<commit_message>
Preparing to fix new issue
</commit_message>
<xml_diff>
--- a/Outputs/net_over_time_avg.xlsx
+++ b/Outputs/net_over_time_avg.xlsx
@@ -162,7 +162,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Net vs time this session (06/15/21): 10-hand moving averages</a:t>
+              <a:t>Net vs time this session (06/21/21): 10-hand moving averages</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -194,7 +194,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$B$2:$B$96</f>
+              <f>'data'!$B$2:$B$284</f>
             </numRef>
           </val>
         </ser>
@@ -221,7 +221,61 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$C$2:$C$96</f>
+              <f>'data'!$C$2:$C$284</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <strRef>
+              <f>'data'!D1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'data'!$D$2:$D$284</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <strRef>
+              <f>'data'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'data'!$E$2:$E$284</f>
             </numRef>
           </val>
         </ser>
@@ -591,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:E284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,10 +661,20 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Scott</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Raymond</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cedric</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Fish</t>
         </is>
@@ -626,16 +690,22 @@
       <c r="C2" t="n">
         <v>0</v>
       </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.15</v>
+        <v>-0.3</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.15</v>
+        <v>0.4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.1</v>
       </c>
     </row>
     <row r="4">
@@ -643,10 +713,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.05</v>
+        <v>-0.9</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05</v>
+        <v>0.53</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.37</v>
       </c>
     </row>
     <row r="5">
@@ -654,10 +727,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-1.15</v>
       </c>
       <c r="C5" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.55</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.6</v>
       </c>
     </row>
     <row r="6">
@@ -665,10 +741,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.15</v>
+        <v>-1.3</v>
       </c>
       <c r="C6" t="n">
-        <v>0.15</v>
+        <v>0.54</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.76</v>
       </c>
     </row>
     <row r="7">
@@ -676,10 +755,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.25</v>
+        <v>-1.38</v>
       </c>
       <c r="C7" t="n">
-        <v>0.25</v>
+        <v>0.53</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.85</v>
       </c>
     </row>
     <row r="8">
@@ -687,10 +769,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.43</v>
+        <v>-1.46</v>
       </c>
       <c r="C8" t="n">
-        <v>0.43</v>
+        <v>0.31</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.14</v>
       </c>
     </row>
     <row r="9">
@@ -698,10 +783,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.57</v>
+        <v>-1.51</v>
       </c>
       <c r="C9" t="n">
-        <v>0.57</v>
+        <v>0.14</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.38</v>
       </c>
     </row>
     <row r="10">
@@ -709,10 +797,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.67</v>
+        <v>-1.44</v>
       </c>
       <c r="C10" t="n">
-        <v>0.67</v>
+        <v>-0.11</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.54</v>
       </c>
     </row>
     <row r="11">
@@ -720,10 +811,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.79</v>
+        <v>-0.82</v>
       </c>
       <c r="C11" t="n">
-        <v>0.79</v>
+        <v>-0.86</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.68</v>
       </c>
     </row>
     <row r="12">
@@ -731,10 +825,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.79</v>
+        <v>-0.82</v>
       </c>
       <c r="C12" t="n">
-        <v>0.79</v>
+        <v>-0.86</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.68</v>
       </c>
     </row>
     <row r="13">
@@ -742,10 +839,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.93</v>
+        <v>-0.35</v>
       </c>
       <c r="C13" t="n">
-        <v>0.93</v>
+        <v>-1.51</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.85</v>
       </c>
     </row>
     <row r="14">
@@ -753,10 +853,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-1.52</v>
+        <v>-0.01</v>
       </c>
       <c r="C14" t="n">
-        <v>1.52</v>
+        <v>-2.23</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.24</v>
       </c>
     </row>
     <row r="15">
@@ -764,10 +867,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-2.01</v>
+        <v>0.46</v>
       </c>
       <c r="C15" t="n">
-        <v>2.01</v>
+        <v>-2.98</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.52</v>
       </c>
     </row>
     <row r="16">
@@ -775,10 +881,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-2.4</v>
+        <v>0.83</v>
       </c>
       <c r="C16" t="n">
-        <v>2.4</v>
+        <v>-3.6</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.77</v>
       </c>
     </row>
     <row r="17">
@@ -786,10 +895,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-2.74</v>
+        <v>1.21</v>
       </c>
       <c r="C17" t="n">
-        <v>2.74</v>
+        <v>-4.21</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3.01</v>
       </c>
     </row>
     <row r="18">
@@ -797,10 +909,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-3.06</v>
+        <v>1.32</v>
       </c>
       <c r="C18" t="n">
-        <v>3.06</v>
+        <v>-4.85</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3.53</v>
       </c>
     </row>
     <row r="19">
@@ -808,10 +923,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-3.33</v>
+        <v>1.44</v>
       </c>
       <c r="C19" t="n">
-        <v>3.33</v>
+        <v>-5.35</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3.9</v>
       </c>
     </row>
     <row r="20">
@@ -819,10 +937,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-3.51</v>
+        <v>2.05</v>
       </c>
       <c r="C20" t="n">
-        <v>3.51</v>
+        <v>-5.83</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3.78</v>
       </c>
     </row>
     <row r="21">
@@ -830,10 +951,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-3.82</v>
+        <v>2.55</v>
       </c>
       <c r="C21" t="n">
-        <v>3.82</v>
+        <v>-6.21</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3.66</v>
       </c>
     </row>
     <row r="22">
@@ -841,10 +965,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-4.04</v>
+        <v>1.9</v>
       </c>
       <c r="C22" t="n">
-        <v>4.04</v>
+        <v>-6.04</v>
+      </c>
+      <c r="D22" t="n">
+        <v>4.14</v>
       </c>
     </row>
     <row r="23">
@@ -852,10 +979,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-4.13</v>
+        <v>1.27</v>
       </c>
       <c r="C23" t="n">
-        <v>4.13</v>
+        <v>-5.99</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4.72</v>
       </c>
     </row>
     <row r="24">
@@ -863,10 +993,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-3.8</v>
+        <v>0.82</v>
       </c>
       <c r="C24" t="n">
-        <v>3.8</v>
+        <v>-5.96</v>
+      </c>
+      <c r="D24" t="n">
+        <v>5.14</v>
       </c>
     </row>
     <row r="25">
@@ -874,10 +1007,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-3.5</v>
+        <v>0.38</v>
       </c>
       <c r="C25" t="n">
-        <v>3.5</v>
+        <v>-5.89</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5.51</v>
       </c>
     </row>
     <row r="26">
@@ -885,10 +1021,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-3.53</v>
+        <v>-0.06</v>
       </c>
       <c r="C26" t="n">
-        <v>3.53</v>
+        <v>-5.92</v>
+      </c>
+      <c r="D26" t="n">
+        <v>5.98</v>
       </c>
     </row>
     <row r="27">
@@ -896,10 +1035,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-3.6</v>
+        <v>-0.52</v>
       </c>
       <c r="C27" t="n">
-        <v>3.6</v>
+        <v>-5.97</v>
+      </c>
+      <c r="D27" t="n">
+        <v>6.49</v>
       </c>
     </row>
     <row r="28">
@@ -907,10 +1049,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-3.7</v>
+        <v>-0.72</v>
       </c>
       <c r="C28" t="n">
-        <v>3.7</v>
+        <v>-6.01</v>
+      </c>
+      <c r="D28" t="n">
+        <v>6.73</v>
       </c>
     </row>
     <row r="29">
@@ -918,10 +1063,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>-3.71</v>
+        <v>-1.42</v>
       </c>
       <c r="C29" t="n">
-        <v>3.71</v>
+        <v>-6.04</v>
+      </c>
+      <c r="D29" t="n">
+        <v>7.46</v>
       </c>
     </row>
     <row r="30">
@@ -929,10 +1077,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-3.74</v>
+        <v>-2.59</v>
       </c>
       <c r="C30" t="n">
-        <v>3.74</v>
+        <v>-6.09</v>
+      </c>
+      <c r="D30" t="n">
+        <v>8.68</v>
       </c>
     </row>
     <row r="31">
@@ -940,10 +1091,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-3.63</v>
+        <v>-3.72</v>
       </c>
       <c r="C31" t="n">
-        <v>3.63</v>
+        <v>-6.16</v>
+      </c>
+      <c r="D31" t="n">
+        <v>9.880000000000001</v>
       </c>
     </row>
     <row r="32">
@@ -951,10 +1105,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-3.73</v>
+        <v>-4.41</v>
       </c>
       <c r="C32" t="n">
-        <v>3.73</v>
+        <v>-6.22</v>
+      </c>
+      <c r="D32" t="n">
+        <v>10.63</v>
       </c>
     </row>
     <row r="33">
@@ -962,10 +1119,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-4.1</v>
+        <v>-5.11</v>
       </c>
       <c r="C33" t="n">
-        <v>4.1</v>
+        <v>-6.2</v>
+      </c>
+      <c r="D33" t="n">
+        <v>11.32</v>
       </c>
     </row>
     <row r="34">
@@ -973,10 +1133,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-4.55</v>
+        <v>-5.79</v>
       </c>
       <c r="C34" t="n">
-        <v>4.55</v>
+        <v>-6.14</v>
+      </c>
+      <c r="D34" t="n">
+        <v>11.95</v>
       </c>
     </row>
     <row r="35">
@@ -984,10 +1147,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-5.04</v>
+        <v>-6.37</v>
       </c>
       <c r="C35" t="n">
-        <v>5.04</v>
+        <v>-6.1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>12.5</v>
       </c>
     </row>
     <row r="36">
@@ -995,10 +1161,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-5.64</v>
+        <v>-4.62</v>
       </c>
       <c r="C36" t="n">
-        <v>5.64</v>
+        <v>-6.21</v>
+      </c>
+      <c r="D36" t="n">
+        <v>10.87</v>
       </c>
     </row>
     <row r="37">
@@ -1006,10 +1175,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-6.21</v>
+        <v>-2.83</v>
       </c>
       <c r="C37" t="n">
-        <v>6.21</v>
+        <v>-6.31</v>
+      </c>
+      <c r="D37" t="n">
+        <v>9.19</v>
       </c>
     </row>
     <row r="38">
@@ -1017,10 +1189,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-6.71</v>
+        <v>-1.03</v>
       </c>
       <c r="C38" t="n">
-        <v>6.71</v>
+        <v>-6.4</v>
+      </c>
+      <c r="D38" t="n">
+        <v>7.49</v>
       </c>
     </row>
     <row r="39">
@@ -1028,10 +1203,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-7.35</v>
+        <v>1.26</v>
       </c>
       <c r="C39" t="n">
-        <v>7.35</v>
+        <v>-6.48</v>
+      </c>
+      <c r="D39" t="n">
+        <v>5.29</v>
       </c>
     </row>
     <row r="40">
@@ -1039,10 +1217,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-8.130000000000001</v>
+        <v>3.33</v>
       </c>
       <c r="C40" t="n">
-        <v>8.130000000000001</v>
+        <v>-6.74</v>
+      </c>
+      <c r="D40" t="n">
+        <v>3.49</v>
       </c>
     </row>
     <row r="41">
@@ -1050,10 +1231,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-8.869999999999999</v>
+        <v>5.38</v>
       </c>
       <c r="C41" t="n">
-        <v>8.869999999999999</v>
+        <v>-6.99</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1.7</v>
       </c>
     </row>
     <row r="42">
@@ -1061,10 +1245,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-8.550000000000001</v>
+        <v>7.59</v>
       </c>
       <c r="C42" t="n">
-        <v>8.550000000000001</v>
+        <v>-7.26</v>
+      </c>
+      <c r="D42" t="n">
+        <v>-0.23</v>
       </c>
     </row>
     <row r="43">
@@ -1072,10 +1259,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>-8.17</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="C43" t="n">
-        <v>8.17</v>
+        <v>-7.59</v>
+      </c>
+      <c r="D43" t="n">
+        <v>-2.11</v>
       </c>
     </row>
     <row r="44">
@@ -1083,10 +1273,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-7.71</v>
+        <v>11.94</v>
       </c>
       <c r="C44" t="n">
-        <v>7.71</v>
+        <v>-7.8</v>
+      </c>
+      <c r="D44" t="n">
+        <v>-4.04</v>
       </c>
     </row>
     <row r="45">
@@ -1094,10 +1287,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>-7.37</v>
+        <v>13.97</v>
       </c>
       <c r="C45" t="n">
-        <v>7.37</v>
+        <v>-8</v>
+      </c>
+      <c r="D45" t="n">
+        <v>-5.87</v>
       </c>
     </row>
     <row r="46">
@@ -1105,10 +1301,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-6.73</v>
+        <v>13.78</v>
       </c>
       <c r="C46" t="n">
-        <v>6.73</v>
+        <v>-8.06</v>
+      </c>
+      <c r="D46" t="n">
+        <v>-5.62</v>
       </c>
     </row>
     <row r="47">
@@ -1116,10 +1315,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>-6.09</v>
+        <v>13.57</v>
       </c>
       <c r="C47" t="n">
-        <v>6.09</v>
+        <v>-8.109999999999999</v>
+      </c>
+      <c r="D47" t="n">
+        <v>-5.36</v>
       </c>
     </row>
     <row r="48">
@@ -1127,10 +1329,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-5.49</v>
+        <v>13.34</v>
       </c>
       <c r="C48" t="n">
-        <v>5.49</v>
+        <v>-8.15</v>
+      </c>
+      <c r="D48" t="n">
+        <v>-5.09</v>
       </c>
     </row>
     <row r="49">
@@ -1138,10 +1343,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-4.81</v>
+        <v>13.12</v>
       </c>
       <c r="C49" t="n">
-        <v>4.81</v>
+        <v>-8.26</v>
+      </c>
+      <c r="D49" t="n">
+        <v>-4.76</v>
       </c>
     </row>
     <row r="50">
@@ -1149,10 +1357,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-4.04</v>
+        <v>13.2</v>
       </c>
       <c r="C50" t="n">
-        <v>4.04</v>
+        <v>-8.17</v>
+      </c>
+      <c r="D50" t="n">
+        <v>-4.93</v>
       </c>
     </row>
     <row r="51">
@@ -1160,10 +1371,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-3.64</v>
+        <v>13.26</v>
       </c>
       <c r="C51" t="n">
-        <v>3.64</v>
+        <v>-8.07</v>
+      </c>
+      <c r="D51" t="n">
+        <v>-5.09</v>
       </c>
     </row>
     <row r="52">
@@ -1171,10 +1385,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-4.18</v>
+        <v>13.3</v>
       </c>
       <c r="C52" t="n">
-        <v>4.18</v>
+        <v>-8.07</v>
+      </c>
+      <c r="D52" t="n">
+        <v>-5.13</v>
       </c>
     </row>
     <row r="53">
@@ -1182,10 +1399,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-4.58</v>
+        <v>13.14</v>
       </c>
       <c r="C53" t="n">
-        <v>4.58</v>
+        <v>-8.09</v>
+      </c>
+      <c r="D53" t="n">
+        <v>-4.95</v>
       </c>
     </row>
     <row r="54">
@@ -1193,10 +1413,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-4.83</v>
+        <v>13.05</v>
       </c>
       <c r="C54" t="n">
-        <v>4.83</v>
+        <v>-8.199999999999999</v>
+      </c>
+      <c r="D54" t="n">
+        <v>-4.74</v>
       </c>
     </row>
     <row r="55">
@@ -1204,10 +1427,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>-4.91</v>
+        <v>12.97</v>
       </c>
       <c r="C55" t="n">
-        <v>4.91</v>
+        <v>-8.32</v>
+      </c>
+      <c r="D55" t="n">
+        <v>-4.53</v>
       </c>
     </row>
     <row r="56">
@@ -1215,10 +1441,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>-4.98</v>
+        <v>12.86</v>
       </c>
       <c r="C56" t="n">
-        <v>4.98</v>
+        <v>-8.43</v>
+      </c>
+      <c r="D56" t="n">
+        <v>-4.3</v>
       </c>
     </row>
     <row r="57">
@@ -1226,10 +1455,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-4.99</v>
+        <v>12.73</v>
       </c>
       <c r="C57" t="n">
-        <v>4.99</v>
+        <v>-8.59</v>
+      </c>
+      <c r="D57" t="n">
+        <v>-4.01</v>
       </c>
     </row>
     <row r="58">
@@ -1237,10 +1469,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>-4.97</v>
+        <v>12.58</v>
       </c>
       <c r="C58" t="n">
-        <v>4.97</v>
+        <v>-8.74</v>
+      </c>
+      <c r="D58" t="n">
+        <v>-3.71</v>
       </c>
     </row>
     <row r="59">
@@ -1248,10 +1483,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>-4.97</v>
+        <v>12.43</v>
       </c>
       <c r="C59" t="n">
-        <v>4.97</v>
+        <v>-8.76</v>
+      </c>
+      <c r="D59" t="n">
+        <v>-3.54</v>
       </c>
     </row>
     <row r="60">
@@ -1259,10 +1497,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>-5.04</v>
+        <v>12.2</v>
       </c>
       <c r="C60" t="n">
-        <v>5.04</v>
+        <v>-8.789999999999999</v>
+      </c>
+      <c r="D60" t="n">
+        <v>-3.28</v>
       </c>
     </row>
     <row r="61">
@@ -1270,10 +1511,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>-4.91</v>
+        <v>11.97</v>
       </c>
       <c r="C61" t="n">
-        <v>4.91</v>
+        <v>-8.81</v>
+      </c>
+      <c r="D61" t="n">
+        <v>-3.03</v>
       </c>
     </row>
     <row r="62">
@@ -1281,10 +1525,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>-4.77</v>
+        <v>11.74</v>
       </c>
       <c r="C62" t="n">
-        <v>4.77</v>
+        <v>-8.65</v>
+      </c>
+      <c r="D62" t="n">
+        <v>-2.96</v>
       </c>
     </row>
     <row r="63">
@@ -1292,10 +1539,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>-4.71</v>
+        <v>11.81</v>
       </c>
       <c r="C63" t="n">
-        <v>4.71</v>
+        <v>-8.5</v>
+      </c>
+      <c r="D63" t="n">
+        <v>-3.18</v>
       </c>
     </row>
     <row r="64">
@@ -1303,10 +1553,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>-4.85</v>
+        <v>10.82</v>
       </c>
       <c r="C64" t="n">
-        <v>4.85</v>
+        <v>-8.48</v>
+      </c>
+      <c r="D64" t="n">
+        <v>-2.22</v>
       </c>
     </row>
     <row r="65">
@@ -1314,10 +1567,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>-5.01</v>
+        <v>9.539999999999999</v>
       </c>
       <c r="C65" t="n">
-        <v>5.01</v>
+        <v>-8.470000000000001</v>
+      </c>
+      <c r="D65" t="n">
+        <v>-0.96</v>
       </c>
     </row>
     <row r="66">
@@ -1325,10 +1581,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>-5.13</v>
+        <v>8.27</v>
       </c>
       <c r="C66" t="n">
-        <v>5.13</v>
+        <v>-8.470000000000001</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="67">
@@ -1336,10 +1595,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>-5.34</v>
+        <v>6.99</v>
       </c>
       <c r="C67" t="n">
-        <v>5.34</v>
+        <v>-8.390000000000001</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1.5</v>
       </c>
     </row>
     <row r="68">
@@ -1347,10 +1609,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-5.54</v>
+        <v>5.74</v>
       </c>
       <c r="C68" t="n">
-        <v>5.54</v>
+        <v>-8.279999999999999</v>
+      </c>
+      <c r="D68" t="n">
+        <v>2.64</v>
       </c>
     </row>
     <row r="69">
@@ -1358,10 +1623,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>-5.73</v>
+        <v>4.43</v>
       </c>
       <c r="C69" t="n">
-        <v>5.73</v>
+        <v>-8.119999999999999</v>
+      </c>
+      <c r="D69" t="n">
+        <v>3.78</v>
       </c>
     </row>
     <row r="70">
@@ -1369,10 +1637,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>-5.84</v>
+        <v>3.13</v>
       </c>
       <c r="C70" t="n">
-        <v>5.84</v>
+        <v>-7.97</v>
+      </c>
+      <c r="D70" t="n">
+        <v>4.95</v>
       </c>
     </row>
     <row r="71">
@@ -1380,10 +1651,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-5.83</v>
+        <v>1.86</v>
       </c>
       <c r="C71" t="n">
-        <v>5.83</v>
+        <v>-7.85</v>
+      </c>
+      <c r="D71" t="n">
+        <v>6.09</v>
       </c>
     </row>
     <row r="72">
@@ -1391,10 +1665,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>-5.82</v>
+        <v>0.57</v>
       </c>
       <c r="C72" t="n">
-        <v>5.82</v>
+        <v>-7.78</v>
+      </c>
+      <c r="D72" t="n">
+        <v>7.31</v>
       </c>
     </row>
     <row r="73">
@@ -1402,10 +1679,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>-5.81</v>
+        <v>-1.06</v>
       </c>
       <c r="C73" t="n">
-        <v>5.81</v>
+        <v>-7.74</v>
+      </c>
+      <c r="D73" t="n">
+        <v>8.890000000000001</v>
       </c>
     </row>
     <row r="74">
@@ -1413,10 +1693,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>-5.74</v>
+        <v>-1.64</v>
       </c>
       <c r="C74" t="n">
-        <v>5.74</v>
+        <v>-7.58</v>
+      </c>
+      <c r="D74" t="n">
+        <v>9.32</v>
       </c>
     </row>
     <row r="75">
@@ -1424,10 +1707,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-5.65</v>
+        <v>-1.86</v>
       </c>
       <c r="C75" t="n">
-        <v>5.65</v>
+        <v>-7.46</v>
+      </c>
+      <c r="D75" t="n">
+        <v>9.42</v>
       </c>
     </row>
     <row r="76">
@@ -1435,10 +1721,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>-5.68</v>
+        <v>-2.05</v>
       </c>
       <c r="C76" t="n">
-        <v>5.68</v>
+        <v>-7.37</v>
+      </c>
+      <c r="D76" t="n">
+        <v>9.51</v>
       </c>
     </row>
     <row r="77">
@@ -1446,10 +1735,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>-5.66</v>
+        <v>-2.21</v>
       </c>
       <c r="C77" t="n">
-        <v>5.66</v>
+        <v>-7.27</v>
+      </c>
+      <c r="D77" t="n">
+        <v>9.59</v>
       </c>
     </row>
     <row r="78">
@@ -1457,10 +1749,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>-5.7</v>
+        <v>-2.37</v>
       </c>
       <c r="C78" t="n">
-        <v>5.7</v>
+        <v>-7.24</v>
+      </c>
+      <c r="D78" t="n">
+        <v>9.710000000000001</v>
       </c>
     </row>
     <row r="79">
@@ -1468,10 +1763,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>-5.74</v>
+        <v>-2.48</v>
       </c>
       <c r="C79" t="n">
-        <v>5.74</v>
+        <v>-7.31</v>
+      </c>
+      <c r="D79" t="n">
+        <v>9.890000000000001</v>
       </c>
     </row>
     <row r="80">
@@ -1479,10 +1777,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>-5.87</v>
+        <v>-2.61</v>
       </c>
       <c r="C80" t="n">
-        <v>5.87</v>
+        <v>-7.34</v>
+      </c>
+      <c r="D80" t="n">
+        <v>10.05</v>
       </c>
     </row>
     <row r="81">
@@ -1490,10 +1791,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>-6.02</v>
+        <v>-2.79</v>
       </c>
       <c r="C81" t="n">
-        <v>6.02</v>
+        <v>-7.36</v>
+      </c>
+      <c r="D81" t="n">
+        <v>10.25</v>
       </c>
     </row>
     <row r="82">
@@ -1501,10 +1805,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>-6.2</v>
+        <v>-2.87</v>
       </c>
       <c r="C82" t="n">
-        <v>6.2</v>
+        <v>-7.4</v>
+      </c>
+      <c r="D82" t="n">
+        <v>10.37</v>
       </c>
     </row>
     <row r="83">
@@ -1512,10 +1819,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>-6.37</v>
+        <v>-3.8</v>
       </c>
       <c r="C83" t="n">
-        <v>6.37</v>
+        <v>-6.31</v>
+      </c>
+      <c r="D83" t="n">
+        <v>10.21</v>
       </c>
     </row>
     <row r="84">
@@ -1523,10 +1833,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>-6.75</v>
+        <v>-4.61</v>
       </c>
       <c r="C84" t="n">
-        <v>6.75</v>
+        <v>-5.26</v>
+      </c>
+      <c r="D84" t="n">
+        <v>9.970000000000001</v>
       </c>
     </row>
     <row r="85">
@@ -1534,10 +1847,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>-6.91</v>
+        <v>-5.48</v>
       </c>
       <c r="C85" t="n">
-        <v>6.91</v>
+        <v>-4.16</v>
+      </c>
+      <c r="D85" t="n">
+        <v>9.74</v>
       </c>
     </row>
     <row r="86">
@@ -1545,10 +1861,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>-6.62</v>
+        <v>-6.31</v>
       </c>
       <c r="C86" t="n">
-        <v>6.62</v>
+        <v>-3.1</v>
+      </c>
+      <c r="D86" t="n">
+        <v>9.51</v>
       </c>
     </row>
     <row r="87">
@@ -1556,10 +1875,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>-6.57</v>
+        <v>-7.13</v>
       </c>
       <c r="C87" t="n">
-        <v>6.57</v>
+        <v>-2.06</v>
+      </c>
+      <c r="D87" t="n">
+        <v>9.300000000000001</v>
       </c>
     </row>
     <row r="88">
@@ -1567,10 +1889,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>-6.5</v>
+        <v>-7.98</v>
       </c>
       <c r="C88" t="n">
-        <v>6.5</v>
+        <v>-1</v>
+      </c>
+      <c r="D88" t="n">
+        <v>9.1</v>
       </c>
     </row>
     <row r="89">
@@ -1578,10 +1903,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>-6.43</v>
+        <v>-8.84</v>
       </c>
       <c r="C89" t="n">
-        <v>6.43</v>
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D89" t="n">
+        <v>8.9</v>
       </c>
     </row>
     <row r="90">
@@ -1589,10 +1917,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>-6.69</v>
+        <v>-9.68</v>
       </c>
       <c r="C90" t="n">
-        <v>6.69</v>
+        <v>1.1</v>
+      </c>
+      <c r="D90" t="n">
+        <v>8.720000000000001</v>
       </c>
     </row>
     <row r="91">
@@ -1600,10 +1931,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>-6.97</v>
+        <v>-10.52</v>
       </c>
       <c r="C91" t="n">
-        <v>6.97</v>
+        <v>2.15</v>
+      </c>
+      <c r="D91" t="n">
+        <v>8.52</v>
       </c>
     </row>
     <row r="92">
@@ -1611,10 +1945,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>-7.39</v>
+        <v>-11.34</v>
       </c>
       <c r="C92" t="n">
-        <v>7.39</v>
+        <v>3.12</v>
+      </c>
+      <c r="D92" t="n">
+        <v>8.380000000000001</v>
       </c>
     </row>
     <row r="93">
@@ -1622,10 +1959,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>-7.81</v>
+        <v>-11.05</v>
       </c>
       <c r="C93" t="n">
-        <v>7.81</v>
+        <v>2.96</v>
+      </c>
+      <c r="D93" t="n">
+        <v>8.26</v>
       </c>
     </row>
     <row r="94">
@@ -1633,10 +1973,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>-8.050000000000001</v>
+        <v>-10.85</v>
       </c>
       <c r="C94" t="n">
-        <v>8.050000000000001</v>
+        <v>2.79</v>
+      </c>
+      <c r="D94" t="n">
+        <v>8.24</v>
       </c>
     </row>
     <row r="95">
@@ -1644,10 +1987,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>-8.41</v>
+        <v>-10.65</v>
       </c>
       <c r="C95" t="n">
-        <v>8.41</v>
+        <v>2.62</v>
+      </c>
+      <c r="D95" t="n">
+        <v>8.220000000000001</v>
       </c>
     </row>
     <row r="96">
@@ -1655,10 +2001,2912 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>-8.970000000000001</v>
+        <v>-10.66</v>
       </c>
       <c r="C96" t="n">
-        <v>8.970000000000001</v>
+        <v>2.63</v>
+      </c>
+      <c r="D96" t="n">
+        <v>8.220000000000001</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>-10.69</v>
+      </c>
+      <c r="C97" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="D97" t="n">
+        <v>8.220000000000001</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>-9.99</v>
+      </c>
+      <c r="C98" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="D98" t="n">
+        <v>8.210000000000001</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>-9.23</v>
+      </c>
+      <c r="C99" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="D99" t="n">
+        <v>8.17</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>-8.550000000000001</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="D100" t="n">
+        <v>8.130000000000001</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>-7.83</v>
+      </c>
+      <c r="C101" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="D101" t="n">
+        <v>8.07</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="n">
+        <v>-7.2</v>
+      </c>
+      <c r="C102" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="D102" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="n">
+        <v>-6.59</v>
+      </c>
+      <c r="C103" t="n">
+        <v>-1.13</v>
+      </c>
+      <c r="D103" t="n">
+        <v>7.86</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="n">
+        <v>-5.97</v>
+      </c>
+      <c r="C104" t="n">
+        <v>-1.6</v>
+      </c>
+      <c r="D104" t="n">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="n">
+        <v>-5.42</v>
+      </c>
+      <c r="C105" t="n">
+        <v>-2.06</v>
+      </c>
+      <c r="D105" t="n">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="n">
+        <v>-4.76</v>
+      </c>
+      <c r="C106" t="n">
+        <v>-2.63</v>
+      </c>
+      <c r="D106" t="n">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="n">
+        <v>-4.08</v>
+      </c>
+      <c r="C107" t="n">
+        <v>-3.2</v>
+      </c>
+      <c r="D107" t="n">
+        <v>7.38</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="n">
+        <v>-4.11</v>
+      </c>
+      <c r="C108" t="n">
+        <v>-3.05</v>
+      </c>
+      <c r="D108" t="n">
+        <v>7.26</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="n">
+        <v>-4.15</v>
+      </c>
+      <c r="C109" t="n">
+        <v>-2.92</v>
+      </c>
+      <c r="D109" t="n">
+        <v>7.17</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="n">
+        <v>-4.1</v>
+      </c>
+      <c r="C110" t="n">
+        <v>-2.86</v>
+      </c>
+      <c r="D110" t="n">
+        <v>7.06</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="n">
+        <v>-4.28</v>
+      </c>
+      <c r="C111" t="n">
+        <v>-2.79</v>
+      </c>
+      <c r="D111" t="n">
+        <v>7.17</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="n">
+        <v>-4.39</v>
+      </c>
+      <c r="C112" t="n">
+        <v>-2.74</v>
+      </c>
+      <c r="D112" t="n">
+        <v>7.23</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="n">
+        <v>-4.49</v>
+      </c>
+      <c r="C113" t="n">
+        <v>-3.22</v>
+      </c>
+      <c r="D113" t="n">
+        <v>7.81</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="n">
+        <v>-4.8</v>
+      </c>
+      <c r="C114" t="n">
+        <v>-3.5</v>
+      </c>
+      <c r="D114" t="n">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="n">
+        <v>-5.17</v>
+      </c>
+      <c r="C115" t="n">
+        <v>-3.66</v>
+      </c>
+      <c r="D115" t="n">
+        <v>8.93</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="n">
+        <v>-5.54</v>
+      </c>
+      <c r="C116" t="n">
+        <v>-3.8</v>
+      </c>
+      <c r="D116" t="n">
+        <v>9.44</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="n">
+        <v>-5.92</v>
+      </c>
+      <c r="C117" t="n">
+        <v>-3.94</v>
+      </c>
+      <c r="D117" t="n">
+        <v>9.960000000000001</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="n">
+        <v>-6.32</v>
+      </c>
+      <c r="C118" t="n">
+        <v>-4.07</v>
+      </c>
+      <c r="D118" t="n">
+        <v>10.49</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="n">
+        <v>-6.82</v>
+      </c>
+      <c r="C119" t="n">
+        <v>-4.08</v>
+      </c>
+      <c r="D119" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="n">
+        <v>-7.41</v>
+      </c>
+      <c r="C120" t="n">
+        <v>-4.01</v>
+      </c>
+      <c r="D120" t="n">
+        <v>11.52</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="n">
+        <v>-9.69</v>
+      </c>
+      <c r="C121" t="n">
+        <v>-1.97</v>
+      </c>
+      <c r="D121" t="n">
+        <v>11.76</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="n">
+        <v>-12.05</v>
+      </c>
+      <c r="C122" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D122" t="n">
+        <v>12.07</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" t="n">
+        <v>-14.41</v>
+      </c>
+      <c r="C123" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="D123" t="n">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="n">
+        <v>-16.58</v>
+      </c>
+      <c r="C124" t="n">
+        <v>5.15</v>
+      </c>
+      <c r="D124" t="n">
+        <v>11.53</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="n">
+        <v>-18.64</v>
+      </c>
+      <c r="C125" t="n">
+        <v>7.49</v>
+      </c>
+      <c r="D125" t="n">
+        <v>11.24</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="n">
+        <v>-20.69</v>
+      </c>
+      <c r="C126" t="n">
+        <v>9.710000000000001</v>
+      </c>
+      <c r="D126" t="n">
+        <v>11.08</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" t="n">
+        <v>-22.73</v>
+      </c>
+      <c r="C127" t="n">
+        <v>11.86</v>
+      </c>
+      <c r="D127" t="n">
+        <v>10.96</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" t="n">
+        <v>-24.64</v>
+      </c>
+      <c r="C128" t="n">
+        <v>13.95</v>
+      </c>
+      <c r="D128" t="n">
+        <v>10.79</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" t="n">
+        <v>-26.48</v>
+      </c>
+      <c r="C129" t="n">
+        <v>15.94</v>
+      </c>
+      <c r="D129" t="n">
+        <v>10.64</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" t="n">
+        <v>-28.33</v>
+      </c>
+      <c r="C130" t="n">
+        <v>17.93</v>
+      </c>
+      <c r="D130" t="n">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" t="n">
+        <v>-28.58</v>
+      </c>
+      <c r="C131" t="n">
+        <v>18.25</v>
+      </c>
+      <c r="D131" t="n">
+        <v>10.44</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" t="n">
+        <v>-28.85</v>
+      </c>
+      <c r="C132" t="n">
+        <v>18.59</v>
+      </c>
+      <c r="D132" t="n">
+        <v>10.36</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" t="n">
+        <v>-29.11</v>
+      </c>
+      <c r="C133" t="n">
+        <v>18.79</v>
+      </c>
+      <c r="D133" t="n">
+        <v>10.42</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" t="n">
+        <v>-29.6</v>
+      </c>
+      <c r="C134" t="n">
+        <v>19.21</v>
+      </c>
+      <c r="D134" t="n">
+        <v>10.49</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" t="n">
+        <v>-30.12</v>
+      </c>
+      <c r="C135" t="n">
+        <v>19.64</v>
+      </c>
+      <c r="D135" t="n">
+        <v>10.57</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" t="n">
+        <v>-30.64</v>
+      </c>
+      <c r="C136" t="n">
+        <v>20.19</v>
+      </c>
+      <c r="D136" t="n">
+        <v>10.56</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" t="n">
+        <v>-31.16</v>
+      </c>
+      <c r="C137" t="n">
+        <v>20.76</v>
+      </c>
+      <c r="D137" t="n">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" t="n">
+        <v>-31.77</v>
+      </c>
+      <c r="C138" t="n">
+        <v>21.37</v>
+      </c>
+      <c r="D138" t="n">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" t="n">
+        <v>-32.49</v>
+      </c>
+      <c r="C139" t="n">
+        <v>22.09</v>
+      </c>
+      <c r="D139" t="n">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" t="n">
+        <v>-33.11</v>
+      </c>
+      <c r="C140" t="n">
+        <v>22.74</v>
+      </c>
+      <c r="D140" t="n">
+        <v>10.47</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="n">
+        <v>-33.61</v>
+      </c>
+      <c r="C141" t="n">
+        <v>23.09</v>
+      </c>
+      <c r="D141" t="n">
+        <v>10.62</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="n">
+        <v>-34.08</v>
+      </c>
+      <c r="C142" t="n">
+        <v>23.41</v>
+      </c>
+      <c r="D142" t="n">
+        <v>10.77</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" t="n">
+        <v>-34.56</v>
+      </c>
+      <c r="C143" t="n">
+        <v>23.76</v>
+      </c>
+      <c r="D143" t="n">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" t="n">
+        <v>-35.05</v>
+      </c>
+      <c r="C144" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="D144" t="n">
+        <v>11.35</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" t="n">
+        <v>-35.5</v>
+      </c>
+      <c r="C145" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="D145" t="n">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" t="n">
+        <v>-35.91</v>
+      </c>
+      <c r="C146" t="n">
+        <v>23.78</v>
+      </c>
+      <c r="D146" t="n">
+        <v>12.23</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B147" t="n">
+        <v>-36.29</v>
+      </c>
+      <c r="C147" t="n">
+        <v>23.77</v>
+      </c>
+      <c r="D147" t="n">
+        <v>12.62</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B148" t="n">
+        <v>-36.7</v>
+      </c>
+      <c r="C148" t="n">
+        <v>23.79</v>
+      </c>
+      <c r="D148" t="n">
+        <v>13.01</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B149" t="n">
+        <v>-36.99</v>
+      </c>
+      <c r="C149" t="n">
+        <v>23.71</v>
+      </c>
+      <c r="D149" t="n">
+        <v>13.38</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B150" t="n">
+        <v>-37.24</v>
+      </c>
+      <c r="C150" t="n">
+        <v>23.64</v>
+      </c>
+      <c r="D150" t="n">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B151" t="n">
+        <v>-37.88</v>
+      </c>
+      <c r="C151" t="n">
+        <v>23.55</v>
+      </c>
+      <c r="D151" t="n">
+        <v>14.43</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B152" t="n">
+        <v>-38.55</v>
+      </c>
+      <c r="C152" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="D152" t="n">
+        <v>15.15</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B153" t="n">
+        <v>-39.15</v>
+      </c>
+      <c r="C153" t="n">
+        <v>23.37</v>
+      </c>
+      <c r="D153" t="n">
+        <v>15.88</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B154" t="n">
+        <v>-39.38</v>
+      </c>
+      <c r="C154" t="n">
+        <v>23.26</v>
+      </c>
+      <c r="D154" t="n">
+        <v>16.22</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B155" t="n">
+        <v>-39.62</v>
+      </c>
+      <c r="C155" t="n">
+        <v>23.18</v>
+      </c>
+      <c r="D155" t="n">
+        <v>16.55</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B156" t="n">
+        <v>-39.9</v>
+      </c>
+      <c r="C156" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="D156" t="n">
+        <v>16.9</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B157" t="n">
+        <v>-40.22</v>
+      </c>
+      <c r="C157" t="n">
+        <v>23.04</v>
+      </c>
+      <c r="D157" t="n">
+        <v>17.29</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B158" t="n">
+        <v>-40.53</v>
+      </c>
+      <c r="C158" t="n">
+        <v>22.9</v>
+      </c>
+      <c r="D158" t="n">
+        <v>17.73</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B159" t="n">
+        <v>-40.84</v>
+      </c>
+      <c r="C159" t="n">
+        <v>22.76</v>
+      </c>
+      <c r="D159" t="n">
+        <v>18.18</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="n">
+        <v>-40.18</v>
+      </c>
+      <c r="C160" t="n">
+        <v>21.59</v>
+      </c>
+      <c r="D160" t="n">
+        <v>18.69</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B161" t="n">
+        <v>-38.96</v>
+      </c>
+      <c r="C161" t="n">
+        <v>20.45</v>
+      </c>
+      <c r="D161" t="n">
+        <v>18.61</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B162" t="n">
+        <v>-37.73</v>
+      </c>
+      <c r="C162" t="n">
+        <v>19.27</v>
+      </c>
+      <c r="D162" t="n">
+        <v>18.56</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B163" t="n">
+        <v>-36.59</v>
+      </c>
+      <c r="C163" t="n">
+        <v>18.18</v>
+      </c>
+      <c r="D163" t="n">
+        <v>18.51</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B164" t="n">
+        <v>-34.49</v>
+      </c>
+      <c r="C164" t="n">
+        <v>16.09</v>
+      </c>
+      <c r="D164" t="n">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B165" t="n">
+        <v>-32.38</v>
+      </c>
+      <c r="C165" t="n">
+        <v>13.96</v>
+      </c>
+      <c r="D165" t="n">
+        <v>18.52</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B166" t="n">
+        <v>-30.26</v>
+      </c>
+      <c r="C166" t="n">
+        <v>11.85</v>
+      </c>
+      <c r="D166" t="n">
+        <v>18.51</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B167" t="n">
+        <v>-28.01</v>
+      </c>
+      <c r="C167" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="D167" t="n">
+        <v>18.51</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B168" t="n">
+        <v>-25.77</v>
+      </c>
+      <c r="C168" t="n">
+        <v>7.41</v>
+      </c>
+      <c r="D168" t="n">
+        <v>18.46</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B169" t="n">
+        <v>-23.41</v>
+      </c>
+      <c r="C169" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="D169" t="n">
+        <v>18.37</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B170" t="n">
+        <v>-22.11</v>
+      </c>
+      <c r="C170" t="n">
+        <v>3.94</v>
+      </c>
+      <c r="D170" t="n">
+        <v>18.28</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B171" t="n">
+        <v>-20.82</v>
+      </c>
+      <c r="C171" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="D171" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B172" t="n">
+        <v>-19.51</v>
+      </c>
+      <c r="C172" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="D172" t="n">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" t="n">
+        <v>-18.16</v>
+      </c>
+      <c r="C173" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="D173" t="n">
+        <v>17.41</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" t="n">
+        <v>-17.9</v>
+      </c>
+      <c r="C174" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="D174" t="n">
+        <v>17.16</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" t="n">
+        <v>-17.65</v>
+      </c>
+      <c r="C175" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D175" t="n">
+        <v>16.9</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="n">
+        <v>-17.49</v>
+      </c>
+      <c r="C176" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="D176" t="n">
+        <v>16.64</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="n">
+        <v>-17.44</v>
+      </c>
+      <c r="C177" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="D177" t="n">
+        <v>16.33</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="n">
+        <v>-17.29</v>
+      </c>
+      <c r="C178" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="D178" t="n">
+        <v>15.94</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="n">
+        <v>-17.31</v>
+      </c>
+      <c r="C179" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="D179" t="n">
+        <v>15.84</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="n">
+        <v>-17.31</v>
+      </c>
+      <c r="C180" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="D180" t="n">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="n">
+        <v>-17.43</v>
+      </c>
+      <c r="C181" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="D181" t="n">
+        <v>15.94</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" t="n">
+        <v>-17.54</v>
+      </c>
+      <c r="C182" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="D182" t="n">
+        <v>16.15</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" t="n">
+        <v>-17.17</v>
+      </c>
+      <c r="C183" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="D183" t="n">
+        <v>16.06</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" t="n">
+        <v>-16.79</v>
+      </c>
+      <c r="C184" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="D184" t="n">
+        <v>15.95</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" t="n">
+        <v>-16.37</v>
+      </c>
+      <c r="C185" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="D185" t="n">
+        <v>15.83</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" t="n">
+        <v>-15.89</v>
+      </c>
+      <c r="C186" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D186" t="n">
+        <v>15.74</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="n">
+        <v>-15.56</v>
+      </c>
+      <c r="C187" t="n">
+        <v>0</v>
+      </c>
+      <c r="D187" t="n">
+        <v>15.66</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="n">
+        <v>-15.65</v>
+      </c>
+      <c r="C188" t="n">
+        <v>-0.21</v>
+      </c>
+      <c r="D188" t="n">
+        <v>15.96</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="n">
+        <v>-15.57</v>
+      </c>
+      <c r="C189" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="D189" t="n">
+        <v>15.94</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" t="n">
+        <v>-15.5</v>
+      </c>
+      <c r="C190" t="n">
+        <v>-0.32</v>
+      </c>
+      <c r="D190" t="n">
+        <v>15.93</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" t="n">
+        <v>-15.3</v>
+      </c>
+      <c r="C191" t="n">
+        <v>-0.39</v>
+      </c>
+      <c r="D191" t="n">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" t="n">
+        <v>-15.12</v>
+      </c>
+      <c r="C192" t="n">
+        <v>-0.46</v>
+      </c>
+      <c r="D192" t="n">
+        <v>15.67</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" t="n">
+        <v>-15.06</v>
+      </c>
+      <c r="C193" t="n">
+        <v>-0.32</v>
+      </c>
+      <c r="D193" t="n">
+        <v>15.48</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" t="n">
+        <v>-15.03</v>
+      </c>
+      <c r="C194" t="n">
+        <v>-0.17</v>
+      </c>
+      <c r="D194" t="n">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" t="n">
+        <v>-15.02</v>
+      </c>
+      <c r="C195" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="D195" t="n">
+        <v>15.13</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" t="n">
+        <v>-15.06</v>
+      </c>
+      <c r="C196" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D196" t="n">
+        <v>15.06</v>
+      </c>
+      <c r="E196" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" t="n">
+        <v>-14.94</v>
+      </c>
+      <c r="C197" t="n">
+        <v>0</v>
+      </c>
+      <c r="D197" t="n">
+        <v>15.05</v>
+      </c>
+      <c r="E197" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="n">
+        <v>-14.51</v>
+      </c>
+      <c r="C198" t="n">
+        <v>-0.11</v>
+      </c>
+      <c r="D198" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="E198" t="n">
+        <v>-0.75</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="n">
+        <v>-14.19</v>
+      </c>
+      <c r="C199" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="D199" t="n">
+        <v>14.41</v>
+      </c>
+      <c r="E199" t="n">
+        <v>-1.175</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="n">
+        <v>-13.87</v>
+      </c>
+      <c r="C200" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="D200" t="n">
+        <v>14.14</v>
+      </c>
+      <c r="E200" t="n">
+        <v>-1.43</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" t="n">
+        <v>-13.58</v>
+      </c>
+      <c r="C201" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="D201" t="n">
+        <v>13.91</v>
+      </c>
+      <c r="E201" t="n">
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" t="n">
+        <v>-13.27</v>
+      </c>
+      <c r="C202" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="D202" t="n">
+        <v>13.66</v>
+      </c>
+      <c r="E202" t="n">
+        <v>-1.835714285714286</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" t="n">
+        <v>-13.41</v>
+      </c>
+      <c r="C203" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="D203" t="n">
+        <v>13.93</v>
+      </c>
+      <c r="E203" t="n">
+        <v>-2.08375</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" t="n">
+        <v>-13.59</v>
+      </c>
+      <c r="C204" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="D204" t="n">
+        <v>14.15</v>
+      </c>
+      <c r="E204" t="n">
+        <v>-2.298888888888889</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" t="n">
+        <v>-13.63</v>
+      </c>
+      <c r="C205" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="D205" t="n">
+        <v>14.26</v>
+      </c>
+      <c r="E205" t="n">
+        <v>-2.471</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B206" t="n">
+        <v>-13.64</v>
+      </c>
+      <c r="C206" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="D206" t="n">
+        <v>14.23</v>
+      </c>
+      <c r="E206" t="n">
+        <v>-2.471</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" t="n">
+        <v>-13.67</v>
+      </c>
+      <c r="C207" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="D207" t="n">
+        <v>14.32</v>
+      </c>
+      <c r="E207" t="n">
+        <v>-2.93</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="n">
+        <v>-13.71</v>
+      </c>
+      <c r="C208" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="D208" t="n">
+        <v>14.42</v>
+      </c>
+      <c r="E208" t="n">
+        <v>-3.409</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="n">
+        <v>-13.77</v>
+      </c>
+      <c r="C209" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="D209" t="n">
+        <v>14.54</v>
+      </c>
+      <c r="E209" t="n">
+        <v>-3.553</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="n">
+        <v>-13.78</v>
+      </c>
+      <c r="C210" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="D210" t="n">
+        <v>14.64</v>
+      </c>
+      <c r="E210" t="n">
+        <v>-3.717</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="n">
+        <v>-13.77</v>
+      </c>
+      <c r="C211" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="D211" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="E211" t="n">
+        <v>-3.901</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="n">
+        <v>-13.85</v>
+      </c>
+      <c r="C212" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="D212" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="E212" t="n">
+        <v>-2.374</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="n">
+        <v>-13.88</v>
+      </c>
+      <c r="C213" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="D213" t="n">
+        <v>14.72</v>
+      </c>
+      <c r="E213" t="n">
+        <v>-0.9329999999999996</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="n">
+        <v>-13.46</v>
+      </c>
+      <c r="C214" t="n">
+        <v>-1.45</v>
+      </c>
+      <c r="D214" t="n">
+        <v>14.56</v>
+      </c>
+      <c r="E214" t="n">
+        <v>0.445</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="n">
+        <v>-13.18</v>
+      </c>
+      <c r="C215" t="n">
+        <v>-3.07</v>
+      </c>
+      <c r="D215" t="n">
+        <v>14.58</v>
+      </c>
+      <c r="E215" t="n">
+        <v>1.763</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="n">
+        <v>-12.71</v>
+      </c>
+      <c r="C216" t="n">
+        <v>-4.78</v>
+      </c>
+      <c r="D216" t="n">
+        <v>14.57</v>
+      </c>
+      <c r="E216" t="n">
+        <v>3.024</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="n">
+        <v>-12.39</v>
+      </c>
+      <c r="C217" t="n">
+        <v>-6.29</v>
+      </c>
+      <c r="D217" t="n">
+        <v>14.44</v>
+      </c>
+      <c r="E217" t="n">
+        <v>4.341999999999999</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="n">
+        <v>-11.78</v>
+      </c>
+      <c r="C218" t="n">
+        <v>-7.81</v>
+      </c>
+      <c r="D218" t="n">
+        <v>14.06</v>
+      </c>
+      <c r="E218" t="n">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="n">
+        <v>-11.21</v>
+      </c>
+      <c r="C219" t="n">
+        <v>-9.31</v>
+      </c>
+      <c r="D219" t="n">
+        <v>13.27</v>
+      </c>
+      <c r="E219" t="n">
+        <v>7.348000000000001</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="n">
+        <v>-10.76</v>
+      </c>
+      <c r="C220" t="n">
+        <v>-10.79</v>
+      </c>
+      <c r="D220" t="n">
+        <v>12.66</v>
+      </c>
+      <c r="E220" t="n">
+        <v>8.995999999999999</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="n">
+        <v>-10.32</v>
+      </c>
+      <c r="C221" t="n">
+        <v>-12.38</v>
+      </c>
+      <c r="D221" t="n">
+        <v>12.05</v>
+      </c>
+      <c r="E221" t="n">
+        <v>10.744</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="n">
+        <v>-9.73</v>
+      </c>
+      <c r="C222" t="n">
+        <v>-12.41</v>
+      </c>
+      <c r="D222" t="n">
+        <v>11.52</v>
+      </c>
+      <c r="E222" t="n">
+        <v>10.721</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="n">
+        <v>-9.19</v>
+      </c>
+      <c r="C223" t="n">
+        <v>-12.3</v>
+      </c>
+      <c r="D223" t="n">
+        <v>10.78</v>
+      </c>
+      <c r="E223" t="n">
+        <v>10.807</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="n">
+        <v>-9.01</v>
+      </c>
+      <c r="C224" t="n">
+        <v>-12.2</v>
+      </c>
+      <c r="D224" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="E224" t="n">
+        <v>11.013</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="n">
+        <v>-8.91</v>
+      </c>
+      <c r="C225" t="n">
+        <v>-12.12</v>
+      </c>
+      <c r="D225" t="n">
+        <v>10.04</v>
+      </c>
+      <c r="E225" t="n">
+        <v>11.089</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="n">
+        <v>-8.99</v>
+      </c>
+      <c r="C226" t="n">
+        <v>-11.97</v>
+      </c>
+      <c r="D226" t="n">
+        <v>9.83</v>
+      </c>
+      <c r="E226" t="n">
+        <v>11.232</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="n">
+        <v>-8.93</v>
+      </c>
+      <c r="C227" t="n">
+        <v>-11.98</v>
+      </c>
+      <c r="D227" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="E227" t="n">
+        <v>11.415</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="n">
+        <v>-9.17</v>
+      </c>
+      <c r="C228" t="n">
+        <v>-11.96</v>
+      </c>
+      <c r="D228" t="n">
+        <v>9.609999999999999</v>
+      </c>
+      <c r="E228" t="n">
+        <v>11.618</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="n">
+        <v>-9.35</v>
+      </c>
+      <c r="C229" t="n">
+        <v>-11.94</v>
+      </c>
+      <c r="D229" t="n">
+        <v>10.02</v>
+      </c>
+      <c r="E229" t="n">
+        <v>11.371</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="n">
+        <v>-9.449999999999999</v>
+      </c>
+      <c r="C230" t="n">
+        <v>-11.84</v>
+      </c>
+      <c r="D230" t="n">
+        <v>10.26</v>
+      </c>
+      <c r="E230" t="n">
+        <v>11.127</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="n">
+        <v>-9.550000000000001</v>
+      </c>
+      <c r="C231" t="n">
+        <v>-11.64</v>
+      </c>
+      <c r="D231" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E231" t="n">
+        <v>10.793</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="n">
+        <v>-9.74</v>
+      </c>
+      <c r="C232" t="n">
+        <v>-11.35</v>
+      </c>
+      <c r="D232" t="n">
+        <v>10.74</v>
+      </c>
+      <c r="E232" t="n">
+        <v>10.449</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="n">
+        <v>-9.93</v>
+      </c>
+      <c r="C233" t="n">
+        <v>-11.18</v>
+      </c>
+      <c r="D233" t="n">
+        <v>10.96</v>
+      </c>
+      <c r="E233" t="n">
+        <v>10.252</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="n">
+        <v>-9.92</v>
+      </c>
+      <c r="C234" t="n">
+        <v>-10.99</v>
+      </c>
+      <c r="D234" t="n">
+        <v>10.98</v>
+      </c>
+      <c r="E234" t="n">
+        <v>10.035</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="n">
+        <v>-9.91</v>
+      </c>
+      <c r="C235" t="n">
+        <v>-10.55</v>
+      </c>
+      <c r="D235" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="E235" t="n">
+        <v>9.856</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="n">
+        <v>-9.9</v>
+      </c>
+      <c r="C236" t="n">
+        <v>-10.31</v>
+      </c>
+      <c r="D236" t="n">
+        <v>10.74</v>
+      </c>
+      <c r="E236" t="n">
+        <v>9.577000000000002</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="n">
+        <v>-9.880000000000001</v>
+      </c>
+      <c r="C237" t="n">
+        <v>-9.98</v>
+      </c>
+      <c r="D237" t="n">
+        <v>10.78</v>
+      </c>
+      <c r="E237" t="n">
+        <v>9.178000000000001</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="n">
+        <v>-9.84</v>
+      </c>
+      <c r="C238" t="n">
+        <v>-9.66</v>
+      </c>
+      <c r="D238" t="n">
+        <v>10.64</v>
+      </c>
+      <c r="E238" t="n">
+        <v>8.959</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="n">
+        <v>-9.640000000000001</v>
+      </c>
+      <c r="C239" t="n">
+        <v>-9.33</v>
+      </c>
+      <c r="D239" t="n">
+        <v>10.52</v>
+      </c>
+      <c r="E239" t="n">
+        <v>8.56</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="B240" t="n">
+        <v>-9.460000000000001</v>
+      </c>
+      <c r="C240" t="n">
+        <v>-9.15</v>
+      </c>
+      <c r="D240" t="n">
+        <v>10.19</v>
+      </c>
+      <c r="E240" t="n">
+        <v>8.523</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="B241" t="n">
+        <v>-9.279999999999999</v>
+      </c>
+      <c r="C241" t="n">
+        <v>-9.02</v>
+      </c>
+      <c r="D241" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="E241" t="n">
+        <v>8.496</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="B242" t="n">
+        <v>-9.09</v>
+      </c>
+      <c r="C242" t="n">
+        <v>-8.9</v>
+      </c>
+      <c r="D242" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="E242" t="n">
+        <v>8.481999999999999</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="n">
+        <v>-8.82</v>
+      </c>
+      <c r="C243" t="n">
+        <v>-8.77</v>
+      </c>
+      <c r="D243" t="n">
+        <v>9.32</v>
+      </c>
+      <c r="E243" t="n">
+        <v>8.367999999999999</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n">
+        <v>242</v>
+      </c>
+      <c r="B244" t="n">
+        <v>-8.84</v>
+      </c>
+      <c r="C244" t="n">
+        <v>-8.33</v>
+      </c>
+      <c r="D244" t="n">
+        <v>9.220000000000001</v>
+      </c>
+      <c r="E244" t="n">
+        <v>8.054</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n">
+        <v>243</v>
+      </c>
+      <c r="B245" t="n">
+        <v>-9</v>
+      </c>
+      <c r="C245" t="n">
+        <v>-7.18</v>
+      </c>
+      <c r="D245" t="n">
+        <v>8.390000000000001</v>
+      </c>
+      <c r="E245" t="n">
+        <v>7.892</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="n">
+        <v>244</v>
+      </c>
+      <c r="B246" t="n">
+        <v>-8.69</v>
+      </c>
+      <c r="C246" t="n">
+        <v>-5.82</v>
+      </c>
+      <c r="D246" t="n">
+        <v>6.93</v>
+      </c>
+      <c r="E246" t="n">
+        <v>7.680000000000001</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="B247" t="n">
+        <v>-8.369999999999999</v>
+      </c>
+      <c r="C247" t="n">
+        <v>-4.56</v>
+      </c>
+      <c r="D247" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="E247" t="n">
+        <v>7.537999999999999</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="n">
+        <v>246</v>
+      </c>
+      <c r="B248" t="n">
+        <v>-8.06</v>
+      </c>
+      <c r="C248" t="n">
+        <v>-3.22</v>
+      </c>
+      <c r="D248" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="E248" t="n">
+        <v>7.146000000000001</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="n">
+        <v>247</v>
+      </c>
+      <c r="B249" t="n">
+        <v>-8.119999999999999</v>
+      </c>
+      <c r="C249" t="n">
+        <v>-1.88</v>
+      </c>
+      <c r="D249" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="E249" t="n">
+        <v>6.884</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="n">
+        <v>248</v>
+      </c>
+      <c r="B250" t="n">
+        <v>-8.16</v>
+      </c>
+      <c r="C250" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="D250" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="E250" t="n">
+        <v>6.316999999999999</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="n">
+        <v>249</v>
+      </c>
+      <c r="B251" t="n">
+        <v>-8.68</v>
+      </c>
+      <c r="C251" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="D251" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="E251" t="n">
+        <v>6.249999999999999</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="n">
+        <v>-9.220000000000001</v>
+      </c>
+      <c r="C252" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="D252" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="E252" t="n">
+        <v>6.289999999999999</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="n">
+        <v>251</v>
+      </c>
+      <c r="B253" t="n">
+        <v>-9.82</v>
+      </c>
+      <c r="C253" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D253" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E253" t="n">
+        <v>6.029999999999999</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="n">
+        <v>252</v>
+      </c>
+      <c r="B254" t="n">
+        <v>-10.83</v>
+      </c>
+      <c r="C254" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="D254" t="n">
+        <v>-0.91</v>
+      </c>
+      <c r="E254" t="n">
+        <v>5.97</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="B255" t="n">
+        <v>-11.63</v>
+      </c>
+      <c r="C255" t="n">
+        <v>7.27</v>
+      </c>
+      <c r="D255" t="n">
+        <v>-1.44</v>
+      </c>
+      <c r="E255" t="n">
+        <v>5.91</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="B256" t="n">
+        <v>-12.96</v>
+      </c>
+      <c r="C256" t="n">
+        <v>8.49</v>
+      </c>
+      <c r="D256" t="n">
+        <v>-1.84</v>
+      </c>
+      <c r="E256" t="n">
+        <v>6.409999999999999</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="B257" t="n">
+        <v>-14.29</v>
+      </c>
+      <c r="C257" t="n">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="D257" t="n">
+        <v>-2.08</v>
+      </c>
+      <c r="E257" t="n">
+        <v>6.775</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="n">
+        <v>256</v>
+      </c>
+      <c r="B258" t="n">
+        <v>-15.53</v>
+      </c>
+      <c r="C258" t="n">
+        <v>10.77</v>
+      </c>
+      <c r="D258" t="n">
+        <v>-2.33</v>
+      </c>
+      <c r="E258" t="n">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="n">
+        <v>257</v>
+      </c>
+      <c r="B259" t="n">
+        <v>-17.27</v>
+      </c>
+      <c r="C259" t="n">
+        <v>11.85</v>
+      </c>
+      <c r="D259" t="n">
+        <v>-2.83</v>
+      </c>
+      <c r="E259" t="n">
+        <v>8.344999999999999</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="B260" t="n">
+        <v>-18.93</v>
+      </c>
+      <c r="C260" t="n">
+        <v>12.85</v>
+      </c>
+      <c r="D260" t="n">
+        <v>-3.34</v>
+      </c>
+      <c r="E260" t="n">
+        <v>9.52</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="n">
+        <v>259</v>
+      </c>
+      <c r="B261" t="n">
+        <v>-20.09</v>
+      </c>
+      <c r="C261" t="n">
+        <v>13.84</v>
+      </c>
+      <c r="D261" t="n">
+        <v>-3.95</v>
+      </c>
+      <c r="E261" t="n">
+        <v>10.295</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B262" t="n">
+        <v>-21.16</v>
+      </c>
+      <c r="C262" t="n">
+        <v>14.87</v>
+      </c>
+      <c r="D262" t="n">
+        <v>-4.61</v>
+      </c>
+      <c r="E262" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="B263" t="n">
+        <v>-21.89</v>
+      </c>
+      <c r="C263" t="n">
+        <v>15.91</v>
+      </c>
+      <c r="D263" t="n">
+        <v>-5.74</v>
+      </c>
+      <c r="E263" t="n">
+        <v>11.815</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1" t="n">
+        <v>262</v>
+      </c>
+      <c r="B264" t="n">
+        <v>-22.22</v>
+      </c>
+      <c r="C264" t="n">
+        <v>15.63</v>
+      </c>
+      <c r="D264" t="n">
+        <v>-5.96</v>
+      </c>
+      <c r="E264" t="n">
+        <v>12.65</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1" t="n">
+        <v>263</v>
+      </c>
+      <c r="B265" t="n">
+        <v>-22.59</v>
+      </c>
+      <c r="C265" t="n">
+        <v>15.33</v>
+      </c>
+      <c r="D265" t="n">
+        <v>-6.12</v>
+      </c>
+      <c r="E265" t="n">
+        <v>13.485</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1" t="n">
+        <v>264</v>
+      </c>
+      <c r="B266" t="n">
+        <v>-22.78</v>
+      </c>
+      <c r="C266" t="n">
+        <v>15.21</v>
+      </c>
+      <c r="D266" t="n">
+        <v>-6.17</v>
+      </c>
+      <c r="E266" t="n">
+        <v>13.84</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="B267" t="n">
+        <v>-22.99</v>
+      </c>
+      <c r="C267" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="D267" t="n">
+        <v>-6.21</v>
+      </c>
+      <c r="E267" t="n">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="B268" t="n">
+        <v>-22.6</v>
+      </c>
+      <c r="C268" t="n">
+        <v>14.39</v>
+      </c>
+      <c r="D268" t="n">
+        <v>-6.24</v>
+      </c>
+      <c r="E268" t="n">
+        <v>14.56</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="B269" t="n">
+        <v>-21.56</v>
+      </c>
+      <c r="C269" t="n">
+        <v>13.66</v>
+      </c>
+      <c r="D269" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="E269" t="n">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="B270" t="n">
+        <v>-20.56</v>
+      </c>
+      <c r="C270" t="n">
+        <v>13.02</v>
+      </c>
+      <c r="D270" t="n">
+        <v>-6.17</v>
+      </c>
+      <c r="E270" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="B271" t="n">
+        <v>-19.59</v>
+      </c>
+      <c r="C271" t="n">
+        <v>12.38</v>
+      </c>
+      <c r="D271" t="n">
+        <v>-6.02</v>
+      </c>
+      <c r="E271" t="n">
+        <v>13.33</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="B272" t="n">
+        <v>-18.31</v>
+      </c>
+      <c r="C272" t="n">
+        <v>11.37</v>
+      </c>
+      <c r="D272" t="n">
+        <v>-5.81</v>
+      </c>
+      <c r="E272" t="n">
+        <v>12.86</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="B273" t="n">
+        <v>-17.32</v>
+      </c>
+      <c r="C273" t="n">
+        <v>10.34</v>
+      </c>
+      <c r="D273" t="n">
+        <v>-5.51</v>
+      </c>
+      <c r="E273" t="n">
+        <v>12.59</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="B274" t="n">
+        <v>-16.18</v>
+      </c>
+      <c r="C274" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="D274" t="n">
+        <v>-5.22</v>
+      </c>
+      <c r="E274" t="n">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="n">
+        <v>273</v>
+      </c>
+      <c r="B275" t="n">
+        <v>-14.96</v>
+      </c>
+      <c r="C275" t="n">
+        <v>8.07</v>
+      </c>
+      <c r="D275" t="n">
+        <v>-5.03</v>
+      </c>
+      <c r="E275" t="n">
+        <v>12.02</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="B276" t="n">
+        <v>-13.88</v>
+      </c>
+      <c r="C276" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="D276" t="n">
+        <v>-5.08</v>
+      </c>
+      <c r="E276" t="n">
+        <v>11.71</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="n">
+        <v>275</v>
+      </c>
+      <c r="B277" t="n">
+        <v>-12.77</v>
+      </c>
+      <c r="C277" t="n">
+        <v>6.61</v>
+      </c>
+      <c r="D277" t="n">
+        <v>-5.31</v>
+      </c>
+      <c r="E277" t="n">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1" t="n">
+        <v>276</v>
+      </c>
+      <c r="B278" t="n">
+        <v>-12.55</v>
+      </c>
+      <c r="C278" t="n">
+        <v>6.54</v>
+      </c>
+      <c r="D278" t="n">
+        <v>-5.6</v>
+      </c>
+      <c r="E278" t="n">
+        <v>11.705</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1" t="n">
+        <v>277</v>
+      </c>
+      <c r="B279" t="n">
+        <v>-12.33</v>
+      </c>
+      <c r="C279" t="n">
+        <v>6.62</v>
+      </c>
+      <c r="D279" t="n">
+        <v>-5.96</v>
+      </c>
+      <c r="E279" t="n">
+        <v>11.77</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="n">
+        <v>278</v>
+      </c>
+      <c r="B280" t="n">
+        <v>-12.13</v>
+      </c>
+      <c r="C280" t="n">
+        <v>6.68</v>
+      </c>
+      <c r="D280" t="n">
+        <v>-6.31</v>
+      </c>
+      <c r="E280" t="n">
+        <v>11.855</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="n">
+        <v>279</v>
+      </c>
+      <c r="B281" t="n">
+        <v>-11.92</v>
+      </c>
+      <c r="C281" t="n">
+        <v>6.72</v>
+      </c>
+      <c r="D281" t="n">
+        <v>-6.71</v>
+      </c>
+      <c r="E281" t="n">
+        <v>12.01</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="n">
+        <v>280</v>
+      </c>
+      <c r="B282" t="n">
+        <v>-12.37</v>
+      </c>
+      <c r="C282" t="n">
+        <v>7.14</v>
+      </c>
+      <c r="D282" t="n">
+        <v>-7.17</v>
+      </c>
+      <c r="E282" t="n">
+        <v>12.495</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="n">
+        <v>281</v>
+      </c>
+      <c r="B283" t="n">
+        <v>-12.54</v>
+      </c>
+      <c r="C283" t="n">
+        <v>7.57</v>
+      </c>
+      <c r="D283" t="n">
+        <v>-7.9</v>
+      </c>
+      <c r="E283" t="n">
+        <v>12.97</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="n">
+        <v>282</v>
+      </c>
+      <c r="B284" t="n">
+        <v>-12.82</v>
+      </c>
+      <c r="C284" t="n">
+        <v>8.08</v>
+      </c>
+      <c r="D284" t="n">
+        <v>-8.619999999999999</v>
+      </c>
+      <c r="E284" t="n">
+        <v>13.465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Preparing to fix a few issues
</commit_message>
<xml_diff>
--- a/Outputs/net_over_time_avg.xlsx
+++ b/Outputs/net_over_time_avg.xlsx
@@ -162,7 +162,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Net vs time this session (05/13/21): 10-hand moving averages</a:t>
+              <a:t>Net vs time this session (06/21/21): 10-hand moving averages</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -194,7 +194,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$B$2:$B$214</f>
+              <f>'data'!$B$2:$B$284</f>
             </numRef>
           </val>
         </ser>
@@ -221,7 +221,61 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$C$2:$C$214</f>
+              <f>'data'!$C$2:$C$284</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <strRef>
+              <f>'data'!D1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'data'!$D$2:$D$284</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <strRef>
+              <f>'data'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'data'!$E$2:$E$284</f>
             </numRef>
           </val>
         </ser>
@@ -591,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:E284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,12 +661,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Fish</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Scott</t>
+          <t>Raymond</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cedric</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fish</t>
         </is>
       </c>
     </row>
@@ -626,16 +690,22 @@
       <c r="C2" t="n">
         <v>0</v>
       </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.15</v>
+        <v>-0.3</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.15</v>
+        <v>0.4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.1</v>
       </c>
     </row>
     <row r="4">
@@ -643,10 +713,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3</v>
+        <v>-0.9</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.3</v>
+        <v>0.53</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.37</v>
       </c>
     </row>
     <row r="5">
@@ -654,10 +727,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>-1.15</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>-0.6</v>
       </c>
     </row>
     <row r="6">
@@ -665,10 +741,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8</v>
+        <v>-1.3</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.8</v>
+        <v>0.54</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.76</v>
       </c>
     </row>
     <row r="7">
@@ -676,10 +755,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.78</v>
+        <v>-1.38</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.78</v>
+        <v>0.53</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.85</v>
       </c>
     </row>
     <row r="8">
@@ -687,10 +769,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5</v>
+        <v>-1.46</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.5</v>
+        <v>0.31</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.14</v>
       </c>
     </row>
     <row r="9">
@@ -698,10 +783,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.26</v>
+        <v>-1.51</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.26</v>
+        <v>0.14</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.38</v>
       </c>
     </row>
     <row r="10">
@@ -709,10 +797,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.12</v>
+        <v>-1.44</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.12</v>
+        <v>-0.11</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.54</v>
       </c>
     </row>
     <row r="11">
@@ -720,10 +811,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.01</v>
+        <v>-0.82</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.01</v>
+        <v>-0.86</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.68</v>
       </c>
     </row>
     <row r="12">
@@ -731,10 +825,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.01</v>
+        <v>-0.82</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.01</v>
+        <v>-0.86</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.68</v>
       </c>
     </row>
     <row r="13">
@@ -742,10 +839,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.24</v>
+        <v>-0.35</v>
       </c>
       <c r="C13" t="n">
-        <v>0.24</v>
+        <v>-1.51</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.85</v>
       </c>
     </row>
     <row r="14">
@@ -753,10 +853,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.5</v>
+        <v>-0.01</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5</v>
+        <v>-2.23</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.24</v>
       </c>
     </row>
     <row r="15">
@@ -764,10 +867,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-0.8100000000000001</v>
+        <v>0.46</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8100000000000001</v>
+        <v>-2.98</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.52</v>
       </c>
     </row>
     <row r="16">
@@ -775,10 +881,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-1.21</v>
+        <v>0.83</v>
       </c>
       <c r="C16" t="n">
-        <v>1.21</v>
+        <v>-3.6</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.77</v>
       </c>
     </row>
     <row r="17">
@@ -786,10 +895,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-1.77</v>
+        <v>1.21</v>
       </c>
       <c r="C17" t="n">
-        <v>1.77</v>
+        <v>-4.21</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3.01</v>
       </c>
     </row>
     <row r="18">
@@ -797,10 +909,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-2.24</v>
+        <v>1.32</v>
       </c>
       <c r="C18" t="n">
-        <v>2.24</v>
+        <v>-4.85</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3.53</v>
       </c>
     </row>
     <row r="19">
@@ -808,10 +923,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-2.5</v>
+        <v>1.44</v>
       </c>
       <c r="C19" t="n">
-        <v>2.5</v>
+        <v>-5.35</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3.9</v>
       </c>
     </row>
     <row r="20">
@@ -819,10 +937,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-3.02</v>
+        <v>2.05</v>
       </c>
       <c r="C20" t="n">
-        <v>3.02</v>
+        <v>-5.83</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3.78</v>
       </c>
     </row>
     <row r="21">
@@ -830,10 +951,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-3.58</v>
+        <v>2.55</v>
       </c>
       <c r="C21" t="n">
-        <v>3.58</v>
+        <v>-6.21</v>
+      </c>
+      <c r="D21" t="n">
+        <v>3.66</v>
       </c>
     </row>
     <row r="22">
@@ -841,10 +965,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-4.13</v>
+        <v>1.9</v>
       </c>
       <c r="C22" t="n">
-        <v>4.13</v>
+        <v>-6.04</v>
+      </c>
+      <c r="D22" t="n">
+        <v>4.14</v>
       </c>
     </row>
     <row r="23">
@@ -852,10 +979,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-4.61</v>
+        <v>1.27</v>
       </c>
       <c r="C23" t="n">
-        <v>4.61</v>
+        <v>-5.99</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4.72</v>
       </c>
     </row>
     <row r="24">
@@ -863,10 +993,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-5.09</v>
+        <v>0.82</v>
       </c>
       <c r="C24" t="n">
-        <v>5.09</v>
+        <v>-5.96</v>
+      </c>
+      <c r="D24" t="n">
+        <v>5.14</v>
       </c>
     </row>
     <row r="25">
@@ -874,10 +1007,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-5.58</v>
+        <v>0.38</v>
       </c>
       <c r="C25" t="n">
-        <v>5.58</v>
+        <v>-5.89</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5.51</v>
       </c>
     </row>
     <row r="26">
@@ -885,10 +1021,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-6.07</v>
+        <v>-0.06</v>
       </c>
       <c r="C26" t="n">
-        <v>6.07</v>
+        <v>-5.92</v>
+      </c>
+      <c r="D26" t="n">
+        <v>5.98</v>
       </c>
     </row>
     <row r="27">
@@ -896,10 +1035,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-6.38</v>
+        <v>-0.52</v>
       </c>
       <c r="C27" t="n">
-        <v>6.38</v>
+        <v>-5.97</v>
+      </c>
+      <c r="D27" t="n">
+        <v>6.49</v>
       </c>
     </row>
     <row r="28">
@@ -907,10 +1049,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-6.71</v>
+        <v>-0.72</v>
       </c>
       <c r="C28" t="n">
-        <v>6.71</v>
+        <v>-6.01</v>
+      </c>
+      <c r="D28" t="n">
+        <v>6.73</v>
       </c>
     </row>
     <row r="29">
@@ -918,10 +1063,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>-7.03</v>
+        <v>-1.42</v>
       </c>
       <c r="C29" t="n">
-        <v>7.03</v>
+        <v>-6.04</v>
+      </c>
+      <c r="D29" t="n">
+        <v>7.46</v>
       </c>
     </row>
     <row r="30">
@@ -929,10 +1077,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-7.09</v>
+        <v>-2.59</v>
       </c>
       <c r="C30" t="n">
-        <v>7.09</v>
+        <v>-6.09</v>
+      </c>
+      <c r="D30" t="n">
+        <v>8.68</v>
       </c>
     </row>
     <row r="31">
@@ -940,10 +1091,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-7.32</v>
+        <v>-3.72</v>
       </c>
       <c r="C31" t="n">
-        <v>7.32</v>
+        <v>-6.16</v>
+      </c>
+      <c r="D31" t="n">
+        <v>9.880000000000001</v>
       </c>
     </row>
     <row r="32">
@@ -951,10 +1105,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-6.67</v>
+        <v>-4.41</v>
       </c>
       <c r="C32" t="n">
-        <v>7.67</v>
+        <v>-6.22</v>
+      </c>
+      <c r="D32" t="n">
+        <v>10.63</v>
       </c>
     </row>
     <row r="33">
@@ -962,10 +1119,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-6.98</v>
+        <v>-5.11</v>
       </c>
       <c r="C33" t="n">
-        <v>7.98</v>
+        <v>-6.2</v>
+      </c>
+      <c r="D33" t="n">
+        <v>11.32</v>
       </c>
     </row>
     <row r="34">
@@ -973,10 +1133,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-7.26</v>
+        <v>-5.79</v>
       </c>
       <c r="C34" t="n">
-        <v>8.26</v>
+        <v>-6.14</v>
+      </c>
+      <c r="D34" t="n">
+        <v>11.95</v>
       </c>
     </row>
     <row r="35">
@@ -984,10 +1147,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-7.45</v>
+        <v>-6.37</v>
       </c>
       <c r="C35" t="n">
-        <v>8.449999999999999</v>
+        <v>-6.1</v>
+      </c>
+      <c r="D35" t="n">
+        <v>12.5</v>
       </c>
     </row>
     <row r="36">
@@ -995,10 +1161,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-7.65</v>
+        <v>-4.62</v>
       </c>
       <c r="C36" t="n">
-        <v>8.65</v>
+        <v>-6.21</v>
+      </c>
+      <c r="D36" t="n">
+        <v>10.87</v>
       </c>
     </row>
     <row r="37">
@@ -1006,10 +1175,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-8.140000000000001</v>
+        <v>-2.83</v>
       </c>
       <c r="C37" t="n">
-        <v>9.140000000000001</v>
+        <v>-6.31</v>
+      </c>
+      <c r="D37" t="n">
+        <v>9.19</v>
       </c>
     </row>
     <row r="38">
@@ -1017,10 +1189,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-8.630000000000001</v>
+        <v>-1.03</v>
       </c>
       <c r="C38" t="n">
-        <v>9.630000000000001</v>
+        <v>-6.4</v>
+      </c>
+      <c r="D38" t="n">
+        <v>7.49</v>
       </c>
     </row>
     <row r="39">
@@ -1028,10 +1203,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-9.050000000000001</v>
+        <v>1.26</v>
       </c>
       <c r="C39" t="n">
-        <v>10.05</v>
+        <v>-6.48</v>
+      </c>
+      <c r="D39" t="n">
+        <v>5.29</v>
       </c>
     </row>
     <row r="40">
@@ -1039,10 +1217,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-9.369999999999999</v>
+        <v>3.33</v>
       </c>
       <c r="C40" t="n">
-        <v>10.37</v>
+        <v>-6.74</v>
+      </c>
+      <c r="D40" t="n">
+        <v>3.49</v>
       </c>
     </row>
     <row r="41">
@@ -1050,10 +1231,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-9.470000000000001</v>
+        <v>5.38</v>
       </c>
       <c r="C41" t="n">
-        <v>10.47</v>
+        <v>-6.99</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1.7</v>
       </c>
     </row>
     <row r="42">
@@ -1061,10 +1245,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-10.57</v>
+        <v>7.59</v>
       </c>
       <c r="C42" t="n">
-        <v>10.57</v>
+        <v>-7.26</v>
+      </c>
+      <c r="D42" t="n">
+        <v>-0.23</v>
       </c>
     </row>
     <row r="43">
@@ -1072,10 +1259,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>-10.61</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="C43" t="n">
-        <v>10.61</v>
+        <v>-7.59</v>
+      </c>
+      <c r="D43" t="n">
+        <v>-2.11</v>
       </c>
     </row>
     <row r="44">
@@ -1083,10 +1273,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-10.64</v>
+        <v>11.94</v>
       </c>
       <c r="C44" t="n">
-        <v>10.64</v>
+        <v>-7.8</v>
+      </c>
+      <c r="D44" t="n">
+        <v>-4.04</v>
       </c>
     </row>
     <row r="45">
@@ -1094,10 +1287,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>-10.74</v>
+        <v>13.97</v>
       </c>
       <c r="C45" t="n">
-        <v>10.74</v>
+        <v>-8</v>
+      </c>
+      <c r="D45" t="n">
+        <v>-5.87</v>
       </c>
     </row>
     <row r="46">
@@ -1105,10 +1301,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-10.86</v>
+        <v>13.78</v>
       </c>
       <c r="C46" t="n">
-        <v>10.86</v>
+        <v>-8.06</v>
+      </c>
+      <c r="D46" t="n">
+        <v>-5.62</v>
       </c>
     </row>
     <row r="47">
@@ -1116,10 +1315,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>-10.8</v>
+        <v>13.57</v>
       </c>
       <c r="C47" t="n">
-        <v>10.8</v>
+        <v>-8.109999999999999</v>
+      </c>
+      <c r="D47" t="n">
+        <v>-5.36</v>
       </c>
     </row>
     <row r="48">
@@ -1127,10 +1329,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-10.72</v>
+        <v>13.34</v>
       </c>
       <c r="C48" t="n">
-        <v>10.72</v>
+        <v>-8.15</v>
+      </c>
+      <c r="D48" t="n">
+        <v>-5.09</v>
       </c>
     </row>
     <row r="49">
@@ -1138,10 +1343,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-10.74</v>
+        <v>13.12</v>
       </c>
       <c r="C49" t="n">
-        <v>10.74</v>
+        <v>-8.26</v>
+      </c>
+      <c r="D49" t="n">
+        <v>-4.76</v>
       </c>
     </row>
     <row r="50">
@@ -1149,10 +1357,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-10.93</v>
+        <v>13.2</v>
       </c>
       <c r="C50" t="n">
-        <v>10.93</v>
+        <v>-8.17</v>
+      </c>
+      <c r="D50" t="n">
+        <v>-4.93</v>
       </c>
     </row>
     <row r="51">
@@ -1160,10 +1371,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-10.7</v>
+        <v>13.26</v>
       </c>
       <c r="C51" t="n">
-        <v>10.7</v>
+        <v>-8.07</v>
+      </c>
+      <c r="D51" t="n">
+        <v>-5.09</v>
       </c>
     </row>
     <row r="52">
@@ -1171,10 +1385,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-10.37</v>
+        <v>13.3</v>
       </c>
       <c r="C52" t="n">
-        <v>10.37</v>
+        <v>-8.07</v>
+      </c>
+      <c r="D52" t="n">
+        <v>-5.13</v>
       </c>
     </row>
     <row r="53">
@@ -1182,10 +1399,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-9.98</v>
+        <v>13.14</v>
       </c>
       <c r="C53" t="n">
-        <v>9.98</v>
+        <v>-8.09</v>
+      </c>
+      <c r="D53" t="n">
+        <v>-4.95</v>
       </c>
     </row>
     <row r="54">
@@ -1193,10 +1413,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-9.710000000000001</v>
+        <v>13.05</v>
       </c>
       <c r="C54" t="n">
-        <v>9.710000000000001</v>
+        <v>-8.199999999999999</v>
+      </c>
+      <c r="D54" t="n">
+        <v>-4.74</v>
       </c>
     </row>
     <row r="55">
@@ -1204,10 +1427,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>-9.390000000000001</v>
+        <v>12.97</v>
       </c>
       <c r="C55" t="n">
-        <v>9.390000000000001</v>
+        <v>-8.32</v>
+      </c>
+      <c r="D55" t="n">
+        <v>-4.53</v>
       </c>
     </row>
     <row r="56">
@@ -1215,10 +1441,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>-8.81</v>
+        <v>12.86</v>
       </c>
       <c r="C56" t="n">
-        <v>8.81</v>
+        <v>-8.43</v>
+      </c>
+      <c r="D56" t="n">
+        <v>-4.3</v>
       </c>
     </row>
     <row r="57">
@@ -1226,10 +1455,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-8.119999999999999</v>
+        <v>12.73</v>
       </c>
       <c r="C57" t="n">
-        <v>8.119999999999999</v>
+        <v>-8.59</v>
+      </c>
+      <c r="D57" t="n">
+        <v>-4.01</v>
       </c>
     </row>
     <row r="58">
@@ -1237,10 +1469,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>-7.43</v>
+        <v>12.58</v>
       </c>
       <c r="C58" t="n">
-        <v>7.43</v>
+        <v>-8.74</v>
+      </c>
+      <c r="D58" t="n">
+        <v>-3.71</v>
       </c>
     </row>
     <row r="59">
@@ -1248,10 +1483,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>-6.74</v>
+        <v>12.43</v>
       </c>
       <c r="C59" t="n">
-        <v>6.74</v>
+        <v>-8.76</v>
+      </c>
+      <c r="D59" t="n">
+        <v>-3.54</v>
       </c>
     </row>
     <row r="60">
@@ -1259,10 +1497,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>-6</v>
+        <v>12.2</v>
       </c>
       <c r="C60" t="n">
-        <v>6</v>
+        <v>-8.789999999999999</v>
+      </c>
+      <c r="D60" t="n">
+        <v>-3.28</v>
       </c>
     </row>
     <row r="61">
@@ -1270,10 +1511,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>-5.8</v>
+        <v>11.97</v>
       </c>
       <c r="C61" t="n">
-        <v>5.8</v>
+        <v>-8.81</v>
+      </c>
+      <c r="D61" t="n">
+        <v>-3.03</v>
       </c>
     </row>
     <row r="62">
@@ -1281,10 +1525,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>-5.64</v>
+        <v>11.74</v>
       </c>
       <c r="C62" t="n">
-        <v>5.64</v>
+        <v>-8.65</v>
+      </c>
+      <c r="D62" t="n">
+        <v>-2.96</v>
       </c>
     </row>
     <row r="63">
@@ -1292,10 +1539,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>-5.56</v>
+        <v>11.81</v>
       </c>
       <c r="C63" t="n">
-        <v>5.56</v>
+        <v>-8.5</v>
+      </c>
+      <c r="D63" t="n">
+        <v>-3.18</v>
       </c>
     </row>
     <row r="64">
@@ -1303,10 +1553,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>-5.41</v>
+        <v>10.82</v>
       </c>
       <c r="C64" t="n">
-        <v>5.41</v>
+        <v>-8.48</v>
+      </c>
+      <c r="D64" t="n">
+        <v>-2.22</v>
       </c>
     </row>
     <row r="65">
@@ -1314,10 +1567,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>-5.31</v>
+        <v>9.539999999999999</v>
       </c>
       <c r="C65" t="n">
-        <v>5.31</v>
+        <v>-8.470000000000001</v>
+      </c>
+      <c r="D65" t="n">
+        <v>-0.96</v>
       </c>
     </row>
     <row r="66">
@@ -1325,10 +1581,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>-5.44</v>
+        <v>8.27</v>
       </c>
       <c r="C66" t="n">
-        <v>5.44</v>
+        <v>-8.470000000000001</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="67">
@@ -1336,10 +1595,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>-5.61</v>
+        <v>6.99</v>
       </c>
       <c r="C67" t="n">
-        <v>5.61</v>
+        <v>-8.390000000000001</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1.5</v>
       </c>
     </row>
     <row r="68">
@@ -1347,10 +1609,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-5.81</v>
+        <v>5.74</v>
       </c>
       <c r="C68" t="n">
-        <v>5.81</v>
+        <v>-8.279999999999999</v>
+      </c>
+      <c r="D68" t="n">
+        <v>2.64</v>
       </c>
     </row>
     <row r="69">
@@ -1358,10 +1623,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>-5.92</v>
+        <v>4.43</v>
       </c>
       <c r="C69" t="n">
-        <v>5.92</v>
+        <v>-8.119999999999999</v>
+      </c>
+      <c r="D69" t="n">
+        <v>3.78</v>
       </c>
     </row>
     <row r="70">
@@ -1369,10 +1637,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>-5.63</v>
+        <v>3.13</v>
       </c>
       <c r="C70" t="n">
-        <v>5.63</v>
+        <v>-7.97</v>
+      </c>
+      <c r="D70" t="n">
+        <v>4.95</v>
       </c>
     </row>
     <row r="71">
@@ -1380,10 +1651,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-5.27</v>
+        <v>1.86</v>
       </c>
       <c r="C71" t="n">
-        <v>5.27</v>
+        <v>-7.85</v>
+      </c>
+      <c r="D71" t="n">
+        <v>6.09</v>
       </c>
     </row>
     <row r="72">
@@ -1391,10 +1665,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>-4.92</v>
+        <v>0.57</v>
       </c>
       <c r="C72" t="n">
-        <v>4.92</v>
+        <v>-7.78</v>
+      </c>
+      <c r="D72" t="n">
+        <v>7.31</v>
       </c>
     </row>
     <row r="73">
@@ -1402,10 +1679,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>-4.54</v>
+        <v>-1.06</v>
       </c>
       <c r="C73" t="n">
-        <v>4.54</v>
+        <v>-7.74</v>
+      </c>
+      <c r="D73" t="n">
+        <v>8.890000000000001</v>
       </c>
     </row>
     <row r="74">
@@ -1413,10 +1693,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>-4.17</v>
+        <v>-1.64</v>
       </c>
       <c r="C74" t="n">
-        <v>4.17</v>
+        <v>-7.58</v>
+      </c>
+      <c r="D74" t="n">
+        <v>9.32</v>
       </c>
     </row>
     <row r="75">
@@ -1424,10 +1707,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-3.8</v>
+        <v>-1.86</v>
       </c>
       <c r="C75" t="n">
-        <v>3.8</v>
+        <v>-7.46</v>
+      </c>
+      <c r="D75" t="n">
+        <v>9.42</v>
       </c>
     </row>
     <row r="76">
@@ -1435,10 +1721,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>-3.42</v>
+        <v>-2.05</v>
       </c>
       <c r="C76" t="n">
-        <v>3.42</v>
+        <v>-7.37</v>
+      </c>
+      <c r="D76" t="n">
+        <v>9.51</v>
       </c>
     </row>
     <row r="77">
@@ -1446,10 +1735,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>-3.12</v>
+        <v>-2.21</v>
       </c>
       <c r="C77" t="n">
-        <v>3.12</v>
+        <v>-7.27</v>
+      </c>
+      <c r="D77" t="n">
+        <v>9.59</v>
       </c>
     </row>
     <row r="78">
@@ -1457,10 +1749,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>-2.82</v>
+        <v>-2.37</v>
       </c>
       <c r="C78" t="n">
-        <v>2.82</v>
+        <v>-7.24</v>
+      </c>
+      <c r="D78" t="n">
+        <v>9.710000000000001</v>
       </c>
     </row>
     <row r="79">
@@ -1468,10 +1763,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>-2.58</v>
+        <v>-2.48</v>
       </c>
       <c r="C79" t="n">
-        <v>2.58</v>
+        <v>-7.31</v>
+      </c>
+      <c r="D79" t="n">
+        <v>9.890000000000001</v>
       </c>
     </row>
     <row r="80">
@@ -1479,10 +1777,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>-2.62</v>
+        <v>-2.61</v>
       </c>
       <c r="C80" t="n">
-        <v>2.62</v>
+        <v>-7.34</v>
+      </c>
+      <c r="D80" t="n">
+        <v>10.05</v>
       </c>
     </row>
     <row r="81">
@@ -1490,10 +1791,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>-2.6</v>
+        <v>-2.79</v>
       </c>
       <c r="C81" t="n">
-        <v>2.6</v>
+        <v>-7.36</v>
+      </c>
+      <c r="D81" t="n">
+        <v>10.25</v>
       </c>
     </row>
     <row r="82">
@@ -1501,10 +1805,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>-2.54</v>
+        <v>-2.87</v>
       </c>
       <c r="C82" t="n">
-        <v>2.54</v>
+        <v>-7.4</v>
+      </c>
+      <c r="D82" t="n">
+        <v>10.37</v>
       </c>
     </row>
     <row r="83">
@@ -1512,10 +1819,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>-2.55</v>
+        <v>-3.8</v>
       </c>
       <c r="C83" t="n">
-        <v>2.55</v>
+        <v>-6.31</v>
+      </c>
+      <c r="D83" t="n">
+        <v>10.21</v>
       </c>
     </row>
     <row r="84">
@@ -1523,10 +1833,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>-2.56</v>
+        <v>-4.61</v>
       </c>
       <c r="C84" t="n">
-        <v>2.56</v>
+        <v>-5.26</v>
+      </c>
+      <c r="D84" t="n">
+        <v>9.970000000000001</v>
       </c>
     </row>
     <row r="85">
@@ -1534,10 +1847,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>-2.57</v>
+        <v>-5.48</v>
       </c>
       <c r="C85" t="n">
-        <v>2.57</v>
+        <v>-4.16</v>
+      </c>
+      <c r="D85" t="n">
+        <v>9.74</v>
       </c>
     </row>
     <row r="86">
@@ -1545,10 +1861,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>-2.55</v>
+        <v>-6.31</v>
       </c>
       <c r="C86" t="n">
-        <v>2.55</v>
+        <v>-3.1</v>
+      </c>
+      <c r="D86" t="n">
+        <v>9.51</v>
       </c>
     </row>
     <row r="87">
@@ -1556,10 +1875,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>-2.52</v>
+        <v>-7.13</v>
       </c>
       <c r="C87" t="n">
-        <v>2.52</v>
+        <v>-2.06</v>
+      </c>
+      <c r="D87" t="n">
+        <v>9.300000000000001</v>
       </c>
     </row>
     <row r="88">
@@ -1567,10 +1889,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>-2.5</v>
+        <v>-7.98</v>
       </c>
       <c r="C88" t="n">
-        <v>2.5</v>
+        <v>-1</v>
+      </c>
+      <c r="D88" t="n">
+        <v>9.1</v>
       </c>
     </row>
     <row r="89">
@@ -1578,10 +1903,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>-2.51</v>
+        <v>-8.84</v>
       </c>
       <c r="C89" t="n">
-        <v>2.51</v>
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D89" t="n">
+        <v>8.9</v>
       </c>
     </row>
     <row r="90">
@@ -1589,10 +1917,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>-2.54</v>
+        <v>-9.68</v>
       </c>
       <c r="C90" t="n">
-        <v>2.54</v>
+        <v>1.1</v>
+      </c>
+      <c r="D90" t="n">
+        <v>8.720000000000001</v>
       </c>
     </row>
     <row r="91">
@@ -1600,10 +1931,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>-2.56</v>
+        <v>-10.52</v>
       </c>
       <c r="C91" t="n">
-        <v>2.56</v>
+        <v>2.15</v>
+      </c>
+      <c r="D91" t="n">
+        <v>8.52</v>
       </c>
     </row>
     <row r="92">
@@ -1611,10 +1945,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>-3.25</v>
+        <v>-11.34</v>
       </c>
       <c r="C92" t="n">
-        <v>3.25</v>
+        <v>3.12</v>
+      </c>
+      <c r="D92" t="n">
+        <v>8.380000000000001</v>
       </c>
     </row>
     <row r="93">
@@ -1622,10 +1959,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>-4</v>
+        <v>-11.05</v>
       </c>
       <c r="C93" t="n">
-        <v>4</v>
+        <v>2.96</v>
+      </c>
+      <c r="D93" t="n">
+        <v>8.26</v>
       </c>
     </row>
     <row r="94">
@@ -1633,10 +1973,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>-4.73</v>
+        <v>-10.85</v>
       </c>
       <c r="C94" t="n">
-        <v>4.73</v>
+        <v>2.79</v>
+      </c>
+      <c r="D94" t="n">
+        <v>8.24</v>
       </c>
     </row>
     <row r="95">
@@ -1644,10 +1987,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>-5.72</v>
+        <v>-10.65</v>
       </c>
       <c r="C95" t="n">
-        <v>5.72</v>
+        <v>2.62</v>
+      </c>
+      <c r="D95" t="n">
+        <v>8.220000000000001</v>
       </c>
     </row>
     <row r="96">
@@ -1655,10 +2001,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>-6.75</v>
+        <v>-10.66</v>
       </c>
       <c r="C96" t="n">
-        <v>6.75</v>
+        <v>2.63</v>
+      </c>
+      <c r="D96" t="n">
+        <v>8.220000000000001</v>
       </c>
     </row>
     <row r="97">
@@ -1666,10 +2015,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>-7.7</v>
+        <v>-10.69</v>
       </c>
       <c r="C97" t="n">
-        <v>7.7</v>
+        <v>2.67</v>
+      </c>
+      <c r="D97" t="n">
+        <v>8.220000000000001</v>
       </c>
     </row>
     <row r="98">
@@ -1677,10 +2029,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>-8.220000000000001</v>
+        <v>-9.99</v>
       </c>
       <c r="C98" t="n">
-        <v>8.220000000000001</v>
+        <v>1.96</v>
+      </c>
+      <c r="D98" t="n">
+        <v>8.210000000000001</v>
       </c>
     </row>
     <row r="99">
@@ -1688,10 +2043,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>-8.75</v>
+        <v>-9.23</v>
       </c>
       <c r="C99" t="n">
-        <v>8.75</v>
+        <v>1.24</v>
+      </c>
+      <c r="D99" t="n">
+        <v>8.17</v>
       </c>
     </row>
     <row r="100">
@@ -1699,10 +2057,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>-9.32</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="C100" t="n">
-        <v>9.32</v>
+        <v>0.59</v>
+      </c>
+      <c r="D100" t="n">
+        <v>8.130000000000001</v>
       </c>
     </row>
     <row r="101">
@@ -1710,10 +2071,13 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>-9.960000000000001</v>
+        <v>-7.83</v>
       </c>
       <c r="C101" t="n">
-        <v>9.960000000000001</v>
+        <v>-0.08</v>
+      </c>
+      <c r="D101" t="n">
+        <v>8.07</v>
       </c>
     </row>
     <row r="102">
@@ -1721,10 +2085,13 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>-9.93</v>
+        <v>-7.2</v>
       </c>
       <c r="C102" t="n">
-        <v>9.93</v>
+        <v>-0.65</v>
+      </c>
+      <c r="D102" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="103">
@@ -1732,10 +2099,13 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>-9.710000000000001</v>
+        <v>-6.59</v>
       </c>
       <c r="C103" t="n">
-        <v>9.710000000000001</v>
+        <v>-1.13</v>
+      </c>
+      <c r="D103" t="n">
+        <v>7.86</v>
       </c>
     </row>
     <row r="104">
@@ -1743,10 +2113,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>-9.51</v>
+        <v>-5.97</v>
       </c>
       <c r="C104" t="n">
-        <v>9.51</v>
+        <v>-1.6</v>
+      </c>
+      <c r="D104" t="n">
+        <v>7.7</v>
       </c>
     </row>
     <row r="105">
@@ -1754,10 +2127,13 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>-9.08</v>
+        <v>-5.42</v>
       </c>
       <c r="C105" t="n">
-        <v>9.08</v>
+        <v>-2.06</v>
+      </c>
+      <c r="D105" t="n">
+        <v>7.6</v>
       </c>
     </row>
     <row r="106">
@@ -1765,10 +2141,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>-7.53</v>
+        <v>-4.76</v>
       </c>
       <c r="C106" t="n">
-        <v>7.53</v>
+        <v>-2.63</v>
+      </c>
+      <c r="D106" t="n">
+        <v>7.5</v>
       </c>
     </row>
     <row r="107">
@@ -1776,10 +2155,13 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>-6.25</v>
+        <v>-4.08</v>
       </c>
       <c r="C107" t="n">
-        <v>6.25</v>
+        <v>-3.2</v>
+      </c>
+      <c r="D107" t="n">
+        <v>7.38</v>
       </c>
     </row>
     <row r="108">
@@ -1787,10 +2169,13 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>-5.37</v>
+        <v>-4.11</v>
       </c>
       <c r="C108" t="n">
-        <v>5.37</v>
+        <v>-3.05</v>
+      </c>
+      <c r="D108" t="n">
+        <v>7.26</v>
       </c>
     </row>
     <row r="109">
@@ -1798,10 +2183,13 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>-4.56</v>
+        <v>-4.15</v>
       </c>
       <c r="C109" t="n">
-        <v>4.56</v>
+        <v>-2.92</v>
+      </c>
+      <c r="D109" t="n">
+        <v>7.17</v>
       </c>
     </row>
     <row r="110">
@@ -1809,10 +2197,13 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>-3.76</v>
+        <v>-4.1</v>
       </c>
       <c r="C110" t="n">
-        <v>3.76</v>
+        <v>-2.86</v>
+      </c>
+      <c r="D110" t="n">
+        <v>7.06</v>
       </c>
     </row>
     <row r="111">
@@ -1820,10 +2211,13 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>-2.65</v>
+        <v>-4.28</v>
       </c>
       <c r="C111" t="n">
-        <v>2.65</v>
+        <v>-2.79</v>
+      </c>
+      <c r="D111" t="n">
+        <v>7.17</v>
       </c>
     </row>
     <row r="112">
@@ -1831,10 +2225,13 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>-1.65</v>
+        <v>-4.39</v>
       </c>
       <c r="C112" t="n">
-        <v>1.65</v>
+        <v>-2.74</v>
+      </c>
+      <c r="D112" t="n">
+        <v>7.23</v>
       </c>
     </row>
     <row r="113">
@@ -1842,10 +2239,13 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>-1.01</v>
+        <v>-4.49</v>
       </c>
       <c r="C113" t="n">
-        <v>1.01</v>
+        <v>-3.22</v>
+      </c>
+      <c r="D113" t="n">
+        <v>7.81</v>
       </c>
     </row>
     <row r="114">
@@ -1853,10 +2253,13 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>-0.45</v>
+        <v>-4.8</v>
       </c>
       <c r="C114" t="n">
-        <v>0.45</v>
+        <v>-3.5</v>
+      </c>
+      <c r="D114" t="n">
+        <v>8.4</v>
       </c>
     </row>
     <row r="115">
@@ -1864,10 +2267,13 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>0.14</v>
+        <v>-5.17</v>
       </c>
       <c r="C115" t="n">
-        <v>-0.14</v>
+        <v>-3.66</v>
+      </c>
+      <c r="D115" t="n">
+        <v>8.93</v>
       </c>
     </row>
     <row r="116">
@@ -1875,10 +2281,13 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>-0.44</v>
+        <v>-5.54</v>
       </c>
       <c r="C116" t="n">
-        <v>0.44</v>
+        <v>-3.8</v>
+      </c>
+      <c r="D116" t="n">
+        <v>9.44</v>
       </c>
     </row>
     <row r="117">
@@ -1886,10 +2295,13 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>-0.76</v>
+        <v>-5.92</v>
       </c>
       <c r="C117" t="n">
-        <v>0.76</v>
+        <v>-3.94</v>
+      </c>
+      <c r="D117" t="n">
+        <v>9.960000000000001</v>
       </c>
     </row>
     <row r="118">
@@ -1897,10 +2309,13 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>-1.21</v>
+        <v>-6.32</v>
       </c>
       <c r="C118" t="n">
-        <v>1.21</v>
+        <v>-4.07</v>
+      </c>
+      <c r="D118" t="n">
+        <v>10.49</v>
       </c>
     </row>
     <row r="119">
@@ -1908,10 +2323,13 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>-1.58</v>
+        <v>-6.82</v>
       </c>
       <c r="C119" t="n">
-        <v>1.58</v>
+        <v>-4.08</v>
+      </c>
+      <c r="D119" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="120">
@@ -1919,10 +2337,13 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>-2.21</v>
+        <v>-7.41</v>
       </c>
       <c r="C120" t="n">
-        <v>2.21</v>
+        <v>-4.01</v>
+      </c>
+      <c r="D120" t="n">
+        <v>11.52</v>
       </c>
     </row>
     <row r="121">
@@ -1930,10 +2351,13 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>-3.18</v>
+        <v>-9.69</v>
       </c>
       <c r="C121" t="n">
-        <v>3.18</v>
+        <v>-1.97</v>
+      </c>
+      <c r="D121" t="n">
+        <v>11.76</v>
       </c>
     </row>
     <row r="122">
@@ -1941,10 +2365,13 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>-4.09</v>
+        <v>-12.05</v>
       </c>
       <c r="C122" t="n">
-        <v>4.09</v>
+        <v>0.08</v>
+      </c>
+      <c r="D122" t="n">
+        <v>12.07</v>
       </c>
     </row>
     <row r="123">
@@ -1952,10 +2379,13 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>-4.53</v>
+        <v>-14.41</v>
       </c>
       <c r="C123" t="n">
-        <v>4.53</v>
+        <v>2.7</v>
+      </c>
+      <c r="D123" t="n">
+        <v>11.8</v>
       </c>
     </row>
     <row r="124">
@@ -1963,10 +2393,13 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>-4.94</v>
+        <v>-16.58</v>
       </c>
       <c r="C124" t="n">
-        <v>4.94</v>
+        <v>5.15</v>
+      </c>
+      <c r="D124" t="n">
+        <v>11.53</v>
       </c>
     </row>
     <row r="125">
@@ -1974,10 +2407,13 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>-5.66</v>
+        <v>-18.64</v>
       </c>
       <c r="C125" t="n">
-        <v>5.66</v>
+        <v>7.49</v>
+      </c>
+      <c r="D125" t="n">
+        <v>11.24</v>
       </c>
     </row>
     <row r="126">
@@ -1985,10 +2421,13 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>-6.41</v>
+        <v>-20.69</v>
       </c>
       <c r="C126" t="n">
-        <v>6.41</v>
+        <v>9.710000000000001</v>
+      </c>
+      <c r="D126" t="n">
+        <v>11.08</v>
       </c>
     </row>
     <row r="127">
@@ -1996,10 +2435,13 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>-7.16</v>
+        <v>-22.73</v>
       </c>
       <c r="C127" t="n">
-        <v>7.16</v>
+        <v>11.86</v>
+      </c>
+      <c r="D127" t="n">
+        <v>10.96</v>
       </c>
     </row>
     <row r="128">
@@ -2007,10 +2449,13 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>-7.78</v>
+        <v>-24.64</v>
       </c>
       <c r="C128" t="n">
-        <v>7.78</v>
+        <v>13.95</v>
+      </c>
+      <c r="D128" t="n">
+        <v>10.79</v>
       </c>
     </row>
     <row r="129">
@@ -2018,10 +2463,13 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>-8.390000000000001</v>
+        <v>-26.48</v>
       </c>
       <c r="C129" t="n">
-        <v>8.390000000000001</v>
+        <v>15.94</v>
+      </c>
+      <c r="D129" t="n">
+        <v>10.64</v>
       </c>
     </row>
     <row r="130">
@@ -2029,10 +2477,13 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>-8.77</v>
+        <v>-28.33</v>
       </c>
       <c r="C130" t="n">
-        <v>8.77</v>
+        <v>17.93</v>
+      </c>
+      <c r="D130" t="n">
+        <v>10.5</v>
       </c>
     </row>
     <row r="131">
@@ -2040,10 +2491,13 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>-9.119999999999999</v>
+        <v>-28.58</v>
       </c>
       <c r="C131" t="n">
-        <v>9.119999999999999</v>
+        <v>18.25</v>
+      </c>
+      <c r="D131" t="n">
+        <v>10.44</v>
       </c>
     </row>
     <row r="132">
@@ -2051,10 +2505,13 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>-9.43</v>
+        <v>-28.85</v>
       </c>
       <c r="C132" t="n">
-        <v>9.43</v>
+        <v>18.59</v>
+      </c>
+      <c r="D132" t="n">
+        <v>10.36</v>
       </c>
     </row>
     <row r="133">
@@ -2062,10 +2519,13 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>-9.949999999999999</v>
+        <v>-29.11</v>
       </c>
       <c r="C133" t="n">
-        <v>9.949999999999999</v>
+        <v>18.79</v>
+      </c>
+      <c r="D133" t="n">
+        <v>10.42</v>
       </c>
     </row>
     <row r="134">
@@ -2073,10 +2533,13 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>-10.39</v>
+        <v>-29.6</v>
       </c>
       <c r="C134" t="n">
-        <v>10.39</v>
+        <v>19.21</v>
+      </c>
+      <c r="D134" t="n">
+        <v>10.49</v>
       </c>
     </row>
     <row r="135">
@@ -2084,10 +2547,13 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>-10.53</v>
+        <v>-30.12</v>
       </c>
       <c r="C135" t="n">
-        <v>10.53</v>
+        <v>19.64</v>
+      </c>
+      <c r="D135" t="n">
+        <v>10.57</v>
       </c>
     </row>
     <row r="136">
@@ -2095,10 +2561,13 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>-10.59</v>
+        <v>-30.64</v>
       </c>
       <c r="C136" t="n">
-        <v>10.59</v>
+        <v>20.19</v>
+      </c>
+      <c r="D136" t="n">
+        <v>10.56</v>
       </c>
     </row>
     <row r="137">
@@ -2106,10 +2575,13 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>-10.48</v>
+        <v>-31.16</v>
       </c>
       <c r="C137" t="n">
-        <v>10.48</v>
+        <v>20.76</v>
+      </c>
+      <c r="D137" t="n">
+        <v>10.5</v>
       </c>
     </row>
     <row r="138">
@@ -2117,10 +2589,13 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>-10.38</v>
+        <v>-31.77</v>
       </c>
       <c r="C138" t="n">
-        <v>10.38</v>
+        <v>21.37</v>
+      </c>
+      <c r="D138" t="n">
+        <v>10.5</v>
       </c>
     </row>
     <row r="139">
@@ -2128,10 +2603,13 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>-10.18</v>
+        <v>-32.49</v>
       </c>
       <c r="C139" t="n">
-        <v>10.18</v>
+        <v>22.09</v>
+      </c>
+      <c r="D139" t="n">
+        <v>10.5</v>
       </c>
     </row>
     <row r="140">
@@ -2139,10 +2617,13 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>-10.02</v>
+        <v>-33.11</v>
       </c>
       <c r="C140" t="n">
-        <v>10.02</v>
+        <v>22.74</v>
+      </c>
+      <c r="D140" t="n">
+        <v>10.47</v>
       </c>
     </row>
     <row r="141">
@@ -2150,10 +2631,13 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>-9.800000000000001</v>
+        <v>-33.61</v>
       </c>
       <c r="C141" t="n">
-        <v>9.800000000000001</v>
+        <v>23.09</v>
+      </c>
+      <c r="D141" t="n">
+        <v>10.62</v>
       </c>
     </row>
     <row r="142">
@@ -2161,10 +2645,13 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>-9.09</v>
+        <v>-34.08</v>
       </c>
       <c r="C142" t="n">
-        <v>9.09</v>
+        <v>23.41</v>
+      </c>
+      <c r="D142" t="n">
+        <v>10.77</v>
       </c>
     </row>
     <row r="143">
@@ -2172,10 +2659,13 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>-8.380000000000001</v>
+        <v>-34.56</v>
       </c>
       <c r="C143" t="n">
-        <v>8.380000000000001</v>
+        <v>23.76</v>
+      </c>
+      <c r="D143" t="n">
+        <v>10.9</v>
       </c>
     </row>
     <row r="144">
@@ -2183,10 +2673,13 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>-7.66</v>
+        <v>-35.05</v>
       </c>
       <c r="C144" t="n">
-        <v>7.66</v>
+        <v>23.8</v>
+      </c>
+      <c r="D144" t="n">
+        <v>11.35</v>
       </c>
     </row>
     <row r="145">
@@ -2194,10 +2687,13 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>-6.94</v>
+        <v>-35.5</v>
       </c>
       <c r="C145" t="n">
-        <v>6.94</v>
+        <v>23.8</v>
+      </c>
+      <c r="D145" t="n">
+        <v>11.8</v>
       </c>
     </row>
     <row r="146">
@@ -2205,10 +2701,13 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>-5.73</v>
+        <v>-35.91</v>
       </c>
       <c r="C146" t="n">
-        <v>5.73</v>
+        <v>23.78</v>
+      </c>
+      <c r="D146" t="n">
+        <v>12.23</v>
       </c>
     </row>
     <row r="147">
@@ -2216,10 +2715,13 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>-4.68</v>
+        <v>-36.29</v>
       </c>
       <c r="C147" t="n">
-        <v>4.68</v>
+        <v>23.77</v>
+      </c>
+      <c r="D147" t="n">
+        <v>12.62</v>
       </c>
     </row>
     <row r="148">
@@ -2227,10 +2729,13 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>-3.84</v>
+        <v>-36.7</v>
       </c>
       <c r="C148" t="n">
-        <v>3.84</v>
+        <v>23.79</v>
+      </c>
+      <c r="D148" t="n">
+        <v>13.01</v>
       </c>
     </row>
     <row r="149">
@@ -2238,10 +2743,13 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>-3.07</v>
+        <v>-36.99</v>
       </c>
       <c r="C149" t="n">
-        <v>3.07</v>
+        <v>23.71</v>
+      </c>
+      <c r="D149" t="n">
+        <v>13.38</v>
       </c>
     </row>
     <row r="150">
@@ -2249,10 +2757,13 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>-2.34</v>
+        <v>-37.24</v>
       </c>
       <c r="C150" t="n">
-        <v>2.34</v>
+        <v>23.64</v>
+      </c>
+      <c r="D150" t="n">
+        <v>13.7</v>
       </c>
     </row>
     <row r="151">
@@ -2260,10 +2771,13 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>-1.46</v>
+        <v>-37.88</v>
       </c>
       <c r="C151" t="n">
-        <v>1.46</v>
+        <v>23.55</v>
+      </c>
+      <c r="D151" t="n">
+        <v>14.43</v>
       </c>
     </row>
     <row r="152">
@@ -2271,10 +2785,13 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>-1.11</v>
+        <v>-38.55</v>
       </c>
       <c r="C152" t="n">
-        <v>1.11</v>
+        <v>23.5</v>
+      </c>
+      <c r="D152" t="n">
+        <v>15.15</v>
       </c>
     </row>
     <row r="153">
@@ -2282,10 +2799,13 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>-0.72</v>
+        <v>-39.15</v>
       </c>
       <c r="C153" t="n">
-        <v>0.72</v>
+        <v>23.37</v>
+      </c>
+      <c r="D153" t="n">
+        <v>15.88</v>
       </c>
     </row>
     <row r="154">
@@ -2293,10 +2813,13 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>-0.36</v>
+        <v>-39.38</v>
       </c>
       <c r="C154" t="n">
-        <v>0.36</v>
+        <v>23.26</v>
+      </c>
+      <c r="D154" t="n">
+        <v>16.22</v>
       </c>
     </row>
     <row r="155">
@@ -2304,10 +2827,13 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>-0.02</v>
+        <v>-39.62</v>
       </c>
       <c r="C155" t="n">
-        <v>0.02</v>
+        <v>23.18</v>
+      </c>
+      <c r="D155" t="n">
+        <v>16.55</v>
       </c>
     </row>
     <row r="156">
@@ -2315,10 +2841,13 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>-0.17</v>
+        <v>-39.9</v>
       </c>
       <c r="C156" t="n">
-        <v>0.17</v>
+        <v>23.1</v>
+      </c>
+      <c r="D156" t="n">
+        <v>16.9</v>
       </c>
     </row>
     <row r="157">
@@ -2326,10 +2855,13 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>-0.25</v>
+        <v>-40.22</v>
       </c>
       <c r="C157" t="n">
-        <v>0.25</v>
+        <v>23.04</v>
+      </c>
+      <c r="D157" t="n">
+        <v>17.29</v>
       </c>
     </row>
     <row r="158">
@@ -2337,10 +2869,13 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>0.32</v>
+        <v>-40.53</v>
       </c>
       <c r="C158" t="n">
-        <v>-0.32</v>
+        <v>22.9</v>
+      </c>
+      <c r="D158" t="n">
+        <v>17.73</v>
       </c>
     </row>
     <row r="159">
@@ -2348,10 +2883,13 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>0.86</v>
+        <v>-40.84</v>
       </c>
       <c r="C159" t="n">
-        <v>-0.86</v>
+        <v>22.76</v>
+      </c>
+      <c r="D159" t="n">
+        <v>18.18</v>
       </c>
     </row>
     <row r="160">
@@ -2359,10 +2897,13 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>1.3</v>
+        <v>-40.18</v>
       </c>
       <c r="C160" t="n">
-        <v>-1.3</v>
+        <v>21.59</v>
+      </c>
+      <c r="D160" t="n">
+        <v>18.69</v>
       </c>
     </row>
     <row r="161">
@@ -2370,10 +2911,13 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>1.59</v>
+        <v>-38.96</v>
       </c>
       <c r="C161" t="n">
-        <v>-1.59</v>
+        <v>20.45</v>
+      </c>
+      <c r="D161" t="n">
+        <v>18.61</v>
       </c>
     </row>
     <row r="162">
@@ -2381,10 +2925,13 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>1.57</v>
+        <v>-37.73</v>
       </c>
       <c r="C162" t="n">
-        <v>-1.57</v>
+        <v>19.27</v>
+      </c>
+      <c r="D162" t="n">
+        <v>18.56</v>
       </c>
     </row>
     <row r="163">
@@ -2392,10 +2939,13 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>1.05</v>
+        <v>-36.59</v>
       </c>
       <c r="C163" t="n">
-        <v>-1.05</v>
+        <v>18.18</v>
+      </c>
+      <c r="D163" t="n">
+        <v>18.51</v>
       </c>
     </row>
     <row r="164">
@@ -2403,10 +2953,13 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>0.5</v>
+        <v>-34.49</v>
       </c>
       <c r="C164" t="n">
-        <v>-0.5</v>
+        <v>16.09</v>
+      </c>
+      <c r="D164" t="n">
+        <v>18.5</v>
       </c>
     </row>
     <row r="165">
@@ -2414,10 +2967,13 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>-0.04</v>
+        <v>-32.38</v>
       </c>
       <c r="C165" t="n">
-        <v>0.04</v>
+        <v>13.96</v>
+      </c>
+      <c r="D165" t="n">
+        <v>18.52</v>
       </c>
     </row>
     <row r="166">
@@ -2425,10 +2981,13 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>-0.55</v>
+        <v>-30.26</v>
       </c>
       <c r="C166" t="n">
-        <v>0.55</v>
+        <v>11.85</v>
+      </c>
+      <c r="D166" t="n">
+        <v>18.51</v>
       </c>
     </row>
     <row r="167">
@@ -2436,10 +2995,13 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>-1.23</v>
+        <v>-28.01</v>
       </c>
       <c r="C167" t="n">
-        <v>1.23</v>
+        <v>9.6</v>
+      </c>
+      <c r="D167" t="n">
+        <v>18.51</v>
       </c>
     </row>
     <row r="168">
@@ -2447,10 +3009,13 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>-2.17</v>
+        <v>-25.77</v>
       </c>
       <c r="C168" t="n">
-        <v>2.17</v>
+        <v>7.41</v>
+      </c>
+      <c r="D168" t="n">
+        <v>18.46</v>
       </c>
     </row>
     <row r="169">
@@ -2458,10 +3023,13 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>-3.1</v>
+        <v>-23.41</v>
       </c>
       <c r="C169" t="n">
-        <v>3.1</v>
+        <v>5.14</v>
+      </c>
+      <c r="D169" t="n">
+        <v>18.37</v>
       </c>
     </row>
     <row r="170">
@@ -2469,10 +3037,13 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>-3.88</v>
+        <v>-22.11</v>
       </c>
       <c r="C170" t="n">
-        <v>3.88</v>
+        <v>3.94</v>
+      </c>
+      <c r="D170" t="n">
+        <v>18.28</v>
       </c>
     </row>
     <row r="171">
@@ -2480,10 +3051,13 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>-4.92</v>
+        <v>-20.82</v>
       </c>
       <c r="C171" t="n">
-        <v>4.92</v>
+        <v>2.92</v>
+      </c>
+      <c r="D171" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="172">
@@ -2491,10 +3065,13 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>-5.6</v>
+        <v>-19.51</v>
       </c>
       <c r="C172" t="n">
-        <v>5.6</v>
+        <v>1.91</v>
+      </c>
+      <c r="D172" t="n">
+        <v>17.7</v>
       </c>
     </row>
     <row r="173">
@@ -2502,10 +3079,13 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>-5.84</v>
+        <v>-18.16</v>
       </c>
       <c r="C173" t="n">
-        <v>5.84</v>
+        <v>0.84</v>
+      </c>
+      <c r="D173" t="n">
+        <v>17.41</v>
       </c>
     </row>
     <row r="174">
@@ -2513,10 +3093,13 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>-6</v>
+        <v>-17.9</v>
       </c>
       <c r="C174" t="n">
-        <v>6</v>
+        <v>0.84</v>
+      </c>
+      <c r="D174" t="n">
+        <v>17.16</v>
       </c>
     </row>
     <row r="175">
@@ -2524,10 +3107,13 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>-6.14</v>
+        <v>-17.65</v>
       </c>
       <c r="C175" t="n">
-        <v>6.14</v>
+        <v>0.85</v>
+      </c>
+      <c r="D175" t="n">
+        <v>16.9</v>
       </c>
     </row>
     <row r="176">
@@ -2535,10 +3121,13 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>-6.38</v>
+        <v>-17.49</v>
       </c>
       <c r="C176" t="n">
-        <v>6.38</v>
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="D176" t="n">
+        <v>16.64</v>
       </c>
     </row>
     <row r="177">
@@ -2546,10 +3135,13 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>-6.5</v>
+        <v>-17.44</v>
       </c>
       <c r="C177" t="n">
-        <v>6.5</v>
+        <v>1.22</v>
+      </c>
+      <c r="D177" t="n">
+        <v>16.33</v>
       </c>
     </row>
     <row r="178">
@@ -2557,10 +3149,13 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>-6.79</v>
+        <v>-17.29</v>
       </c>
       <c r="C178" t="n">
-        <v>6.79</v>
+        <v>1.44</v>
+      </c>
+      <c r="D178" t="n">
+        <v>15.94</v>
       </c>
     </row>
     <row r="179">
@@ -2568,10 +3163,13 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>-7.03</v>
+        <v>-17.31</v>
       </c>
       <c r="C179" t="n">
-        <v>7.03</v>
+        <v>1.56</v>
+      </c>
+      <c r="D179" t="n">
+        <v>15.84</v>
       </c>
     </row>
     <row r="180">
@@ -2579,10 +3177,13 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>-7.33</v>
+        <v>-17.31</v>
       </c>
       <c r="C180" t="n">
-        <v>7.33</v>
+        <v>1.66</v>
+      </c>
+      <c r="D180" t="n">
+        <v>15.74</v>
       </c>
     </row>
     <row r="181">
@@ -2590,10 +3191,13 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>-7.37</v>
+        <v>-17.43</v>
       </c>
       <c r="C181" t="n">
-        <v>7.37</v>
+        <v>1.59</v>
+      </c>
+      <c r="D181" t="n">
+        <v>15.94</v>
       </c>
     </row>
     <row r="182">
@@ -2601,10 +3205,13 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>-7.41</v>
+        <v>-17.54</v>
       </c>
       <c r="C182" t="n">
-        <v>7.41</v>
+        <v>1.49</v>
+      </c>
+      <c r="D182" t="n">
+        <v>16.15</v>
       </c>
     </row>
     <row r="183">
@@ -2612,10 +3219,13 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>-7.49</v>
+        <v>-17.17</v>
       </c>
       <c r="C183" t="n">
-        <v>7.49</v>
+        <v>1.21</v>
+      </c>
+      <c r="D183" t="n">
+        <v>16.06</v>
       </c>
     </row>
     <row r="184">
@@ -2623,10 +3233,13 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>-7.66</v>
+        <v>-16.79</v>
       </c>
       <c r="C184" t="n">
-        <v>7.66</v>
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="D184" t="n">
+        <v>15.95</v>
       </c>
     </row>
     <row r="185">
@@ -2634,10 +3247,13 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>-7.88</v>
+        <v>-16.37</v>
       </c>
       <c r="C185" t="n">
-        <v>7.88</v>
+        <v>0.64</v>
+      </c>
+      <c r="D185" t="n">
+        <v>15.83</v>
       </c>
     </row>
     <row r="186">
@@ -2645,10 +3261,13 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>-8.050000000000001</v>
+        <v>-15.89</v>
       </c>
       <c r="C186" t="n">
-        <v>8.050000000000001</v>
+        <v>0.25</v>
+      </c>
+      <c r="D186" t="n">
+        <v>15.74</v>
       </c>
     </row>
     <row r="187">
@@ -2656,10 +3275,13 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>-8.23</v>
+        <v>-15.56</v>
       </c>
       <c r="C187" t="n">
-        <v>8.23</v>
+        <v>0</v>
+      </c>
+      <c r="D187" t="n">
+        <v>15.66</v>
       </c>
     </row>
     <row r="188">
@@ -2667,10 +3289,13 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>-8.43</v>
+        <v>-15.65</v>
       </c>
       <c r="C188" t="n">
-        <v>8.43</v>
+        <v>-0.21</v>
+      </c>
+      <c r="D188" t="n">
+        <v>15.96</v>
       </c>
     </row>
     <row r="189">
@@ -2678,10 +3303,13 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>-8.640000000000001</v>
+        <v>-15.57</v>
       </c>
       <c r="C189" t="n">
-        <v>8.640000000000001</v>
+        <v>-0.27</v>
+      </c>
+      <c r="D189" t="n">
+        <v>15.94</v>
       </c>
     </row>
     <row r="190">
@@ -2689,10 +3317,13 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>-8.779999999999999</v>
+        <v>-15.5</v>
       </c>
       <c r="C190" t="n">
-        <v>8.779999999999999</v>
+        <v>-0.32</v>
+      </c>
+      <c r="D190" t="n">
+        <v>15.93</v>
       </c>
     </row>
     <row r="191">
@@ -2700,10 +3331,13 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>-8.949999999999999</v>
+        <v>-15.3</v>
       </c>
       <c r="C191" t="n">
-        <v>8.949999999999999</v>
+        <v>-0.39</v>
+      </c>
+      <c r="D191" t="n">
+        <v>15.8</v>
       </c>
     </row>
     <row r="192">
@@ -2711,10 +3345,13 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>-9.119999999999999</v>
+        <v>-15.12</v>
       </c>
       <c r="C192" t="n">
-        <v>9.119999999999999</v>
+        <v>-0.46</v>
+      </c>
+      <c r="D192" t="n">
+        <v>15.67</v>
       </c>
     </row>
     <row r="193">
@@ -2722,10 +3359,13 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>-9.17</v>
+        <v>-15.06</v>
       </c>
       <c r="C193" t="n">
-        <v>9.17</v>
+        <v>-0.32</v>
+      </c>
+      <c r="D193" t="n">
+        <v>15.48</v>
       </c>
     </row>
     <row r="194">
@@ -2733,10 +3373,13 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>-9.699999999999999</v>
+        <v>-15.03</v>
       </c>
       <c r="C194" t="n">
-        <v>9.699999999999999</v>
+        <v>-0.17</v>
+      </c>
+      <c r="D194" t="n">
+        <v>15.3</v>
       </c>
     </row>
     <row r="195">
@@ -2744,10 +3387,13 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>-10.21</v>
+        <v>-15.02</v>
       </c>
       <c r="C195" t="n">
-        <v>10.21</v>
+        <v>-0.01</v>
+      </c>
+      <c r="D195" t="n">
+        <v>15.13</v>
       </c>
     </row>
     <row r="196">
@@ -2755,10 +3401,16 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>-10.97</v>
+        <v>-15.06</v>
       </c>
       <c r="C196" t="n">
-        <v>10.97</v>
+        <v>0.1</v>
+      </c>
+      <c r="D196" t="n">
+        <v>15.06</v>
+      </c>
+      <c r="E196" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -2766,10 +3418,16 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>-11.75</v>
+        <v>-14.94</v>
       </c>
       <c r="C197" t="n">
-        <v>11.75</v>
+        <v>0</v>
+      </c>
+      <c r="D197" t="n">
+        <v>15.05</v>
+      </c>
+      <c r="E197" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="198">
@@ -2777,10 +3435,16 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>-12.49</v>
+        <v>-14.51</v>
       </c>
       <c r="C198" t="n">
-        <v>12.49</v>
+        <v>-0.11</v>
+      </c>
+      <c r="D198" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="E198" t="n">
+        <v>-0.75</v>
       </c>
     </row>
     <row r="199">
@@ -2788,10 +3452,16 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>-13.19</v>
+        <v>-14.19</v>
       </c>
       <c r="C199" t="n">
-        <v>13.19</v>
+        <v>0.11</v>
+      </c>
+      <c r="D199" t="n">
+        <v>14.41</v>
+      </c>
+      <c r="E199" t="n">
+        <v>-1.175</v>
       </c>
     </row>
     <row r="200">
@@ -2799,10 +3469,16 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>-13.94</v>
+        <v>-13.87</v>
       </c>
       <c r="C200" t="n">
-        <v>13.94</v>
+        <v>0.29</v>
+      </c>
+      <c r="D200" t="n">
+        <v>14.14</v>
+      </c>
+      <c r="E200" t="n">
+        <v>-1.43</v>
       </c>
     </row>
     <row r="201">
@@ -2810,10 +3486,16 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>-14.65</v>
+        <v>-13.58</v>
       </c>
       <c r="C201" t="n">
-        <v>14.65</v>
+        <v>0.48</v>
+      </c>
+      <c r="D201" t="n">
+        <v>13.91</v>
+      </c>
+      <c r="E201" t="n">
+        <v>-1.6</v>
       </c>
     </row>
     <row r="202">
@@ -2821,10 +3503,16 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>-15.4</v>
+        <v>-13.27</v>
       </c>
       <c r="C202" t="n">
-        <v>15.4</v>
+        <v>0.67</v>
+      </c>
+      <c r="D202" t="n">
+        <v>13.66</v>
+      </c>
+      <c r="E202" t="n">
+        <v>-1.835714285714286</v>
       </c>
     </row>
     <row r="203">
@@ -2832,10 +3520,16 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
-        <v>-16.22</v>
+        <v>-13.41</v>
       </c>
       <c r="C203" t="n">
-        <v>16.22</v>
+        <v>0.86</v>
+      </c>
+      <c r="D203" t="n">
+        <v>13.93</v>
+      </c>
+      <c r="E203" t="n">
+        <v>-2.08375</v>
       </c>
     </row>
     <row r="204">
@@ -2843,10 +3537,16 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
-        <v>-16.51</v>
+        <v>-13.59</v>
       </c>
       <c r="C204" t="n">
-        <v>16.51</v>
+        <v>1.21</v>
+      </c>
+      <c r="D204" t="n">
+        <v>14.15</v>
+      </c>
+      <c r="E204" t="n">
+        <v>-2.298888888888889</v>
       </c>
     </row>
     <row r="205">
@@ -2854,10 +3554,16 @@
         <v>203</v>
       </c>
       <c r="B205" t="n">
-        <v>-16.8</v>
+        <v>-13.63</v>
       </c>
       <c r="C205" t="n">
-        <v>16.8</v>
+        <v>1.55</v>
+      </c>
+      <c r="D205" t="n">
+        <v>14.26</v>
+      </c>
+      <c r="E205" t="n">
+        <v>-2.471</v>
       </c>
     </row>
     <row r="206">
@@ -2865,10 +3571,16 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>-16.94</v>
+        <v>-13.64</v>
       </c>
       <c r="C206" t="n">
-        <v>16.94</v>
+        <v>1.98</v>
+      </c>
+      <c r="D206" t="n">
+        <v>14.23</v>
+      </c>
+      <c r="E206" t="n">
+        <v>-2.471</v>
       </c>
     </row>
     <row r="207">
@@ -2876,10 +3588,16 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>-17.06</v>
+        <v>-13.67</v>
       </c>
       <c r="C207" t="n">
-        <v>17.06</v>
+        <v>2.38</v>
+      </c>
+      <c r="D207" t="n">
+        <v>14.32</v>
+      </c>
+      <c r="E207" t="n">
+        <v>-2.93</v>
       </c>
     </row>
     <row r="208">
@@ -2887,10 +3605,16 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>-17.2</v>
+        <v>-13.71</v>
       </c>
       <c r="C208" t="n">
-        <v>17.2</v>
+        <v>2.8</v>
+      </c>
+      <c r="D208" t="n">
+        <v>14.42</v>
+      </c>
+      <c r="E208" t="n">
+        <v>-3.409</v>
       </c>
     </row>
     <row r="209">
@@ -2898,10 +3622,16 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>-17.39</v>
+        <v>-13.77</v>
       </c>
       <c r="C209" t="n">
-        <v>17.39</v>
+        <v>2.88</v>
+      </c>
+      <c r="D209" t="n">
+        <v>14.54</v>
+      </c>
+      <c r="E209" t="n">
+        <v>-3.553</v>
       </c>
     </row>
     <row r="210">
@@ -2909,10 +3639,16 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>-17.58</v>
+        <v>-13.78</v>
       </c>
       <c r="C210" t="n">
-        <v>17.58</v>
+        <v>2.96</v>
+      </c>
+      <c r="D210" t="n">
+        <v>14.64</v>
+      </c>
+      <c r="E210" t="n">
+        <v>-3.717</v>
       </c>
     </row>
     <row r="211">
@@ -2920,10 +3656,16 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>-17.59</v>
+        <v>-13.77</v>
       </c>
       <c r="C211" t="n">
-        <v>17.59</v>
+        <v>3.08</v>
+      </c>
+      <c r="D211" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="E211" t="n">
+        <v>-3.901</v>
       </c>
     </row>
     <row r="212">
@@ -2931,10 +3673,16 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>-17.57</v>
+        <v>-13.85</v>
       </c>
       <c r="C212" t="n">
-        <v>17.57</v>
+        <v>1.65</v>
+      </c>
+      <c r="D212" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="E212" t="n">
+        <v>-2.374</v>
       </c>
     </row>
     <row r="213">
@@ -2942,10 +3690,16 @@
         <v>211</v>
       </c>
       <c r="B213" t="n">
-        <v>-17.57</v>
+        <v>-13.88</v>
       </c>
       <c r="C213" t="n">
-        <v>17.57</v>
+        <v>0.19</v>
+      </c>
+      <c r="D213" t="n">
+        <v>14.72</v>
+      </c>
+      <c r="E213" t="n">
+        <v>-0.9329999999999996</v>
       </c>
     </row>
     <row r="214">
@@ -2953,10 +3707,1206 @@
         <v>212</v>
       </c>
       <c r="B214" t="n">
-        <v>-17.54</v>
+        <v>-13.46</v>
       </c>
       <c r="C214" t="n">
-        <v>17.54</v>
+        <v>-1.45</v>
+      </c>
+      <c r="D214" t="n">
+        <v>14.56</v>
+      </c>
+      <c r="E214" t="n">
+        <v>0.445</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="n">
+        <v>-13.18</v>
+      </c>
+      <c r="C215" t="n">
+        <v>-3.07</v>
+      </c>
+      <c r="D215" t="n">
+        <v>14.58</v>
+      </c>
+      <c r="E215" t="n">
+        <v>1.763</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="n">
+        <v>-12.71</v>
+      </c>
+      <c r="C216" t="n">
+        <v>-4.78</v>
+      </c>
+      <c r="D216" t="n">
+        <v>14.57</v>
+      </c>
+      <c r="E216" t="n">
+        <v>3.024</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="n">
+        <v>-12.39</v>
+      </c>
+      <c r="C217" t="n">
+        <v>-6.29</v>
+      </c>
+      <c r="D217" t="n">
+        <v>14.44</v>
+      </c>
+      <c r="E217" t="n">
+        <v>4.341999999999999</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="n">
+        <v>-11.78</v>
+      </c>
+      <c r="C218" t="n">
+        <v>-7.81</v>
+      </c>
+      <c r="D218" t="n">
+        <v>14.06</v>
+      </c>
+      <c r="E218" t="n">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="n">
+        <v>-11.21</v>
+      </c>
+      <c r="C219" t="n">
+        <v>-9.31</v>
+      </c>
+      <c r="D219" t="n">
+        <v>13.27</v>
+      </c>
+      <c r="E219" t="n">
+        <v>7.348000000000001</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="n">
+        <v>-10.76</v>
+      </c>
+      <c r="C220" t="n">
+        <v>-10.79</v>
+      </c>
+      <c r="D220" t="n">
+        <v>12.66</v>
+      </c>
+      <c r="E220" t="n">
+        <v>8.995999999999999</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="n">
+        <v>-10.32</v>
+      </c>
+      <c r="C221" t="n">
+        <v>-12.38</v>
+      </c>
+      <c r="D221" t="n">
+        <v>12.05</v>
+      </c>
+      <c r="E221" t="n">
+        <v>10.744</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="n">
+        <v>-9.73</v>
+      </c>
+      <c r="C222" t="n">
+        <v>-12.41</v>
+      </c>
+      <c r="D222" t="n">
+        <v>11.52</v>
+      </c>
+      <c r="E222" t="n">
+        <v>10.721</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="n">
+        <v>-9.19</v>
+      </c>
+      <c r="C223" t="n">
+        <v>-12.3</v>
+      </c>
+      <c r="D223" t="n">
+        <v>10.78</v>
+      </c>
+      <c r="E223" t="n">
+        <v>10.807</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="n">
+        <v>-9.01</v>
+      </c>
+      <c r="C224" t="n">
+        <v>-12.2</v>
+      </c>
+      <c r="D224" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="E224" t="n">
+        <v>11.013</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="n">
+        <v>-8.91</v>
+      </c>
+      <c r="C225" t="n">
+        <v>-12.12</v>
+      </c>
+      <c r="D225" t="n">
+        <v>10.04</v>
+      </c>
+      <c r="E225" t="n">
+        <v>11.089</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="n">
+        <v>-8.99</v>
+      </c>
+      <c r="C226" t="n">
+        <v>-11.97</v>
+      </c>
+      <c r="D226" t="n">
+        <v>9.83</v>
+      </c>
+      <c r="E226" t="n">
+        <v>11.232</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="n">
+        <v>-8.93</v>
+      </c>
+      <c r="C227" t="n">
+        <v>-11.98</v>
+      </c>
+      <c r="D227" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="E227" t="n">
+        <v>11.415</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="n">
+        <v>-9.17</v>
+      </c>
+      <c r="C228" t="n">
+        <v>-11.96</v>
+      </c>
+      <c r="D228" t="n">
+        <v>9.609999999999999</v>
+      </c>
+      <c r="E228" t="n">
+        <v>11.618</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="n">
+        <v>-9.35</v>
+      </c>
+      <c r="C229" t="n">
+        <v>-11.94</v>
+      </c>
+      <c r="D229" t="n">
+        <v>10.02</v>
+      </c>
+      <c r="E229" t="n">
+        <v>11.371</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="n">
+        <v>-9.449999999999999</v>
+      </c>
+      <c r="C230" t="n">
+        <v>-11.84</v>
+      </c>
+      <c r="D230" t="n">
+        <v>10.26</v>
+      </c>
+      <c r="E230" t="n">
+        <v>11.127</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="n">
+        <v>-9.550000000000001</v>
+      </c>
+      <c r="C231" t="n">
+        <v>-11.64</v>
+      </c>
+      <c r="D231" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="E231" t="n">
+        <v>10.793</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="n">
+        <v>-9.74</v>
+      </c>
+      <c r="C232" t="n">
+        <v>-11.35</v>
+      </c>
+      <c r="D232" t="n">
+        <v>10.74</v>
+      </c>
+      <c r="E232" t="n">
+        <v>10.449</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="n">
+        <v>-9.93</v>
+      </c>
+      <c r="C233" t="n">
+        <v>-11.18</v>
+      </c>
+      <c r="D233" t="n">
+        <v>10.96</v>
+      </c>
+      <c r="E233" t="n">
+        <v>10.252</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="n">
+        <v>-9.92</v>
+      </c>
+      <c r="C234" t="n">
+        <v>-10.99</v>
+      </c>
+      <c r="D234" t="n">
+        <v>10.98</v>
+      </c>
+      <c r="E234" t="n">
+        <v>10.035</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="n">
+        <v>-9.91</v>
+      </c>
+      <c r="C235" t="n">
+        <v>-10.55</v>
+      </c>
+      <c r="D235" t="n">
+        <v>10.7</v>
+      </c>
+      <c r="E235" t="n">
+        <v>9.856</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="n">
+        <v>-9.9</v>
+      </c>
+      <c r="C236" t="n">
+        <v>-10.31</v>
+      </c>
+      <c r="D236" t="n">
+        <v>10.74</v>
+      </c>
+      <c r="E236" t="n">
+        <v>9.577000000000002</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="n">
+        <v>-9.880000000000001</v>
+      </c>
+      <c r="C237" t="n">
+        <v>-9.98</v>
+      </c>
+      <c r="D237" t="n">
+        <v>10.78</v>
+      </c>
+      <c r="E237" t="n">
+        <v>9.178000000000001</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="n">
+        <v>-9.84</v>
+      </c>
+      <c r="C238" t="n">
+        <v>-9.66</v>
+      </c>
+      <c r="D238" t="n">
+        <v>10.64</v>
+      </c>
+      <c r="E238" t="n">
+        <v>8.959</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="n">
+        <v>-9.640000000000001</v>
+      </c>
+      <c r="C239" t="n">
+        <v>-9.33</v>
+      </c>
+      <c r="D239" t="n">
+        <v>10.52</v>
+      </c>
+      <c r="E239" t="n">
+        <v>8.56</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="B240" t="n">
+        <v>-9.460000000000001</v>
+      </c>
+      <c r="C240" t="n">
+        <v>-9.15</v>
+      </c>
+      <c r="D240" t="n">
+        <v>10.19</v>
+      </c>
+      <c r="E240" t="n">
+        <v>8.523</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="B241" t="n">
+        <v>-9.279999999999999</v>
+      </c>
+      <c r="C241" t="n">
+        <v>-9.02</v>
+      </c>
+      <c r="D241" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="E241" t="n">
+        <v>8.496</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="B242" t="n">
+        <v>-9.09</v>
+      </c>
+      <c r="C242" t="n">
+        <v>-8.9</v>
+      </c>
+      <c r="D242" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="E242" t="n">
+        <v>8.481999999999999</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="n">
+        <v>-8.82</v>
+      </c>
+      <c r="C243" t="n">
+        <v>-8.77</v>
+      </c>
+      <c r="D243" t="n">
+        <v>9.32</v>
+      </c>
+      <c r="E243" t="n">
+        <v>8.367999999999999</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n">
+        <v>242</v>
+      </c>
+      <c r="B244" t="n">
+        <v>-8.84</v>
+      </c>
+      <c r="C244" t="n">
+        <v>-8.33</v>
+      </c>
+      <c r="D244" t="n">
+        <v>9.220000000000001</v>
+      </c>
+      <c r="E244" t="n">
+        <v>8.054</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n">
+        <v>243</v>
+      </c>
+      <c r="B245" t="n">
+        <v>-9</v>
+      </c>
+      <c r="C245" t="n">
+        <v>-7.18</v>
+      </c>
+      <c r="D245" t="n">
+        <v>8.390000000000001</v>
+      </c>
+      <c r="E245" t="n">
+        <v>7.892</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="n">
+        <v>244</v>
+      </c>
+      <c r="B246" t="n">
+        <v>-8.69</v>
+      </c>
+      <c r="C246" t="n">
+        <v>-5.82</v>
+      </c>
+      <c r="D246" t="n">
+        <v>6.93</v>
+      </c>
+      <c r="E246" t="n">
+        <v>7.680000000000001</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="B247" t="n">
+        <v>-8.369999999999999</v>
+      </c>
+      <c r="C247" t="n">
+        <v>-4.56</v>
+      </c>
+      <c r="D247" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="E247" t="n">
+        <v>7.537999999999999</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="n">
+        <v>246</v>
+      </c>
+      <c r="B248" t="n">
+        <v>-8.06</v>
+      </c>
+      <c r="C248" t="n">
+        <v>-3.22</v>
+      </c>
+      <c r="D248" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="E248" t="n">
+        <v>7.146000000000001</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="n">
+        <v>247</v>
+      </c>
+      <c r="B249" t="n">
+        <v>-8.119999999999999</v>
+      </c>
+      <c r="C249" t="n">
+        <v>-1.88</v>
+      </c>
+      <c r="D249" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="E249" t="n">
+        <v>6.884</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="n">
+        <v>248</v>
+      </c>
+      <c r="B250" t="n">
+        <v>-8.16</v>
+      </c>
+      <c r="C250" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="D250" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="E250" t="n">
+        <v>6.316999999999999</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="n">
+        <v>249</v>
+      </c>
+      <c r="B251" t="n">
+        <v>-8.68</v>
+      </c>
+      <c r="C251" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="D251" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="E251" t="n">
+        <v>6.249999999999999</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="n">
+        <v>-9.220000000000001</v>
+      </c>
+      <c r="C252" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="D252" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="E252" t="n">
+        <v>6.289999999999999</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="n">
+        <v>251</v>
+      </c>
+      <c r="B253" t="n">
+        <v>-9.82</v>
+      </c>
+      <c r="C253" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D253" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E253" t="n">
+        <v>6.029999999999999</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="n">
+        <v>252</v>
+      </c>
+      <c r="B254" t="n">
+        <v>-10.83</v>
+      </c>
+      <c r="C254" t="n">
+        <v>5.87</v>
+      </c>
+      <c r="D254" t="n">
+        <v>-0.91</v>
+      </c>
+      <c r="E254" t="n">
+        <v>5.97</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="n">
+        <v>253</v>
+      </c>
+      <c r="B255" t="n">
+        <v>-11.63</v>
+      </c>
+      <c r="C255" t="n">
+        <v>7.27</v>
+      </c>
+      <c r="D255" t="n">
+        <v>-1.44</v>
+      </c>
+      <c r="E255" t="n">
+        <v>5.91</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="B256" t="n">
+        <v>-12.96</v>
+      </c>
+      <c r="C256" t="n">
+        <v>8.49</v>
+      </c>
+      <c r="D256" t="n">
+        <v>-1.84</v>
+      </c>
+      <c r="E256" t="n">
+        <v>6.409999999999999</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="B257" t="n">
+        <v>-14.29</v>
+      </c>
+      <c r="C257" t="n">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="D257" t="n">
+        <v>-2.08</v>
+      </c>
+      <c r="E257" t="n">
+        <v>6.775</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="n">
+        <v>256</v>
+      </c>
+      <c r="B258" t="n">
+        <v>-15.53</v>
+      </c>
+      <c r="C258" t="n">
+        <v>10.77</v>
+      </c>
+      <c r="D258" t="n">
+        <v>-2.33</v>
+      </c>
+      <c r="E258" t="n">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="n">
+        <v>257</v>
+      </c>
+      <c r="B259" t="n">
+        <v>-17.27</v>
+      </c>
+      <c r="C259" t="n">
+        <v>11.85</v>
+      </c>
+      <c r="D259" t="n">
+        <v>-2.83</v>
+      </c>
+      <c r="E259" t="n">
+        <v>8.344999999999999</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="n">
+        <v>258</v>
+      </c>
+      <c r="B260" t="n">
+        <v>-18.93</v>
+      </c>
+      <c r="C260" t="n">
+        <v>12.85</v>
+      </c>
+      <c r="D260" t="n">
+        <v>-3.34</v>
+      </c>
+      <c r="E260" t="n">
+        <v>9.52</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="n">
+        <v>259</v>
+      </c>
+      <c r="B261" t="n">
+        <v>-20.09</v>
+      </c>
+      <c r="C261" t="n">
+        <v>13.84</v>
+      </c>
+      <c r="D261" t="n">
+        <v>-3.95</v>
+      </c>
+      <c r="E261" t="n">
+        <v>10.295</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="B262" t="n">
+        <v>-21.16</v>
+      </c>
+      <c r="C262" t="n">
+        <v>14.87</v>
+      </c>
+      <c r="D262" t="n">
+        <v>-4.61</v>
+      </c>
+      <c r="E262" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="n">
+        <v>261</v>
+      </c>
+      <c r="B263" t="n">
+        <v>-21.89</v>
+      </c>
+      <c r="C263" t="n">
+        <v>15.91</v>
+      </c>
+      <c r="D263" t="n">
+        <v>-5.74</v>
+      </c>
+      <c r="E263" t="n">
+        <v>11.815</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1" t="n">
+        <v>262</v>
+      </c>
+      <c r="B264" t="n">
+        <v>-22.22</v>
+      </c>
+      <c r="C264" t="n">
+        <v>15.63</v>
+      </c>
+      <c r="D264" t="n">
+        <v>-5.96</v>
+      </c>
+      <c r="E264" t="n">
+        <v>12.65</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1" t="n">
+        <v>263</v>
+      </c>
+      <c r="B265" t="n">
+        <v>-22.59</v>
+      </c>
+      <c r="C265" t="n">
+        <v>15.33</v>
+      </c>
+      <c r="D265" t="n">
+        <v>-6.12</v>
+      </c>
+      <c r="E265" t="n">
+        <v>13.485</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1" t="n">
+        <v>264</v>
+      </c>
+      <c r="B266" t="n">
+        <v>-22.78</v>
+      </c>
+      <c r="C266" t="n">
+        <v>15.21</v>
+      </c>
+      <c r="D266" t="n">
+        <v>-6.17</v>
+      </c>
+      <c r="E266" t="n">
+        <v>13.84</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="1" t="n">
+        <v>265</v>
+      </c>
+      <c r="B267" t="n">
+        <v>-22.99</v>
+      </c>
+      <c r="C267" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="D267" t="n">
+        <v>-6.21</v>
+      </c>
+      <c r="E267" t="n">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="B268" t="n">
+        <v>-22.6</v>
+      </c>
+      <c r="C268" t="n">
+        <v>14.39</v>
+      </c>
+      <c r="D268" t="n">
+        <v>-6.24</v>
+      </c>
+      <c r="E268" t="n">
+        <v>14.56</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="B269" t="n">
+        <v>-21.56</v>
+      </c>
+      <c r="C269" t="n">
+        <v>13.66</v>
+      </c>
+      <c r="D269" t="n">
+        <v>-6.2</v>
+      </c>
+      <c r="E269" t="n">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>268</v>
+      </c>
+      <c r="B270" t="n">
+        <v>-20.56</v>
+      </c>
+      <c r="C270" t="n">
+        <v>13.02</v>
+      </c>
+      <c r="D270" t="n">
+        <v>-6.17</v>
+      </c>
+      <c r="E270" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="B271" t="n">
+        <v>-19.59</v>
+      </c>
+      <c r="C271" t="n">
+        <v>12.38</v>
+      </c>
+      <c r="D271" t="n">
+        <v>-6.02</v>
+      </c>
+      <c r="E271" t="n">
+        <v>13.33</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="B272" t="n">
+        <v>-18.31</v>
+      </c>
+      <c r="C272" t="n">
+        <v>11.37</v>
+      </c>
+      <c r="D272" t="n">
+        <v>-5.81</v>
+      </c>
+      <c r="E272" t="n">
+        <v>12.86</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="B273" t="n">
+        <v>-17.32</v>
+      </c>
+      <c r="C273" t="n">
+        <v>10.34</v>
+      </c>
+      <c r="D273" t="n">
+        <v>-5.51</v>
+      </c>
+      <c r="E273" t="n">
+        <v>12.59</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>272</v>
+      </c>
+      <c r="B274" t="n">
+        <v>-16.18</v>
+      </c>
+      <c r="C274" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="D274" t="n">
+        <v>-5.22</v>
+      </c>
+      <c r="E274" t="n">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="n">
+        <v>273</v>
+      </c>
+      <c r="B275" t="n">
+        <v>-14.96</v>
+      </c>
+      <c r="C275" t="n">
+        <v>8.07</v>
+      </c>
+      <c r="D275" t="n">
+        <v>-5.03</v>
+      </c>
+      <c r="E275" t="n">
+        <v>12.02</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="B276" t="n">
+        <v>-13.88</v>
+      </c>
+      <c r="C276" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="D276" t="n">
+        <v>-5.08</v>
+      </c>
+      <c r="E276" t="n">
+        <v>11.71</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="n">
+        <v>275</v>
+      </c>
+      <c r="B277" t="n">
+        <v>-12.77</v>
+      </c>
+      <c r="C277" t="n">
+        <v>6.61</v>
+      </c>
+      <c r="D277" t="n">
+        <v>-5.31</v>
+      </c>
+      <c r="E277" t="n">
+        <v>11.57</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1" t="n">
+        <v>276</v>
+      </c>
+      <c r="B278" t="n">
+        <v>-12.55</v>
+      </c>
+      <c r="C278" t="n">
+        <v>6.54</v>
+      </c>
+      <c r="D278" t="n">
+        <v>-5.6</v>
+      </c>
+      <c r="E278" t="n">
+        <v>11.705</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1" t="n">
+        <v>277</v>
+      </c>
+      <c r="B279" t="n">
+        <v>-12.33</v>
+      </c>
+      <c r="C279" t="n">
+        <v>6.62</v>
+      </c>
+      <c r="D279" t="n">
+        <v>-5.96</v>
+      </c>
+      <c r="E279" t="n">
+        <v>11.77</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="n">
+        <v>278</v>
+      </c>
+      <c r="B280" t="n">
+        <v>-12.13</v>
+      </c>
+      <c r="C280" t="n">
+        <v>6.68</v>
+      </c>
+      <c r="D280" t="n">
+        <v>-6.31</v>
+      </c>
+      <c r="E280" t="n">
+        <v>11.855</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="n">
+        <v>279</v>
+      </c>
+      <c r="B281" t="n">
+        <v>-11.92</v>
+      </c>
+      <c r="C281" t="n">
+        <v>6.72</v>
+      </c>
+      <c r="D281" t="n">
+        <v>-6.71</v>
+      </c>
+      <c r="E281" t="n">
+        <v>12.01</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="n">
+        <v>280</v>
+      </c>
+      <c r="B282" t="n">
+        <v>-12.37</v>
+      </c>
+      <c r="C282" t="n">
+        <v>7.14</v>
+      </c>
+      <c r="D282" t="n">
+        <v>-7.17</v>
+      </c>
+      <c r="E282" t="n">
+        <v>12.495</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="n">
+        <v>281</v>
+      </c>
+      <c r="B283" t="n">
+        <v>-12.54</v>
+      </c>
+      <c r="C283" t="n">
+        <v>7.57</v>
+      </c>
+      <c r="D283" t="n">
+        <v>-7.9</v>
+      </c>
+      <c r="E283" t="n">
+        <v>12.97</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="n">
+        <v>282</v>
+      </c>
+      <c r="B284" t="n">
+        <v>-12.82</v>
+      </c>
+      <c r="C284" t="n">
+        <v>8.08</v>
+      </c>
+      <c r="D284" t="n">
+        <v>-8.619999999999999</v>
+      </c>
+      <c r="E284" t="n">
+        <v>13.465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A few good changes made
Old data is wiped from current session stats in Excel. For example, if PLO isn't played that session, no PLO sheet is shown. This is for clarity. Also, regex expressions were not added; I didn't find them too necessary.
</commit_message>
<xml_diff>
--- a/Outputs/net_over_time_avg.xlsx
+++ b/Outputs/net_over_time_avg.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId1"/>
@@ -26,7 +25,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +50,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +75,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -149,7 +162,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Net vs time this session (07/05/21): 10-hand moving averages</a:t>
+              <a:t>Net vs time this session (06/24/21): 10-hand moving averages</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -181,7 +194,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$B$2:$B$176</f>
+              <f>'data'!$B$2:$B$227</f>
             </numRef>
           </val>
         </ser>
@@ -208,7 +221,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$C$2:$C$176</f>
+              <f>'data'!$C$2:$C$227</f>
             </numRef>
           </val>
         </ser>
@@ -235,7 +248,61 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$D$2:$D$176</f>
+              <f>'data'!$D$2:$D$227</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <strRef>
+              <f>'data'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'data'!$E$2:$E$227</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <strRef>
+              <f>'data'!F1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'data'!$F$2:$F$227</f>
             </numRef>
           </val>
         </ser>
@@ -605,9 +672,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D176"/>
+  <dimension ref="A1:F227"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -621,7 +688,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Fish</t>
+          <t>Scott</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -631,7 +698,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Scott</t>
+          <t>Cedric</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Cheyenne</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Fish</t>
         </is>
       </c>
     </row>
@@ -654,13 +731,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.35</v>
+        <v>-1</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.05</v>
+        <v>1.1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="4">
@@ -668,13 +745,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.7</v>
+        <v>-1.33</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2</v>
+        <v>1.43</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="5">
@@ -682,13 +759,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.02</v>
+        <v>1.95</v>
       </c>
       <c r="C5" t="n">
-        <v>0.17</v>
+        <v>1.46</v>
       </c>
       <c r="D5" t="n">
-        <v>0.85</v>
+        <v>-3.41</v>
       </c>
     </row>
     <row r="6">
@@ -696,13 +773,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.26</v>
+        <v>3.9</v>
       </c>
       <c r="C6" t="n">
-        <v>0.14</v>
+        <v>1.49</v>
       </c>
       <c r="D6" t="n">
-        <v>1.12</v>
+        <v>-5.4</v>
       </c>
     </row>
     <row r="7">
@@ -710,13 +787,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.52</v>
+        <v>5.25</v>
       </c>
       <c r="C7" t="n">
-        <v>0.12</v>
+        <v>1.5</v>
       </c>
       <c r="D7" t="n">
-        <v>1.4</v>
+        <v>-6.75</v>
       </c>
     </row>
     <row r="8">
@@ -724,13 +801,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.67</v>
+        <v>6.23</v>
       </c>
       <c r="C8" t="n">
-        <v>0.07000000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="D8" t="n">
-        <v>1.6</v>
+        <v>-7.74</v>
       </c>
     </row>
     <row r="9">
@@ -738,13 +815,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.94</v>
+        <v>6.96</v>
       </c>
       <c r="C9" t="n">
-        <v>0.19</v>
+        <v>1.52</v>
       </c>
       <c r="D9" t="n">
-        <v>1.75</v>
+        <v>-8.470000000000001</v>
       </c>
     </row>
     <row r="10">
@@ -752,13 +829,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.21</v>
+        <v>7.6</v>
       </c>
       <c r="C10" t="n">
-        <v>0.34</v>
+        <v>1.52</v>
       </c>
       <c r="D10" t="n">
-        <v>1.87</v>
+        <v>-9.119999999999999</v>
       </c>
     </row>
     <row r="11">
@@ -766,13 +843,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-2.37</v>
+        <v>8.119999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>0.41</v>
+        <v>1.52</v>
       </c>
       <c r="D11" t="n">
-        <v>1.96</v>
+        <v>-9.640000000000001</v>
       </c>
     </row>
     <row r="12">
@@ -780,13 +857,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-2.37</v>
+        <v>8.119999999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>0.41</v>
+        <v>1.52</v>
       </c>
       <c r="D12" t="n">
-        <v>1.96</v>
+        <v>-9.640000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -794,13 +871,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-2.77</v>
+        <v>9.390000000000001</v>
       </c>
       <c r="C13" t="n">
-        <v>0.53</v>
+        <v>1.65</v>
       </c>
       <c r="D13" t="n">
-        <v>2.24</v>
+        <v>-11.04</v>
       </c>
     </row>
     <row r="14">
@@ -808,13 +885,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-3.16</v>
+        <v>11.31</v>
       </c>
       <c r="C14" t="n">
-        <v>0.72</v>
+        <v>1.56</v>
       </c>
       <c r="D14" t="n">
-        <v>2.44</v>
+        <v>-12.87</v>
       </c>
     </row>
     <row r="15">
@@ -822,13 +899,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-3.42</v>
+        <v>13.25</v>
       </c>
       <c r="C15" t="n">
-        <v>0.77</v>
+        <v>1.47</v>
       </c>
       <c r="D15" t="n">
-        <v>2.65</v>
+        <v>-14.72</v>
       </c>
     </row>
     <row r="16">
@@ -836,13 +913,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-3.63</v>
+        <v>13.8</v>
       </c>
       <c r="C16" t="n">
-        <v>0.89</v>
+        <v>1.45</v>
       </c>
       <c r="D16" t="n">
-        <v>2.74</v>
+        <v>-15.25</v>
       </c>
     </row>
     <row r="17">
@@ -850,13 +927,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-3.81</v>
+        <v>13.79</v>
       </c>
       <c r="C17" t="n">
-        <v>1.01</v>
+        <v>2.06</v>
       </c>
       <c r="D17" t="n">
-        <v>2.8</v>
+        <v>-15.85</v>
       </c>
     </row>
     <row r="18">
@@ -864,13 +941,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-3.99</v>
+        <v>13.45</v>
       </c>
       <c r="C18" t="n">
-        <v>1.19</v>
+        <v>3</v>
       </c>
       <c r="D18" t="n">
-        <v>2.8</v>
+        <v>-16.45</v>
       </c>
     </row>
     <row r="19">
@@ -878,13 +955,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-4.16</v>
+        <v>13.09</v>
       </c>
       <c r="C19" t="n">
-        <v>1.39</v>
+        <v>3.99</v>
       </c>
       <c r="D19" t="n">
-        <v>2.77</v>
+        <v>-17.08</v>
       </c>
     </row>
     <row r="20">
@@ -892,13 +969,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-4.03</v>
+        <v>12.82</v>
       </c>
       <c r="C20" t="n">
-        <v>1.29</v>
+        <v>4.9</v>
       </c>
       <c r="D20" t="n">
-        <v>2.74</v>
+        <v>-17.72</v>
       </c>
     </row>
     <row r="21">
@@ -906,13 +983,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-3.81</v>
+        <v>12.49</v>
       </c>
       <c r="C21" t="n">
-        <v>1.12</v>
+        <v>5.81</v>
       </c>
       <c r="D21" t="n">
-        <v>2.69</v>
+        <v>-18.3</v>
       </c>
     </row>
     <row r="22">
@@ -920,13 +997,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-3.67</v>
+        <v>12.27</v>
       </c>
       <c r="C22" t="n">
-        <v>1.04</v>
+        <v>6.67</v>
       </c>
       <c r="D22" t="n">
-        <v>2.63</v>
+        <v>-18.94</v>
       </c>
     </row>
     <row r="23">
@@ -934,13 +1011,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-3.45</v>
+        <v>12.16</v>
       </c>
       <c r="C23" t="n">
-        <v>0.88</v>
+        <v>7.47</v>
       </c>
       <c r="D23" t="n">
-        <v>2.57</v>
+        <v>-19.62</v>
       </c>
     </row>
     <row r="24">
@@ -948,13 +1025,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-2.98</v>
+        <v>11.61</v>
       </c>
       <c r="C24" t="n">
-        <v>0.49</v>
+        <v>8.27</v>
       </c>
       <c r="D24" t="n">
-        <v>2.51</v>
+        <v>-19.88</v>
       </c>
     </row>
     <row r="25">
@@ -962,13 +1039,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-2.59</v>
+        <v>11.03</v>
       </c>
       <c r="C25" t="n">
-        <v>0.18</v>
+        <v>9.09</v>
       </c>
       <c r="D25" t="n">
-        <v>2.45</v>
+        <v>-20.12</v>
       </c>
     </row>
     <row r="26">
@@ -976,13 +1053,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-2.2</v>
+        <v>10.27</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.13</v>
+        <v>11.51</v>
       </c>
       <c r="D26" t="n">
-        <v>2.39</v>
+        <v>-21.78</v>
       </c>
     </row>
     <row r="27">
@@ -990,13 +1067,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-1.81</v>
+        <v>10.07</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.44</v>
+        <v>13.3</v>
       </c>
       <c r="D27" t="n">
-        <v>2.33</v>
+        <v>-23.37</v>
       </c>
     </row>
     <row r="28">
@@ -1004,13 +1081,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-1.37</v>
+        <v>10.24</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.8</v>
+        <v>14.75</v>
       </c>
       <c r="D28" t="n">
-        <v>2.27</v>
+        <v>-24.99</v>
       </c>
     </row>
     <row r="29">
@@ -1018,13 +1095,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>-1.02</v>
+        <v>10.42</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.1</v>
+        <v>16.16</v>
       </c>
       <c r="D29" t="n">
-        <v>2.24</v>
+        <v>-26.58</v>
       </c>
     </row>
     <row r="30">
@@ -1032,13 +1109,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.86</v>
+        <v>10.5</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.21</v>
+        <v>17.65</v>
       </c>
       <c r="D30" t="n">
-        <v>2.21</v>
+        <v>-28.18</v>
       </c>
     </row>
     <row r="31">
@@ -1046,13 +1123,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.75</v>
+        <v>10.59</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.29</v>
+        <v>19.14</v>
       </c>
       <c r="D31" t="n">
-        <v>2.2</v>
+        <v>-29.79</v>
       </c>
     </row>
     <row r="32">
@@ -1060,13 +1137,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.68</v>
+        <v>10.5</v>
       </c>
       <c r="C32" t="n">
-        <v>-1.34</v>
+        <v>20.69</v>
       </c>
       <c r="D32" t="n">
-        <v>2.2</v>
+        <v>-31.28</v>
       </c>
     </row>
     <row r="33">
@@ -1074,13 +1151,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.66</v>
+        <v>10.25</v>
       </c>
       <c r="C33" t="n">
-        <v>-1.34</v>
+        <v>22.35</v>
       </c>
       <c r="D33" t="n">
-        <v>2.2</v>
+        <v>-32.69</v>
       </c>
     </row>
     <row r="34">
@@ -1088,13 +1165,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.84</v>
+        <v>10.04</v>
       </c>
       <c r="C34" t="n">
-        <v>-1.16</v>
+        <v>23.98</v>
       </c>
       <c r="D34" t="n">
-        <v>2.2</v>
+        <v>-34.11</v>
       </c>
     </row>
     <row r="35">
@@ -1102,13 +1179,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.99</v>
+        <v>9.92</v>
       </c>
       <c r="C35" t="n">
-        <v>-1.01</v>
+        <v>25.6</v>
       </c>
       <c r="D35" t="n">
-        <v>2.2</v>
+        <v>-35.61</v>
       </c>
     </row>
     <row r="36">
@@ -1116,13 +1193,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-1.11</v>
+        <v>9.94</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.89</v>
+        <v>25.72</v>
       </c>
       <c r="D36" t="n">
-        <v>2.2</v>
+        <v>-35.75</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1130,13 +1210,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-1.26</v>
+        <v>9.949999999999999</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.74</v>
+        <v>25.83</v>
       </c>
       <c r="D37" t="n">
-        <v>2.2</v>
+        <v>-35.87</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1144,13 +1227,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-1.46</v>
+        <v>9.84</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.54</v>
+        <v>26.07</v>
       </c>
       <c r="D38" t="n">
-        <v>2.2</v>
+        <v>-36.01</v>
+      </c>
+      <c r="E38" t="n">
+        <v>-0.06666666666666667</v>
       </c>
     </row>
     <row r="39">
@@ -1158,13 +1244,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-1.62</v>
+        <v>9.76</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.38</v>
+        <v>26.3</v>
       </c>
       <c r="D39" t="n">
-        <v>2.2</v>
+        <v>-36.12</v>
+      </c>
+      <c r="E39" t="n">
+        <v>-0.125</v>
       </c>
     </row>
     <row r="40">
@@ -1172,13 +1261,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-1.89</v>
+        <v>9.720000000000001</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.11</v>
+        <v>26.5</v>
       </c>
       <c r="D40" t="n">
-        <v>2.18</v>
+        <v>-36.23</v>
+      </c>
+      <c r="E40" t="n">
+        <v>-0.16</v>
       </c>
     </row>
     <row r="41">
@@ -1186,13 +1278,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-2.16</v>
+        <v>9.84</v>
       </c>
       <c r="C41" t="n">
-        <v>0.14</v>
+        <v>26.7</v>
       </c>
       <c r="D41" t="n">
-        <v>2.18</v>
+        <v>-36.48</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-0.2833333333333333</v>
       </c>
     </row>
     <row r="42">
@@ -1200,13 +1295,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-2.31</v>
+        <v>10.08</v>
       </c>
       <c r="C42" t="n">
-        <v>0.27</v>
+        <v>26.89</v>
       </c>
       <c r="D42" t="n">
-        <v>2.18</v>
+        <v>-36.8</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-0.4</v>
       </c>
     </row>
     <row r="43">
@@ -1214,13 +1312,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>-2.47</v>
+        <v>10.47</v>
       </c>
       <c r="C43" t="n">
-        <v>0.4</v>
+        <v>27.05</v>
       </c>
       <c r="D43" t="n">
-        <v>2.19</v>
+        <v>-37.25</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-0.4999999999999999</v>
       </c>
     </row>
     <row r="44">
@@ -1228,13 +1329,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-2.55</v>
+        <v>10.81</v>
       </c>
       <c r="C44" t="n">
-        <v>0.46</v>
+        <v>27.26</v>
       </c>
       <c r="D44" t="n">
-        <v>2.19</v>
+        <v>-37.67</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-0.5777777777777778</v>
       </c>
     </row>
     <row r="45">
@@ -1242,13 +1346,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>-2.49</v>
+        <v>11.07</v>
       </c>
       <c r="C45" t="n">
-        <v>0.46</v>
+        <v>27.52</v>
       </c>
       <c r="D45" t="n">
-        <v>2.11</v>
+        <v>-38.07</v>
+      </c>
+      <c r="E45" t="n">
+        <v>-0.6399999999999999</v>
       </c>
     </row>
     <row r="46">
@@ -1256,13 +1363,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-2.51</v>
+        <v>11.45</v>
       </c>
       <c r="C46" t="n">
-        <v>0.46</v>
+        <v>27.61</v>
       </c>
       <c r="D46" t="n">
-        <v>2.11</v>
+        <v>-38.42</v>
+      </c>
+      <c r="E46" t="n">
+        <v>-0.6399999999999999</v>
       </c>
     </row>
     <row r="47">
@@ -1270,13 +1380,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>-2.26</v>
+        <v>11.86</v>
       </c>
       <c r="C47" t="n">
-        <v>0.2</v>
+        <v>27.71</v>
       </c>
       <c r="D47" t="n">
-        <v>2.1</v>
+        <v>-38.78</v>
+      </c>
+      <c r="E47" t="n">
+        <v>-0.78</v>
       </c>
     </row>
     <row r="48">
@@ -1284,13 +1397,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-2.01</v>
+        <v>12.39</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.14</v>
+        <v>27.63</v>
       </c>
       <c r="D48" t="n">
-        <v>2.17</v>
+        <v>-39.09</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-0.93</v>
       </c>
     </row>
     <row r="49">
@@ -1298,13 +1414,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-1.77</v>
+        <v>12.9</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.51</v>
+        <v>27.54</v>
       </c>
       <c r="D49" t="n">
-        <v>2.27</v>
+        <v>-39.43</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-1.01</v>
       </c>
     </row>
     <row r="50">
@@ -1312,13 +1431,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-1.47</v>
+        <v>13.39</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.99</v>
+        <v>27.48</v>
       </c>
       <c r="D50" t="n">
-        <v>2.46</v>
+        <v>-39.79</v>
+      </c>
+      <c r="E50" t="n">
+        <v>-1.08</v>
       </c>
     </row>
     <row r="51">
@@ -1326,13 +1448,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-1.16</v>
+        <v>13.7</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.99</v>
+        <v>27.45</v>
       </c>
       <c r="D51" t="n">
-        <v>2.15</v>
+        <v>-39.98</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-1.17</v>
       </c>
     </row>
     <row r="52">
@@ -1340,13 +1465,19 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.91</v>
+        <v>13.94</v>
       </c>
       <c r="C52" t="n">
-        <v>-1.08</v>
+        <v>27.45</v>
       </c>
       <c r="D52" t="n">
-        <v>1.99</v>
+        <v>-40.18</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-1.21</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1354,13 +1485,19 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-0.68</v>
+        <v>14.1</v>
       </c>
       <c r="C53" t="n">
-        <v>-1.15</v>
+        <v>27.39</v>
       </c>
       <c r="D53" t="n">
-        <v>1.84</v>
+        <v>-40.26</v>
+      </c>
+      <c r="E53" t="n">
+        <v>-1.23</v>
+      </c>
+      <c r="F53" t="n">
+        <v>-0.1</v>
       </c>
     </row>
     <row r="54">
@@ -1368,13 +1505,19 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-0.5</v>
+        <v>14.25</v>
       </c>
       <c r="C54" t="n">
-        <v>-1.19</v>
+        <v>27.33</v>
       </c>
       <c r="D54" t="n">
-        <v>1.7</v>
+        <v>-40.32</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-1.24</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-0.2</v>
       </c>
     </row>
     <row r="55">
@@ -1382,13 +1525,19 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>-0.5</v>
+        <v>14.45</v>
       </c>
       <c r="C55" t="n">
-        <v>-1.16</v>
+        <v>27.2</v>
       </c>
       <c r="D55" t="n">
-        <v>1.66</v>
+        <v>-40.34</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-1.25</v>
+      </c>
+      <c r="F55" t="n">
+        <v>-0.25</v>
       </c>
     </row>
     <row r="56">
@@ -1396,13 +1545,19 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>-0.57</v>
+        <v>14.64</v>
       </c>
       <c r="C56" t="n">
-        <v>-1.12</v>
+        <v>27.13</v>
       </c>
       <c r="D56" t="n">
-        <v>1.54</v>
+        <v>-40.35</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-1.32</v>
+      </c>
+      <c r="F56" t="n">
+        <v>-0.28</v>
       </c>
     </row>
     <row r="57">
@@ -1410,13 +1565,19 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.36</v>
+        <v>14.81</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.6899999999999999</v>
+        <v>27.07</v>
       </c>
       <c r="D57" t="n">
-        <v>0.89</v>
+        <v>-40.36</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-1.38</v>
+      </c>
+      <c r="F57" t="n">
+        <v>-0.3</v>
       </c>
     </row>
     <row r="58">
@@ -1424,13 +1585,19 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.02</v>
+        <v>14.91</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.25</v>
+        <v>27.06</v>
       </c>
       <c r="D58" t="n">
-        <v>0.08</v>
+        <v>-40.39</v>
+      </c>
+      <c r="E58" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="F58" t="n">
+        <v>-0.3428571428571429</v>
       </c>
     </row>
     <row r="59">
@@ -1438,13 +1605,19 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.79</v>
+        <v>14.81</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.17</v>
+        <v>28.24</v>
       </c>
       <c r="D59" t="n">
-        <v>-0.77</v>
+        <v>-41.34</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-1.47</v>
+      </c>
+      <c r="F59" t="n">
+        <v>-0.6600000000000001</v>
       </c>
     </row>
     <row r="60">
@@ -1452,13 +1625,19 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>1.65</v>
+        <v>14.64</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.11</v>
+        <v>29.7</v>
       </c>
       <c r="D60" t="n">
-        <v>-1.69</v>
+        <v>-42.28</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-1.54</v>
+      </c>
+      <c r="F60" t="n">
+        <v>-0.9955555555555556</v>
       </c>
     </row>
     <row r="61">
@@ -1466,13 +1645,19 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>2.62</v>
+        <v>14.59</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.63</v>
+        <v>31.13</v>
       </c>
       <c r="D61" t="n">
-        <v>-2.15</v>
+        <v>-43.21</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-1.61</v>
+      </c>
+      <c r="F61" t="n">
+        <v>-1.264</v>
       </c>
     </row>
     <row r="62">
@@ -1480,13 +1665,19 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>3.6</v>
+        <v>14.71</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.99</v>
+        <v>32.37</v>
       </c>
       <c r="D62" t="n">
-        <v>-2.77</v>
+        <v>-44.13</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-1.68</v>
+      </c>
+      <c r="F62" t="n">
+        <v>-1.264</v>
       </c>
     </row>
     <row r="63">
@@ -1494,13 +1685,19 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>4.54</v>
+        <v>14.83</v>
       </c>
       <c r="C63" t="n">
-        <v>-1.55</v>
+        <v>33.64</v>
       </c>
       <c r="D63" t="n">
-        <v>-3.15</v>
+        <v>-45.11</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-1.56</v>
+      </c>
+      <c r="F63" t="n">
+        <v>-1.802</v>
       </c>
     </row>
     <row r="64">
@@ -1508,13 +1705,19 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>5.41</v>
+        <v>14.18</v>
       </c>
       <c r="C64" t="n">
-        <v>-2.09</v>
+        <v>35.74</v>
       </c>
       <c r="D64" t="n">
-        <v>-3.47</v>
+        <v>-46.11</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-1.44</v>
+      </c>
+      <c r="F64" t="n">
+        <v>-2.377</v>
       </c>
     </row>
     <row r="65">
@@ -1522,13 +1725,19 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>6.22</v>
+        <v>13.5</v>
       </c>
       <c r="C65" t="n">
-        <v>-2.8</v>
+        <v>37.85</v>
       </c>
       <c r="D65" t="n">
-        <v>-3.57</v>
+        <v>-47.09</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-1.34</v>
+      </c>
+      <c r="F65" t="n">
+        <v>-2.922</v>
       </c>
     </row>
     <row r="66">
@@ -1536,13 +1745,19 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>7.06</v>
+        <v>12.76</v>
       </c>
       <c r="C66" t="n">
-        <v>-3.4</v>
+        <v>40.05</v>
       </c>
       <c r="D66" t="n">
-        <v>-3.66</v>
+        <v>-48.06</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-1.2</v>
+      </c>
+      <c r="F66" t="n">
+        <v>-3.547</v>
       </c>
     </row>
     <row r="67">
@@ -1550,13 +1765,19 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>7.36</v>
+        <v>12.02</v>
       </c>
       <c r="C67" t="n">
-        <v>-4.13</v>
+        <v>42.12</v>
       </c>
       <c r="D67" t="n">
-        <v>-3.23</v>
+        <v>-49.04</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-1.05</v>
+      </c>
+      <c r="F67" t="n">
+        <v>-4.052</v>
       </c>
     </row>
     <row r="68">
@@ -1564,13 +1785,19 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>7.64</v>
+        <v>11.1</v>
       </c>
       <c r="C68" t="n">
-        <v>-4.91</v>
+        <v>44.21</v>
       </c>
       <c r="D68" t="n">
-        <v>-2.73</v>
+        <v>-50</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-0.93</v>
+      </c>
+      <c r="F68" t="n">
+        <v>-4.377000000000001</v>
       </c>
     </row>
     <row r="69">
@@ -1578,13 +1805,19 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>7.52</v>
+        <v>10.54</v>
       </c>
       <c r="C69" t="n">
-        <v>-5.3</v>
+        <v>45.11</v>
       </c>
       <c r="D69" t="n">
-        <v>-2.22</v>
+        <v>-50</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-0.8899999999999999</v>
+      </c>
+      <c r="F69" t="n">
+        <v>-4.762000000000001</v>
       </c>
     </row>
     <row r="70">
@@ -1592,13 +1825,19 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>7.39</v>
+        <v>9.98</v>
       </c>
       <c r="C70" t="n">
-        <v>-5.76</v>
+        <v>45.71</v>
       </c>
       <c r="D70" t="n">
-        <v>-1.63</v>
+        <v>-50</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-0.86</v>
+      </c>
+      <c r="F70" t="n">
+        <v>-4.829000000000001</v>
       </c>
     </row>
     <row r="71">
@@ -1606,13 +1845,19 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>7.28</v>
+        <v>9.32</v>
       </c>
       <c r="C71" t="n">
-        <v>-6.14</v>
+        <v>46.25</v>
       </c>
       <c r="D71" t="n">
-        <v>-1.14</v>
+        <v>-50</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-0.8099999999999998</v>
+      </c>
+      <c r="F71" t="n">
+        <v>-4.756000000000001</v>
       </c>
     </row>
     <row r="72">
@@ -1620,13 +1865,19 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>7.14</v>
+        <v>8.550000000000001</v>
       </c>
       <c r="C72" t="n">
-        <v>-6.5</v>
+        <v>46.96</v>
       </c>
       <c r="D72" t="n">
-        <v>-0.64</v>
+        <v>-50</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-0.7899999999999998</v>
+      </c>
+      <c r="F72" t="n">
+        <v>-4.723000000000001</v>
       </c>
     </row>
     <row r="73">
@@ -1634,13 +1885,19 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>6.91</v>
+        <v>7.71</v>
       </c>
       <c r="C73" t="n">
-        <v>-6.67</v>
+        <v>47.69</v>
       </c>
       <c r="D73" t="n">
-        <v>-0.24</v>
+        <v>-50</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-1.22</v>
+      </c>
+      <c r="F73" t="n">
+        <v>-4.180000000000001</v>
       </c>
     </row>
     <row r="74">
@@ -1648,13 +1905,19 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>6.59</v>
+        <v>7.71</v>
       </c>
       <c r="C74" t="n">
-        <v>-6.83</v>
+        <v>47.53</v>
       </c>
       <c r="D74" t="n">
-        <v>0.24</v>
+        <v>-50</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-1.660000000000001</v>
+      </c>
+      <c r="F74" t="n">
+        <v>-3.58</v>
       </c>
     </row>
     <row r="75">
@@ -1662,13 +1925,19 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>6.33</v>
+        <v>7.73</v>
       </c>
       <c r="C75" t="n">
-        <v>-6.81</v>
+        <v>47.36</v>
       </c>
       <c r="D75" t="n">
-        <v>0.47</v>
+        <v>-50</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-2.08</v>
+      </c>
+      <c r="F75" t="n">
+        <v>-3.009999999999999</v>
       </c>
     </row>
     <row r="76">
@@ -1676,13 +1945,19 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>6.19</v>
+        <v>7.5</v>
       </c>
       <c r="C76" t="n">
-        <v>-6.84</v>
+        <v>47.09</v>
       </c>
       <c r="D76" t="n">
-        <v>0.65</v>
+        <v>-50</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-2.48</v>
+      </c>
+      <c r="F76" t="n">
+        <v>-2.11</v>
       </c>
     </row>
     <row r="77">
@@ -1690,13 +1965,19 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>6.07</v>
+        <v>7.26</v>
       </c>
       <c r="C77" t="n">
-        <v>-6.89</v>
+        <v>46.94</v>
       </c>
       <c r="D77" t="n">
-        <v>0.82</v>
+        <v>-50</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="F77" t="n">
+        <v>-1.3</v>
       </c>
     </row>
     <row r="78">
@@ -1704,13 +1985,19 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>5.86</v>
+        <v>7.2</v>
       </c>
       <c r="C78" t="n">
-        <v>-6.87</v>
+        <v>46.77</v>
       </c>
       <c r="D78" t="n">
-        <v>1.01</v>
+        <v>-50</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-3.3</v>
+      </c>
+      <c r="F78" t="n">
+        <v>-0.67</v>
       </c>
     </row>
     <row r="79">
@@ -1718,13 +2005,19 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>5.67</v>
+        <v>6.64</v>
       </c>
       <c r="C79" t="n">
-        <v>-6.87</v>
+        <v>47.04</v>
       </c>
       <c r="D79" t="n">
-        <v>1.2</v>
+        <v>-50</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-3.699999999999999</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.02000000000000011</v>
       </c>
     </row>
     <row r="80">
@@ -1732,13 +2025,19 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>5.62</v>
+        <v>6.16</v>
       </c>
       <c r="C80" t="n">
-        <v>-6.79</v>
+        <v>47.33</v>
       </c>
       <c r="D80" t="n">
-        <v>1.17</v>
+        <v>-50</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-4.089999999999999</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.6000000000000001</v>
       </c>
     </row>
     <row r="81">
@@ -1746,13 +2045,19 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>5.55</v>
+        <v>4.75</v>
       </c>
       <c r="C81" t="n">
-        <v>-6.81</v>
+        <v>48.7</v>
       </c>
       <c r="D81" t="n">
-        <v>1.25</v>
+        <v>-50</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-4.499999999999999</v>
+      </c>
+      <c r="F81" t="n">
+        <v>1.05</v>
       </c>
     </row>
     <row r="82">
@@ -1760,13 +2065,19 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>5.59</v>
+        <v>3.26</v>
       </c>
       <c r="C82" t="n">
-        <v>-6.86</v>
+        <v>50.1</v>
       </c>
       <c r="D82" t="n">
-        <v>1.27</v>
+        <v>-50</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-4.88</v>
+      </c>
+      <c r="F82" t="n">
+        <v>1.52</v>
       </c>
     </row>
     <row r="83">
@@ -1774,13 +2085,19 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>5.75</v>
+        <v>1.78</v>
       </c>
       <c r="C83" t="n">
-        <v>-6.87</v>
+        <v>51.5</v>
       </c>
       <c r="D83" t="n">
-        <v>1.12</v>
+        <v>-50</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-5</v>
+      </c>
+      <c r="F83" t="n">
+        <v>1.72</v>
       </c>
     </row>
     <row r="84">
@@ -1788,13 +2105,19 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>6.22</v>
+        <v>0.25</v>
       </c>
       <c r="C84" t="n">
-        <v>-6.9</v>
+        <v>52.95</v>
       </c>
       <c r="D84" t="n">
-        <v>0.68</v>
+        <v>-50</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-5.11</v>
+      </c>
+      <c r="F84" t="n">
+        <v>1.91</v>
       </c>
     </row>
     <row r="85">
@@ -1802,13 +2125,19 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>6.71</v>
+        <v>-1.29</v>
       </c>
       <c r="C85" t="n">
-        <v>-6.95</v>
+        <v>54.41</v>
       </c>
       <c r="D85" t="n">
-        <v>0.24</v>
+        <v>-50</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-5.24</v>
+      </c>
+      <c r="F85" t="n">
+        <v>2.12</v>
       </c>
     </row>
     <row r="86">
@@ -1816,13 +2145,19 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>7.28</v>
+        <v>-2.58</v>
       </c>
       <c r="C86" t="n">
-        <v>-7.06</v>
+        <v>55.79</v>
       </c>
       <c r="D86" t="n">
-        <v>-0.21</v>
+        <v>-50</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-5.39</v>
+      </c>
+      <c r="F86" t="n">
+        <v>2.18</v>
       </c>
     </row>
     <row r="87">
@@ -1830,13 +2165,19 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>7.92</v>
+        <v>-5.16</v>
       </c>
       <c r="C87" t="n">
-        <v>-7.19</v>
+        <v>58.55</v>
       </c>
       <c r="D87" t="n">
-        <v>-0.73</v>
+        <v>-50</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-5.52</v>
+      </c>
+      <c r="F87" t="n">
+        <v>2.13</v>
       </c>
     </row>
     <row r="88">
@@ -1844,13 +2185,19 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>8.5</v>
+        <v>-7.73</v>
       </c>
       <c r="C88" t="n">
-        <v>-7.34</v>
+        <v>61.27</v>
       </c>
       <c r="D88" t="n">
-        <v>-1.17</v>
+        <v>-50</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-5.726999999999999</v>
+      </c>
+      <c r="F88" t="n">
+        <v>2.194</v>
       </c>
     </row>
     <row r="89">
@@ -1858,13 +2205,19 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>9.27</v>
+        <v>-9.970000000000001</v>
       </c>
       <c r="C89" t="n">
-        <v>-7.48</v>
+        <v>63.67</v>
       </c>
       <c r="D89" t="n">
-        <v>-1.79</v>
+        <v>-50.12</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-5.864</v>
+      </c>
+      <c r="F89" t="n">
+        <v>2.278</v>
       </c>
     </row>
     <row r="90">
@@ -1872,13 +2225,19 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>9.869999999999999</v>
+        <v>-12.23</v>
       </c>
       <c r="C90" t="n">
-        <v>-7.68</v>
+        <v>66.18000000000001</v>
       </c>
       <c r="D90" t="n">
-        <v>-2.2</v>
+        <v>-50.25</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-6.081</v>
+      </c>
+      <c r="F90" t="n">
+        <v>2.382000000000001</v>
       </c>
     </row>
     <row r="91">
@@ -1886,13 +2245,19 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>10.38</v>
+        <v>-13.55</v>
       </c>
       <c r="C91" t="n">
-        <v>-7.84</v>
+        <v>67.66</v>
       </c>
       <c r="D91" t="n">
-        <v>-2.54</v>
+        <v>-50.41</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-6.278</v>
+      </c>
+      <c r="F91" t="n">
+        <v>2.576</v>
       </c>
     </row>
     <row r="92">
@@ -1900,13 +2265,19 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>10.88</v>
+        <v>-14.81</v>
       </c>
       <c r="C92" t="n">
-        <v>-7.99</v>
+        <v>69.12</v>
       </c>
       <c r="D92" t="n">
-        <v>-2.9</v>
+        <v>-50.57</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-6.464999999999999</v>
+      </c>
+      <c r="F92" t="n">
+        <v>2.73</v>
       </c>
     </row>
     <row r="93">
@@ -1914,13 +2285,19 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>11.4</v>
+        <v>-16.62</v>
       </c>
       <c r="C93" t="n">
-        <v>-8.16</v>
+        <v>70.58</v>
       </c>
       <c r="D93" t="n">
-        <v>-3.24</v>
+        <v>-50.1</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-6.672</v>
+      </c>
+      <c r="F93" t="n">
+        <v>2.813999999999999</v>
       </c>
     </row>
     <row r="94">
@@ -1928,13 +2305,19 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>11.82</v>
+        <v>-18.44</v>
       </c>
       <c r="C94" t="n">
-        <v>-8.32</v>
+        <v>71.97</v>
       </c>
       <c r="D94" t="n">
-        <v>-3.5</v>
+        <v>-49.64</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-6.889</v>
+      </c>
+      <c r="F94" t="n">
+        <v>2.988</v>
       </c>
     </row>
     <row r="95">
@@ -1942,13 +2325,19 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>12.3</v>
+        <v>-20.24</v>
       </c>
       <c r="C95" t="n">
-        <v>-8.470000000000001</v>
+        <v>73.36</v>
       </c>
       <c r="D95" t="n">
-        <v>-3.83</v>
+        <v>-49.19</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-7.086</v>
+      </c>
+      <c r="F95" t="n">
+        <v>3.161999999999999</v>
       </c>
     </row>
     <row r="96">
@@ -1956,13 +2345,19 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>12.76</v>
+        <v>-22.05</v>
       </c>
       <c r="C96" t="n">
-        <v>-8.68</v>
+        <v>74.84999999999999</v>
       </c>
       <c r="D96" t="n">
-        <v>-4.08</v>
+        <v>-48.76</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-7.263</v>
+      </c>
+      <c r="F96" t="n">
+        <v>3.216</v>
       </c>
     </row>
     <row r="97">
@@ -1970,13 +2365,19 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>13.12</v>
+        <v>-22.3</v>
       </c>
       <c r="C97" t="n">
-        <v>-8.720000000000001</v>
+        <v>74.97</v>
       </c>
       <c r="D97" t="n">
-        <v>-4.4</v>
+        <v>-48.57</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-7.44</v>
+      </c>
+      <c r="F97" t="n">
+        <v>3.34</v>
       </c>
     </row>
     <row r="98">
@@ -1984,13 +2385,19 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>13.55</v>
+        <v>-22.37</v>
       </c>
       <c r="C98" t="n">
-        <v>-8.75</v>
+        <v>75.15000000000001</v>
       </c>
       <c r="D98" t="n">
-        <v>-4.8</v>
+        <v>-48.39</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-7.58</v>
+      </c>
+      <c r="F98" t="n">
+        <v>3.185</v>
       </c>
     </row>
     <row r="99">
@@ -1998,13 +2405,19 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>13.78</v>
+        <v>-22.43</v>
       </c>
       <c r="C99" t="n">
-        <v>-8.76</v>
+        <v>75.28</v>
       </c>
       <c r="D99" t="n">
-        <v>-5.02</v>
+        <v>-48.15</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-7.73</v>
+      </c>
+      <c r="F99" t="n">
+        <v>3.03</v>
       </c>
     </row>
     <row r="100">
@@ -2012,13 +2425,19 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>14.05</v>
+        <v>-24.39</v>
       </c>
       <c r="C100" t="n">
-        <v>-8.720000000000001</v>
+        <v>75.31</v>
       </c>
       <c r="D100" t="n">
-        <v>-5.33</v>
+        <v>-45.91</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-7.799999999999999</v>
+      </c>
+      <c r="F100" t="n">
+        <v>2.795</v>
       </c>
     </row>
     <row r="101">
@@ -2026,13 +2445,19 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>14.33</v>
+        <v>-26.35</v>
       </c>
       <c r="C101" t="n">
-        <v>-8.619999999999999</v>
+        <v>75.34</v>
       </c>
       <c r="D101" t="n">
-        <v>-5.71</v>
+        <v>-43.64</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-7.869999999999999</v>
+      </c>
+      <c r="F101" t="n">
+        <v>2.52</v>
       </c>
     </row>
     <row r="102">
@@ -2040,13 +2465,19 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>14.47</v>
+        <v>-28.37</v>
       </c>
       <c r="C102" t="n">
-        <v>-8.460000000000001</v>
+        <v>75.36</v>
       </c>
       <c r="D102" t="n">
-        <v>-6.01</v>
+        <v>-41.38</v>
+      </c>
+      <c r="E102" t="n">
+        <v>-7.959999999999999</v>
+      </c>
+      <c r="F102" t="n">
+        <v>2.345</v>
       </c>
     </row>
     <row r="103">
@@ -2054,13 +2485,19 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>14.65</v>
+        <v>-29.78</v>
       </c>
       <c r="C103" t="n">
-        <v>-8.32</v>
+        <v>75.36</v>
       </c>
       <c r="D103" t="n">
-        <v>-6.33</v>
+        <v>-39.71</v>
+      </c>
+      <c r="E103" t="n">
+        <v>-8.039999999999999</v>
+      </c>
+      <c r="F103" t="n">
+        <v>2.17</v>
       </c>
     </row>
     <row r="104">
@@ -2068,13 +2505,19 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>14.68</v>
+        <v>-31.2</v>
       </c>
       <c r="C104" t="n">
-        <v>-8.17</v>
+        <v>75.81</v>
       </c>
       <c r="D104" t="n">
-        <v>-6.51</v>
+        <v>-38.06</v>
+      </c>
+      <c r="E104" t="n">
+        <v>-8.109999999999999</v>
+      </c>
+      <c r="F104" t="n">
+        <v>1.565</v>
       </c>
     </row>
     <row r="105">
@@ -2082,13 +2525,19 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>15.29</v>
+        <v>-32.65</v>
       </c>
       <c r="C105" t="n">
-        <v>-8.66</v>
+        <v>76.33</v>
       </c>
       <c r="D105" t="n">
-        <v>-6.63</v>
+        <v>-36.41</v>
+      </c>
+      <c r="E105" t="n">
+        <v>-8.18</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0.9029999999999999</v>
       </c>
     </row>
     <row r="106">
@@ -2096,13 +2545,19 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>15.84</v>
+        <v>-34.12</v>
       </c>
       <c r="C106" t="n">
-        <v>-9.07</v>
+        <v>77.06</v>
       </c>
       <c r="D106" t="n">
-        <v>-6.77</v>
+        <v>-34.74</v>
+      </c>
+      <c r="E106" t="n">
+        <v>-8.27</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.07600000000000011</v>
       </c>
     </row>
     <row r="107">
@@ -2110,13 +2565,19 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>16.31</v>
+        <v>-35.84</v>
       </c>
       <c r="C107" t="n">
-        <v>-9.630000000000001</v>
+        <v>77.79000000000001</v>
       </c>
       <c r="D107" t="n">
-        <v>-6.68</v>
+        <v>-32.83</v>
+      </c>
+      <c r="E107" t="n">
+        <v>-8.379999999999999</v>
+      </c>
+      <c r="F107" t="n">
+        <v>-0.7409999999999999</v>
       </c>
     </row>
     <row r="108">
@@ -2124,13 +2585,19 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>17</v>
+        <v>-36.74</v>
       </c>
       <c r="C108" t="n">
-        <v>-10.21</v>
+        <v>77.53</v>
       </c>
       <c r="D108" t="n">
-        <v>-6.79</v>
+        <v>-30.91</v>
+      </c>
+      <c r="E108" t="n">
+        <v>-8.48</v>
+      </c>
+      <c r="F108" t="n">
+        <v>-1.393</v>
       </c>
     </row>
     <row r="109">
@@ -2138,13 +2605,19 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>17.63</v>
+        <v>-37.65</v>
       </c>
       <c r="C109" t="n">
-        <v>-10.71</v>
+        <v>77.17</v>
       </c>
       <c r="D109" t="n">
-        <v>-6.92</v>
+        <v>-28.95</v>
+      </c>
+      <c r="E109" t="n">
+        <v>-8.56</v>
+      </c>
+      <c r="F109" t="n">
+        <v>-2.015</v>
       </c>
     </row>
     <row r="110">
@@ -2152,13 +2625,19 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>17.99</v>
+        <v>-36.24</v>
       </c>
       <c r="C110" t="n">
-        <v>-11.2</v>
+        <v>76.83</v>
       </c>
       <c r="D110" t="n">
-        <v>-6.79</v>
+        <v>-29.03</v>
+      </c>
+      <c r="E110" t="n">
+        <v>-8.699999999999999</v>
+      </c>
+      <c r="F110" t="n">
+        <v>-2.857</v>
       </c>
     </row>
     <row r="111">
@@ -2166,13 +2645,19 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>18.33</v>
+        <v>-34.81</v>
       </c>
       <c r="C111" t="n">
-        <v>-11.52</v>
+        <v>76.48999999999999</v>
       </c>
       <c r="D111" t="n">
-        <v>-6.81</v>
+        <v>-29.13</v>
+      </c>
+      <c r="E111" t="n">
+        <v>-8.860000000000001</v>
+      </c>
+      <c r="F111" t="n">
+        <v>-3.689</v>
       </c>
     </row>
     <row r="112">
@@ -2180,13 +2665,19 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>19.19</v>
+        <v>-33.45</v>
       </c>
       <c r="C112" t="n">
-        <v>-12.35</v>
+        <v>76.31</v>
       </c>
       <c r="D112" t="n">
-        <v>-6.84</v>
+        <v>-29.28</v>
+      </c>
+      <c r="E112" t="n">
+        <v>-9.02</v>
+      </c>
+      <c r="F112" t="n">
+        <v>-4.561</v>
       </c>
     </row>
     <row r="113">
@@ -2194,13 +2685,19 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>20</v>
+        <v>-32.08</v>
       </c>
       <c r="C113" t="n">
-        <v>-13.13</v>
+        <v>76.06</v>
       </c>
       <c r="D113" t="n">
-        <v>-6.87</v>
+        <v>-29.46</v>
+      </c>
+      <c r="E113" t="n">
+        <v>-9.25</v>
+      </c>
+      <c r="F113" t="n">
+        <v>-5.273000000000001</v>
       </c>
     </row>
     <row r="114">
@@ -2208,13 +2705,19 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>20.95</v>
+        <v>-30.98</v>
       </c>
       <c r="C114" t="n">
-        <v>-13.97</v>
+        <v>75.37</v>
       </c>
       <c r="D114" t="n">
-        <v>-6.98</v>
+        <v>-29.64</v>
+      </c>
+      <c r="E114" t="n">
+        <v>-9.030000000000001</v>
+      </c>
+      <c r="F114" t="n">
+        <v>-5.715000000000002</v>
       </c>
     </row>
     <row r="115">
@@ -2222,13 +2725,19 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>21.26</v>
+        <v>-29.82</v>
       </c>
       <c r="C115" t="n">
-        <v>-14.19</v>
+        <v>74.61</v>
       </c>
       <c r="D115" t="n">
-        <v>-7.06</v>
+        <v>-29.82</v>
+      </c>
+      <c r="E115" t="n">
+        <v>-8.81</v>
+      </c>
+      <c r="F115" t="n">
+        <v>-6.160000000000001</v>
       </c>
     </row>
     <row r="116">
@@ -2236,13 +2745,19 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>21.75</v>
+        <v>-28.46</v>
       </c>
       <c r="C116" t="n">
-        <v>-14.44</v>
+        <v>73.62</v>
       </c>
       <c r="D116" t="n">
-        <v>-7.31</v>
+        <v>-30.08</v>
+      </c>
+      <c r="E116" t="n">
+        <v>-8.57</v>
+      </c>
+      <c r="F116" t="n">
+        <v>-6.5</v>
       </c>
     </row>
     <row r="117">
@@ -2250,13 +2765,19 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>22.02</v>
+        <v>-30.5</v>
       </c>
       <c r="C117" t="n">
-        <v>-14.38</v>
+        <v>76.15000000000001</v>
       </c>
       <c r="D117" t="n">
-        <v>-7.64</v>
+        <v>-30.41</v>
+      </c>
+      <c r="E117" t="n">
+        <v>-8.329999999999998</v>
+      </c>
+      <c r="F117" t="n">
+        <v>-6.910000000000001</v>
       </c>
     </row>
     <row r="118">
@@ -2264,13 +2785,19 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>22.07</v>
+        <v>-33.52</v>
       </c>
       <c r="C118" t="n">
-        <v>-14.31</v>
+        <v>79.76000000000001</v>
       </c>
       <c r="D118" t="n">
-        <v>-7.76</v>
+        <v>-30.74</v>
+      </c>
+      <c r="E118" t="n">
+        <v>-8.1</v>
+      </c>
+      <c r="F118" t="n">
+        <v>-7.400000000000001</v>
       </c>
     </row>
     <row r="119">
@@ -2278,13 +2805,19 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>22.13</v>
+        <v>-36.55</v>
       </c>
       <c r="C119" t="n">
-        <v>-14.27</v>
+        <v>83.38</v>
       </c>
       <c r="D119" t="n">
-        <v>-7.86</v>
+        <v>-31.04</v>
+      </c>
+      <c r="E119" t="n">
+        <v>-7.869999999999999</v>
+      </c>
+      <c r="F119" t="n">
+        <v>-7.92</v>
       </c>
     </row>
     <row r="120">
@@ -2292,13 +2825,19 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>22.42</v>
+        <v>-40</v>
       </c>
       <c r="C120" t="n">
-        <v>-14.21</v>
+        <v>87</v>
       </c>
       <c r="D120" t="n">
-        <v>-8.210000000000001</v>
+        <v>-31.18</v>
+      </c>
+      <c r="E120" t="n">
+        <v>-7.659999999999998</v>
+      </c>
+      <c r="F120" t="n">
+        <v>-8.16</v>
       </c>
     </row>
     <row r="121">
@@ -2306,13 +2845,19 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>22.7</v>
+        <v>-43.48</v>
       </c>
       <c r="C121" t="n">
-        <v>-14.57</v>
+        <v>90.61</v>
       </c>
       <c r="D121" t="n">
-        <v>-8.130000000000001</v>
+        <v>-31.32</v>
+      </c>
+      <c r="E121" t="n">
+        <v>-7.489999999999999</v>
+      </c>
+      <c r="F121" t="n">
+        <v>-8.33</v>
       </c>
     </row>
     <row r="122">
@@ -2320,13 +2865,19 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>22.59</v>
+        <v>-46.88</v>
       </c>
       <c r="C122" t="n">
-        <v>-14.55</v>
+        <v>93.87</v>
       </c>
       <c r="D122" t="n">
-        <v>-8.039999999999999</v>
+        <v>-31.39</v>
+      </c>
+      <c r="E122" t="n">
+        <v>-6.599999999999999</v>
+      </c>
+      <c r="F122" t="n">
+        <v>-9</v>
       </c>
     </row>
     <row r="123">
@@ -2334,13 +2885,19 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>22.49</v>
+        <v>-50.29</v>
       </c>
       <c r="C123" t="n">
-        <v>-14.53</v>
+        <v>97.2</v>
       </c>
       <c r="D123" t="n">
-        <v>-7.94</v>
+        <v>-31.48</v>
+      </c>
+      <c r="E123" t="n">
+        <v>-5.028999999999999</v>
+      </c>
+      <c r="F123" t="n">
+        <v>-10.401</v>
       </c>
     </row>
     <row r="124">
@@ -2348,13 +2905,19 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>22.34</v>
+        <v>-53.43</v>
       </c>
       <c r="C124" t="n">
-        <v>-14.47</v>
+        <v>100.61</v>
       </c>
       <c r="D124" t="n">
-        <v>-7.83</v>
+        <v>-31.56</v>
+      </c>
+      <c r="E124" t="n">
+        <v>-3.908</v>
+      </c>
+      <c r="F124" t="n">
+        <v>-11.72</v>
       </c>
     </row>
     <row r="125">
@@ -2362,13 +2925,19 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>22.17</v>
+        <v>-56.63</v>
       </c>
       <c r="C125" t="n">
-        <v>-14.41</v>
+        <v>104.09</v>
       </c>
       <c r="D125" t="n">
-        <v>-7.72</v>
+        <v>-31.63</v>
+      </c>
+      <c r="E125" t="n">
+        <v>-2.85</v>
+      </c>
+      <c r="F125" t="n">
+        <v>-12.973</v>
       </c>
     </row>
     <row r="126">
@@ -2376,13 +2945,19 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>22.05</v>
+        <v>-60</v>
       </c>
       <c r="C126" t="n">
-        <v>-14.57</v>
+        <v>107.57</v>
       </c>
       <c r="D126" t="n">
-        <v>-7.44</v>
+        <v>-31.62</v>
+      </c>
+      <c r="E126" t="n">
+        <v>-1.802</v>
+      </c>
+      <c r="F126" t="n">
+        <v>-14.146</v>
       </c>
     </row>
     <row r="127">
@@ -2390,13 +2965,19 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>22.71</v>
+        <v>-60</v>
       </c>
       <c r="C127" t="n">
-        <v>-15.45</v>
+        <v>107.26</v>
       </c>
       <c r="D127" t="n">
-        <v>-7.22</v>
+        <v>-31.28</v>
+      </c>
+      <c r="E127" t="n">
+        <v>-0.7339999999999998</v>
+      </c>
+      <c r="F127" t="n">
+        <v>-15.249</v>
       </c>
     </row>
     <row r="128">
@@ -2404,13 +2985,19 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>23.32</v>
+        <v>-60</v>
       </c>
       <c r="C128" t="n">
-        <v>-16.34</v>
+        <v>106.86</v>
       </c>
       <c r="D128" t="n">
-        <v>-6.94</v>
+        <v>-30.96</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0.3830000000000003</v>
+      </c>
+      <c r="F128" t="n">
+        <v>-16.281</v>
       </c>
     </row>
     <row r="129">
@@ -2418,13 +3005,19 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>24.01</v>
+        <v>-60</v>
       </c>
       <c r="C129" t="n">
-        <v>-17.31</v>
+        <v>106.55</v>
       </c>
       <c r="D129" t="n">
-        <v>-6.66</v>
+        <v>-30.65</v>
+      </c>
+      <c r="E129" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="F129" t="n">
+        <v>-17.313</v>
       </c>
     </row>
     <row r="130">
@@ -2432,13 +3025,19 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>24.69</v>
+        <v>-60</v>
       </c>
       <c r="C130" t="n">
-        <v>-18.3</v>
+        <v>106.26</v>
       </c>
       <c r="D130" t="n">
-        <v>-6.35</v>
+        <v>-30.44</v>
+      </c>
+      <c r="E130" t="n">
+        <v>2.507</v>
+      </c>
+      <c r="F130" t="n">
+        <v>-18.325</v>
       </c>
     </row>
     <row r="131">
@@ -2446,13 +3045,19 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>25.2</v>
+        <v>-60</v>
       </c>
       <c r="C131" t="n">
-        <v>-19.13</v>
+        <v>105.9</v>
       </c>
       <c r="D131" t="n">
-        <v>-6.03</v>
+        <v>-30.17</v>
+      </c>
+      <c r="E131" t="n">
+        <v>3.663999999999999</v>
+      </c>
+      <c r="F131" t="n">
+        <v>-19.397</v>
       </c>
     </row>
     <row r="132">
@@ -2460,13 +3065,19 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>26.1</v>
+        <v>-60</v>
       </c>
       <c r="C132" t="n">
-        <v>-19.9</v>
+        <v>105.75</v>
       </c>
       <c r="D132" t="n">
-        <v>-6.16</v>
+        <v>-29.88</v>
+      </c>
+      <c r="E132" t="n">
+        <v>4.101</v>
+      </c>
+      <c r="F132" t="n">
+        <v>-19.969</v>
       </c>
     </row>
     <row r="133">
@@ -2474,13 +3085,19 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>26.8</v>
+        <v>-60</v>
       </c>
       <c r="C133" t="n">
-        <v>-21.38</v>
+        <v>105.58</v>
       </c>
       <c r="D133" t="n">
-        <v>-5.4</v>
+        <v>-29.54</v>
+      </c>
+      <c r="E133" t="n">
+        <v>3.927</v>
+      </c>
+      <c r="F133" t="n">
+        <v>-19.97</v>
       </c>
     </row>
     <row r="134">
@@ -2488,13 +3105,19 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>27.34</v>
+        <v>-60</v>
       </c>
       <c r="C134" t="n">
-        <v>-22.67</v>
+        <v>105.31</v>
       </c>
       <c r="D134" t="n">
-        <v>-4.67</v>
+        <v>-29.19</v>
+      </c>
+      <c r="E134" t="n">
+        <v>3.733000000000001</v>
+      </c>
+      <c r="F134" t="n">
+        <v>-19.833</v>
       </c>
     </row>
     <row r="135">
@@ -2502,13 +3125,19 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>27.84</v>
+        <v>-60</v>
       </c>
       <c r="C135" t="n">
-        <v>-23.99</v>
+        <v>104.88</v>
       </c>
       <c r="D135" t="n">
-        <v>-3.85</v>
+        <v>-28.84</v>
+      </c>
+      <c r="E135" t="n">
+        <v>3.742</v>
+      </c>
+      <c r="F135" t="n">
+        <v>-19.742</v>
       </c>
     </row>
     <row r="136">
@@ -2516,13 +3145,19 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>27.49</v>
+        <v>-60</v>
       </c>
       <c r="C136" t="n">
-        <v>-25.11</v>
+        <v>104.72</v>
       </c>
       <c r="D136" t="n">
-        <v>-2.37</v>
+        <v>-28.49</v>
+      </c>
+      <c r="E136" t="n">
+        <v>3.704</v>
+      </c>
+      <c r="F136" t="n">
+        <v>-19.879</v>
       </c>
     </row>
     <row r="137">
@@ -2530,13 +3165,19 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>26.56</v>
+        <v>-60</v>
       </c>
       <c r="C137" t="n">
-        <v>-25.71</v>
+        <v>104.81</v>
       </c>
       <c r="D137" t="n">
-        <v>-0.86</v>
+        <v>-28.42</v>
+      </c>
+      <c r="E137" t="n">
+        <v>3.586</v>
+      </c>
+      <c r="F137" t="n">
+        <v>-19.916</v>
       </c>
     </row>
     <row r="138">
@@ -2544,13 +3185,19 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>25.93</v>
+        <v>-60</v>
       </c>
       <c r="C138" t="n">
-        <v>-26.51</v>
+        <v>104.88</v>
       </c>
       <c r="D138" t="n">
-        <v>0.58</v>
+        <v>-28.32</v>
+      </c>
+      <c r="E138" t="n">
+        <v>3.439</v>
+      </c>
+      <c r="F138" t="n">
+        <v>-19.944</v>
       </c>
     </row>
     <row r="139">
@@ -2558,13 +3205,19 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>25.28</v>
+        <v>-60</v>
       </c>
       <c r="C139" t="n">
-        <v>-27.37</v>
+        <v>104.87</v>
       </c>
       <c r="D139" t="n">
-        <v>2.09</v>
+        <v>-28.24</v>
+      </c>
+      <c r="E139" t="n">
+        <v>3.382</v>
+      </c>
+      <c r="F139" t="n">
+        <v>-19.952</v>
       </c>
     </row>
     <row r="140">
@@ -2572,13 +3225,19 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>24.64</v>
+        <v>-60</v>
       </c>
       <c r="C140" t="n">
-        <v>-28.22</v>
+        <v>104.84</v>
       </c>
       <c r="D140" t="n">
-        <v>3.58</v>
+        <v>-28.18</v>
+      </c>
+      <c r="E140" t="n">
+        <v>3.365</v>
+      </c>
+      <c r="F140" t="n">
+        <v>-19.97</v>
       </c>
     </row>
     <row r="141">
@@ -2586,13 +3245,19 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>24.05</v>
+        <v>-60</v>
       </c>
       <c r="C141" t="n">
-        <v>-28.99</v>
+        <v>104.86</v>
       </c>
       <c r="D141" t="n">
-        <v>4.95</v>
+        <v>-28.18</v>
+      </c>
+      <c r="E141" t="n">
+        <v>3.338</v>
+      </c>
+      <c r="F141" t="n">
+        <v>-19.958</v>
       </c>
     </row>
     <row r="142">
@@ -2600,13 +3265,19 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>22.93</v>
+        <v>-60</v>
       </c>
       <c r="C142" t="n">
-        <v>-29.71</v>
+        <v>104.87</v>
       </c>
       <c r="D142" t="n">
-        <v>6.77</v>
+        <v>-28.22</v>
+      </c>
+      <c r="E142" t="n">
+        <v>3.241000000000001</v>
+      </c>
+      <c r="F142" t="n">
+        <v>-19.826</v>
       </c>
     </row>
     <row r="143">
@@ -2614,13 +3285,19 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>22.02</v>
+        <v>-60</v>
       </c>
       <c r="C143" t="n">
-        <v>-29.66</v>
+        <v>104.92</v>
       </c>
       <c r="D143" t="n">
-        <v>7.65</v>
+        <v>-28.3</v>
+      </c>
+      <c r="E143" t="n">
+        <v>3.154</v>
+      </c>
+      <c r="F143" t="n">
+        <v>-19.714</v>
       </c>
     </row>
     <row r="144">
@@ -2628,13 +3305,19 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>21.39</v>
+        <v>-60</v>
       </c>
       <c r="C144" t="n">
-        <v>-29.81</v>
+        <v>105.11</v>
       </c>
       <c r="D144" t="n">
-        <v>8.42</v>
+        <v>-28.38</v>
+      </c>
+      <c r="E144" t="n">
+        <v>3.067</v>
+      </c>
+      <c r="F144" t="n">
+        <v>-19.752</v>
       </c>
     </row>
     <row r="145">
@@ -2642,13 +3325,19 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>20.92</v>
+        <v>-60</v>
       </c>
       <c r="C145" t="n">
-        <v>-29.92</v>
+        <v>105.33</v>
       </c>
       <c r="D145" t="n">
-        <v>9</v>
+        <v>-28.39</v>
+      </c>
+      <c r="E145" t="n">
+        <v>2.830000000000001</v>
+      </c>
+      <c r="F145" t="n">
+        <v>-19.75</v>
       </c>
     </row>
     <row r="146">
@@ -2656,13 +3345,19 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>21.07</v>
+        <v>-60</v>
       </c>
       <c r="C146" t="n">
-        <v>-30.02</v>
+        <v>105.65</v>
       </c>
       <c r="D146" t="n">
-        <v>8.949999999999999</v>
+        <v>-28.42</v>
+      </c>
+      <c r="E146" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="F146" t="n">
+        <v>-19.86</v>
       </c>
     </row>
     <row r="147">
@@ -2670,13 +3365,19 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>21.49</v>
+        <v>-60</v>
       </c>
       <c r="C147" t="n">
-        <v>-30.22</v>
+        <v>105.99</v>
       </c>
       <c r="D147" t="n">
-        <v>8.73</v>
+        <v>-28.39</v>
+      </c>
+      <c r="E147" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="F147" t="n">
+        <v>-20.09</v>
       </c>
     </row>
     <row r="148">
@@ -2684,13 +3385,19 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>21.62</v>
+        <v>-60</v>
       </c>
       <c r="C148" t="n">
-        <v>-30.4</v>
+        <v>106.34</v>
       </c>
       <c r="D148" t="n">
-        <v>8.779999999999999</v>
+        <v>-28.33</v>
+      </c>
+      <c r="E148" t="n">
+        <v>2.330000000000001</v>
+      </c>
+      <c r="F148" t="n">
+        <v>-20.34</v>
       </c>
     </row>
     <row r="149">
@@ -2698,13 +3405,19 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>21.76</v>
+        <v>-60</v>
       </c>
       <c r="C149" t="n">
-        <v>-30.49</v>
+        <v>106.67</v>
       </c>
       <c r="D149" t="n">
-        <v>8.73</v>
+        <v>-28.01</v>
+      </c>
+      <c r="E149" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="F149" t="n">
+        <v>-20.79</v>
       </c>
     </row>
     <row r="150">
@@ -2712,13 +3425,19 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>21.88</v>
+        <v>-60</v>
       </c>
       <c r="C150" t="n">
-        <v>-30.57</v>
+        <v>106.99</v>
       </c>
       <c r="D150" t="n">
-        <v>8.699999999999999</v>
+        <v>-27.64</v>
+      </c>
+      <c r="E150" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="F150" t="n">
+        <v>-21.25</v>
       </c>
     </row>
     <row r="151">
@@ -2726,13 +3445,19 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>22.17</v>
+        <v>-60</v>
       </c>
       <c r="C151" t="n">
-        <v>-30.68</v>
+        <v>107.33</v>
       </c>
       <c r="D151" t="n">
-        <v>8.51</v>
+        <v>-27.29</v>
+      </c>
+      <c r="E151" t="n">
+        <v>1.015</v>
+      </c>
+      <c r="F151" t="n">
+        <v>-21.055</v>
       </c>
     </row>
     <row r="152">
@@ -2740,13 +3465,19 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>22.75</v>
+        <v>-60</v>
       </c>
       <c r="C152" t="n">
-        <v>-30.85</v>
+        <v>107.68</v>
       </c>
       <c r="D152" t="n">
-        <v>8.109999999999999</v>
+        <v>-27.18</v>
+      </c>
+      <c r="E152" t="n">
+        <v>0.1999999999999997</v>
+      </c>
+      <c r="F152" t="n">
+        <v>-20.7</v>
       </c>
     </row>
     <row r="153">
@@ -2754,13 +3485,19 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>23.21</v>
+        <v>-60</v>
       </c>
       <c r="C153" t="n">
-        <v>-31.09</v>
+        <v>108.03</v>
       </c>
       <c r="D153" t="n">
-        <v>7.88</v>
+        <v>-27.08</v>
+      </c>
+      <c r="E153" t="n">
+        <v>-0.6249999999999999</v>
+      </c>
+      <c r="F153" t="n">
+        <v>-20.325</v>
       </c>
     </row>
     <row r="154">
@@ -2768,13 +3505,19 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>23.49</v>
+        <v>-60</v>
       </c>
       <c r="C154" t="n">
-        <v>-30.17</v>
+        <v>107.41</v>
       </c>
       <c r="D154" t="n">
-        <v>6.68</v>
+        <v>-27</v>
+      </c>
+      <c r="E154" t="n">
+        <v>-1.45</v>
+      </c>
+      <c r="F154" t="n">
+        <v>-18.96</v>
       </c>
     </row>
     <row r="155">
@@ -2782,13 +3525,19 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>23.6</v>
+        <v>-60</v>
       </c>
       <c r="C155" t="n">
-        <v>-29.24</v>
+        <v>106.85</v>
       </c>
       <c r="D155" t="n">
-        <v>5.64</v>
+        <v>-27</v>
+      </c>
+      <c r="E155" t="n">
+        <v>-2.285</v>
+      </c>
+      <c r="F155" t="n">
+        <v>-17.565</v>
       </c>
     </row>
     <row r="156">
@@ -2796,13 +3545,19 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>23.65</v>
+        <v>-60</v>
       </c>
       <c r="C156" t="n">
-        <v>-28.3</v>
+        <v>105.91</v>
       </c>
       <c r="D156" t="n">
-        <v>4.65</v>
+        <v>-26.98</v>
+      </c>
+      <c r="E156" t="n">
+        <v>-3.089999999999999</v>
+      </c>
+      <c r="F156" t="n">
+        <v>-15.84</v>
       </c>
     </row>
     <row r="157">
@@ -2810,13 +3565,19 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>23.53</v>
+        <v>-60</v>
       </c>
       <c r="C157" t="n">
-        <v>-27.38</v>
+        <v>104.98</v>
       </c>
       <c r="D157" t="n">
-        <v>3.85</v>
+        <v>-27</v>
+      </c>
+      <c r="E157" t="n">
+        <v>-3.884999999999999</v>
+      </c>
+      <c r="F157" t="n">
+        <v>-14.095</v>
       </c>
     </row>
     <row r="158">
@@ -2824,13 +3585,19 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>24.38</v>
+        <v>-60</v>
       </c>
       <c r="C158" t="n">
-        <v>-27.16</v>
+        <v>103.99</v>
       </c>
       <c r="D158" t="n">
-        <v>2.78</v>
+        <v>-27.12</v>
+      </c>
+      <c r="E158" t="n">
+        <v>-4.659999999999999</v>
+      </c>
+      <c r="F158" t="n">
+        <v>-12.21</v>
       </c>
     </row>
     <row r="159">
@@ -2838,13 +3605,19 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>25.25</v>
+        <v>-60</v>
       </c>
       <c r="C159" t="n">
-        <v>-26.96</v>
+        <v>103.85</v>
       </c>
       <c r="D159" t="n">
-        <v>1.71</v>
+        <v>-28.12</v>
+      </c>
+      <c r="E159" t="n">
+        <v>-5.487</v>
+      </c>
+      <c r="F159" t="n">
+        <v>-10.237</v>
       </c>
     </row>
     <row r="160">
@@ -2852,13 +3625,19 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>26.01</v>
+        <v>-60</v>
       </c>
       <c r="C160" t="n">
-        <v>-26.58</v>
+        <v>103.59</v>
       </c>
       <c r="D160" t="n">
-        <v>0.57</v>
+        <v>-29.16</v>
+      </c>
+      <c r="E160" t="n">
+        <v>-6.334</v>
+      </c>
+      <c r="F160" t="n">
+        <v>-8.1</v>
       </c>
     </row>
     <row r="161">
@@ -2866,13 +3645,19 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>26.58</v>
+        <v>-60</v>
       </c>
       <c r="C161" t="n">
-        <v>-26</v>
+        <v>103.42</v>
       </c>
       <c r="D161" t="n">
-        <v>-0.58</v>
+        <v>-30.24</v>
+      </c>
+      <c r="E161" t="n">
+        <v>-6.525999999999999</v>
+      </c>
+      <c r="F161" t="n">
+        <v>-6.648000000000001</v>
       </c>
     </row>
     <row r="162">
@@ -2880,13 +3665,19 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>26.74</v>
+        <v>-60</v>
       </c>
       <c r="C162" t="n">
-        <v>-25.4</v>
+        <v>103.46</v>
       </c>
       <c r="D162" t="n">
-        <v>-1.34</v>
+        <v>-31.17</v>
+      </c>
+      <c r="E162" t="n">
+        <v>-6.717999999999999</v>
+      </c>
+      <c r="F162" t="n">
+        <v>-5.576</v>
       </c>
     </row>
     <row r="163">
@@ -2894,13 +3685,19 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>27.12</v>
+        <v>-60</v>
       </c>
       <c r="C163" t="n">
-        <v>-24.91</v>
+        <v>103.47</v>
       </c>
       <c r="D163" t="n">
-        <v>-2.21</v>
+        <v>-32.15</v>
+      </c>
+      <c r="E163" t="n">
+        <v>-6.74</v>
+      </c>
+      <c r="F163" t="n">
+        <v>-4.584</v>
       </c>
     </row>
     <row r="164">
@@ -2908,13 +3705,19 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>27.48</v>
+        <v>-60</v>
       </c>
       <c r="C164" t="n">
-        <v>-25.47</v>
+        <v>104.43</v>
       </c>
       <c r="D164" t="n">
-        <v>-2.01</v>
+        <v>-33.13</v>
+      </c>
+      <c r="E164" t="n">
+        <v>-7.002</v>
+      </c>
+      <c r="F164" t="n">
+        <v>-4.292000000000001</v>
       </c>
     </row>
     <row r="165">
@@ -2922,13 +3725,19 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>27.89</v>
+        <v>-60</v>
       </c>
       <c r="C165" t="n">
-        <v>-26.02</v>
+        <v>105.36</v>
       </c>
       <c r="D165" t="n">
-        <v>-1.87</v>
+        <v>-34.11</v>
+      </c>
+      <c r="E165" t="n">
+        <v>-7.203999999999999</v>
+      </c>
+      <c r="F165" t="n">
+        <v>-4.050000000000001</v>
       </c>
     </row>
     <row r="166">
@@ -2936,13 +3745,19 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>28.48</v>
+        <v>-60</v>
       </c>
       <c r="C166" t="n">
-        <v>-26.63</v>
+        <v>106.31</v>
       </c>
       <c r="D166" t="n">
-        <v>-1.85</v>
+        <v>-35.1</v>
+      </c>
+      <c r="E166" t="n">
+        <v>-7.406000000000001</v>
+      </c>
+      <c r="F166" t="n">
+        <v>-3.798</v>
       </c>
     </row>
     <row r="167">
@@ -2950,13 +3765,19 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>29.05</v>
+        <v>-60</v>
       </c>
       <c r="C167" t="n">
-        <v>-27.23</v>
+        <v>107.24</v>
       </c>
       <c r="D167" t="n">
-        <v>-1.82</v>
+        <v>-36.08</v>
+      </c>
+      <c r="E167" t="n">
+        <v>-7.597999999999999</v>
+      </c>
+      <c r="F167" t="n">
+        <v>-3.566</v>
       </c>
     </row>
     <row r="168">
@@ -2964,13 +3785,19 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>28.96</v>
+        <v>-60</v>
       </c>
       <c r="C168" t="n">
-        <v>-27.12</v>
+        <v>108.23</v>
       </c>
       <c r="D168" t="n">
-        <v>-1.84</v>
+        <v>-37.05</v>
+      </c>
+      <c r="E168" t="n">
+        <v>-7.970000000000001</v>
+      </c>
+      <c r="F168" t="n">
+        <v>-3.214</v>
       </c>
     </row>
     <row r="169">
@@ -2978,13 +3805,19 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>28.86</v>
+        <v>-60</v>
       </c>
       <c r="C169" t="n">
-        <v>-27.02</v>
+        <v>108.38</v>
       </c>
       <c r="D169" t="n">
-        <v>-1.84</v>
+        <v>-37.6</v>
+      </c>
+      <c r="E169" t="n">
+        <v>-7.870000000000002</v>
+      </c>
+      <c r="F169" t="n">
+        <v>-2.91</v>
       </c>
     </row>
     <row r="170">
@@ -2992,13 +3825,19 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>28.89</v>
+        <v>-60</v>
       </c>
       <c r="C170" t="n">
-        <v>-27.11</v>
+        <v>108.81</v>
       </c>
       <c r="D170" t="n">
-        <v>-1.79</v>
+        <v>-38.23</v>
+      </c>
+      <c r="E170" t="n">
+        <v>-7.750000000000002</v>
+      </c>
+      <c r="F170" t="n">
+        <v>-2.83</v>
       </c>
     </row>
     <row r="171">
@@ -3006,13 +3845,19 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>29.34</v>
+        <v>-60</v>
       </c>
       <c r="C171" t="n">
-        <v>-27.44</v>
+        <v>109.09</v>
       </c>
       <c r="D171" t="n">
-        <v>-1.9</v>
+        <v>-38.8</v>
+      </c>
+      <c r="E171" t="n">
+        <v>-7.69</v>
+      </c>
+      <c r="F171" t="n">
+        <v>-2.6</v>
       </c>
     </row>
     <row r="172">
@@ -3020,13 +3865,19 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>29.95</v>
+        <v>-60</v>
       </c>
       <c r="C172" t="n">
-        <v>-27.79</v>
+        <v>109.15</v>
       </c>
       <c r="D172" t="n">
-        <v>-2.16</v>
+        <v>-39.27</v>
+      </c>
+      <c r="E172" t="n">
+        <v>-8.15</v>
+      </c>
+      <c r="F172" t="n">
+        <v>-1.73</v>
       </c>
     </row>
     <row r="173">
@@ -3034,13 +3885,19 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>30.46</v>
+        <v>-60</v>
       </c>
       <c r="C173" t="n">
-        <v>-28.05</v>
+        <v>109.19</v>
       </c>
       <c r="D173" t="n">
-        <v>-2.44</v>
+        <v>-39.66</v>
+      </c>
+      <c r="E173" t="n">
+        <v>-8.75</v>
+      </c>
+      <c r="F173" t="n">
+        <v>-0.78</v>
       </c>
     </row>
     <row r="174">
@@ -3048,13 +3905,19 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>31.04</v>
+        <v>-60</v>
       </c>
       <c r="C174" t="n">
-        <v>-28.39</v>
+        <v>109.22</v>
       </c>
       <c r="D174" t="n">
-        <v>-2.71</v>
+        <v>-39.09</v>
+      </c>
+      <c r="E174" t="n">
+        <v>-9.875999999999999</v>
+      </c>
+      <c r="F174" t="n">
+        <v>-0.2500000000000001</v>
       </c>
     </row>
     <row r="175">
@@ -3062,13 +3925,19 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>31.65</v>
+        <v>-60</v>
       </c>
       <c r="C175" t="n">
-        <v>-28.73</v>
+        <v>109.27</v>
       </c>
       <c r="D175" t="n">
-        <v>-3.01</v>
+        <v>-38.54</v>
+      </c>
+      <c r="E175" t="n">
+        <v>-11.042</v>
+      </c>
+      <c r="F175" t="n">
+        <v>0.3100000000000001</v>
       </c>
     </row>
     <row r="176">
@@ -3076,17 +3945,1043 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>32.14</v>
+        <v>-60</v>
       </c>
       <c r="C176" t="n">
-        <v>-28.7</v>
+        <v>108.33</v>
       </c>
       <c r="D176" t="n">
-        <v>-3.56</v>
+        <v>-37.96</v>
+      </c>
+      <c r="E176" t="n">
+        <v>-12.218</v>
+      </c>
+      <c r="F176" t="n">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C177" t="n">
+        <v>106.89</v>
+      </c>
+      <c r="D177" t="n">
+        <v>-36.71</v>
+      </c>
+      <c r="E177" t="n">
+        <v>-13.394</v>
+      </c>
+      <c r="F177" t="n">
+        <v>3.21</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C178" t="n">
+        <v>105.27</v>
+      </c>
+      <c r="D178" t="n">
+        <v>-35.4</v>
+      </c>
+      <c r="E178" t="n">
+        <v>-14.39</v>
+      </c>
+      <c r="F178" t="n">
+        <v>4.521</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C179" t="n">
+        <v>103.59</v>
+      </c>
+      <c r="D179" t="n">
+        <v>-33.95</v>
+      </c>
+      <c r="E179" t="n">
+        <v>-15.766</v>
+      </c>
+      <c r="F179" t="n">
+        <v>6.132000000000001</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C180" t="n">
+        <v>101.67</v>
+      </c>
+      <c r="D180" t="n">
+        <v>-32.45</v>
+      </c>
+      <c r="E180" t="n">
+        <v>-17.142</v>
+      </c>
+      <c r="F180" t="n">
+        <v>7.923</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C181" t="n">
+        <v>99.52</v>
+      </c>
+      <c r="D181" t="n">
+        <v>-30.61</v>
+      </c>
+      <c r="E181" t="n">
+        <v>-18.448</v>
+      </c>
+      <c r="F181" t="n">
+        <v>9.544</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C182" t="n">
+        <v>97.34999999999999</v>
+      </c>
+      <c r="D182" t="n">
+        <v>-28.8</v>
+      </c>
+      <c r="E182" t="n">
+        <v>-19.214</v>
+      </c>
+      <c r="F182" t="n">
+        <v>10.665</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C183" t="n">
+        <v>95</v>
+      </c>
+      <c r="D183" t="n">
+        <v>-27.07</v>
+      </c>
+      <c r="E183" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F183" t="n">
+        <v>12.066</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C184" t="n">
+        <v>92.69</v>
+      </c>
+      <c r="D184" t="n">
+        <v>-26.28</v>
+      </c>
+      <c r="E184" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F184" t="n">
+        <v>13.587</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C185" t="n">
+        <v>90.37</v>
+      </c>
+      <c r="D185" t="n">
+        <v>-25.57</v>
+      </c>
+      <c r="E185" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F185" t="n">
+        <v>15.198</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C186" t="n">
+        <v>88.94</v>
+      </c>
+      <c r="D186" t="n">
+        <v>-24.87</v>
+      </c>
+      <c r="E186" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F186" t="n">
+        <v>15.929</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C187" t="n">
+        <v>88.08</v>
+      </c>
+      <c r="D187" t="n">
+        <v>-24.88</v>
+      </c>
+      <c r="E187" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F187" t="n">
+        <v>16.803</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C188" t="n">
+        <v>87.38</v>
+      </c>
+      <c r="D188" t="n">
+        <v>-24.9</v>
+      </c>
+      <c r="E188" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F188" t="n">
+        <v>17.526</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C189" t="n">
+        <v>86.75</v>
+      </c>
+      <c r="D189" t="n">
+        <v>-24.84</v>
+      </c>
+      <c r="E189" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F189" t="n">
+        <v>18.089</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C190" t="n">
+        <v>86.2</v>
+      </c>
+      <c r="D190" t="n">
+        <v>-24.77</v>
+      </c>
+      <c r="E190" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F190" t="n">
+        <v>18.572</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C191" t="n">
+        <v>85.95999999999999</v>
+      </c>
+      <c r="D191" t="n">
+        <v>-25.02</v>
+      </c>
+      <c r="E191" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F191" t="n">
+        <v>19.065</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C192" t="n">
+        <v>85.72</v>
+      </c>
+      <c r="D192" t="n">
+        <v>-25.27</v>
+      </c>
+      <c r="E192" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F192" t="n">
+        <v>19.548</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C193" t="n">
+        <v>85.72</v>
+      </c>
+      <c r="D193" t="n">
+        <v>-25.45</v>
+      </c>
+      <c r="E193" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F193" t="n">
+        <v>19.751</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C194" t="n">
+        <v>86.14</v>
+      </c>
+      <c r="D194" t="n">
+        <v>-26.07</v>
+      </c>
+      <c r="E194" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F194" t="n">
+        <v>19.954</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C195" t="n">
+        <v>86.31</v>
+      </c>
+      <c r="D195" t="n">
+        <v>-26.62</v>
+      </c>
+      <c r="E195" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F195" t="n">
+        <v>20.327</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C196" t="n">
+        <v>86.55</v>
+      </c>
+      <c r="D196" t="n">
+        <v>-27.12</v>
+      </c>
+      <c r="E196" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F196" t="n">
+        <v>20.59</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C197" t="n">
+        <v>86.73999999999999</v>
+      </c>
+      <c r="D197" t="n">
+        <v>-27.63</v>
+      </c>
+      <c r="E197" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F197" t="n">
+        <v>20.91</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C198" t="n">
+        <v>87.51000000000001</v>
+      </c>
+      <c r="D198" t="n">
+        <v>-28.18</v>
+      </c>
+      <c r="E198" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F198" t="n">
+        <v>20.685</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C199" t="n">
+        <v>88.43000000000001</v>
+      </c>
+      <c r="D199" t="n">
+        <v>-28.85</v>
+      </c>
+      <c r="E199" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F199" t="n">
+        <v>20.44</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C200" t="n">
+        <v>89.38</v>
+      </c>
+      <c r="D200" t="n">
+        <v>-29.53</v>
+      </c>
+      <c r="E200" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F200" t="n">
+        <v>20.175</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C201" t="n">
+        <v>90.31</v>
+      </c>
+      <c r="D201" t="n">
+        <v>-30.22</v>
+      </c>
+      <c r="E201" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F201" t="n">
+        <v>19.93</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C202" t="n">
+        <v>91.20999999999999</v>
+      </c>
+      <c r="D202" t="n">
+        <v>-30.93</v>
+      </c>
+      <c r="E202" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F202" t="n">
+        <v>19.735</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C203" t="n">
+        <v>92.06999999999999</v>
+      </c>
+      <c r="D203" t="n">
+        <v>-31.59</v>
+      </c>
+      <c r="E203" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F203" t="n">
+        <v>19.52</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C204" t="n">
+        <v>92.48</v>
+      </c>
+      <c r="D204" t="n">
+        <v>-31.88</v>
+      </c>
+      <c r="E204" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F204" t="n">
+        <v>19.394</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C205" t="n">
+        <v>93.17</v>
+      </c>
+      <c r="D205" t="n">
+        <v>-32.15</v>
+      </c>
+      <c r="E205" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F205" t="n">
+        <v>18.988</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B206" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C206" t="n">
+        <v>93.81</v>
+      </c>
+      <c r="D206" t="n">
+        <v>-32.4</v>
+      </c>
+      <c r="E206" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F206" t="n">
+        <v>18.592</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C207" t="n">
+        <v>94.43000000000001</v>
+      </c>
+      <c r="D207" t="n">
+        <v>-32.63</v>
+      </c>
+      <c r="E207" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F207" t="n">
+        <v>18.196</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C208" t="n">
+        <v>94.19</v>
+      </c>
+      <c r="D208" t="n">
+        <v>-32.8</v>
+      </c>
+      <c r="E208" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F208" t="n">
+        <v>18.605</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C209" t="n">
+        <v>93.83</v>
+      </c>
+      <c r="D209" t="n">
+        <v>-32.86</v>
+      </c>
+      <c r="E209" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F209" t="n">
+        <v>19.034</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C210" t="n">
+        <v>93.8</v>
+      </c>
+      <c r="D210" t="n">
+        <v>-33.19</v>
+      </c>
+      <c r="E210" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F210" t="n">
+        <v>19.393</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C211" t="n">
+        <v>93.75</v>
+      </c>
+      <c r="D211" t="n">
+        <v>-33.41</v>
+      </c>
+      <c r="E211" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F211" t="n">
+        <v>19.662</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C212" t="n">
+        <v>93.62</v>
+      </c>
+      <c r="D212" t="n">
+        <v>-33.47</v>
+      </c>
+      <c r="E212" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F212" t="n">
+        <v>19.851</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C213" t="n">
+        <v>92.43000000000001</v>
+      </c>
+      <c r="D213" t="n">
+        <v>-32.47</v>
+      </c>
+      <c r="E213" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F213" t="n">
+        <v>20.04</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C214" t="n">
+        <v>91.25</v>
+      </c>
+      <c r="D214" t="n">
+        <v>-31.4</v>
+      </c>
+      <c r="E214" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F214" t="n">
+        <v>20.15</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C215" t="n">
+        <v>90.52</v>
+      </c>
+      <c r="D215" t="n">
+        <v>-30.35</v>
+      </c>
+      <c r="E215" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F215" t="n">
+        <v>19.83000000000001</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C216" t="n">
+        <v>89.84999999999999</v>
+      </c>
+      <c r="D216" t="n">
+        <v>-29.38</v>
+      </c>
+      <c r="E216" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F216" t="n">
+        <v>19.53</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C217" t="n">
+        <v>88.98</v>
+      </c>
+      <c r="D217" t="n">
+        <v>-28.01</v>
+      </c>
+      <c r="E217" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F217" t="n">
+        <v>19.03</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C218" t="n">
+        <v>88.33</v>
+      </c>
+      <c r="D218" t="n">
+        <v>-26.72</v>
+      </c>
+      <c r="E218" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F218" t="n">
+        <v>18.39</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C219" t="n">
+        <v>87.66</v>
+      </c>
+      <c r="D219" t="n">
+        <v>-25.42</v>
+      </c>
+      <c r="E219" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F219" t="n">
+        <v>17.76</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C220" t="n">
+        <v>86.81999999999999</v>
+      </c>
+      <c r="D220" t="n">
+        <v>-23.84</v>
+      </c>
+      <c r="E220" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F220" t="n">
+        <v>17.02</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C221" t="n">
+        <v>85.98999999999999</v>
+      </c>
+      <c r="D221" t="n">
+        <v>-22.4</v>
+      </c>
+      <c r="E221" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F221" t="n">
+        <v>16.41</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C222" t="n">
+        <v>85.28</v>
+      </c>
+      <c r="D222" t="n">
+        <v>-21.09</v>
+      </c>
+      <c r="E222" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F222" t="n">
+        <v>15.81</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C223" t="n">
+        <v>85.56999999999999</v>
+      </c>
+      <c r="D223" t="n">
+        <v>-20.79</v>
+      </c>
+      <c r="E223" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F223" t="n">
+        <v>15.22</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C224" t="n">
+        <v>85.87</v>
+      </c>
+      <c r="D224" t="n">
+        <v>-20.51</v>
+      </c>
+      <c r="E224" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F224" t="n">
+        <v>14.64</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C225" t="n">
+        <v>86.2</v>
+      </c>
+      <c r="D225" t="n">
+        <v>-21.19</v>
+      </c>
+      <c r="E225" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F225" t="n">
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C226" t="n">
+        <v>86.53</v>
+      </c>
+      <c r="D226" t="n">
+        <v>-21.85</v>
+      </c>
+      <c r="E226" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F226" t="n">
+        <v>15.32</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="n">
+        <v>-60</v>
+      </c>
+      <c r="C227" t="n">
+        <v>87.05</v>
+      </c>
+      <c r="D227" t="n">
+        <v>-22.9</v>
+      </c>
+      <c r="E227" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F227" t="n">
+        <v>15.85</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Functions moved to fewer files
My last commit from the Jackson Square office. It has been a good run. I've enjoyed writing this program from scratch. I hope it runs bug free and is useful forever, to me and to others.

There are many helper functions in the PokerStats program. Before now, each had their own file, as in MATLAB. Now, a bunch of functions are in a few files, for conciseness.
</commit_message>
<xml_diff>
--- a/Outputs/net_over_time_avg.xlsx
+++ b/Outputs/net_over_time_avg.xlsx
@@ -162,7 +162,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Net vs time this session (05/20/21): 10-hand moving averages</a:t>
+              <a:t>Net vs time this session (07/05/21): 10-hand moving averages</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -194,7 +194,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$B$2:$B$224</f>
+              <f>'data'!$B$2:$B$176</f>
             </numRef>
           </val>
         </ser>
@@ -221,7 +221,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$C$2:$C$224</f>
+              <f>'data'!$C$2:$C$176</f>
             </numRef>
           </val>
         </ser>
@@ -248,34 +248,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$D$2:$D$224</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <strRef>
-              <f>'data'!E1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'data'!$E$2:$E$224</f>
+              <f>'data'!$D$2:$D$176</f>
             </numRef>
           </val>
         </ser>
@@ -645,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E224"/>
+  <dimension ref="A1:D176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,7 +639,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cedric</t>
+          <t>Raymond</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -674,11 +647,6 @@
           <t>Scott</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Xavier</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -690,16 +658,22 @@
       <c r="C2" t="n">
         <v>0</v>
       </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1</v>
+        <v>-0.35</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1</v>
+        <v>-0.05</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="4">
@@ -707,10 +681,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.47</v>
+        <v>-0.7</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.47</v>
+        <v>0.2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5">
@@ -718,10 +695,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.68</v>
+        <v>-1.02</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.68</v>
+        <v>0.17</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.85</v>
       </c>
     </row>
     <row r="6">
@@ -729,10 +709,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.76</v>
+        <v>-1.26</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.76</v>
+        <v>0.14</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.12</v>
       </c>
     </row>
     <row r="7">
@@ -740,10 +723,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.72</v>
+        <v>-1.52</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.72</v>
+        <v>0.12</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.4</v>
       </c>
     </row>
     <row r="8">
@@ -751,10 +737,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.74</v>
+        <v>-1.67</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.74</v>
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.6</v>
       </c>
     </row>
     <row r="9">
@@ -762,10 +751,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.74</v>
+        <v>-1.94</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.74</v>
+        <v>0.19</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.75</v>
       </c>
     </row>
     <row r="10">
@@ -773,10 +765,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.67</v>
+        <v>-2.21</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.67</v>
+        <v>0.34</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.87</v>
       </c>
     </row>
     <row r="11">
@@ -784,10 +779,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.97</v>
+        <v>-2.37</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.97</v>
+        <v>0.41</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.96</v>
       </c>
     </row>
     <row r="12">
@@ -795,10 +793,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.97</v>
+        <v>-2.37</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.97</v>
+        <v>0.41</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.96</v>
       </c>
     </row>
     <row r="13">
@@ -806,10 +807,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1.36</v>
+        <v>-2.77</v>
       </c>
       <c r="C13" t="n">
-        <v>-1.36</v>
+        <v>0.53</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.24</v>
       </c>
     </row>
     <row r="14">
@@ -817,10 +821,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1.85</v>
+        <v>-3.16</v>
       </c>
       <c r="C14" t="n">
-        <v>-1.85</v>
+        <v>0.72</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.44</v>
       </c>
     </row>
     <row r="15">
@@ -828,10 +835,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>2.18</v>
+        <v>-3.42</v>
       </c>
       <c r="C15" t="n">
-        <v>-2.18</v>
+        <v>0.77</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.65</v>
       </c>
     </row>
     <row r="16">
@@ -839,10 +849,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>2.35</v>
+        <v>-3.63</v>
       </c>
       <c r="C16" t="n">
-        <v>-2.35</v>
+        <v>0.89</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.74</v>
       </c>
     </row>
     <row r="17">
@@ -850,10 +863,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>2.64</v>
+        <v>-3.81</v>
       </c>
       <c r="C17" t="n">
-        <v>-2.64</v>
+        <v>1.01</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.8</v>
       </c>
     </row>
     <row r="18">
@@ -861,10 +877,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>-3.99</v>
       </c>
       <c r="C18" t="n">
-        <v>-3</v>
+        <v>1.19</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.8</v>
       </c>
     </row>
     <row r="19">
@@ -872,10 +891,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>3.44</v>
+        <v>-4.16</v>
       </c>
       <c r="C19" t="n">
-        <v>-3.44</v>
+        <v>1.39</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.77</v>
       </c>
     </row>
     <row r="20">
@@ -883,10 +905,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>3.91</v>
+        <v>-4.03</v>
       </c>
       <c r="C20" t="n">
-        <v>-3.91</v>
+        <v>1.29</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.74</v>
       </c>
     </row>
     <row r="21">
@@ -894,10 +919,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>4.46</v>
+        <v>-3.81</v>
       </c>
       <c r="C21" t="n">
-        <v>-4.46</v>
+        <v>1.12</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2.69</v>
       </c>
     </row>
     <row r="22">
@@ -905,10 +933,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>4.41</v>
+        <v>-3.67</v>
       </c>
       <c r="C22" t="n">
-        <v>-4.41</v>
+        <v>1.04</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2.63</v>
       </c>
     </row>
     <row r="23">
@@ -916,13 +947,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>4.36</v>
+        <v>-3.45</v>
       </c>
       <c r="C23" t="n">
-        <v>-4.36</v>
+        <v>0.88</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="24">
@@ -930,13 +961,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>3.85</v>
+        <v>-2.98</v>
       </c>
       <c r="C24" t="n">
-        <v>-4.23</v>
+        <v>0.49</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.05</v>
+        <v>2.51</v>
       </c>
     </row>
     <row r="25">
@@ -944,13 +975,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>3.25</v>
+        <v>-2.59</v>
       </c>
       <c r="C25" t="n">
-        <v>-4</v>
+        <v>0.18</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.06666666666666667</v>
+        <v>2.45</v>
       </c>
     </row>
     <row r="26">
@@ -958,13 +989,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>2.82</v>
+        <v>-2.2</v>
       </c>
       <c r="C26" t="n">
-        <v>-3.94</v>
+        <v>-0.13</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.025</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="27">
@@ -972,13 +1003,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>2.27</v>
+        <v>-1.81</v>
       </c>
       <c r="C27" t="n">
-        <v>-3.78</v>
+        <v>-0.44</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.04</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="28">
@@ -986,13 +1017,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.53</v>
+        <v>-1.37</v>
       </c>
       <c r="C28" t="n">
-        <v>-3.41</v>
+        <v>-0.8</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.1166666666666667</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="29">
@@ -1000,13 +1031,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.73</v>
+        <v>-1.02</v>
       </c>
       <c r="C29" t="n">
-        <v>-2.94</v>
+        <v>-1.1</v>
       </c>
       <c r="D29" t="n">
-        <v>0.05714285714285716</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="30">
@@ -1014,13 +1045,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.23</v>
+        <v>-0.86</v>
       </c>
       <c r="C30" t="n">
-        <v>-2.47</v>
+        <v>-1.21</v>
       </c>
       <c r="D30" t="n">
-        <v>0.1625</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="31">
@@ -1028,13 +1059,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-1.23</v>
+        <v>-0.75</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.94</v>
+        <v>-1.29</v>
       </c>
       <c r="D31" t="n">
-        <v>0.2444444444444445</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="32">
@@ -1042,13 +1073,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-1.98</v>
+        <v>-0.68</v>
       </c>
       <c r="C32" t="n">
-        <v>-1.66</v>
+        <v>-1.34</v>
       </c>
       <c r="D32" t="n">
-        <v>0.95</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="33">
@@ -1056,13 +1087,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-3.36</v>
+        <v>-0.66</v>
       </c>
       <c r="C33" t="n">
-        <v>-1.39</v>
+        <v>-1.34</v>
       </c>
       <c r="D33" t="n">
-        <v>0.95</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="34">
@@ -1070,13 +1101,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-4.38</v>
+        <v>-0.84</v>
       </c>
       <c r="C34" t="n">
-        <v>-1.09</v>
+        <v>-1.16</v>
       </c>
       <c r="D34" t="n">
-        <v>1.67</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="35">
@@ -1084,13 +1115,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-5.11</v>
+        <v>-0.99</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.96</v>
+        <v>-1.01</v>
       </c>
       <c r="D35" t="n">
-        <v>2.274999999999999</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="36">
@@ -1098,13 +1129,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-5.88</v>
+        <v>-1.11</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.82</v>
+        <v>-0.89</v>
       </c>
       <c r="D36" t="n">
-        <v>2.9</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="37">
@@ -1112,13 +1143,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-6.63</v>
+        <v>-1.26</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.6899999999999999</v>
+        <v>-0.74</v>
       </c>
       <c r="D37" t="n">
-        <v>3.524999999999999</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="38">
@@ -1126,13 +1157,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-7.2</v>
+        <v>-1.46</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.77</v>
+        <v>-0.54</v>
       </c>
       <c r="D38" t="n">
-        <v>4.17</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="39">
@@ -1140,13 +1171,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-7.83</v>
+        <v>-1.62</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.9</v>
+        <v>-0.38</v>
       </c>
       <c r="D39" t="n">
-        <v>4.924999999999999</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="40">
@@ -1154,13 +1185,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-8.31</v>
+        <v>-1.89</v>
       </c>
       <c r="C40" t="n">
-        <v>-1.03</v>
+        <v>-0.11</v>
       </c>
       <c r="D40" t="n">
-        <v>5.54</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="41">
@@ -1168,13 +1199,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-8.859999999999999</v>
+        <v>-2.16</v>
       </c>
       <c r="C41" t="n">
-        <v>-1.11</v>
+        <v>0.14</v>
       </c>
       <c r="D41" t="n">
-        <v>6.175</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="42">
@@ -1182,13 +1213,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-9.44</v>
+        <v>-2.31</v>
       </c>
       <c r="C42" t="n">
-        <v>-1.18</v>
+        <v>0.27</v>
       </c>
       <c r="D42" t="n">
-        <v>6.82</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="43">
@@ -1196,13 +1227,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>-9.289999999999999</v>
+        <v>-2.47</v>
       </c>
       <c r="C43" t="n">
-        <v>-1.25</v>
+        <v>0.4</v>
       </c>
       <c r="D43" t="n">
-        <v>6.745</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="44">
@@ -1210,13 +1241,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-9.119999999999999</v>
+        <v>-2.55</v>
       </c>
       <c r="C44" t="n">
-        <v>-1.36</v>
+        <v>0.46</v>
       </c>
       <c r="D44" t="n">
-        <v>6.68</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="45">
@@ -1224,13 +1255,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>-9.779999999999999</v>
+        <v>-2.49</v>
       </c>
       <c r="C45" t="n">
-        <v>-1.46</v>
+        <v>0.46</v>
       </c>
       <c r="D45" t="n">
-        <v>7.44</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="46">
@@ -1238,13 +1269,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-10.14</v>
+        <v>-2.51</v>
       </c>
       <c r="C46" t="n">
-        <v>-1.82</v>
+        <v>0.46</v>
       </c>
       <c r="D46" t="n">
-        <v>8.159999999999998</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="47">
@@ -1252,13 +1283,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>-10.49</v>
+        <v>-2.26</v>
       </c>
       <c r="C47" t="n">
-        <v>-2.17</v>
+        <v>0.2</v>
       </c>
       <c r="D47" t="n">
-        <v>8.859999999999998</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="48">
@@ -1266,13 +1297,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-10.86</v>
+        <v>-2.01</v>
       </c>
       <c r="C48" t="n">
-        <v>-2.51</v>
+        <v>-0.14</v>
       </c>
       <c r="D48" t="n">
-        <v>9.569999999999999</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="49">
@@ -1280,13 +1311,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-11.22</v>
+        <v>-1.77</v>
       </c>
       <c r="C49" t="n">
-        <v>-2.97</v>
+        <v>-0.51</v>
       </c>
       <c r="D49" t="n">
-        <v>10.39</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="50">
@@ -1294,13 +1325,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-11.56</v>
+        <v>-1.47</v>
       </c>
       <c r="C50" t="n">
-        <v>-3.43</v>
+        <v>-0.99</v>
       </c>
       <c r="D50" t="n">
-        <v>11.19</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="51">
@@ -1308,13 +1339,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-11.89</v>
+        <v>-1.16</v>
       </c>
       <c r="C51" t="n">
-        <v>-4.46</v>
+        <v>-0.99</v>
       </c>
       <c r="D51" t="n">
-        <v>12.55</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="52">
@@ -1322,13 +1353,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-12.21</v>
+        <v>-0.91</v>
       </c>
       <c r="C52" t="n">
-        <v>-5.51</v>
+        <v>-1.08</v>
       </c>
       <c r="D52" t="n">
-        <v>13.92</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="53">
@@ -1336,16 +1367,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-12.5</v>
+        <v>-0.68</v>
       </c>
       <c r="C53" t="n">
-        <v>-6.55</v>
+        <v>-1.15</v>
       </c>
       <c r="D53" t="n">
-        <v>15.245</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="54">
@@ -1353,16 +1381,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-12.78</v>
+        <v>-0.5</v>
       </c>
       <c r="C54" t="n">
-        <v>-7.53</v>
+        <v>-1.19</v>
       </c>
       <c r="D54" t="n">
-        <v>16.51</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="55">
@@ -1370,16 +1395,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>-12.43</v>
+        <v>-0.5</v>
       </c>
       <c r="C55" t="n">
-        <v>-8.210000000000001</v>
+        <v>-1.16</v>
       </c>
       <c r="D55" t="n">
-        <v>16.835</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0.06666666666666667</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="56">
@@ -1387,16 +1409,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>-12.35</v>
+        <v>-0.57</v>
       </c>
       <c r="C56" t="n">
-        <v>-8.65</v>
+        <v>-1.12</v>
       </c>
       <c r="D56" t="n">
-        <v>17.18</v>
-      </c>
-      <c r="E56" t="n">
-        <v>0.5</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="57">
@@ -1404,16 +1423,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-12.31</v>
+        <v>-0.36</v>
       </c>
       <c r="C57" t="n">
-        <v>-9.220000000000001</v>
+        <v>-0.6899999999999999</v>
       </c>
       <c r="D57" t="n">
-        <v>17.525</v>
-      </c>
-      <c r="E57" t="n">
-        <v>-0.18</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="58">
@@ -1421,16 +1437,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>-12.31</v>
+        <v>0.02</v>
       </c>
       <c r="C58" t="n">
-        <v>-9.789999999999999</v>
+        <v>-0.25</v>
       </c>
       <c r="D58" t="n">
-        <v>18.39</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0.6333333333333334</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="59">
@@ -1438,16 +1451,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>-12.38</v>
+        <v>0.79</v>
       </c>
       <c r="C59" t="n">
-        <v>-10.2</v>
+        <v>-0.17</v>
       </c>
       <c r="D59" t="n">
-        <v>18.405</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0.9428571428571428</v>
+        <v>-0.77</v>
       </c>
     </row>
     <row r="60">
@@ -1455,16 +1465,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>-12.53</v>
+        <v>1.65</v>
       </c>
       <c r="C60" t="n">
-        <v>-10.6</v>
+        <v>-0.11</v>
       </c>
       <c r="D60" t="n">
-        <v>18.67</v>
-      </c>
-      <c r="E60" t="n">
-        <v>-0.4712499999999999</v>
+        <v>-1.69</v>
       </c>
     </row>
     <row r="61">
@@ -1472,16 +1479,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>-12.67</v>
+        <v>2.62</v>
       </c>
       <c r="C61" t="n">
-        <v>-8.859999999999999</v>
+        <v>-0.63</v>
       </c>
       <c r="D61" t="n">
-        <v>18.105</v>
-      </c>
-      <c r="E61" t="n">
-        <v>-1.482222222222222</v>
+        <v>-2.15</v>
       </c>
     </row>
     <row r="62">
@@ -1489,16 +1493,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>-12.88</v>
+        <v>3.6</v>
       </c>
       <c r="C62" t="n">
-        <v>-7.19</v>
+        <v>-0.99</v>
       </c>
       <c r="D62" t="n">
-        <v>17.6</v>
-      </c>
-      <c r="E62" t="n">
-        <v>-2.531</v>
+        <v>-2.77</v>
       </c>
     </row>
     <row r="63">
@@ -1506,16 +1507,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>-12.96</v>
+        <v>4.54</v>
       </c>
       <c r="C63" t="n">
-        <v>-5.52</v>
+        <v>-1.55</v>
       </c>
       <c r="D63" t="n">
-        <v>17.21</v>
-      </c>
-      <c r="E63" t="n">
-        <v>-2.531</v>
+        <v>-3.15</v>
       </c>
     </row>
     <row r="64">
@@ -1523,16 +1521,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>-13.12</v>
+        <v>5.41</v>
       </c>
       <c r="C64" t="n">
-        <v>-3.87</v>
+        <v>-2.09</v>
       </c>
       <c r="D64" t="n">
-        <v>16.94</v>
-      </c>
-      <c r="E64" t="n">
-        <v>-3.748</v>
+        <v>-3.47</v>
       </c>
     </row>
     <row r="65">
@@ -1540,16 +1535,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>-13.24</v>
+        <v>6.22</v>
       </c>
       <c r="C65" t="n">
-        <v>-2.52</v>
+        <v>-2.8</v>
       </c>
       <c r="D65" t="n">
-        <v>16.75</v>
-      </c>
-      <c r="E65" t="n">
-        <v>-4.784999999999999</v>
+        <v>-3.57</v>
       </c>
     </row>
     <row r="66">
@@ -1557,16 +1549,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>-13.42</v>
+        <v>7.06</v>
       </c>
       <c r="C66" t="n">
-        <v>-1.16</v>
+        <v>-3.4</v>
       </c>
       <c r="D66" t="n">
-        <v>16.62</v>
-      </c>
-      <c r="E66" t="n">
-        <v>-5.842</v>
+        <v>-3.66</v>
       </c>
     </row>
     <row r="67">
@@ -1574,16 +1563,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>-13.58</v>
+        <v>7.36</v>
       </c>
       <c r="C67" t="n">
-        <v>0.33</v>
+        <v>-4.13</v>
       </c>
       <c r="D67" t="n">
-        <v>16.58</v>
-      </c>
-      <c r="E67" t="n">
-        <v>-7.129</v>
+        <v>-3.23</v>
       </c>
     </row>
     <row r="68">
@@ -1591,16 +1577,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-13.22</v>
+        <v>7.64</v>
       </c>
       <c r="C68" t="n">
-        <v>1.81</v>
+        <v>-4.91</v>
       </c>
       <c r="D68" t="n">
-        <v>16.01</v>
-      </c>
-      <c r="E68" t="n">
-        <v>-8.391</v>
+        <v>-2.73</v>
       </c>
     </row>
     <row r="69">
@@ -1608,16 +1591,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>-12.35</v>
+        <v>7.52</v>
       </c>
       <c r="C69" t="n">
-        <v>3.3</v>
+        <v>-5.3</v>
       </c>
       <c r="D69" t="n">
-        <v>16.11</v>
-      </c>
-      <c r="E69" t="n">
-        <v>-10.861</v>
+        <v>-2.22</v>
       </c>
     </row>
     <row r="70">
@@ -1625,16 +1605,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>-11.44</v>
+        <v>7.39</v>
       </c>
       <c r="C70" t="n">
-        <v>4.81</v>
+        <v>-5.76</v>
       </c>
       <c r="D70" t="n">
-        <v>15.97</v>
-      </c>
-      <c r="E70" t="n">
-        <v>-13.141</v>
+        <v>-1.63</v>
       </c>
     </row>
     <row r="71">
@@ -1642,16 +1619,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-9.76</v>
+        <v>7.28</v>
       </c>
       <c r="C71" t="n">
-        <v>4.59</v>
+        <v>-6.14</v>
       </c>
       <c r="D71" t="n">
-        <v>16.09</v>
-      </c>
-      <c r="E71" t="n">
-        <v>-14.724</v>
+        <v>-1.14</v>
       </c>
     </row>
     <row r="72">
@@ -1659,16 +1633,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>-8.01</v>
+        <v>7.14</v>
       </c>
       <c r="C72" t="n">
-        <v>4.49</v>
+        <v>-6.5</v>
       </c>
       <c r="D72" t="n">
-        <v>16.13</v>
-      </c>
-      <c r="E72" t="n">
-        <v>-16.407</v>
+        <v>-0.64</v>
       </c>
     </row>
     <row r="73">
@@ -1676,16 +1647,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>-6.62</v>
+        <v>6.91</v>
       </c>
       <c r="C73" t="n">
-        <v>4.85</v>
+        <v>-6.67</v>
       </c>
       <c r="D73" t="n">
-        <v>16.18</v>
-      </c>
-      <c r="E73" t="n">
-        <v>-18.21</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="74">
@@ -1693,16 +1661,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>-4.91</v>
+        <v>6.59</v>
       </c>
       <c r="C74" t="n">
-        <v>5.17</v>
+        <v>-6.83</v>
       </c>
       <c r="D74" t="n">
-        <v>15.93</v>
-      </c>
-      <c r="E74" t="n">
-        <v>-19.993</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="75">
@@ -1710,16 +1675,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-3.17</v>
+        <v>6.33</v>
       </c>
       <c r="C75" t="n">
-        <v>5.33</v>
+        <v>-6.81</v>
       </c>
       <c r="D75" t="n">
-        <v>16</v>
-      </c>
-      <c r="E75" t="n">
-        <v>-21.956</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="76">
@@ -1727,16 +1689,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>-1.38</v>
+        <v>6.19</v>
       </c>
       <c r="C76" t="n">
-        <v>5.48</v>
+        <v>-6.84</v>
       </c>
       <c r="D76" t="n">
-        <v>16.354</v>
-      </c>
-      <c r="E76" t="n">
-        <v>-24.253</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="77">
@@ -1744,16 +1703,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.26</v>
+        <v>6.07</v>
       </c>
       <c r="C77" t="n">
-        <v>5.65</v>
+        <v>-6.89</v>
       </c>
       <c r="D77" t="n">
-        <v>16.618</v>
-      </c>
-      <c r="E77" t="n">
-        <v>-26.33</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="78">
@@ -1761,16 +1717,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>1.59</v>
+        <v>5.86</v>
       </c>
       <c r="C78" t="n">
-        <v>5.83</v>
+        <v>-6.87</v>
       </c>
       <c r="D78" t="n">
-        <v>16.812</v>
-      </c>
-      <c r="E78" t="n">
-        <v>-28.032</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="79">
@@ -1778,16 +1731,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>2.41</v>
+        <v>5.67</v>
       </c>
       <c r="C79" t="n">
-        <v>6.01</v>
+        <v>-6.87</v>
       </c>
       <c r="D79" t="n">
-        <v>17.626</v>
-      </c>
-      <c r="E79" t="n">
-        <v>-29.846</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="80">
@@ -1795,16 +1745,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>3.32</v>
+        <v>5.62</v>
       </c>
       <c r="C80" t="n">
-        <v>6.19</v>
+        <v>-6.79</v>
       </c>
       <c r="D80" t="n">
-        <v>18.43</v>
-      </c>
-      <c r="E80" t="n">
-        <v>-31.74</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="81">
@@ -1812,16 +1759,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>3.52</v>
+        <v>5.55</v>
       </c>
       <c r="C81" t="n">
-        <v>6.44</v>
+        <v>-6.81</v>
       </c>
       <c r="D81" t="n">
-        <v>18.819</v>
-      </c>
-      <c r="E81" t="n">
-        <v>-32.57899999999999</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="82">
@@ -1829,16 +1773,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>4.26</v>
+        <v>5.59</v>
       </c>
       <c r="C82" t="n">
-        <v>6.65</v>
+        <v>-6.86</v>
       </c>
       <c r="D82" t="n">
-        <v>18.948</v>
-      </c>
-      <c r="E82" t="n">
-        <v>-33.658</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="83">
@@ -1846,16 +1787,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>5.26</v>
+        <v>5.75</v>
       </c>
       <c r="C83" t="n">
-        <v>6.42</v>
+        <v>-6.87</v>
       </c>
       <c r="D83" t="n">
-        <v>19.077</v>
-      </c>
-      <c r="E83" t="n">
-        <v>-34.557</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="84">
@@ -1863,16 +1801,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>5.95</v>
+        <v>6.22</v>
       </c>
       <c r="C84" t="n">
-        <v>6.25</v>
+        <v>-6.9</v>
       </c>
       <c r="D84" t="n">
-        <v>19.261</v>
-      </c>
-      <c r="E84" t="n">
-        <v>-35.261</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="85">
@@ -1880,16 +1815,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>6.57</v>
+        <v>6.71</v>
       </c>
       <c r="C85" t="n">
-        <v>6.24</v>
+        <v>-6.95</v>
       </c>
       <c r="D85" t="n">
-        <v>19.275</v>
-      </c>
-      <c r="E85" t="n">
-        <v>-35.88500000000001</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="86">
@@ -1897,16 +1829,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>7.21</v>
+        <v>7.28</v>
       </c>
       <c r="C86" t="n">
-        <v>6.24</v>
+        <v>-7.06</v>
       </c>
       <c r="D86" t="n">
-        <v>18.945</v>
-      </c>
-      <c r="E86" t="n">
-        <v>-36.195</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="87">
@@ -1914,16 +1843,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>8.18</v>
+        <v>7.92</v>
       </c>
       <c r="C87" t="n">
-        <v>6.24</v>
+        <v>-7.19</v>
       </c>
       <c r="D87" t="n">
-        <v>18.545</v>
-      </c>
-      <c r="E87" t="n">
-        <v>-36.765</v>
+        <v>-0.73</v>
       </c>
     </row>
     <row r="88">
@@ -1931,16 +1857,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>9.130000000000001</v>
+        <v>8.5</v>
       </c>
       <c r="C88" t="n">
-        <v>6.17</v>
+        <v>-7.34</v>
       </c>
       <c r="D88" t="n">
-        <v>18.195</v>
-      </c>
-      <c r="E88" t="n">
-        <v>-37.285</v>
+        <v>-1.17</v>
       </c>
     </row>
     <row r="89">
@@ -1948,16 +1871,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>10.11</v>
+        <v>9.27</v>
       </c>
       <c r="C89" t="n">
-        <v>6.01</v>
+        <v>-7.48</v>
       </c>
       <c r="D89" t="n">
-        <v>17.225</v>
-      </c>
-      <c r="E89" t="n">
-        <v>-37.145</v>
+        <v>-1.79</v>
       </c>
     </row>
     <row r="90">
@@ -1965,16 +1885,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>11</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="C90" t="n">
-        <v>5.9</v>
+        <v>-7.68</v>
       </c>
       <c r="D90" t="n">
-        <v>16.255</v>
-      </c>
-      <c r="E90" t="n">
-        <v>-36.94500000000001</v>
+        <v>-2.2</v>
       </c>
     </row>
     <row r="91">
@@ -1982,16 +1899,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>11.71</v>
+        <v>10.38</v>
       </c>
       <c r="C91" t="n">
-        <v>5.78</v>
+        <v>-7.84</v>
       </c>
       <c r="D91" t="n">
-        <v>14.97</v>
-      </c>
-      <c r="E91" t="n">
-        <v>-36.255</v>
+        <v>-2.54</v>
       </c>
     </row>
     <row r="92">
@@ -1999,16 +1913,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>11.83</v>
+        <v>10.88</v>
       </c>
       <c r="C92" t="n">
-        <v>5.65</v>
+        <v>-7.99</v>
       </c>
       <c r="D92" t="n">
-        <v>13.935</v>
-      </c>
-      <c r="E92" t="n">
-        <v>-35.205</v>
+        <v>-2.9</v>
       </c>
     </row>
     <row r="93">
@@ -2016,16 +1927,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>11.75</v>
+        <v>11.4</v>
       </c>
       <c r="C93" t="n">
-        <v>5.55</v>
+        <v>-8.16</v>
       </c>
       <c r="D93" t="n">
-        <v>12.9</v>
-      </c>
-      <c r="E93" t="n">
-        <v>-33.995</v>
+        <v>-3.24</v>
       </c>
     </row>
     <row r="94">
@@ -2033,16 +1941,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>11.66</v>
+        <v>11.82</v>
       </c>
       <c r="C94" t="n">
-        <v>5.92</v>
+        <v>-8.32</v>
       </c>
       <c r="D94" t="n">
-        <v>12.05</v>
-      </c>
-      <c r="E94" t="n">
-        <v>-33.42</v>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="95">
@@ -2050,16 +1955,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>11.54</v>
+        <v>12.3</v>
       </c>
       <c r="C95" t="n">
-        <v>5.25</v>
+        <v>-8.470000000000001</v>
       </c>
       <c r="D95" t="n">
-        <v>11.12</v>
-      </c>
-      <c r="E95" t="n">
-        <v>-31.71</v>
+        <v>-3.83</v>
       </c>
     </row>
     <row r="96">
@@ -2067,16 +1969,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>11.25</v>
+        <v>12.76</v>
       </c>
       <c r="C96" t="n">
-        <v>2.31</v>
+        <v>-8.68</v>
       </c>
       <c r="D96" t="n">
-        <v>12.778</v>
-      </c>
-      <c r="E96" t="n">
-        <v>-30.14</v>
+        <v>-4.08</v>
       </c>
     </row>
     <row r="97">
@@ -2084,16 +1983,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>10.79</v>
+        <v>13.12</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.61</v>
+        <v>-8.720000000000001</v>
       </c>
       <c r="D97" t="n">
-        <v>14.506</v>
-      </c>
-      <c r="E97" t="n">
-        <v>-28.48</v>
+        <v>-4.4</v>
       </c>
     </row>
     <row r="98">
@@ -2101,16 +1997,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>10.2</v>
+        <v>13.55</v>
       </c>
       <c r="C98" t="n">
-        <v>-3.28</v>
+        <v>-8.75</v>
       </c>
       <c r="D98" t="n">
-        <v>16.168</v>
-      </c>
-      <c r="E98" t="n">
-        <v>-26.886</v>
+        <v>-4.8</v>
       </c>
     </row>
     <row r="99">
@@ -2118,16 +2011,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>9.630000000000001</v>
+        <v>13.78</v>
       </c>
       <c r="C99" t="n">
-        <v>-5.68</v>
+        <v>-8.76</v>
       </c>
       <c r="D99" t="n">
-        <v>17.83</v>
-      </c>
-      <c r="E99" t="n">
-        <v>-25.562</v>
+        <v>-5.02</v>
       </c>
     </row>
     <row r="100">
@@ -2135,16 +2025,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>9.140000000000001</v>
+        <v>14.05</v>
       </c>
       <c r="C100" t="n">
-        <v>-8.130000000000001</v>
+        <v>-8.720000000000001</v>
       </c>
       <c r="D100" t="n">
-        <v>19.492</v>
-      </c>
-      <c r="E100" t="n">
-        <v>-24.258</v>
+        <v>-5.33</v>
       </c>
     </row>
     <row r="101">
@@ -2152,16 +2039,13 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>8.81</v>
+        <v>14.33</v>
       </c>
       <c r="C101" t="n">
-        <v>-10.54</v>
+        <v>-8.619999999999999</v>
       </c>
       <c r="D101" t="n">
-        <v>21.894</v>
-      </c>
-      <c r="E101" t="n">
-        <v>-23.899</v>
+        <v>-5.71</v>
       </c>
     </row>
     <row r="102">
@@ -2169,16 +2053,13 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>8.380000000000001</v>
+        <v>14.47</v>
       </c>
       <c r="C102" t="n">
-        <v>-12.96</v>
+        <v>-8.460000000000001</v>
       </c>
       <c r="D102" t="n">
-        <v>24.306</v>
-      </c>
-      <c r="E102" t="n">
-        <v>-23.45</v>
+        <v>-6.01</v>
       </c>
     </row>
     <row r="103">
@@ -2186,16 +2067,13 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>7.97</v>
+        <v>14.65</v>
       </c>
       <c r="C103" t="n">
-        <v>-15.42</v>
+        <v>-8.32</v>
       </c>
       <c r="D103" t="n">
-        <v>26.718</v>
-      </c>
-      <c r="E103" t="n">
-        <v>-22.971</v>
+        <v>-6.33</v>
       </c>
     </row>
     <row r="104">
@@ -2203,16 +2081,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>7.68</v>
+        <v>14.68</v>
       </c>
       <c r="C104" t="n">
-        <v>-18.36</v>
+        <v>-8.17</v>
       </c>
       <c r="D104" t="n">
-        <v>29.13</v>
-      </c>
-      <c r="E104" t="n">
-        <v>-22.13200000000001</v>
+        <v>-6.51</v>
       </c>
     </row>
     <row r="105">
@@ -2220,16 +2095,13 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>7.05</v>
+        <v>15.29</v>
       </c>
       <c r="C105" t="n">
-        <v>-19.8</v>
+        <v>-8.66</v>
       </c>
       <c r="D105" t="n">
-        <v>31.63200000000001</v>
-      </c>
-      <c r="E105" t="n">
-        <v>-22.54800000000001</v>
+        <v>-6.63</v>
       </c>
     </row>
     <row r="106">
@@ -2237,16 +2109,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>6.58</v>
+        <v>15.84</v>
       </c>
       <c r="C106" t="n">
-        <v>-18.98</v>
+        <v>-9.07</v>
       </c>
       <c r="D106" t="n">
-        <v>31.546</v>
-      </c>
-      <c r="E106" t="n">
-        <v>-22.794</v>
+        <v>-6.77</v>
       </c>
     </row>
     <row r="107">
@@ -2254,16 +2123,13 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>6.1</v>
+        <v>16.31</v>
       </c>
       <c r="C107" t="n">
-        <v>-18.18</v>
+        <v>-9.630000000000001</v>
       </c>
       <c r="D107" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E107" t="n">
-        <v>-23</v>
+        <v>-6.68</v>
       </c>
     </row>
     <row r="108">
@@ -2271,16 +2137,13 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>6.02</v>
+        <v>17</v>
       </c>
       <c r="C108" t="n">
-        <v>-17.57</v>
+        <v>-10.21</v>
       </c>
       <c r="D108" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E108" t="n">
-        <v>-23.51</v>
+        <v>-6.79</v>
       </c>
     </row>
     <row r="109">
@@ -2288,16 +2151,13 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>5.92</v>
+        <v>17.63</v>
       </c>
       <c r="C109" t="n">
-        <v>-17.17</v>
+        <v>-10.71</v>
       </c>
       <c r="D109" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E109" t="n">
-        <v>-23.81</v>
+        <v>-6.92</v>
       </c>
     </row>
     <row r="110">
@@ -2305,16 +2165,13 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>5.57</v>
+        <v>17.99</v>
       </c>
       <c r="C110" t="n">
-        <v>-16.16</v>
+        <v>-11.2</v>
       </c>
       <c r="D110" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E110" t="n">
-        <v>-24.47</v>
+        <v>-6.79</v>
       </c>
     </row>
     <row r="111">
@@ -2322,16 +2179,13 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>5.57</v>
+        <v>18.33</v>
       </c>
       <c r="C111" t="n">
-        <v>-15.21</v>
+        <v>-11.52</v>
       </c>
       <c r="D111" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E111" t="n">
-        <v>-25.42</v>
+        <v>-6.81</v>
       </c>
     </row>
     <row r="112">
@@ -2339,16 +2193,13 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>5.6</v>
+        <v>19.19</v>
       </c>
       <c r="C112" t="n">
-        <v>-14.26</v>
+        <v>-12.35</v>
       </c>
       <c r="D112" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E112" t="n">
-        <v>-26.405</v>
+        <v>-6.84</v>
       </c>
     </row>
     <row r="113">
@@ -2356,16 +2207,13 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>5.55</v>
+        <v>20</v>
       </c>
       <c r="C113" t="n">
-        <v>-13.37</v>
+        <v>-13.13</v>
       </c>
       <c r="D113" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E113" t="n">
-        <v>-27.24</v>
+        <v>-6.87</v>
       </c>
     </row>
     <row r="114">
@@ -2373,16 +2221,13 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>6.21</v>
+        <v>20.95</v>
       </c>
       <c r="C114" t="n">
-        <v>-12.48</v>
+        <v>-13.97</v>
       </c>
       <c r="D114" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E114" t="n">
-        <v>-28.785</v>
+        <v>-6.98</v>
       </c>
     </row>
     <row r="115">
@@ -2390,16 +2235,13 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>7.21</v>
+        <v>21.26</v>
       </c>
       <c r="C115" t="n">
-        <v>-10.82</v>
+        <v>-14.19</v>
       </c>
       <c r="D115" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E115" t="n">
-        <v>-31.45499999999999</v>
+        <v>-7.06</v>
       </c>
     </row>
     <row r="116">
@@ -2407,16 +2249,13 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>8.390000000000001</v>
+        <v>21.75</v>
       </c>
       <c r="C116" t="n">
-        <v>-9.32</v>
+        <v>-14.44</v>
       </c>
       <c r="D116" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E116" t="n">
-        <v>-34.13499999999999</v>
+        <v>-7.31</v>
       </c>
     </row>
     <row r="117">
@@ -2424,16 +2263,13 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>9.539999999999999</v>
+        <v>22.02</v>
       </c>
       <c r="C117" t="n">
-        <v>-7.77</v>
+        <v>-14.38</v>
       </c>
       <c r="D117" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E117" t="n">
-        <v>-36.83499999999999</v>
+        <v>-7.64</v>
       </c>
     </row>
     <row r="118">
@@ -2441,16 +2277,13 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>10.21</v>
+        <v>22.07</v>
       </c>
       <c r="C118" t="n">
-        <v>-6.13</v>
+        <v>-14.31</v>
       </c>
       <c r="D118" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E118" t="n">
-        <v>-39.145</v>
+        <v>-7.76</v>
       </c>
     </row>
     <row r="119">
@@ -2458,16 +2291,13 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>10.93</v>
+        <v>22.13</v>
       </c>
       <c r="C119" t="n">
-        <v>-4.5</v>
+        <v>-14.27</v>
       </c>
       <c r="D119" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E119" t="n">
-        <v>-41.495</v>
+        <v>-7.86</v>
       </c>
     </row>
     <row r="120">
@@ -2475,16 +2305,13 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>11.48</v>
+        <v>22.42</v>
       </c>
       <c r="C120" t="n">
-        <v>-3.1</v>
+        <v>-14.21</v>
       </c>
       <c r="D120" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E120" t="n">
-        <v>-43.44500000000001</v>
+        <v>-8.210000000000001</v>
       </c>
     </row>
     <row r="121">
@@ -2492,16 +2319,13 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>11.61</v>
+        <v>22.7</v>
       </c>
       <c r="C121" t="n">
-        <v>-1.58</v>
+        <v>-14.57</v>
       </c>
       <c r="D121" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E121" t="n">
-        <v>-45.085</v>
+        <v>-8.130000000000001</v>
       </c>
     </row>
     <row r="122">
@@ -2509,16 +2333,13 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>11.89</v>
+        <v>22.59</v>
       </c>
       <c r="C122" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-14.55</v>
       </c>
       <c r="D122" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E122" t="n">
-        <v>-46.88</v>
+        <v>-8.039999999999999</v>
       </c>
     </row>
     <row r="123">
@@ -2526,16 +2347,13 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>12.13</v>
+        <v>22.49</v>
       </c>
       <c r="C123" t="n">
-        <v>1.65</v>
+        <v>-14.53</v>
       </c>
       <c r="D123" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E123" t="n">
-        <v>-48.835</v>
+        <v>-7.94</v>
       </c>
     </row>
     <row r="124">
@@ -2543,16 +2361,13 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>11.57</v>
+        <v>22.34</v>
       </c>
       <c r="C124" t="n">
-        <v>3.37</v>
+        <v>-14.47</v>
       </c>
       <c r="D124" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E124" t="n">
-        <v>-50</v>
+        <v>-7.83</v>
       </c>
     </row>
     <row r="125">
@@ -2560,16 +2375,13 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>11.39</v>
+        <v>22.17</v>
       </c>
       <c r="C125" t="n">
-        <v>3.55</v>
+        <v>-14.41</v>
       </c>
       <c r="D125" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E125" t="n">
-        <v>-50</v>
+        <v>-7.72</v>
       </c>
     </row>
     <row r="126">
@@ -2577,16 +2389,13 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>11.01</v>
+        <v>22.05</v>
       </c>
       <c r="C126" t="n">
-        <v>3.93</v>
+        <v>-14.57</v>
       </c>
       <c r="D126" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E126" t="n">
-        <v>-50</v>
+        <v>-7.44</v>
       </c>
     </row>
     <row r="127">
@@ -2594,16 +2403,13 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>10.68</v>
+        <v>22.71</v>
       </c>
       <c r="C127" t="n">
-        <v>4.26</v>
+        <v>-15.45</v>
       </c>
       <c r="D127" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E127" t="n">
-        <v>-50</v>
+        <v>-7.22</v>
       </c>
     </row>
     <row r="128">
@@ -2611,16 +2417,13 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>10.42</v>
+        <v>23.32</v>
       </c>
       <c r="C128" t="n">
-        <v>4.52</v>
+        <v>-16.34</v>
       </c>
       <c r="D128" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E128" t="n">
-        <v>-50</v>
+        <v>-6.94</v>
       </c>
     </row>
     <row r="129">
@@ -2628,16 +2431,13 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>10.23</v>
+        <v>24.01</v>
       </c>
       <c r="C129" t="n">
-        <v>4.71</v>
+        <v>-17.31</v>
       </c>
       <c r="D129" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E129" t="n">
-        <v>-50</v>
+        <v>-6.66</v>
       </c>
     </row>
     <row r="130">
@@ -2645,16 +2445,13 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>10.34</v>
+        <v>24.69</v>
       </c>
       <c r="C130" t="n">
-        <v>4.6</v>
+        <v>-18.3</v>
       </c>
       <c r="D130" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E130" t="n">
-        <v>-50</v>
+        <v>-6.35</v>
       </c>
     </row>
     <row r="131">
@@ -2662,16 +2459,13 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>10.54</v>
+        <v>25.2</v>
       </c>
       <c r="C131" t="n">
-        <v>4.4</v>
+        <v>-19.13</v>
       </c>
       <c r="D131" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E131" t="n">
-        <v>-50</v>
+        <v>-6.03</v>
       </c>
     </row>
     <row r="132">
@@ -2679,16 +2473,13 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>10.75</v>
+        <v>26.1</v>
       </c>
       <c r="C132" t="n">
-        <v>4.19</v>
+        <v>-19.9</v>
       </c>
       <c r="D132" t="n">
-        <v>31.44</v>
-      </c>
-      <c r="E132" t="n">
-        <v>-50</v>
+        <v>-6.16</v>
       </c>
     </row>
     <row r="133">
@@ -2696,16 +2487,13 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>10.55</v>
+        <v>26.8</v>
       </c>
       <c r="C133" t="n">
-        <v>4.42</v>
+        <v>-21.38</v>
       </c>
       <c r="D133" t="n">
-        <v>31.39</v>
-      </c>
-      <c r="E133" t="n">
-        <v>-50</v>
+        <v>-5.4</v>
       </c>
     </row>
     <row r="134">
@@ -2713,16 +2501,13 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>10.33</v>
+        <v>27.34</v>
       </c>
       <c r="C134" t="n">
-        <v>4.59</v>
+        <v>-22.67</v>
       </c>
       <c r="D134" t="n">
-        <v>31.42</v>
-      </c>
-      <c r="E134" t="n">
-        <v>-50</v>
+        <v>-4.67</v>
       </c>
     </row>
     <row r="135">
@@ -2730,16 +2515,13 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>9.74</v>
+        <v>27.84</v>
       </c>
       <c r="C135" t="n">
-        <v>5.07</v>
+        <v>-23.99</v>
       </c>
       <c r="D135" t="n">
-        <v>31.51</v>
-      </c>
-      <c r="E135" t="n">
-        <v>-50</v>
+        <v>-3.85</v>
       </c>
     </row>
     <row r="136">
@@ -2747,16 +2529,13 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>9.529999999999999</v>
+        <v>27.49</v>
       </c>
       <c r="C136" t="n">
-        <v>5.25</v>
+        <v>-25.11</v>
       </c>
       <c r="D136" t="n">
-        <v>31.52</v>
-      </c>
-      <c r="E136" t="n">
-        <v>-50</v>
+        <v>-2.37</v>
       </c>
     </row>
     <row r="137">
@@ -2764,16 +2543,13 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>9.33</v>
+        <v>26.56</v>
       </c>
       <c r="C137" t="n">
-        <v>5.4</v>
+        <v>-25.71</v>
       </c>
       <c r="D137" t="n">
-        <v>31.6</v>
-      </c>
-      <c r="E137" t="n">
-        <v>-50</v>
+        <v>-0.86</v>
       </c>
     </row>
     <row r="138">
@@ -2781,16 +2557,13 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>9.130000000000001</v>
+        <v>25.93</v>
       </c>
       <c r="C138" t="n">
-        <v>5.56</v>
+        <v>-26.51</v>
       </c>
       <c r="D138" t="n">
-        <v>31.69</v>
-      </c>
-      <c r="E138" t="n">
-        <v>-50</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="139">
@@ -2798,16 +2571,13 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>8.83</v>
+        <v>25.28</v>
       </c>
       <c r="C139" t="n">
-        <v>5.79</v>
+        <v>-27.37</v>
       </c>
       <c r="D139" t="n">
-        <v>31.8</v>
-      </c>
-      <c r="E139" t="n">
-        <v>-50</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="140">
@@ -2815,16 +2585,13 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>8.529999999999999</v>
+        <v>24.64</v>
       </c>
       <c r="C140" t="n">
-        <v>5.9</v>
+        <v>-28.22</v>
       </c>
       <c r="D140" t="n">
-        <v>31.96999999999999</v>
-      </c>
-      <c r="E140" t="n">
-        <v>-50</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="141">
@@ -2832,16 +2599,13 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>8.27</v>
+        <v>24.05</v>
       </c>
       <c r="C141" t="n">
-        <v>5.97</v>
+        <v>-28.99</v>
       </c>
       <c r="D141" t="n">
-        <v>32.14</v>
-      </c>
-      <c r="E141" t="n">
-        <v>-50</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="142">
@@ -2849,16 +2613,13 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>8.140000000000001</v>
+        <v>22.93</v>
       </c>
       <c r="C142" t="n">
-        <v>5.99</v>
+        <v>-29.71</v>
       </c>
       <c r="D142" t="n">
-        <v>32.25</v>
-      </c>
-      <c r="E142" t="n">
-        <v>-50</v>
+        <v>6.77</v>
       </c>
     </row>
     <row r="143">
@@ -2866,16 +2627,13 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>8.539999999999999</v>
+        <v>22.02</v>
       </c>
       <c r="C143" t="n">
-        <v>5.43</v>
+        <v>-29.66</v>
       </c>
       <c r="D143" t="n">
-        <v>32.41</v>
-      </c>
-      <c r="E143" t="n">
-        <v>-50</v>
+        <v>7.65</v>
       </c>
     </row>
     <row r="144">
@@ -2883,16 +2641,13 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>9.029999999999999</v>
+        <v>21.39</v>
       </c>
       <c r="C144" t="n">
-        <v>4.92</v>
+        <v>-29.81</v>
       </c>
       <c r="D144" t="n">
-        <v>32.43</v>
-      </c>
-      <c r="E144" t="n">
-        <v>-50</v>
+        <v>8.42</v>
       </c>
     </row>
     <row r="145">
@@ -2900,16 +2655,13 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>9.56</v>
+        <v>20.92</v>
       </c>
       <c r="C145" t="n">
-        <v>4.15</v>
+        <v>-29.92</v>
       </c>
       <c r="D145" t="n">
-        <v>32.67</v>
-      </c>
-      <c r="E145" t="n">
-        <v>-50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="146">
@@ -2917,16 +2669,13 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>9.710000000000001</v>
+        <v>21.07</v>
       </c>
       <c r="C146" t="n">
-        <v>3.64</v>
+        <v>-30.02</v>
       </c>
       <c r="D146" t="n">
-        <v>33.03</v>
-      </c>
-      <c r="E146" t="n">
-        <v>-50</v>
+        <v>8.949999999999999</v>
       </c>
     </row>
     <row r="147">
@@ -2934,16 +2683,13 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>9.9</v>
+        <v>21.49</v>
       </c>
       <c r="C147" t="n">
-        <v>3.1</v>
+        <v>-30.22</v>
       </c>
       <c r="D147" t="n">
-        <v>33.32</v>
-      </c>
-      <c r="E147" t="n">
-        <v>-50</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="148">
@@ -2951,16 +2697,13 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>10.07</v>
+        <v>21.62</v>
       </c>
       <c r="C148" t="n">
-        <v>2.49</v>
+        <v>-30.4</v>
       </c>
       <c r="D148" t="n">
-        <v>33.7</v>
-      </c>
-      <c r="E148" t="n">
-        <v>-50</v>
+        <v>8.779999999999999</v>
       </c>
     </row>
     <row r="149">
@@ -2968,16 +2711,13 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>9.82</v>
+        <v>21.76</v>
       </c>
       <c r="C149" t="n">
-        <v>1.88</v>
+        <v>-30.49</v>
       </c>
       <c r="D149" t="n">
-        <v>34.49499999999999</v>
-      </c>
-      <c r="E149" t="n">
-        <v>-50</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="150">
@@ -2985,16 +2725,13 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>9.58</v>
+        <v>21.88</v>
       </c>
       <c r="C150" t="n">
-        <v>1.45</v>
+        <v>-30.57</v>
       </c>
       <c r="D150" t="n">
-        <v>35.16999999999999</v>
-      </c>
-      <c r="E150" t="n">
-        <v>-50</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="151">
@@ -3002,16 +2739,13 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>9.43</v>
+        <v>22.17</v>
       </c>
       <c r="C151" t="n">
-        <v>0.95</v>
+        <v>-30.68</v>
       </c>
       <c r="D151" t="n">
-        <v>35.825</v>
-      </c>
-      <c r="E151" t="n">
-        <v>-50</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="152">
@@ -3019,16 +2753,13 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>9.050000000000001</v>
+        <v>22.75</v>
       </c>
       <c r="C152" t="n">
-        <v>0.65</v>
+        <v>-30.85</v>
       </c>
       <c r="D152" t="n">
-        <v>36.49999999999999</v>
-      </c>
-      <c r="E152" t="n">
-        <v>-50</v>
+        <v>8.109999999999999</v>
       </c>
     </row>
     <row r="153">
@@ -3036,16 +2767,13 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>8.68</v>
+        <v>23.21</v>
       </c>
       <c r="C153" t="n">
-        <v>0.36</v>
+        <v>-31.09</v>
       </c>
       <c r="D153" t="n">
-        <v>37.15499999999999</v>
-      </c>
-      <c r="E153" t="n">
-        <v>-50</v>
+        <v>7.88</v>
       </c>
     </row>
     <row r="154">
@@ -3053,16 +2781,13 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>8.27</v>
+        <v>23.49</v>
       </c>
       <c r="C154" t="n">
-        <v>0.08</v>
+        <v>-30.17</v>
       </c>
       <c r="D154" t="n">
-        <v>37.84999999999999</v>
-      </c>
-      <c r="E154" t="n">
-        <v>-50</v>
+        <v>6.68</v>
       </c>
     </row>
     <row r="155">
@@ -3070,16 +2795,13 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>7.88</v>
+        <v>23.6</v>
       </c>
       <c r="C155" t="n">
-        <v>0.16</v>
+        <v>-29.24</v>
       </c>
       <c r="D155" t="n">
-        <v>38.165</v>
-      </c>
-      <c r="E155" t="n">
-        <v>-50</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="156">
@@ -3087,16 +2809,13 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>7.52</v>
+        <v>23.65</v>
       </c>
       <c r="C156" t="n">
-        <v>0.24</v>
+        <v>-28.3</v>
       </c>
       <c r="D156" t="n">
-        <v>38.44</v>
-      </c>
-      <c r="E156" t="n">
-        <v>-50</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="157">
@@ -3104,16 +2823,13 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>6.96</v>
+        <v>23.53</v>
       </c>
       <c r="C157" t="n">
-        <v>0.36</v>
+        <v>-27.38</v>
       </c>
       <c r="D157" t="n">
-        <v>38.87499999999999</v>
-      </c>
-      <c r="E157" t="n">
-        <v>-50</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="158">
@@ -3121,16 +2837,13 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>6.41</v>
+        <v>24.38</v>
       </c>
       <c r="C158" t="n">
-        <v>0.54</v>
+        <v>-27.16</v>
       </c>
       <c r="D158" t="n">
-        <v>39.25</v>
-      </c>
-      <c r="E158" t="n">
-        <v>-50</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="159">
@@ -3138,16 +2851,13 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>6.28</v>
+        <v>25.25</v>
       </c>
       <c r="C159" t="n">
-        <v>0.73</v>
+        <v>-26.96</v>
       </c>
       <c r="D159" t="n">
-        <v>39.19</v>
-      </c>
-      <c r="E159" t="n">
-        <v>-50</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="160">
@@ -3155,16 +2865,13 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>6.17</v>
+        <v>26.01</v>
       </c>
       <c r="C160" t="n">
-        <v>-0.14</v>
+        <v>-26.58</v>
       </c>
       <c r="D160" t="n">
-        <v>40.17</v>
-      </c>
-      <c r="E160" t="n">
-        <v>-50</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="161">
@@ -3172,16 +2879,13 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>5.95</v>
+        <v>26.58</v>
       </c>
       <c r="C161" t="n">
-        <v>-0.47</v>
+        <v>-26</v>
       </c>
       <c r="D161" t="n">
-        <v>40.71999999999999</v>
-      </c>
-      <c r="E161" t="n">
-        <v>-50</v>
+        <v>-0.58</v>
       </c>
     </row>
     <row r="162">
@@ -3189,16 +2893,13 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>5.73</v>
+        <v>26.74</v>
       </c>
       <c r="C162" t="n">
-        <v>-0.33</v>
+        <v>-25.4</v>
       </c>
       <c r="D162" t="n">
-        <v>40.79799999999999</v>
-      </c>
-      <c r="E162" t="n">
-        <v>-50</v>
+        <v>-1.34</v>
       </c>
     </row>
     <row r="163">
@@ -3206,16 +2907,13 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>5.56</v>
+        <v>27.12</v>
       </c>
       <c r="C163" t="n">
-        <v>-0.18</v>
+        <v>-24.91</v>
       </c>
       <c r="D163" t="n">
-        <v>40.816</v>
-      </c>
-      <c r="E163" t="n">
-        <v>-50</v>
+        <v>-2.21</v>
       </c>
     </row>
     <row r="164">
@@ -3223,16 +2921,13 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>5.95</v>
+        <v>27.48</v>
       </c>
       <c r="C164" t="n">
-        <v>-0.04</v>
+        <v>-25.47</v>
       </c>
       <c r="D164" t="n">
-        <v>40.294</v>
-      </c>
-      <c r="E164" t="n">
-        <v>-50</v>
+        <v>-2.01</v>
       </c>
     </row>
     <row r="165">
@@ -3240,16 +2935,13 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>6.36</v>
+        <v>27.89</v>
       </c>
       <c r="C165" t="n">
-        <v>-0.03</v>
+        <v>-26.02</v>
       </c>
       <c r="D165" t="n">
-        <v>39.87199999999999</v>
-      </c>
-      <c r="E165" t="n">
-        <v>-50</v>
+        <v>-1.87</v>
       </c>
     </row>
     <row r="166">
@@ -3257,16 +2949,13 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>6.73</v>
+        <v>28.48</v>
       </c>
       <c r="C166" t="n">
-        <v>-0.14</v>
+        <v>-26.63</v>
       </c>
       <c r="D166" t="n">
-        <v>39.60999999999999</v>
-      </c>
-      <c r="E166" t="n">
-        <v>-50</v>
+        <v>-1.85</v>
       </c>
     </row>
     <row r="167">
@@ -3274,16 +2963,13 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>6.78</v>
+        <v>29.05</v>
       </c>
       <c r="C167" t="n">
-        <v>-0.33</v>
+        <v>-27.23</v>
       </c>
       <c r="D167" t="n">
-        <v>39.74799999999999</v>
-      </c>
-      <c r="E167" t="n">
-        <v>-50</v>
+        <v>-1.82</v>
       </c>
     </row>
     <row r="168">
@@ -3291,16 +2977,13 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>6.86</v>
+        <v>28.96</v>
       </c>
       <c r="C168" t="n">
-        <v>-0.51</v>
+        <v>-27.12</v>
       </c>
       <c r="D168" t="n">
-        <v>39.84599999999999</v>
-      </c>
-      <c r="E168" t="n">
-        <v>-50</v>
+        <v>-1.84</v>
       </c>
     </row>
     <row r="169">
@@ -3308,16 +2991,13 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>6.83</v>
+        <v>28.86</v>
       </c>
       <c r="C169" t="n">
-        <v>-0.67</v>
+        <v>-27.02</v>
       </c>
       <c r="D169" t="n">
-        <v>40.044</v>
-      </c>
-      <c r="E169" t="n">
-        <v>-50</v>
+        <v>-1.84</v>
       </c>
     </row>
     <row r="170">
@@ -3325,16 +3005,13 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>6.38</v>
+        <v>28.89</v>
       </c>
       <c r="C170" t="n">
-        <v>0.57</v>
+        <v>-27.11</v>
       </c>
       <c r="D170" t="n">
-        <v>39.242</v>
-      </c>
-      <c r="E170" t="n">
-        <v>-50</v>
+        <v>-1.79</v>
       </c>
     </row>
     <row r="171">
@@ -3342,16 +3019,13 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>5.75</v>
+        <v>29.34</v>
       </c>
       <c r="C171" t="n">
-        <v>1.36</v>
+        <v>-27.44</v>
       </c>
       <c r="D171" t="n">
-        <v>39.09</v>
-      </c>
-      <c r="E171" t="n">
-        <v>-50</v>
+        <v>-1.9</v>
       </c>
     </row>
     <row r="172">
@@ -3359,16 +3033,13 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>5.23</v>
+        <v>29.95</v>
       </c>
       <c r="C172" t="n">
-        <v>1.56</v>
+        <v>-27.79</v>
       </c>
       <c r="D172" t="n">
-        <v>39.41</v>
-      </c>
-      <c r="E172" t="n">
-        <v>-50</v>
+        <v>-2.16</v>
       </c>
     </row>
     <row r="173">
@@ -3376,16 +3047,13 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>4.63</v>
+        <v>30.46</v>
       </c>
       <c r="C173" t="n">
-        <v>1.86</v>
+        <v>-28.05</v>
       </c>
       <c r="D173" t="n">
-        <v>39.70999999999999</v>
-      </c>
-      <c r="E173" t="n">
-        <v>-50</v>
+        <v>-2.44</v>
       </c>
     </row>
     <row r="174">
@@ -3393,16 +3061,13 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>3.44</v>
+        <v>31.04</v>
       </c>
       <c r="C174" t="n">
-        <v>2.2</v>
+        <v>-28.39</v>
       </c>
       <c r="D174" t="n">
-        <v>40.57</v>
-      </c>
-      <c r="E174" t="n">
-        <v>-50</v>
+        <v>-2.71</v>
       </c>
     </row>
     <row r="175">
@@ -3410,16 +3075,13 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>2.28</v>
+        <v>31.65</v>
       </c>
       <c r="C175" t="n">
-        <v>2.55</v>
+        <v>-28.73</v>
       </c>
       <c r="D175" t="n">
-        <v>41.37</v>
-      </c>
-      <c r="E175" t="n">
-        <v>-50</v>
+        <v>-3.01</v>
       </c>
     </row>
     <row r="176">
@@ -3427,832 +3089,13 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>1.12</v>
+        <v>32.14</v>
       </c>
       <c r="C176" t="n">
-        <v>3.03</v>
+        <v>-28.7</v>
       </c>
       <c r="D176" t="n">
-        <v>42.05</v>
-      </c>
-      <c r="E176" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" s="1" t="n">
-        <v>175</v>
-      </c>
-      <c r="B177" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="C177" t="n">
-        <v>3.58</v>
-      </c>
-      <c r="D177" t="n">
-        <v>42.499</v>
-      </c>
-      <c r="E177" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" s="1" t="n">
-        <v>176</v>
-      </c>
-      <c r="B178" t="n">
-        <v>-0.89</v>
-      </c>
-      <c r="C178" t="n">
-        <v>4.13</v>
-      </c>
-      <c r="D178" t="n">
-        <v>42.95799999999999</v>
-      </c>
-      <c r="E178" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" s="1" t="n">
-        <v>177</v>
-      </c>
-      <c r="B179" t="n">
-        <v>-1.77</v>
-      </c>
-      <c r="C179" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="D179" t="n">
-        <v>43.297</v>
-      </c>
-      <c r="E179" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" s="1" t="n">
-        <v>178</v>
-      </c>
-      <c r="B180" t="n">
-        <v>-2.17</v>
-      </c>
-      <c r="C180" t="n">
-        <v>4.71</v>
-      </c>
-      <c r="D180" t="n">
-        <v>43.656</v>
-      </c>
-      <c r="E180" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" s="1" t="n">
-        <v>179</v>
-      </c>
-      <c r="B181" t="n">
-        <v>-2.38</v>
-      </c>
-      <c r="C181" t="n">
-        <v>4.74</v>
-      </c>
-      <c r="D181" t="n">
-        <v>43.84500000000001</v>
-      </c>
-      <c r="E181" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="B182" t="n">
-        <v>-2.66</v>
-      </c>
-      <c r="C182" t="n">
-        <v>4.83</v>
-      </c>
-      <c r="D182" t="n">
-        <v>44.03400000000001</v>
-      </c>
-      <c r="E182" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="1" t="n">
-        <v>181</v>
-      </c>
-      <c r="B183" t="n">
-        <v>-2.94</v>
-      </c>
-      <c r="C183" t="n">
-        <v>4.84</v>
-      </c>
-      <c r="D183" t="n">
-        <v>44.303</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" s="1" t="n">
-        <v>182</v>
-      </c>
-      <c r="B184" t="n">
-        <v>-2.87</v>
-      </c>
-      <c r="C184" t="n">
-        <v>4.83</v>
-      </c>
-      <c r="D184" t="n">
-        <v>44.23800000000001</v>
-      </c>
-      <c r="E184" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" s="1" t="n">
-        <v>183</v>
-      </c>
-      <c r="B185" t="n">
-        <v>-2.87</v>
-      </c>
-      <c r="C185" t="n">
-        <v>4.86</v>
-      </c>
-      <c r="D185" t="n">
-        <v>44.213</v>
-      </c>
-      <c r="E185" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" s="1" t="n">
-        <v>184</v>
-      </c>
-      <c r="B186" t="n">
-        <v>-2.92</v>
-      </c>
-      <c r="C186" t="n">
-        <v>4.85</v>
-      </c>
-      <c r="D186" t="n">
-        <v>44.26799999999999</v>
-      </c>
-      <c r="E186" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" s="1" t="n">
-        <v>185</v>
-      </c>
-      <c r="B187" t="n">
-        <v>-3.18</v>
-      </c>
-      <c r="C187" t="n">
-        <v>4.85</v>
-      </c>
-      <c r="D187" t="n">
-        <v>44.53399999999999</v>
-      </c>
-      <c r="E187" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" s="1" t="n">
-        <v>186</v>
-      </c>
-      <c r="B188" t="n">
-        <v>-3.25</v>
-      </c>
-      <c r="C188" t="n">
-        <v>4.68</v>
-      </c>
-      <c r="D188" t="n">
-        <v>44.77</v>
-      </c>
-      <c r="E188" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" s="1" t="n">
-        <v>187</v>
-      </c>
-      <c r="B189" t="n">
-        <v>-3.38</v>
-      </c>
-      <c r="C189" t="n">
-        <v>4.47</v>
-      </c>
-      <c r="D189" t="n">
-        <v>45.10600000000001</v>
-      </c>
-      <c r="E189" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" s="1" t="n">
-        <v>188</v>
-      </c>
-      <c r="B190" t="n">
-        <v>-3.39</v>
-      </c>
-      <c r="C190" t="n">
-        <v>4.22</v>
-      </c>
-      <c r="D190" t="n">
-        <v>45.377</v>
-      </c>
-      <c r="E190" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" s="1" t="n">
-        <v>189</v>
-      </c>
-      <c r="B191" t="n">
-        <v>-3.11</v>
-      </c>
-      <c r="C191" t="n">
-        <v>3.71</v>
-      </c>
-      <c r="D191" t="n">
-        <v>45.598</v>
-      </c>
-      <c r="E191" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" s="1" t="n">
-        <v>190</v>
-      </c>
-      <c r="B192" t="n">
-        <v>-2.89</v>
-      </c>
-      <c r="C192" t="n">
-        <v>3.21</v>
-      </c>
-      <c r="D192" t="n">
-        <v>45.879</v>
-      </c>
-      <c r="E192" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" s="1" t="n">
-        <v>191</v>
-      </c>
-      <c r="B193" t="n">
-        <v>-2.74</v>
-      </c>
-      <c r="C193" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D193" t="n">
-        <v>46.44</v>
-      </c>
-      <c r="E193" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" s="1" t="n">
-        <v>192</v>
-      </c>
-      <c r="B194" t="n">
-        <v>-2.91</v>
-      </c>
-      <c r="C194" t="n">
-        <v>1.79</v>
-      </c>
-      <c r="D194" t="n">
-        <v>47.315</v>
-      </c>
-      <c r="E194" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" s="1" t="n">
-        <v>193</v>
-      </c>
-      <c r="B195" t="n">
-        <v>-2.52</v>
-      </c>
-      <c r="C195" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="D195" t="n">
-        <v>48.20999999999999</v>
-      </c>
-      <c r="E195" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" s="1" t="n">
-        <v>194</v>
-      </c>
-      <c r="B196" t="n">
-        <v>-2.1</v>
-      </c>
-      <c r="C196" t="n">
-        <v>-0.51</v>
-      </c>
-      <c r="D196" t="n">
-        <v>48.808</v>
-      </c>
-      <c r="E196" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" s="1" t="n">
-        <v>195</v>
-      </c>
-      <c r="B197" t="n">
-        <v>-1.13</v>
-      </c>
-      <c r="C197" t="n">
-        <v>-1.98</v>
-      </c>
-      <c r="D197" t="n">
-        <v>49.316</v>
-      </c>
-      <c r="E197" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" s="1" t="n">
-        <v>196</v>
-      </c>
-      <c r="B198" t="n">
-        <v>-0.22</v>
-      </c>
-      <c r="C198" t="n">
-        <v>-3.36</v>
-      </c>
-      <c r="D198" t="n">
-        <v>49.78400000000001</v>
-      </c>
-      <c r="E198" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" s="1" t="n">
-        <v>197</v>
-      </c>
-      <c r="B199" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="C199" t="n">
-        <v>-4.69</v>
-      </c>
-      <c r="D199" t="n">
-        <v>50.712</v>
-      </c>
-      <c r="E199" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" s="1" t="n">
-        <v>198</v>
-      </c>
-      <c r="B200" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="C200" t="n">
-        <v>-5.95</v>
-      </c>
-      <c r="D200" t="n">
-        <v>51.725</v>
-      </c>
-      <c r="E200" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" s="1" t="n">
-        <v>199</v>
-      </c>
-      <c r="B201" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="C201" t="n">
-        <v>-6.94</v>
-      </c>
-      <c r="D201" t="n">
-        <v>52.818</v>
-      </c>
-      <c r="E201" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="B202" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="C202" t="n">
-        <v>-7.99</v>
-      </c>
-      <c r="D202" t="n">
-        <v>53.461</v>
-      </c>
-      <c r="E202" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="B203" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="C203" t="n">
-        <v>-8.869999999999999</v>
-      </c>
-      <c r="D203" t="n">
-        <v>54.104</v>
-      </c>
-      <c r="E203" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" s="1" t="n">
-        <v>202</v>
-      </c>
-      <c r="B204" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="C204" t="n">
-        <v>-9.619999999999999</v>
-      </c>
-      <c r="D204" t="n">
-        <v>54.617</v>
-      </c>
-      <c r="E204" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" s="1" t="n">
-        <v>203</v>
-      </c>
-      <c r="B205" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="C205" t="n">
-        <v>-9.84</v>
-      </c>
-      <c r="D205" t="n">
-        <v>55.11999999999999</v>
-      </c>
-      <c r="E205" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" s="1" t="n">
-        <v>204</v>
-      </c>
-      <c r="B206" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C206" t="n">
-        <v>-10.2</v>
-      </c>
-      <c r="D206" t="n">
-        <v>55.8</v>
-      </c>
-      <c r="E206" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" s="1" t="n">
-        <v>205</v>
-      </c>
-      <c r="B207" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="C207" t="n">
-        <v>-10.11</v>
-      </c>
-      <c r="D207" t="n">
-        <v>56.04000000000001</v>
-      </c>
-      <c r="E207" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" s="1" t="n">
-        <v>206</v>
-      </c>
-      <c r="B208" t="n">
-        <v>-0.61</v>
-      </c>
-      <c r="C208" t="n">
-        <v>-9.960000000000001</v>
-      </c>
-      <c r="D208" t="n">
-        <v>56.77</v>
-      </c>
-      <c r="E208" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" s="1" t="n">
-        <v>207</v>
-      </c>
-      <c r="B209" t="n">
-        <v>-0.65</v>
-      </c>
-      <c r="C209" t="n">
-        <v>-9.869999999999999</v>
-      </c>
-      <c r="D209" t="n">
-        <v>56.72000000000001</v>
-      </c>
-      <c r="E209" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" s="1" t="n">
-        <v>208</v>
-      </c>
-      <c r="B210" t="n">
-        <v>-0.68</v>
-      </c>
-      <c r="C210" t="n">
-        <v>-9.75</v>
-      </c>
-      <c r="D210" t="n">
-        <v>56.63000000000001</v>
-      </c>
-      <c r="E210" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" s="1" t="n">
-        <v>209</v>
-      </c>
-      <c r="B211" t="n">
-        <v>-0.65</v>
-      </c>
-      <c r="C211" t="n">
-        <v>-9.81</v>
-      </c>
-      <c r="D211" t="n">
-        <v>56.66</v>
-      </c>
-      <c r="E211" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" s="1" t="n">
-        <v>210</v>
-      </c>
-      <c r="B212" t="n">
-        <v>-1.09</v>
-      </c>
-      <c r="C212" t="n">
-        <v>-9.789999999999999</v>
-      </c>
-      <c r="D212" t="n">
-        <v>57.08</v>
-      </c>
-      <c r="E212" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" s="1" t="n">
-        <v>211</v>
-      </c>
-      <c r="B213" t="n">
-        <v>-1.36</v>
-      </c>
-      <c r="C213" t="n">
-        <v>-9.640000000000001</v>
-      </c>
-      <c r="D213" t="n">
-        <v>57.2</v>
-      </c>
-      <c r="E213" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" s="1" t="n">
-        <v>212</v>
-      </c>
-      <c r="B214" t="n">
-        <v>-0.85</v>
-      </c>
-      <c r="C214" t="n">
-        <v>-9.83</v>
-      </c>
-      <c r="D214" t="n">
-        <v>56.88499999999999</v>
-      </c>
-      <c r="E214" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" s="1" t="n">
-        <v>213</v>
-      </c>
-      <c r="B215" t="n">
-        <v>-0.4</v>
-      </c>
-      <c r="C215" t="n">
-        <v>-9.98</v>
-      </c>
-      <c r="D215" t="n">
-        <v>56.58</v>
-      </c>
-      <c r="E215" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" s="1" t="n">
-        <v>214</v>
-      </c>
-      <c r="B216" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C216" t="n">
-        <v>-10.27</v>
-      </c>
-      <c r="D216" t="n">
-        <v>56.255</v>
-      </c>
-      <c r="E216" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" s="1" t="n">
-        <v>215</v>
-      </c>
-      <c r="B217" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="C217" t="n">
-        <v>-10.62</v>
-      </c>
-      <c r="D217" t="n">
-        <v>55.98</v>
-      </c>
-      <c r="E217" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" s="1" t="n">
-        <v>216</v>
-      </c>
-      <c r="B218" t="n">
-        <v>2.02</v>
-      </c>
-      <c r="C218" t="n">
-        <v>-11.02</v>
-      </c>
-      <c r="D218" t="n">
-        <v>55.205</v>
-      </c>
-      <c r="E218" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" s="1" t="n">
-        <v>217</v>
-      </c>
-      <c r="B219" t="n">
-        <v>2.91</v>
-      </c>
-      <c r="C219" t="n">
-        <v>-11.36</v>
-      </c>
-      <c r="D219" t="n">
-        <v>54.65</v>
-      </c>
-      <c r="E219" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" s="1" t="n">
-        <v>218</v>
-      </c>
-      <c r="B220" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="C220" t="n">
-        <v>-11.64</v>
-      </c>
-      <c r="D220" t="n">
-        <v>54.09500000000001</v>
-      </c>
-      <c r="E220" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" s="1" t="n">
-        <v>219</v>
-      </c>
-      <c r="B221" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="C221" t="n">
-        <v>-11.76</v>
-      </c>
-      <c r="D221" t="n">
-        <v>53.56</v>
-      </c>
-      <c r="E221" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" s="1" t="n">
-        <v>220</v>
-      </c>
-      <c r="B222" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="C222" t="n">
-        <v>-12.21</v>
-      </c>
-      <c r="D222" t="n">
-        <v>53.425</v>
-      </c>
-      <c r="E222" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" s="1" t="n">
-        <v>221</v>
-      </c>
-      <c r="B223" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="C223" t="n">
-        <v>-12.59</v>
-      </c>
-      <c r="D223" t="n">
-        <v>53.19</v>
-      </c>
-      <c r="E223" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" s="1" t="n">
-        <v>222</v>
-      </c>
-      <c r="B224" t="n">
-        <v>5.26</v>
-      </c>
-      <c r="C224" t="n">
-        <v>-12.61</v>
-      </c>
-      <c r="D224" t="n">
-        <v>53.54</v>
-      </c>
-      <c r="E224" t="n">
-        <v>-50</v>
+        <v>-3.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Functions moved to fewer files"
This reverts commit 2b64c9e523a152c1844af1b8e60b857c87e690b1.
</commit_message>
<xml_diff>
--- a/Outputs/net_over_time_avg.xlsx
+++ b/Outputs/net_over_time_avg.xlsx
@@ -162,7 +162,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Net vs time this session (07/05/21): 10-hand moving averages</a:t>
+              <a:t>Net vs time this session (05/20/21): 10-hand moving averages</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -194,7 +194,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$B$2:$B$176</f>
+              <f>'data'!$B$2:$B$224</f>
             </numRef>
           </val>
         </ser>
@@ -221,7 +221,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$C$2:$C$176</f>
+              <f>'data'!$C$2:$C$224</f>
             </numRef>
           </val>
         </ser>
@@ -248,7 +248,34 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$D$2:$D$176</f>
+              <f>'data'!$D$2:$D$224</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <strRef>
+              <f>'data'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <val>
+            <numRef>
+              <f>'data'!$E$2:$E$224</f>
             </numRef>
           </val>
         </ser>
@@ -618,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D176"/>
+  <dimension ref="A1:E224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -639,7 +666,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Raymond</t>
+          <t>Cedric</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -647,6 +674,11 @@
           <t>Scott</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Xavier</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -658,22 +690,16 @@
       <c r="C2" t="n">
         <v>0</v>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.35</v>
+        <v>0.1</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.05</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.4</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="4">
@@ -681,13 +707,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.7</v>
+        <v>0.47</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.5</v>
+        <v>-0.47</v>
       </c>
     </row>
     <row r="5">
@@ -695,13 +718,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-1.02</v>
+        <v>0.68</v>
       </c>
       <c r="C5" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.85</v>
+        <v>-0.68</v>
       </c>
     </row>
     <row r="6">
@@ -709,13 +729,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.26</v>
+        <v>0.76</v>
       </c>
       <c r="C6" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.12</v>
+        <v>-0.76</v>
       </c>
     </row>
     <row r="7">
@@ -723,13 +740,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-1.52</v>
+        <v>0.72</v>
       </c>
       <c r="C7" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1.4</v>
+        <v>-0.72</v>
       </c>
     </row>
     <row r="8">
@@ -737,13 +751,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-1.67</v>
+        <v>0.74</v>
       </c>
       <c r="C8" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.6</v>
+        <v>-0.74</v>
       </c>
     </row>
     <row r="9">
@@ -751,13 +762,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-1.94</v>
+        <v>0.74</v>
       </c>
       <c r="C9" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.75</v>
+        <v>-0.74</v>
       </c>
     </row>
     <row r="10">
@@ -765,13 +773,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.21</v>
+        <v>0.67</v>
       </c>
       <c r="C10" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1.87</v>
+        <v>-0.67</v>
       </c>
     </row>
     <row r="11">
@@ -779,13 +784,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>-2.37</v>
+        <v>0.97</v>
       </c>
       <c r="C11" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1.96</v>
+        <v>-0.97</v>
       </c>
     </row>
     <row r="12">
@@ -793,13 +795,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>-2.37</v>
+        <v>0.97</v>
       </c>
       <c r="C12" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1.96</v>
+        <v>-0.97</v>
       </c>
     </row>
     <row r="13">
@@ -807,13 +806,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-2.77</v>
+        <v>1.36</v>
       </c>
       <c r="C13" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="D13" t="n">
-        <v>2.24</v>
+        <v>-1.36</v>
       </c>
     </row>
     <row r="14">
@@ -821,13 +817,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-3.16</v>
+        <v>1.85</v>
       </c>
       <c r="C14" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="D14" t="n">
-        <v>2.44</v>
+        <v>-1.85</v>
       </c>
     </row>
     <row r="15">
@@ -835,13 +828,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>-3.42</v>
+        <v>2.18</v>
       </c>
       <c r="C15" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="D15" t="n">
-        <v>2.65</v>
+        <v>-2.18</v>
       </c>
     </row>
     <row r="16">
@@ -849,13 +839,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-3.63</v>
+        <v>2.35</v>
       </c>
       <c r="C16" t="n">
-        <v>0.89</v>
-      </c>
-      <c r="D16" t="n">
-        <v>2.74</v>
+        <v>-2.35</v>
       </c>
     </row>
     <row r="17">
@@ -863,13 +850,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>-3.81</v>
+        <v>2.64</v>
       </c>
       <c r="C17" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="D17" t="n">
-        <v>2.8</v>
+        <v>-2.64</v>
       </c>
     </row>
     <row r="18">
@@ -877,13 +861,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>-3.99</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
-        <v>1.19</v>
-      </c>
-      <c r="D18" t="n">
-        <v>2.8</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="19">
@@ -891,13 +872,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-4.16</v>
+        <v>3.44</v>
       </c>
       <c r="C19" t="n">
-        <v>1.39</v>
-      </c>
-      <c r="D19" t="n">
-        <v>2.77</v>
+        <v>-3.44</v>
       </c>
     </row>
     <row r="20">
@@ -905,13 +883,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-4.03</v>
+        <v>3.91</v>
       </c>
       <c r="C20" t="n">
-        <v>1.29</v>
-      </c>
-      <c r="D20" t="n">
-        <v>2.74</v>
+        <v>-3.91</v>
       </c>
     </row>
     <row r="21">
@@ -919,13 +894,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-3.81</v>
+        <v>4.46</v>
       </c>
       <c r="C21" t="n">
-        <v>1.12</v>
-      </c>
-      <c r="D21" t="n">
-        <v>2.69</v>
+        <v>-4.46</v>
       </c>
     </row>
     <row r="22">
@@ -933,13 +905,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>-3.67</v>
+        <v>4.41</v>
       </c>
       <c r="C22" t="n">
-        <v>1.04</v>
-      </c>
-      <c r="D22" t="n">
-        <v>2.63</v>
+        <v>-4.41</v>
       </c>
     </row>
     <row r="23">
@@ -947,13 +916,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>-3.45</v>
+        <v>4.36</v>
       </c>
       <c r="C23" t="n">
-        <v>0.88</v>
+        <v>-4.36</v>
       </c>
       <c r="D23" t="n">
-        <v>2.57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -961,13 +930,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>-2.98</v>
+        <v>3.85</v>
       </c>
       <c r="C24" t="n">
-        <v>0.49</v>
+        <v>-4.23</v>
       </c>
       <c r="D24" t="n">
-        <v>2.51</v>
+        <v>-0.05</v>
       </c>
     </row>
     <row r="25">
@@ -975,13 +944,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-2.59</v>
+        <v>3.25</v>
       </c>
       <c r="C25" t="n">
-        <v>0.18</v>
+        <v>-4</v>
       </c>
       <c r="D25" t="n">
-        <v>2.45</v>
+        <v>-0.06666666666666667</v>
       </c>
     </row>
     <row r="26">
@@ -989,13 +958,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>-2.2</v>
+        <v>2.82</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.13</v>
+        <v>-3.94</v>
       </c>
       <c r="D26" t="n">
-        <v>2.39</v>
+        <v>-0.025</v>
       </c>
     </row>
     <row r="27">
@@ -1003,13 +972,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>-1.81</v>
+        <v>2.27</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.44</v>
+        <v>-3.78</v>
       </c>
       <c r="D27" t="n">
-        <v>2.33</v>
+        <v>-0.04</v>
       </c>
     </row>
     <row r="28">
@@ -1017,13 +986,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>-1.37</v>
+        <v>1.53</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.8</v>
+        <v>-3.41</v>
       </c>
       <c r="D28" t="n">
-        <v>2.27</v>
+        <v>-0.1166666666666667</v>
       </c>
     </row>
     <row r="29">
@@ -1031,13 +1000,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>-1.02</v>
+        <v>0.73</v>
       </c>
       <c r="C29" t="n">
-        <v>-1.1</v>
+        <v>-2.94</v>
       </c>
       <c r="D29" t="n">
-        <v>2.24</v>
+        <v>0.05714285714285716</v>
       </c>
     </row>
     <row r="30">
@@ -1045,13 +1014,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.86</v>
+        <v>-0.23</v>
       </c>
       <c r="C30" t="n">
-        <v>-1.21</v>
+        <v>-2.47</v>
       </c>
       <c r="D30" t="n">
-        <v>2.21</v>
+        <v>0.1625</v>
       </c>
     </row>
     <row r="31">
@@ -1059,13 +1028,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-0.75</v>
+        <v>-1.23</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.29</v>
+        <v>-1.94</v>
       </c>
       <c r="D31" t="n">
-        <v>2.2</v>
+        <v>0.2444444444444445</v>
       </c>
     </row>
     <row r="32">
@@ -1073,13 +1042,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-0.68</v>
+        <v>-1.98</v>
       </c>
       <c r="C32" t="n">
-        <v>-1.34</v>
+        <v>-1.66</v>
       </c>
       <c r="D32" t="n">
-        <v>2.2</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="33">
@@ -1087,13 +1056,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.66</v>
+        <v>-3.36</v>
       </c>
       <c r="C33" t="n">
-        <v>-1.34</v>
+        <v>-1.39</v>
       </c>
       <c r="D33" t="n">
-        <v>2.2</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="34">
@@ -1101,13 +1070,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.84</v>
+        <v>-4.38</v>
       </c>
       <c r="C34" t="n">
-        <v>-1.16</v>
+        <v>-1.09</v>
       </c>
       <c r="D34" t="n">
-        <v>2.2</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="35">
@@ -1115,13 +1084,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.99</v>
+        <v>-5.11</v>
       </c>
       <c r="C35" t="n">
-        <v>-1.01</v>
+        <v>-0.96</v>
       </c>
       <c r="D35" t="n">
-        <v>2.2</v>
+        <v>2.274999999999999</v>
       </c>
     </row>
     <row r="36">
@@ -1129,13 +1098,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-1.11</v>
+        <v>-5.88</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.89</v>
+        <v>-0.82</v>
       </c>
       <c r="D36" t="n">
-        <v>2.2</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="37">
@@ -1143,13 +1112,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-1.26</v>
+        <v>-6.63</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.74</v>
+        <v>-0.6899999999999999</v>
       </c>
       <c r="D37" t="n">
-        <v>2.2</v>
+        <v>3.524999999999999</v>
       </c>
     </row>
     <row r="38">
@@ -1157,13 +1126,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-1.46</v>
+        <v>-7.2</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.54</v>
+        <v>-0.77</v>
       </c>
       <c r="D38" t="n">
-        <v>2.2</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="39">
@@ -1171,13 +1140,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-1.62</v>
+        <v>-7.83</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.38</v>
+        <v>-0.9</v>
       </c>
       <c r="D39" t="n">
-        <v>2.2</v>
+        <v>4.924999999999999</v>
       </c>
     </row>
     <row r="40">
@@ -1185,13 +1154,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-1.89</v>
+        <v>-8.31</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.11</v>
+        <v>-1.03</v>
       </c>
       <c r="D40" t="n">
-        <v>2.18</v>
+        <v>5.54</v>
       </c>
     </row>
     <row r="41">
@@ -1199,13 +1168,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-2.16</v>
+        <v>-8.859999999999999</v>
       </c>
       <c r="C41" t="n">
-        <v>0.14</v>
+        <v>-1.11</v>
       </c>
       <c r="D41" t="n">
-        <v>2.18</v>
+        <v>6.175</v>
       </c>
     </row>
     <row r="42">
@@ -1213,13 +1182,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-2.31</v>
+        <v>-9.44</v>
       </c>
       <c r="C42" t="n">
-        <v>0.27</v>
+        <v>-1.18</v>
       </c>
       <c r="D42" t="n">
-        <v>2.18</v>
+        <v>6.82</v>
       </c>
     </row>
     <row r="43">
@@ -1227,13 +1196,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>-2.47</v>
+        <v>-9.289999999999999</v>
       </c>
       <c r="C43" t="n">
-        <v>0.4</v>
+        <v>-1.25</v>
       </c>
       <c r="D43" t="n">
-        <v>2.19</v>
+        <v>6.745</v>
       </c>
     </row>
     <row r="44">
@@ -1241,13 +1210,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-2.55</v>
+        <v>-9.119999999999999</v>
       </c>
       <c r="C44" t="n">
-        <v>0.46</v>
+        <v>-1.36</v>
       </c>
       <c r="D44" t="n">
-        <v>2.19</v>
+        <v>6.68</v>
       </c>
     </row>
     <row r="45">
@@ -1255,13 +1224,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>-2.49</v>
+        <v>-9.779999999999999</v>
       </c>
       <c r="C45" t="n">
-        <v>0.46</v>
+        <v>-1.46</v>
       </c>
       <c r="D45" t="n">
-        <v>2.11</v>
+        <v>7.44</v>
       </c>
     </row>
     <row r="46">
@@ -1269,13 +1238,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-2.51</v>
+        <v>-10.14</v>
       </c>
       <c r="C46" t="n">
-        <v>0.46</v>
+        <v>-1.82</v>
       </c>
       <c r="D46" t="n">
-        <v>2.11</v>
+        <v>8.159999999999998</v>
       </c>
     </row>
     <row r="47">
@@ -1283,13 +1252,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>-2.26</v>
+        <v>-10.49</v>
       </c>
       <c r="C47" t="n">
-        <v>0.2</v>
+        <v>-2.17</v>
       </c>
       <c r="D47" t="n">
-        <v>2.1</v>
+        <v>8.859999999999998</v>
       </c>
     </row>
     <row r="48">
@@ -1297,13 +1266,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-2.01</v>
+        <v>-10.86</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.14</v>
+        <v>-2.51</v>
       </c>
       <c r="D48" t="n">
-        <v>2.17</v>
+        <v>9.569999999999999</v>
       </c>
     </row>
     <row r="49">
@@ -1311,13 +1280,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-1.77</v>
+        <v>-11.22</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.51</v>
+        <v>-2.97</v>
       </c>
       <c r="D49" t="n">
-        <v>2.27</v>
+        <v>10.39</v>
       </c>
     </row>
     <row r="50">
@@ -1325,13 +1294,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-1.47</v>
+        <v>-11.56</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.99</v>
+        <v>-3.43</v>
       </c>
       <c r="D50" t="n">
-        <v>2.46</v>
+        <v>11.19</v>
       </c>
     </row>
     <row r="51">
@@ -1339,13 +1308,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-1.16</v>
+        <v>-11.89</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.99</v>
+        <v>-4.46</v>
       </c>
       <c r="D51" t="n">
-        <v>2.15</v>
+        <v>12.55</v>
       </c>
     </row>
     <row r="52">
@@ -1353,13 +1322,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.91</v>
+        <v>-12.21</v>
       </c>
       <c r="C52" t="n">
-        <v>-1.08</v>
+        <v>-5.51</v>
       </c>
       <c r="D52" t="n">
-        <v>1.99</v>
+        <v>13.92</v>
       </c>
     </row>
     <row r="53">
@@ -1367,13 +1336,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-0.68</v>
+        <v>-12.5</v>
       </c>
       <c r="C53" t="n">
-        <v>-1.15</v>
+        <v>-6.55</v>
       </c>
       <c r="D53" t="n">
-        <v>1.84</v>
+        <v>15.245</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1381,13 +1353,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-0.5</v>
+        <v>-12.78</v>
       </c>
       <c r="C54" t="n">
-        <v>-1.19</v>
+        <v>-7.53</v>
       </c>
       <c r="D54" t="n">
-        <v>1.7</v>
+        <v>16.51</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1395,13 +1370,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>-0.5</v>
+        <v>-12.43</v>
       </c>
       <c r="C55" t="n">
-        <v>-1.16</v>
+        <v>-8.210000000000001</v>
       </c>
       <c r="D55" t="n">
-        <v>1.66</v>
+        <v>16.835</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.06666666666666667</v>
       </c>
     </row>
     <row r="56">
@@ -1409,13 +1387,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>-0.57</v>
+        <v>-12.35</v>
       </c>
       <c r="C56" t="n">
-        <v>-1.12</v>
+        <v>-8.65</v>
       </c>
       <c r="D56" t="n">
-        <v>1.54</v>
+        <v>17.18</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="57">
@@ -1423,13 +1404,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.36</v>
+        <v>-12.31</v>
       </c>
       <c r="C57" t="n">
-        <v>-0.6899999999999999</v>
+        <v>-9.220000000000001</v>
       </c>
       <c r="D57" t="n">
-        <v>0.89</v>
+        <v>17.525</v>
+      </c>
+      <c r="E57" t="n">
+        <v>-0.18</v>
       </c>
     </row>
     <row r="58">
@@ -1437,13 +1421,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.02</v>
+        <v>-12.31</v>
       </c>
       <c r="C58" t="n">
-        <v>-0.25</v>
+        <v>-9.789999999999999</v>
       </c>
       <c r="D58" t="n">
-        <v>0.08</v>
+        <v>18.39</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.6333333333333334</v>
       </c>
     </row>
     <row r="59">
@@ -1451,13 +1438,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.79</v>
+        <v>-12.38</v>
       </c>
       <c r="C59" t="n">
-        <v>-0.17</v>
+        <v>-10.2</v>
       </c>
       <c r="D59" t="n">
-        <v>-0.77</v>
+        <v>18.405</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.9428571428571428</v>
       </c>
     </row>
     <row r="60">
@@ -1465,13 +1455,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>1.65</v>
+        <v>-12.53</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.11</v>
+        <v>-10.6</v>
       </c>
       <c r="D60" t="n">
-        <v>-1.69</v>
+        <v>18.67</v>
+      </c>
+      <c r="E60" t="n">
+        <v>-0.4712499999999999</v>
       </c>
     </row>
     <row r="61">
@@ -1479,13 +1472,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>2.62</v>
+        <v>-12.67</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.63</v>
+        <v>-8.859999999999999</v>
       </c>
       <c r="D61" t="n">
-        <v>-2.15</v>
+        <v>18.105</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-1.482222222222222</v>
       </c>
     </row>
     <row r="62">
@@ -1493,13 +1489,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>3.6</v>
+        <v>-12.88</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.99</v>
+        <v>-7.19</v>
       </c>
       <c r="D62" t="n">
-        <v>-2.77</v>
+        <v>17.6</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-2.531</v>
       </c>
     </row>
     <row r="63">
@@ -1507,13 +1506,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>4.54</v>
+        <v>-12.96</v>
       </c>
       <c r="C63" t="n">
-        <v>-1.55</v>
+        <v>-5.52</v>
       </c>
       <c r="D63" t="n">
-        <v>-3.15</v>
+        <v>17.21</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-2.531</v>
       </c>
     </row>
     <row r="64">
@@ -1521,13 +1523,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>5.41</v>
+        <v>-13.12</v>
       </c>
       <c r="C64" t="n">
-        <v>-2.09</v>
+        <v>-3.87</v>
       </c>
       <c r="D64" t="n">
-        <v>-3.47</v>
+        <v>16.94</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-3.748</v>
       </c>
     </row>
     <row r="65">
@@ -1535,13 +1540,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>6.22</v>
+        <v>-13.24</v>
       </c>
       <c r="C65" t="n">
-        <v>-2.8</v>
+        <v>-2.52</v>
       </c>
       <c r="D65" t="n">
-        <v>-3.57</v>
+        <v>16.75</v>
+      </c>
+      <c r="E65" t="n">
+        <v>-4.784999999999999</v>
       </c>
     </row>
     <row r="66">
@@ -1549,13 +1557,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>7.06</v>
+        <v>-13.42</v>
       </c>
       <c r="C66" t="n">
-        <v>-3.4</v>
+        <v>-1.16</v>
       </c>
       <c r="D66" t="n">
-        <v>-3.66</v>
+        <v>16.62</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-5.842</v>
       </c>
     </row>
     <row r="67">
@@ -1563,13 +1574,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>7.36</v>
+        <v>-13.58</v>
       </c>
       <c r="C67" t="n">
-        <v>-4.13</v>
+        <v>0.33</v>
       </c>
       <c r="D67" t="n">
-        <v>-3.23</v>
+        <v>16.58</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-7.129</v>
       </c>
     </row>
     <row r="68">
@@ -1577,13 +1591,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>7.64</v>
+        <v>-13.22</v>
       </c>
       <c r="C68" t="n">
-        <v>-4.91</v>
+        <v>1.81</v>
       </c>
       <c r="D68" t="n">
-        <v>-2.73</v>
+        <v>16.01</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-8.391</v>
       </c>
     </row>
     <row r="69">
@@ -1591,13 +1608,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>7.52</v>
+        <v>-12.35</v>
       </c>
       <c r="C69" t="n">
-        <v>-5.3</v>
+        <v>3.3</v>
       </c>
       <c r="D69" t="n">
-        <v>-2.22</v>
+        <v>16.11</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-10.861</v>
       </c>
     </row>
     <row r="70">
@@ -1605,13 +1625,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>7.39</v>
+        <v>-11.44</v>
       </c>
       <c r="C70" t="n">
-        <v>-5.76</v>
+        <v>4.81</v>
       </c>
       <c r="D70" t="n">
-        <v>-1.63</v>
+        <v>15.97</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-13.141</v>
       </c>
     </row>
     <row r="71">
@@ -1619,13 +1642,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>7.28</v>
+        <v>-9.76</v>
       </c>
       <c r="C71" t="n">
-        <v>-6.14</v>
+        <v>4.59</v>
       </c>
       <c r="D71" t="n">
-        <v>-1.14</v>
+        <v>16.09</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-14.724</v>
       </c>
     </row>
     <row r="72">
@@ -1633,13 +1659,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>7.14</v>
+        <v>-8.01</v>
       </c>
       <c r="C72" t="n">
-        <v>-6.5</v>
+        <v>4.49</v>
       </c>
       <c r="D72" t="n">
-        <v>-0.64</v>
+        <v>16.13</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-16.407</v>
       </c>
     </row>
     <row r="73">
@@ -1647,13 +1676,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>6.91</v>
+        <v>-6.62</v>
       </c>
       <c r="C73" t="n">
-        <v>-6.67</v>
+        <v>4.85</v>
       </c>
       <c r="D73" t="n">
-        <v>-0.24</v>
+        <v>16.18</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-18.21</v>
       </c>
     </row>
     <row r="74">
@@ -1661,13 +1693,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>6.59</v>
+        <v>-4.91</v>
       </c>
       <c r="C74" t="n">
-        <v>-6.83</v>
+        <v>5.17</v>
       </c>
       <c r="D74" t="n">
-        <v>0.24</v>
+        <v>15.93</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-19.993</v>
       </c>
     </row>
     <row r="75">
@@ -1675,13 +1710,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>6.33</v>
+        <v>-3.17</v>
       </c>
       <c r="C75" t="n">
-        <v>-6.81</v>
+        <v>5.33</v>
       </c>
       <c r="D75" t="n">
-        <v>0.47</v>
+        <v>16</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-21.956</v>
       </c>
     </row>
     <row r="76">
@@ -1689,13 +1727,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>6.19</v>
+        <v>-1.38</v>
       </c>
       <c r="C76" t="n">
-        <v>-6.84</v>
+        <v>5.48</v>
       </c>
       <c r="D76" t="n">
-        <v>0.65</v>
+        <v>16.354</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-24.253</v>
       </c>
     </row>
     <row r="77">
@@ -1703,13 +1744,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>6.07</v>
+        <v>0.26</v>
       </c>
       <c r="C77" t="n">
-        <v>-6.89</v>
+        <v>5.65</v>
       </c>
       <c r="D77" t="n">
-        <v>0.82</v>
+        <v>16.618</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-26.33</v>
       </c>
     </row>
     <row r="78">
@@ -1717,13 +1761,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>5.86</v>
+        <v>1.59</v>
       </c>
       <c r="C78" t="n">
-        <v>-6.87</v>
+        <v>5.83</v>
       </c>
       <c r="D78" t="n">
-        <v>1.01</v>
+        <v>16.812</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-28.032</v>
       </c>
     </row>
     <row r="79">
@@ -1731,13 +1778,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>5.67</v>
+        <v>2.41</v>
       </c>
       <c r="C79" t="n">
-        <v>-6.87</v>
+        <v>6.01</v>
       </c>
       <c r="D79" t="n">
-        <v>1.2</v>
+        <v>17.626</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-29.846</v>
       </c>
     </row>
     <row r="80">
@@ -1745,13 +1795,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>5.62</v>
+        <v>3.32</v>
       </c>
       <c r="C80" t="n">
-        <v>-6.79</v>
+        <v>6.19</v>
       </c>
       <c r="D80" t="n">
-        <v>1.17</v>
+        <v>18.43</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-31.74</v>
       </c>
     </row>
     <row r="81">
@@ -1759,13 +1812,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>5.55</v>
+        <v>3.52</v>
       </c>
       <c r="C81" t="n">
-        <v>-6.81</v>
+        <v>6.44</v>
       </c>
       <c r="D81" t="n">
-        <v>1.25</v>
+        <v>18.819</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-32.57899999999999</v>
       </c>
     </row>
     <row r="82">
@@ -1773,13 +1829,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>5.59</v>
+        <v>4.26</v>
       </c>
       <c r="C82" t="n">
-        <v>-6.86</v>
+        <v>6.65</v>
       </c>
       <c r="D82" t="n">
-        <v>1.27</v>
+        <v>18.948</v>
+      </c>
+      <c r="E82" t="n">
+        <v>-33.658</v>
       </c>
     </row>
     <row r="83">
@@ -1787,13 +1846,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>5.75</v>
+        <v>5.26</v>
       </c>
       <c r="C83" t="n">
-        <v>-6.87</v>
+        <v>6.42</v>
       </c>
       <c r="D83" t="n">
-        <v>1.12</v>
+        <v>19.077</v>
+      </c>
+      <c r="E83" t="n">
+        <v>-34.557</v>
       </c>
     </row>
     <row r="84">
@@ -1801,13 +1863,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>6.22</v>
+        <v>5.95</v>
       </c>
       <c r="C84" t="n">
-        <v>-6.9</v>
+        <v>6.25</v>
       </c>
       <c r="D84" t="n">
-        <v>0.68</v>
+        <v>19.261</v>
+      </c>
+      <c r="E84" t="n">
+        <v>-35.261</v>
       </c>
     </row>
     <row r="85">
@@ -1815,13 +1880,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>6.71</v>
+        <v>6.57</v>
       </c>
       <c r="C85" t="n">
-        <v>-6.95</v>
+        <v>6.24</v>
       </c>
       <c r="D85" t="n">
-        <v>0.24</v>
+        <v>19.275</v>
+      </c>
+      <c r="E85" t="n">
+        <v>-35.88500000000001</v>
       </c>
     </row>
     <row r="86">
@@ -1829,13 +1897,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>7.28</v>
+        <v>7.21</v>
       </c>
       <c r="C86" t="n">
-        <v>-7.06</v>
+        <v>6.24</v>
       </c>
       <c r="D86" t="n">
-        <v>-0.21</v>
+        <v>18.945</v>
+      </c>
+      <c r="E86" t="n">
+        <v>-36.195</v>
       </c>
     </row>
     <row r="87">
@@ -1843,13 +1914,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>7.92</v>
+        <v>8.18</v>
       </c>
       <c r="C87" t="n">
-        <v>-7.19</v>
+        <v>6.24</v>
       </c>
       <c r="D87" t="n">
-        <v>-0.73</v>
+        <v>18.545</v>
+      </c>
+      <c r="E87" t="n">
+        <v>-36.765</v>
       </c>
     </row>
     <row r="88">
@@ -1857,13 +1931,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>8.5</v>
+        <v>9.130000000000001</v>
       </c>
       <c r="C88" t="n">
-        <v>-7.34</v>
+        <v>6.17</v>
       </c>
       <c r="D88" t="n">
-        <v>-1.17</v>
+        <v>18.195</v>
+      </c>
+      <c r="E88" t="n">
+        <v>-37.285</v>
       </c>
     </row>
     <row r="89">
@@ -1871,13 +1948,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>9.27</v>
+        <v>10.11</v>
       </c>
       <c r="C89" t="n">
-        <v>-7.48</v>
+        <v>6.01</v>
       </c>
       <c r="D89" t="n">
-        <v>-1.79</v>
+        <v>17.225</v>
+      </c>
+      <c r="E89" t="n">
+        <v>-37.145</v>
       </c>
     </row>
     <row r="90">
@@ -1885,13 +1965,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>9.869999999999999</v>
+        <v>11</v>
       </c>
       <c r="C90" t="n">
-        <v>-7.68</v>
+        <v>5.9</v>
       </c>
       <c r="D90" t="n">
-        <v>-2.2</v>
+        <v>16.255</v>
+      </c>
+      <c r="E90" t="n">
+        <v>-36.94500000000001</v>
       </c>
     </row>
     <row r="91">
@@ -1899,13 +1982,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>10.38</v>
+        <v>11.71</v>
       </c>
       <c r="C91" t="n">
-        <v>-7.84</v>
+        <v>5.78</v>
       </c>
       <c r="D91" t="n">
-        <v>-2.54</v>
+        <v>14.97</v>
+      </c>
+      <c r="E91" t="n">
+        <v>-36.255</v>
       </c>
     </row>
     <row r="92">
@@ -1913,13 +1999,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>10.88</v>
+        <v>11.83</v>
       </c>
       <c r="C92" t="n">
-        <v>-7.99</v>
+        <v>5.65</v>
       </c>
       <c r="D92" t="n">
-        <v>-2.9</v>
+        <v>13.935</v>
+      </c>
+      <c r="E92" t="n">
+        <v>-35.205</v>
       </c>
     </row>
     <row r="93">
@@ -1927,13 +2016,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>11.4</v>
+        <v>11.75</v>
       </c>
       <c r="C93" t="n">
-        <v>-8.16</v>
+        <v>5.55</v>
       </c>
       <c r="D93" t="n">
-        <v>-3.24</v>
+        <v>12.9</v>
+      </c>
+      <c r="E93" t="n">
+        <v>-33.995</v>
       </c>
     </row>
     <row r="94">
@@ -1941,13 +2033,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>11.82</v>
+        <v>11.66</v>
       </c>
       <c r="C94" t="n">
-        <v>-8.32</v>
+        <v>5.92</v>
       </c>
       <c r="D94" t="n">
-        <v>-3.5</v>
+        <v>12.05</v>
+      </c>
+      <c r="E94" t="n">
+        <v>-33.42</v>
       </c>
     </row>
     <row r="95">
@@ -1955,13 +2050,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>12.3</v>
+        <v>11.54</v>
       </c>
       <c r="C95" t="n">
-        <v>-8.470000000000001</v>
+        <v>5.25</v>
       </c>
       <c r="D95" t="n">
-        <v>-3.83</v>
+        <v>11.12</v>
+      </c>
+      <c r="E95" t="n">
+        <v>-31.71</v>
       </c>
     </row>
     <row r="96">
@@ -1969,13 +2067,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>12.76</v>
+        <v>11.25</v>
       </c>
       <c r="C96" t="n">
-        <v>-8.68</v>
+        <v>2.31</v>
       </c>
       <c r="D96" t="n">
-        <v>-4.08</v>
+        <v>12.778</v>
+      </c>
+      <c r="E96" t="n">
+        <v>-30.14</v>
       </c>
     </row>
     <row r="97">
@@ -1983,13 +2084,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>13.12</v>
+        <v>10.79</v>
       </c>
       <c r="C97" t="n">
-        <v>-8.720000000000001</v>
+        <v>-0.61</v>
       </c>
       <c r="D97" t="n">
-        <v>-4.4</v>
+        <v>14.506</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-28.48</v>
       </c>
     </row>
     <row r="98">
@@ -1997,13 +2101,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>13.55</v>
+        <v>10.2</v>
       </c>
       <c r="C98" t="n">
-        <v>-8.75</v>
+        <v>-3.28</v>
       </c>
       <c r="D98" t="n">
-        <v>-4.8</v>
+        <v>16.168</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-26.886</v>
       </c>
     </row>
     <row r="99">
@@ -2011,13 +2118,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>13.78</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="C99" t="n">
-        <v>-8.76</v>
+        <v>-5.68</v>
       </c>
       <c r="D99" t="n">
-        <v>-5.02</v>
+        <v>17.83</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-25.562</v>
       </c>
     </row>
     <row r="100">
@@ -2025,13 +2135,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>14.05</v>
+        <v>9.140000000000001</v>
       </c>
       <c r="C100" t="n">
-        <v>-8.720000000000001</v>
+        <v>-8.130000000000001</v>
       </c>
       <c r="D100" t="n">
-        <v>-5.33</v>
+        <v>19.492</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-24.258</v>
       </c>
     </row>
     <row r="101">
@@ -2039,13 +2152,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>14.33</v>
+        <v>8.81</v>
       </c>
       <c r="C101" t="n">
-        <v>-8.619999999999999</v>
+        <v>-10.54</v>
       </c>
       <c r="D101" t="n">
-        <v>-5.71</v>
+        <v>21.894</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-23.899</v>
       </c>
     </row>
     <row r="102">
@@ -2053,13 +2169,16 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>14.47</v>
+        <v>8.380000000000001</v>
       </c>
       <c r="C102" t="n">
-        <v>-8.460000000000001</v>
+        <v>-12.96</v>
       </c>
       <c r="D102" t="n">
-        <v>-6.01</v>
+        <v>24.306</v>
+      </c>
+      <c r="E102" t="n">
+        <v>-23.45</v>
       </c>
     </row>
     <row r="103">
@@ -2067,13 +2186,16 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>14.65</v>
+        <v>7.97</v>
       </c>
       <c r="C103" t="n">
-        <v>-8.32</v>
+        <v>-15.42</v>
       </c>
       <c r="D103" t="n">
-        <v>-6.33</v>
+        <v>26.718</v>
+      </c>
+      <c r="E103" t="n">
+        <v>-22.971</v>
       </c>
     </row>
     <row r="104">
@@ -2081,13 +2203,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>14.68</v>
+        <v>7.68</v>
       </c>
       <c r="C104" t="n">
-        <v>-8.17</v>
+        <v>-18.36</v>
       </c>
       <c r="D104" t="n">
-        <v>-6.51</v>
+        <v>29.13</v>
+      </c>
+      <c r="E104" t="n">
+        <v>-22.13200000000001</v>
       </c>
     </row>
     <row r="105">
@@ -2095,13 +2220,16 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>15.29</v>
+        <v>7.05</v>
       </c>
       <c r="C105" t="n">
-        <v>-8.66</v>
+        <v>-19.8</v>
       </c>
       <c r="D105" t="n">
-        <v>-6.63</v>
+        <v>31.63200000000001</v>
+      </c>
+      <c r="E105" t="n">
+        <v>-22.54800000000001</v>
       </c>
     </row>
     <row r="106">
@@ -2109,13 +2237,16 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>15.84</v>
+        <v>6.58</v>
       </c>
       <c r="C106" t="n">
-        <v>-9.07</v>
+        <v>-18.98</v>
       </c>
       <c r="D106" t="n">
-        <v>-6.77</v>
+        <v>31.546</v>
+      </c>
+      <c r="E106" t="n">
+        <v>-22.794</v>
       </c>
     </row>
     <row r="107">
@@ -2123,13 +2254,16 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>16.31</v>
+        <v>6.1</v>
       </c>
       <c r="C107" t="n">
-        <v>-9.630000000000001</v>
+        <v>-18.18</v>
       </c>
       <c r="D107" t="n">
-        <v>-6.68</v>
+        <v>31.46</v>
+      </c>
+      <c r="E107" t="n">
+        <v>-23</v>
       </c>
     </row>
     <row r="108">
@@ -2137,13 +2271,16 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>17</v>
+        <v>6.02</v>
       </c>
       <c r="C108" t="n">
-        <v>-10.21</v>
+        <v>-17.57</v>
       </c>
       <c r="D108" t="n">
-        <v>-6.79</v>
+        <v>31.46</v>
+      </c>
+      <c r="E108" t="n">
+        <v>-23.51</v>
       </c>
     </row>
     <row r="109">
@@ -2151,13 +2288,16 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>17.63</v>
+        <v>5.92</v>
       </c>
       <c r="C109" t="n">
-        <v>-10.71</v>
+        <v>-17.17</v>
       </c>
       <c r="D109" t="n">
-        <v>-6.92</v>
+        <v>31.46</v>
+      </c>
+      <c r="E109" t="n">
+        <v>-23.81</v>
       </c>
     </row>
     <row r="110">
@@ -2165,13 +2305,16 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>17.99</v>
+        <v>5.57</v>
       </c>
       <c r="C110" t="n">
-        <v>-11.2</v>
+        <v>-16.16</v>
       </c>
       <c r="D110" t="n">
-        <v>-6.79</v>
+        <v>31.46</v>
+      </c>
+      <c r="E110" t="n">
+        <v>-24.47</v>
       </c>
     </row>
     <row r="111">
@@ -2179,13 +2322,16 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>18.33</v>
+        <v>5.57</v>
       </c>
       <c r="C111" t="n">
-        <v>-11.52</v>
+        <v>-15.21</v>
       </c>
       <c r="D111" t="n">
-        <v>-6.81</v>
+        <v>31.46</v>
+      </c>
+      <c r="E111" t="n">
+        <v>-25.42</v>
       </c>
     </row>
     <row r="112">
@@ -2193,13 +2339,16 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>19.19</v>
+        <v>5.6</v>
       </c>
       <c r="C112" t="n">
-        <v>-12.35</v>
+        <v>-14.26</v>
       </c>
       <c r="D112" t="n">
-        <v>-6.84</v>
+        <v>31.46</v>
+      </c>
+      <c r="E112" t="n">
+        <v>-26.405</v>
       </c>
     </row>
     <row r="113">
@@ -2207,13 +2356,16 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>20</v>
+        <v>5.55</v>
       </c>
       <c r="C113" t="n">
-        <v>-13.13</v>
+        <v>-13.37</v>
       </c>
       <c r="D113" t="n">
-        <v>-6.87</v>
+        <v>31.46</v>
+      </c>
+      <c r="E113" t="n">
+        <v>-27.24</v>
       </c>
     </row>
     <row r="114">
@@ -2221,13 +2373,16 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>20.95</v>
+        <v>6.21</v>
       </c>
       <c r="C114" t="n">
-        <v>-13.97</v>
+        <v>-12.48</v>
       </c>
       <c r="D114" t="n">
-        <v>-6.98</v>
+        <v>31.46</v>
+      </c>
+      <c r="E114" t="n">
+        <v>-28.785</v>
       </c>
     </row>
     <row r="115">
@@ -2235,13 +2390,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>21.26</v>
+        <v>7.21</v>
       </c>
       <c r="C115" t="n">
-        <v>-14.19</v>
+        <v>-10.82</v>
       </c>
       <c r="D115" t="n">
-        <v>-7.06</v>
+        <v>31.46</v>
+      </c>
+      <c r="E115" t="n">
+        <v>-31.45499999999999</v>
       </c>
     </row>
     <row r="116">
@@ -2249,13 +2407,16 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>21.75</v>
+        <v>8.390000000000001</v>
       </c>
       <c r="C116" t="n">
-        <v>-14.44</v>
+        <v>-9.32</v>
       </c>
       <c r="D116" t="n">
-        <v>-7.31</v>
+        <v>31.46</v>
+      </c>
+      <c r="E116" t="n">
+        <v>-34.13499999999999</v>
       </c>
     </row>
     <row r="117">
@@ -2263,13 +2424,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>22.02</v>
+        <v>9.539999999999999</v>
       </c>
       <c r="C117" t="n">
-        <v>-14.38</v>
+        <v>-7.77</v>
       </c>
       <c r="D117" t="n">
-        <v>-7.64</v>
+        <v>31.46</v>
+      </c>
+      <c r="E117" t="n">
+        <v>-36.83499999999999</v>
       </c>
     </row>
     <row r="118">
@@ -2277,13 +2441,16 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>22.07</v>
+        <v>10.21</v>
       </c>
       <c r="C118" t="n">
-        <v>-14.31</v>
+        <v>-6.13</v>
       </c>
       <c r="D118" t="n">
-        <v>-7.76</v>
+        <v>31.46</v>
+      </c>
+      <c r="E118" t="n">
+        <v>-39.145</v>
       </c>
     </row>
     <row r="119">
@@ -2291,13 +2458,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>22.13</v>
+        <v>10.93</v>
       </c>
       <c r="C119" t="n">
-        <v>-14.27</v>
+        <v>-4.5</v>
       </c>
       <c r="D119" t="n">
-        <v>-7.86</v>
+        <v>31.46</v>
+      </c>
+      <c r="E119" t="n">
+        <v>-41.495</v>
       </c>
     </row>
     <row r="120">
@@ -2305,13 +2475,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>22.42</v>
+        <v>11.48</v>
       </c>
       <c r="C120" t="n">
-        <v>-14.21</v>
+        <v>-3.1</v>
       </c>
       <c r="D120" t="n">
-        <v>-8.210000000000001</v>
+        <v>31.46</v>
+      </c>
+      <c r="E120" t="n">
+        <v>-43.44500000000001</v>
       </c>
     </row>
     <row r="121">
@@ -2319,13 +2492,16 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>22.7</v>
+        <v>11.61</v>
       </c>
       <c r="C121" t="n">
-        <v>-14.57</v>
+        <v>-1.58</v>
       </c>
       <c r="D121" t="n">
-        <v>-8.130000000000001</v>
+        <v>31.46</v>
+      </c>
+      <c r="E121" t="n">
+        <v>-45.085</v>
       </c>
     </row>
     <row r="122">
@@ -2333,13 +2509,16 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>22.59</v>
+        <v>11.89</v>
       </c>
       <c r="C122" t="n">
-        <v>-14.55</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="D122" t="n">
-        <v>-8.039999999999999</v>
+        <v>31.46</v>
+      </c>
+      <c r="E122" t="n">
+        <v>-46.88</v>
       </c>
     </row>
     <row r="123">
@@ -2347,13 +2526,16 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>22.49</v>
+        <v>12.13</v>
       </c>
       <c r="C123" t="n">
-        <v>-14.53</v>
+        <v>1.65</v>
       </c>
       <c r="D123" t="n">
-        <v>-7.94</v>
+        <v>31.46</v>
+      </c>
+      <c r="E123" t="n">
+        <v>-48.835</v>
       </c>
     </row>
     <row r="124">
@@ -2361,13 +2543,16 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>22.34</v>
+        <v>11.57</v>
       </c>
       <c r="C124" t="n">
-        <v>-14.47</v>
+        <v>3.37</v>
       </c>
       <c r="D124" t="n">
-        <v>-7.83</v>
+        <v>31.46</v>
+      </c>
+      <c r="E124" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="125">
@@ -2375,13 +2560,16 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>22.17</v>
+        <v>11.39</v>
       </c>
       <c r="C125" t="n">
-        <v>-14.41</v>
+        <v>3.55</v>
       </c>
       <c r="D125" t="n">
-        <v>-7.72</v>
+        <v>31.46</v>
+      </c>
+      <c r="E125" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="126">
@@ -2389,13 +2577,16 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>22.05</v>
+        <v>11.01</v>
       </c>
       <c r="C126" t="n">
-        <v>-14.57</v>
+        <v>3.93</v>
       </c>
       <c r="D126" t="n">
-        <v>-7.44</v>
+        <v>31.46</v>
+      </c>
+      <c r="E126" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="127">
@@ -2403,13 +2594,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>22.71</v>
+        <v>10.68</v>
       </c>
       <c r="C127" t="n">
-        <v>-15.45</v>
+        <v>4.26</v>
       </c>
       <c r="D127" t="n">
-        <v>-7.22</v>
+        <v>31.46</v>
+      </c>
+      <c r="E127" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="128">
@@ -2417,13 +2611,16 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>23.32</v>
+        <v>10.42</v>
       </c>
       <c r="C128" t="n">
-        <v>-16.34</v>
+        <v>4.52</v>
       </c>
       <c r="D128" t="n">
-        <v>-6.94</v>
+        <v>31.46</v>
+      </c>
+      <c r="E128" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="129">
@@ -2431,13 +2628,16 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>24.01</v>
+        <v>10.23</v>
       </c>
       <c r="C129" t="n">
-        <v>-17.31</v>
+        <v>4.71</v>
       </c>
       <c r="D129" t="n">
-        <v>-6.66</v>
+        <v>31.46</v>
+      </c>
+      <c r="E129" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="130">
@@ -2445,13 +2645,16 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>24.69</v>
+        <v>10.34</v>
       </c>
       <c r="C130" t="n">
-        <v>-18.3</v>
+        <v>4.6</v>
       </c>
       <c r="D130" t="n">
-        <v>-6.35</v>
+        <v>31.46</v>
+      </c>
+      <c r="E130" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="131">
@@ -2459,13 +2662,16 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>25.2</v>
+        <v>10.54</v>
       </c>
       <c r="C131" t="n">
-        <v>-19.13</v>
+        <v>4.4</v>
       </c>
       <c r="D131" t="n">
-        <v>-6.03</v>
+        <v>31.46</v>
+      </c>
+      <c r="E131" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="132">
@@ -2473,13 +2679,16 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>26.1</v>
+        <v>10.75</v>
       </c>
       <c r="C132" t="n">
-        <v>-19.9</v>
+        <v>4.19</v>
       </c>
       <c r="D132" t="n">
-        <v>-6.16</v>
+        <v>31.44</v>
+      </c>
+      <c r="E132" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="133">
@@ -2487,13 +2696,16 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>26.8</v>
+        <v>10.55</v>
       </c>
       <c r="C133" t="n">
-        <v>-21.38</v>
+        <v>4.42</v>
       </c>
       <c r="D133" t="n">
-        <v>-5.4</v>
+        <v>31.39</v>
+      </c>
+      <c r="E133" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="134">
@@ -2501,13 +2713,16 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>27.34</v>
+        <v>10.33</v>
       </c>
       <c r="C134" t="n">
-        <v>-22.67</v>
+        <v>4.59</v>
       </c>
       <c r="D134" t="n">
-        <v>-4.67</v>
+        <v>31.42</v>
+      </c>
+      <c r="E134" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="135">
@@ -2515,13 +2730,16 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>27.84</v>
+        <v>9.74</v>
       </c>
       <c r="C135" t="n">
-        <v>-23.99</v>
+        <v>5.07</v>
       </c>
       <c r="D135" t="n">
-        <v>-3.85</v>
+        <v>31.51</v>
+      </c>
+      <c r="E135" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="136">
@@ -2529,13 +2747,16 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>27.49</v>
+        <v>9.529999999999999</v>
       </c>
       <c r="C136" t="n">
-        <v>-25.11</v>
+        <v>5.25</v>
       </c>
       <c r="D136" t="n">
-        <v>-2.37</v>
+        <v>31.52</v>
+      </c>
+      <c r="E136" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="137">
@@ -2543,13 +2764,16 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>26.56</v>
+        <v>9.33</v>
       </c>
       <c r="C137" t="n">
-        <v>-25.71</v>
+        <v>5.4</v>
       </c>
       <c r="D137" t="n">
-        <v>-0.86</v>
+        <v>31.6</v>
+      </c>
+      <c r="E137" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="138">
@@ -2557,13 +2781,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>25.93</v>
+        <v>9.130000000000001</v>
       </c>
       <c r="C138" t="n">
-        <v>-26.51</v>
+        <v>5.56</v>
       </c>
       <c r="D138" t="n">
-        <v>0.58</v>
+        <v>31.69</v>
+      </c>
+      <c r="E138" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="139">
@@ -2571,13 +2798,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>25.28</v>
+        <v>8.83</v>
       </c>
       <c r="C139" t="n">
-        <v>-27.37</v>
+        <v>5.79</v>
       </c>
       <c r="D139" t="n">
-        <v>2.09</v>
+        <v>31.8</v>
+      </c>
+      <c r="E139" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="140">
@@ -2585,13 +2815,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>24.64</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="C140" t="n">
-        <v>-28.22</v>
+        <v>5.9</v>
       </c>
       <c r="D140" t="n">
-        <v>3.58</v>
+        <v>31.96999999999999</v>
+      </c>
+      <c r="E140" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="141">
@@ -2599,13 +2832,16 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>24.05</v>
+        <v>8.27</v>
       </c>
       <c r="C141" t="n">
-        <v>-28.99</v>
+        <v>5.97</v>
       </c>
       <c r="D141" t="n">
-        <v>4.95</v>
+        <v>32.14</v>
+      </c>
+      <c r="E141" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="142">
@@ -2613,13 +2849,16 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>22.93</v>
+        <v>8.140000000000001</v>
       </c>
       <c r="C142" t="n">
-        <v>-29.71</v>
+        <v>5.99</v>
       </c>
       <c r="D142" t="n">
-        <v>6.77</v>
+        <v>32.25</v>
+      </c>
+      <c r="E142" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="143">
@@ -2627,13 +2866,16 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>22.02</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="C143" t="n">
-        <v>-29.66</v>
+        <v>5.43</v>
       </c>
       <c r="D143" t="n">
-        <v>7.65</v>
+        <v>32.41</v>
+      </c>
+      <c r="E143" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="144">
@@ -2641,13 +2883,16 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>21.39</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="C144" t="n">
-        <v>-29.81</v>
+        <v>4.92</v>
       </c>
       <c r="D144" t="n">
-        <v>8.42</v>
+        <v>32.43</v>
+      </c>
+      <c r="E144" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="145">
@@ -2655,13 +2900,16 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>20.92</v>
+        <v>9.56</v>
       </c>
       <c r="C145" t="n">
-        <v>-29.92</v>
+        <v>4.15</v>
       </c>
       <c r="D145" t="n">
-        <v>9</v>
+        <v>32.67</v>
+      </c>
+      <c r="E145" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="146">
@@ -2669,13 +2917,16 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>21.07</v>
+        <v>9.710000000000001</v>
       </c>
       <c r="C146" t="n">
-        <v>-30.02</v>
+        <v>3.64</v>
       </c>
       <c r="D146" t="n">
-        <v>8.949999999999999</v>
+        <v>33.03</v>
+      </c>
+      <c r="E146" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="147">
@@ -2683,13 +2934,16 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>21.49</v>
+        <v>9.9</v>
       </c>
       <c r="C147" t="n">
-        <v>-30.22</v>
+        <v>3.1</v>
       </c>
       <c r="D147" t="n">
-        <v>8.73</v>
+        <v>33.32</v>
+      </c>
+      <c r="E147" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="148">
@@ -2697,13 +2951,16 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>21.62</v>
+        <v>10.07</v>
       </c>
       <c r="C148" t="n">
-        <v>-30.4</v>
+        <v>2.49</v>
       </c>
       <c r="D148" t="n">
-        <v>8.779999999999999</v>
+        <v>33.7</v>
+      </c>
+      <c r="E148" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="149">
@@ -2711,13 +2968,16 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>21.76</v>
+        <v>9.82</v>
       </c>
       <c r="C149" t="n">
-        <v>-30.49</v>
+        <v>1.88</v>
       </c>
       <c r="D149" t="n">
-        <v>8.73</v>
+        <v>34.49499999999999</v>
+      </c>
+      <c r="E149" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="150">
@@ -2725,13 +2985,16 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>21.88</v>
+        <v>9.58</v>
       </c>
       <c r="C150" t="n">
-        <v>-30.57</v>
+        <v>1.45</v>
       </c>
       <c r="D150" t="n">
-        <v>8.699999999999999</v>
+        <v>35.16999999999999</v>
+      </c>
+      <c r="E150" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="151">
@@ -2739,13 +3002,16 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>22.17</v>
+        <v>9.43</v>
       </c>
       <c r="C151" t="n">
-        <v>-30.68</v>
+        <v>0.95</v>
       </c>
       <c r="D151" t="n">
-        <v>8.51</v>
+        <v>35.825</v>
+      </c>
+      <c r="E151" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="152">
@@ -2753,13 +3019,16 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>22.75</v>
+        <v>9.050000000000001</v>
       </c>
       <c r="C152" t="n">
-        <v>-30.85</v>
+        <v>0.65</v>
       </c>
       <c r="D152" t="n">
-        <v>8.109999999999999</v>
+        <v>36.49999999999999</v>
+      </c>
+      <c r="E152" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="153">
@@ -2767,13 +3036,16 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>23.21</v>
+        <v>8.68</v>
       </c>
       <c r="C153" t="n">
-        <v>-31.09</v>
+        <v>0.36</v>
       </c>
       <c r="D153" t="n">
-        <v>7.88</v>
+        <v>37.15499999999999</v>
+      </c>
+      <c r="E153" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="154">
@@ -2781,13 +3053,16 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>23.49</v>
+        <v>8.27</v>
       </c>
       <c r="C154" t="n">
-        <v>-30.17</v>
+        <v>0.08</v>
       </c>
       <c r="D154" t="n">
-        <v>6.68</v>
+        <v>37.84999999999999</v>
+      </c>
+      <c r="E154" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="155">
@@ -2795,13 +3070,16 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>23.6</v>
+        <v>7.88</v>
       </c>
       <c r="C155" t="n">
-        <v>-29.24</v>
+        <v>0.16</v>
       </c>
       <c r="D155" t="n">
-        <v>5.64</v>
+        <v>38.165</v>
+      </c>
+      <c r="E155" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="156">
@@ -2809,13 +3087,16 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>23.65</v>
+        <v>7.52</v>
       </c>
       <c r="C156" t="n">
-        <v>-28.3</v>
+        <v>0.24</v>
       </c>
       <c r="D156" t="n">
-        <v>4.65</v>
+        <v>38.44</v>
+      </c>
+      <c r="E156" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="157">
@@ -2823,13 +3104,16 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>23.53</v>
+        <v>6.96</v>
       </c>
       <c r="C157" t="n">
-        <v>-27.38</v>
+        <v>0.36</v>
       </c>
       <c r="D157" t="n">
-        <v>3.85</v>
+        <v>38.87499999999999</v>
+      </c>
+      <c r="E157" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="158">
@@ -2837,13 +3121,16 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>24.38</v>
+        <v>6.41</v>
       </c>
       <c r="C158" t="n">
-        <v>-27.16</v>
+        <v>0.54</v>
       </c>
       <c r="D158" t="n">
-        <v>2.78</v>
+        <v>39.25</v>
+      </c>
+      <c r="E158" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="159">
@@ -2851,13 +3138,16 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>25.25</v>
+        <v>6.28</v>
       </c>
       <c r="C159" t="n">
-        <v>-26.96</v>
+        <v>0.73</v>
       </c>
       <c r="D159" t="n">
-        <v>1.71</v>
+        <v>39.19</v>
+      </c>
+      <c r="E159" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="160">
@@ -2865,13 +3155,16 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>26.01</v>
+        <v>6.17</v>
       </c>
       <c r="C160" t="n">
-        <v>-26.58</v>
+        <v>-0.14</v>
       </c>
       <c r="D160" t="n">
-        <v>0.57</v>
+        <v>40.17</v>
+      </c>
+      <c r="E160" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="161">
@@ -2879,13 +3172,16 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>26.58</v>
+        <v>5.95</v>
       </c>
       <c r="C161" t="n">
-        <v>-26</v>
+        <v>-0.47</v>
       </c>
       <c r="D161" t="n">
-        <v>-0.58</v>
+        <v>40.71999999999999</v>
+      </c>
+      <c r="E161" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="162">
@@ -2893,13 +3189,16 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>26.74</v>
+        <v>5.73</v>
       </c>
       <c r="C162" t="n">
-        <v>-25.4</v>
+        <v>-0.33</v>
       </c>
       <c r="D162" t="n">
-        <v>-1.34</v>
+        <v>40.79799999999999</v>
+      </c>
+      <c r="E162" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="163">
@@ -2907,13 +3206,16 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>27.12</v>
+        <v>5.56</v>
       </c>
       <c r="C163" t="n">
-        <v>-24.91</v>
+        <v>-0.18</v>
       </c>
       <c r="D163" t="n">
-        <v>-2.21</v>
+        <v>40.816</v>
+      </c>
+      <c r="E163" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="164">
@@ -2921,13 +3223,16 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>27.48</v>
+        <v>5.95</v>
       </c>
       <c r="C164" t="n">
-        <v>-25.47</v>
+        <v>-0.04</v>
       </c>
       <c r="D164" t="n">
-        <v>-2.01</v>
+        <v>40.294</v>
+      </c>
+      <c r="E164" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="165">
@@ -2935,13 +3240,16 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>27.89</v>
+        <v>6.36</v>
       </c>
       <c r="C165" t="n">
-        <v>-26.02</v>
+        <v>-0.03</v>
       </c>
       <c r="D165" t="n">
-        <v>-1.87</v>
+        <v>39.87199999999999</v>
+      </c>
+      <c r="E165" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="166">
@@ -2949,13 +3257,16 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>28.48</v>
+        <v>6.73</v>
       </c>
       <c r="C166" t="n">
-        <v>-26.63</v>
+        <v>-0.14</v>
       </c>
       <c r="D166" t="n">
-        <v>-1.85</v>
+        <v>39.60999999999999</v>
+      </c>
+      <c r="E166" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="167">
@@ -2963,13 +3274,16 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>29.05</v>
+        <v>6.78</v>
       </c>
       <c r="C167" t="n">
-        <v>-27.23</v>
+        <v>-0.33</v>
       </c>
       <c r="D167" t="n">
-        <v>-1.82</v>
+        <v>39.74799999999999</v>
+      </c>
+      <c r="E167" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="168">
@@ -2977,13 +3291,16 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>28.96</v>
+        <v>6.86</v>
       </c>
       <c r="C168" t="n">
-        <v>-27.12</v>
+        <v>-0.51</v>
       </c>
       <c r="D168" t="n">
-        <v>-1.84</v>
+        <v>39.84599999999999</v>
+      </c>
+      <c r="E168" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="169">
@@ -2991,13 +3308,16 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>28.86</v>
+        <v>6.83</v>
       </c>
       <c r="C169" t="n">
-        <v>-27.02</v>
+        <v>-0.67</v>
       </c>
       <c r="D169" t="n">
-        <v>-1.84</v>
+        <v>40.044</v>
+      </c>
+      <c r="E169" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="170">
@@ -3005,13 +3325,16 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>28.89</v>
+        <v>6.38</v>
       </c>
       <c r="C170" t="n">
-        <v>-27.11</v>
+        <v>0.57</v>
       </c>
       <c r="D170" t="n">
-        <v>-1.79</v>
+        <v>39.242</v>
+      </c>
+      <c r="E170" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="171">
@@ -3019,13 +3342,16 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>29.34</v>
+        <v>5.75</v>
       </c>
       <c r="C171" t="n">
-        <v>-27.44</v>
+        <v>1.36</v>
       </c>
       <c r="D171" t="n">
-        <v>-1.9</v>
+        <v>39.09</v>
+      </c>
+      <c r="E171" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="172">
@@ -3033,13 +3359,16 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>29.95</v>
+        <v>5.23</v>
       </c>
       <c r="C172" t="n">
-        <v>-27.79</v>
+        <v>1.56</v>
       </c>
       <c r="D172" t="n">
-        <v>-2.16</v>
+        <v>39.41</v>
+      </c>
+      <c r="E172" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="173">
@@ -3047,13 +3376,16 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>30.46</v>
+        <v>4.63</v>
       </c>
       <c r="C173" t="n">
-        <v>-28.05</v>
+        <v>1.86</v>
       </c>
       <c r="D173" t="n">
-        <v>-2.44</v>
+        <v>39.70999999999999</v>
+      </c>
+      <c r="E173" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="174">
@@ -3061,13 +3393,16 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>31.04</v>
+        <v>3.44</v>
       </c>
       <c r="C174" t="n">
-        <v>-28.39</v>
+        <v>2.2</v>
       </c>
       <c r="D174" t="n">
-        <v>-2.71</v>
+        <v>40.57</v>
+      </c>
+      <c r="E174" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="175">
@@ -3075,13 +3410,16 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>31.65</v>
+        <v>2.28</v>
       </c>
       <c r="C175" t="n">
-        <v>-28.73</v>
+        <v>2.55</v>
       </c>
       <c r="D175" t="n">
-        <v>-3.01</v>
+        <v>41.37</v>
+      </c>
+      <c r="E175" t="n">
+        <v>-50</v>
       </c>
     </row>
     <row r="176">
@@ -3089,13 +3427,832 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>32.14</v>
+        <v>1.12</v>
       </c>
       <c r="C176" t="n">
-        <v>-28.7</v>
+        <v>3.03</v>
       </c>
       <c r="D176" t="n">
-        <v>-3.56</v>
+        <v>42.05</v>
+      </c>
+      <c r="E176" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="C177" t="n">
+        <v>3.58</v>
+      </c>
+      <c r="D177" t="n">
+        <v>42.499</v>
+      </c>
+      <c r="E177" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="n">
+        <v>-0.89</v>
+      </c>
+      <c r="C178" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="D178" t="n">
+        <v>42.95799999999999</v>
+      </c>
+      <c r="E178" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="n">
+        <v>-1.77</v>
+      </c>
+      <c r="C179" t="n">
+        <v>4.67</v>
+      </c>
+      <c r="D179" t="n">
+        <v>43.297</v>
+      </c>
+      <c r="E179" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="n">
+        <v>-2.17</v>
+      </c>
+      <c r="C180" t="n">
+        <v>4.71</v>
+      </c>
+      <c r="D180" t="n">
+        <v>43.656</v>
+      </c>
+      <c r="E180" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="n">
+        <v>-2.38</v>
+      </c>
+      <c r="C181" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="D181" t="n">
+        <v>43.84500000000001</v>
+      </c>
+      <c r="E181" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B182" t="n">
+        <v>-2.66</v>
+      </c>
+      <c r="C182" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="D182" t="n">
+        <v>44.03400000000001</v>
+      </c>
+      <c r="E182" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B183" t="n">
+        <v>-2.94</v>
+      </c>
+      <c r="C183" t="n">
+        <v>4.84</v>
+      </c>
+      <c r="D183" t="n">
+        <v>44.303</v>
+      </c>
+      <c r="E183" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B184" t="n">
+        <v>-2.87</v>
+      </c>
+      <c r="C184" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="D184" t="n">
+        <v>44.23800000000001</v>
+      </c>
+      <c r="E184" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B185" t="n">
+        <v>-2.87</v>
+      </c>
+      <c r="C185" t="n">
+        <v>4.86</v>
+      </c>
+      <c r="D185" t="n">
+        <v>44.213</v>
+      </c>
+      <c r="E185" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B186" t="n">
+        <v>-2.92</v>
+      </c>
+      <c r="C186" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="D186" t="n">
+        <v>44.26799999999999</v>
+      </c>
+      <c r="E186" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B187" t="n">
+        <v>-3.18</v>
+      </c>
+      <c r="C187" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="D187" t="n">
+        <v>44.53399999999999</v>
+      </c>
+      <c r="E187" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B188" t="n">
+        <v>-3.25</v>
+      </c>
+      <c r="C188" t="n">
+        <v>4.68</v>
+      </c>
+      <c r="D188" t="n">
+        <v>44.77</v>
+      </c>
+      <c r="E188" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B189" t="n">
+        <v>-3.38</v>
+      </c>
+      <c r="C189" t="n">
+        <v>4.47</v>
+      </c>
+      <c r="D189" t="n">
+        <v>45.10600000000001</v>
+      </c>
+      <c r="E189" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B190" t="n">
+        <v>-3.39</v>
+      </c>
+      <c r="C190" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="D190" t="n">
+        <v>45.377</v>
+      </c>
+      <c r="E190" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B191" t="n">
+        <v>-3.11</v>
+      </c>
+      <c r="C191" t="n">
+        <v>3.71</v>
+      </c>
+      <c r="D191" t="n">
+        <v>45.598</v>
+      </c>
+      <c r="E191" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B192" t="n">
+        <v>-2.89</v>
+      </c>
+      <c r="C192" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="D192" t="n">
+        <v>45.879</v>
+      </c>
+      <c r="E192" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B193" t="n">
+        <v>-2.74</v>
+      </c>
+      <c r="C193" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D193" t="n">
+        <v>46.44</v>
+      </c>
+      <c r="E193" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B194" t="n">
+        <v>-2.91</v>
+      </c>
+      <c r="C194" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="D194" t="n">
+        <v>47.315</v>
+      </c>
+      <c r="E194" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B195" t="n">
+        <v>-2.52</v>
+      </c>
+      <c r="C195" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="D195" t="n">
+        <v>48.20999999999999</v>
+      </c>
+      <c r="E195" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B196" t="n">
+        <v>-2.1</v>
+      </c>
+      <c r="C196" t="n">
+        <v>-0.51</v>
+      </c>
+      <c r="D196" t="n">
+        <v>48.808</v>
+      </c>
+      <c r="E196" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B197" t="n">
+        <v>-1.13</v>
+      </c>
+      <c r="C197" t="n">
+        <v>-1.98</v>
+      </c>
+      <c r="D197" t="n">
+        <v>49.316</v>
+      </c>
+      <c r="E197" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="n">
+        <v>-0.22</v>
+      </c>
+      <c r="C198" t="n">
+        <v>-3.36</v>
+      </c>
+      <c r="D198" t="n">
+        <v>49.78400000000001</v>
+      </c>
+      <c r="E198" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="C199" t="n">
+        <v>-4.69</v>
+      </c>
+      <c r="D199" t="n">
+        <v>50.712</v>
+      </c>
+      <c r="E199" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="C200" t="n">
+        <v>-5.95</v>
+      </c>
+      <c r="D200" t="n">
+        <v>51.725</v>
+      </c>
+      <c r="E200" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="C201" t="n">
+        <v>-6.94</v>
+      </c>
+      <c r="D201" t="n">
+        <v>52.818</v>
+      </c>
+      <c r="E201" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="C202" t="n">
+        <v>-7.99</v>
+      </c>
+      <c r="D202" t="n">
+        <v>53.461</v>
+      </c>
+      <c r="E202" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="C203" t="n">
+        <v>-8.869999999999999</v>
+      </c>
+      <c r="D203" t="n">
+        <v>54.104</v>
+      </c>
+      <c r="E203" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C204" t="n">
+        <v>-9.619999999999999</v>
+      </c>
+      <c r="D204" t="n">
+        <v>54.617</v>
+      </c>
+      <c r="E204" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="C205" t="n">
+        <v>-9.84</v>
+      </c>
+      <c r="D205" t="n">
+        <v>55.11999999999999</v>
+      </c>
+      <c r="E205" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B206" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C206" t="n">
+        <v>-10.2</v>
+      </c>
+      <c r="D206" t="n">
+        <v>55.8</v>
+      </c>
+      <c r="E206" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="C207" t="n">
+        <v>-10.11</v>
+      </c>
+      <c r="D207" t="n">
+        <v>56.04000000000001</v>
+      </c>
+      <c r="E207" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="n">
+        <v>-0.61</v>
+      </c>
+      <c r="C208" t="n">
+        <v>-9.960000000000001</v>
+      </c>
+      <c r="D208" t="n">
+        <v>56.77</v>
+      </c>
+      <c r="E208" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="C209" t="n">
+        <v>-9.869999999999999</v>
+      </c>
+      <c r="D209" t="n">
+        <v>56.72000000000001</v>
+      </c>
+      <c r="E209" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="n">
+        <v>-0.68</v>
+      </c>
+      <c r="C210" t="n">
+        <v>-9.75</v>
+      </c>
+      <c r="D210" t="n">
+        <v>56.63000000000001</v>
+      </c>
+      <c r="E210" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="C211" t="n">
+        <v>-9.81</v>
+      </c>
+      <c r="D211" t="n">
+        <v>56.66</v>
+      </c>
+      <c r="E211" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="n">
+        <v>-1.09</v>
+      </c>
+      <c r="C212" t="n">
+        <v>-9.789999999999999</v>
+      </c>
+      <c r="D212" t="n">
+        <v>57.08</v>
+      </c>
+      <c r="E212" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="n">
+        <v>-1.36</v>
+      </c>
+      <c r="C213" t="n">
+        <v>-9.640000000000001</v>
+      </c>
+      <c r="D213" t="n">
+        <v>57.2</v>
+      </c>
+      <c r="E213" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="n">
+        <v>-0.85</v>
+      </c>
+      <c r="C214" t="n">
+        <v>-9.83</v>
+      </c>
+      <c r="D214" t="n">
+        <v>56.88499999999999</v>
+      </c>
+      <c r="E214" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="C215" t="n">
+        <v>-9.98</v>
+      </c>
+      <c r="D215" t="n">
+        <v>56.58</v>
+      </c>
+      <c r="E215" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="C216" t="n">
+        <v>-10.27</v>
+      </c>
+      <c r="D216" t="n">
+        <v>56.255</v>
+      </c>
+      <c r="E216" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="C217" t="n">
+        <v>-10.62</v>
+      </c>
+      <c r="D217" t="n">
+        <v>55.98</v>
+      </c>
+      <c r="E217" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="C218" t="n">
+        <v>-11.02</v>
+      </c>
+      <c r="D218" t="n">
+        <v>55.205</v>
+      </c>
+      <c r="E218" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="n">
+        <v>2.91</v>
+      </c>
+      <c r="C219" t="n">
+        <v>-11.36</v>
+      </c>
+      <c r="D219" t="n">
+        <v>54.65</v>
+      </c>
+      <c r="E219" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="C220" t="n">
+        <v>-11.64</v>
+      </c>
+      <c r="D220" t="n">
+        <v>54.09500000000001</v>
+      </c>
+      <c r="E220" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="C221" t="n">
+        <v>-11.76</v>
+      </c>
+      <c r="D221" t="n">
+        <v>53.56</v>
+      </c>
+      <c r="E221" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="C222" t="n">
+        <v>-12.21</v>
+      </c>
+      <c r="D222" t="n">
+        <v>53.425</v>
+      </c>
+      <c r="E222" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="C223" t="n">
+        <v>-12.59</v>
+      </c>
+      <c r="D223" t="n">
+        <v>53.19</v>
+      </c>
+      <c r="E223" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="C224" t="n">
+        <v>-12.61</v>
+      </c>
+      <c r="D224" t="n">
+        <v>53.54</v>
+      </c>
+      <c r="E224" t="n">
+        <v>-50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
My last commit from JS
Goodbye! It has been a good run. I hope this code runs bug free and is useful forever.
</commit_message>
<xml_diff>
--- a/Outputs/net_over_time_avg.xlsx
+++ b/Outputs/net_over_time_avg.xlsx
@@ -162,7 +162,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>Net vs time this session (05/20/21): 10-hand moving averages</a:t>
+              <a:t>Net vs time this session (07/05/21): 10-hand moving averages</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -194,7 +194,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$B$2:$B$224</f>
+              <f>'data'!$B$2:$B$176</f>
             </numRef>
           </val>
         </ser>
@@ -221,7 +221,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$C$2:$C$224</f>
+              <f>'data'!$C$2:$C$176</f>
             </numRef>
           </val>
         </ser>
@@ -248,34 +248,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'data'!$D$2:$D$224</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <strRef>
-              <f>'data'!E1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <val>
-            <numRef>
-              <f>'data'!$E$2:$E$224</f>
+              <f>'data'!$D$2:$D$176</f>
             </numRef>
           </val>
         </ser>
@@ -645,7 +618,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E224"/>
+  <dimension ref="A1:D176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,7 +639,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cedric</t>
+          <t>Raymond</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -674,11 +647,6 @@
           <t>Scott</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Xavier</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -690,16 +658,22 @@
       <c r="C2" t="n">
         <v>0</v>
       </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1</v>
+        <v>-0.35</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1</v>
+        <v>-0.05</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.4</v>
       </c>
     </row>
     <row r="4">
@@ -707,10 +681,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.47</v>
+        <v>-0.7</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.47</v>
+        <v>0.2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="5">
@@ -718,10 +695,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.68</v>
+        <v>-1.02</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.68</v>
+        <v>0.17</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.85</v>
       </c>
     </row>
     <row r="6">
@@ -729,10 +709,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.76</v>
+        <v>-1.26</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.76</v>
+        <v>0.14</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.12</v>
       </c>
     </row>
     <row r="7">
@@ -740,10 +723,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.72</v>
+        <v>-1.52</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.72</v>
+        <v>0.12</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.4</v>
       </c>
     </row>
     <row r="8">
@@ -751,10 +737,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.74</v>
+        <v>-1.67</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.74</v>
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.6</v>
       </c>
     </row>
     <row r="9">
@@ -762,10 +751,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.74</v>
+        <v>-1.94</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.74</v>
+        <v>0.19</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.75</v>
       </c>
     </row>
     <row r="10">
@@ -773,10 +765,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.67</v>
+        <v>-2.21</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.67</v>
+        <v>0.34</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.87</v>
       </c>
     </row>
     <row r="11">
@@ -784,10 +779,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.97</v>
+        <v>-2.37</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.97</v>
+        <v>0.41</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.96</v>
       </c>
     </row>
     <row r="12">
@@ -795,10 +793,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.97</v>
+        <v>-2.37</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.97</v>
+        <v>0.41</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.96</v>
       </c>
     </row>
     <row r="13">
@@ -806,10 +807,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1.36</v>
+        <v>-2.77</v>
       </c>
       <c r="C13" t="n">
-        <v>-1.36</v>
+        <v>0.53</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.24</v>
       </c>
     </row>
     <row r="14">
@@ -817,10 +821,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1.85</v>
+        <v>-3.16</v>
       </c>
       <c r="C14" t="n">
-        <v>-1.85</v>
+        <v>0.72</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.44</v>
       </c>
     </row>
     <row r="15">
@@ -828,10 +835,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>2.18</v>
+        <v>-3.42</v>
       </c>
       <c r="C15" t="n">
-        <v>-2.18</v>
+        <v>0.77</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.65</v>
       </c>
     </row>
     <row r="16">
@@ -839,10 +849,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>2.35</v>
+        <v>-3.63</v>
       </c>
       <c r="C16" t="n">
-        <v>-2.35</v>
+        <v>0.89</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.74</v>
       </c>
     </row>
     <row r="17">
@@ -850,10 +863,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>2.64</v>
+        <v>-3.81</v>
       </c>
       <c r="C17" t="n">
-        <v>-2.64</v>
+        <v>1.01</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2.8</v>
       </c>
     </row>
     <row r="18">
@@ -861,10 +877,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>3</v>
+        <v>-3.99</v>
       </c>
       <c r="C18" t="n">
-        <v>-3</v>
+        <v>1.19</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.8</v>
       </c>
     </row>
     <row r="19">
@@ -872,10 +891,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>3.44</v>
+        <v>-4.16</v>
       </c>
       <c r="C19" t="n">
-        <v>-3.44</v>
+        <v>1.39</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.77</v>
       </c>
     </row>
     <row r="20">
@@ -883,10 +905,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>3.91</v>
+        <v>-4.03</v>
       </c>
       <c r="C20" t="n">
-        <v>-3.91</v>
+        <v>1.29</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.74</v>
       </c>
     </row>
     <row r="21">
@@ -894,10 +919,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>4.46</v>
+        <v>-3.81</v>
       </c>
       <c r="C21" t="n">
-        <v>-4.46</v>
+        <v>1.12</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2.69</v>
       </c>
     </row>
     <row r="22">
@@ -905,10 +933,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>4.41</v>
+        <v>-3.67</v>
       </c>
       <c r="C22" t="n">
-        <v>-4.41</v>
+        <v>1.04</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2.63</v>
       </c>
     </row>
     <row r="23">
@@ -916,13 +947,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>4.36</v>
+        <v>-3.45</v>
       </c>
       <c r="C23" t="n">
-        <v>-4.36</v>
+        <v>0.88</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="24">
@@ -930,13 +961,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>3.85</v>
+        <v>-2.98</v>
       </c>
       <c r="C24" t="n">
-        <v>-4.23</v>
+        <v>0.49</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.05</v>
+        <v>2.51</v>
       </c>
     </row>
     <row r="25">
@@ -944,13 +975,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>3.25</v>
+        <v>-2.59</v>
       </c>
       <c r="C25" t="n">
-        <v>-4</v>
+        <v>0.18</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.06666666666666667</v>
+        <v>2.45</v>
       </c>
     </row>
     <row r="26">
@@ -958,13 +989,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>2.82</v>
+        <v>-2.2</v>
       </c>
       <c r="C26" t="n">
-        <v>-3.94</v>
+        <v>-0.13</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.025</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="27">
@@ -972,13 +1003,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>2.27</v>
+        <v>-1.81</v>
       </c>
       <c r="C27" t="n">
-        <v>-3.78</v>
+        <v>-0.44</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.04</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="28">
@@ -986,13 +1017,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1.53</v>
+        <v>-1.37</v>
       </c>
       <c r="C28" t="n">
-        <v>-3.41</v>
+        <v>-0.8</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.1166666666666667</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="29">
@@ -1000,13 +1031,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.73</v>
+        <v>-1.02</v>
       </c>
       <c r="C29" t="n">
-        <v>-2.94</v>
+        <v>-1.1</v>
       </c>
       <c r="D29" t="n">
-        <v>0.05714285714285716</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="30">
@@ -1014,13 +1045,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.23</v>
+        <v>-0.86</v>
       </c>
       <c r="C30" t="n">
-        <v>-2.47</v>
+        <v>-1.21</v>
       </c>
       <c r="D30" t="n">
-        <v>0.1625</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="31">
@@ -1028,13 +1059,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>-1.23</v>
+        <v>-0.75</v>
       </c>
       <c r="C31" t="n">
-        <v>-1.94</v>
+        <v>-1.29</v>
       </c>
       <c r="D31" t="n">
-        <v>0.2444444444444445</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="32">
@@ -1042,13 +1073,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-1.98</v>
+        <v>-0.68</v>
       </c>
       <c r="C32" t="n">
-        <v>-1.66</v>
+        <v>-1.34</v>
       </c>
       <c r="D32" t="n">
-        <v>0.95</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="33">
@@ -1056,13 +1087,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-3.36</v>
+        <v>-0.66</v>
       </c>
       <c r="C33" t="n">
-        <v>-1.39</v>
+        <v>-1.34</v>
       </c>
       <c r="D33" t="n">
-        <v>0.95</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="34">
@@ -1070,13 +1101,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>-4.38</v>
+        <v>-0.84</v>
       </c>
       <c r="C34" t="n">
-        <v>-1.09</v>
+        <v>-1.16</v>
       </c>
       <c r="D34" t="n">
-        <v>1.67</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="35">
@@ -1084,13 +1115,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>-5.11</v>
+        <v>-0.99</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.96</v>
+        <v>-1.01</v>
       </c>
       <c r="D35" t="n">
-        <v>2.274999999999999</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="36">
@@ -1098,13 +1129,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>-5.88</v>
+        <v>-1.11</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.82</v>
+        <v>-0.89</v>
       </c>
       <c r="D36" t="n">
-        <v>2.9</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="37">
@@ -1112,13 +1143,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>-6.63</v>
+        <v>-1.26</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.6899999999999999</v>
+        <v>-0.74</v>
       </c>
       <c r="D37" t="n">
-        <v>3.524999999999999</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="38">
@@ -1126,13 +1157,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>-7.2</v>
+        <v>-1.46</v>
       </c>
       <c r="C38" t="n">
-        <v>-0.77</v>
+        <v>-0.54</v>
       </c>
       <c r="D38" t="n">
-        <v>4.17</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="39">
@@ -1140,13 +1171,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>-7.83</v>
+        <v>-1.62</v>
       </c>
       <c r="C39" t="n">
-        <v>-0.9</v>
+        <v>-0.38</v>
       </c>
       <c r="D39" t="n">
-        <v>4.924999999999999</v>
+        <v>2.2</v>
       </c>
     </row>
     <row r="40">
@@ -1154,13 +1185,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>-8.31</v>
+        <v>-1.89</v>
       </c>
       <c r="C40" t="n">
-        <v>-1.03</v>
+        <v>-0.11</v>
       </c>
       <c r="D40" t="n">
-        <v>5.54</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="41">
@@ -1168,13 +1199,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>-8.859999999999999</v>
+        <v>-2.16</v>
       </c>
       <c r="C41" t="n">
-        <v>-1.11</v>
+        <v>0.14</v>
       </c>
       <c r="D41" t="n">
-        <v>6.175</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="42">
@@ -1182,13 +1213,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-9.44</v>
+        <v>-2.31</v>
       </c>
       <c r="C42" t="n">
-        <v>-1.18</v>
+        <v>0.27</v>
       </c>
       <c r="D42" t="n">
-        <v>6.82</v>
+        <v>2.18</v>
       </c>
     </row>
     <row r="43">
@@ -1196,13 +1227,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>-9.289999999999999</v>
+        <v>-2.47</v>
       </c>
       <c r="C43" t="n">
-        <v>-1.25</v>
+        <v>0.4</v>
       </c>
       <c r="D43" t="n">
-        <v>6.745</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="44">
@@ -1210,13 +1241,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-9.119999999999999</v>
+        <v>-2.55</v>
       </c>
       <c r="C44" t="n">
-        <v>-1.36</v>
+        <v>0.46</v>
       </c>
       <c r="D44" t="n">
-        <v>6.68</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="45">
@@ -1224,13 +1255,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>-9.779999999999999</v>
+        <v>-2.49</v>
       </c>
       <c r="C45" t="n">
-        <v>-1.46</v>
+        <v>0.46</v>
       </c>
       <c r="D45" t="n">
-        <v>7.44</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="46">
@@ -1238,13 +1269,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>-10.14</v>
+        <v>-2.51</v>
       </c>
       <c r="C46" t="n">
-        <v>-1.82</v>
+        <v>0.46</v>
       </c>
       <c r="D46" t="n">
-        <v>8.159999999999998</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="47">
@@ -1252,13 +1283,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>-10.49</v>
+        <v>-2.26</v>
       </c>
       <c r="C47" t="n">
-        <v>-2.17</v>
+        <v>0.2</v>
       </c>
       <c r="D47" t="n">
-        <v>8.859999999999998</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="48">
@@ -1266,13 +1297,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>-10.86</v>
+        <v>-2.01</v>
       </c>
       <c r="C48" t="n">
-        <v>-2.51</v>
+        <v>-0.14</v>
       </c>
       <c r="D48" t="n">
-        <v>9.569999999999999</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="49">
@@ -1280,13 +1311,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>-11.22</v>
+        <v>-1.77</v>
       </c>
       <c r="C49" t="n">
-        <v>-2.97</v>
+        <v>-0.51</v>
       </c>
       <c r="D49" t="n">
-        <v>10.39</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="50">
@@ -1294,13 +1325,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>-11.56</v>
+        <v>-1.47</v>
       </c>
       <c r="C50" t="n">
-        <v>-3.43</v>
+        <v>-0.99</v>
       </c>
       <c r="D50" t="n">
-        <v>11.19</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="51">
@@ -1308,13 +1339,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>-11.89</v>
+        <v>-1.16</v>
       </c>
       <c r="C51" t="n">
-        <v>-4.46</v>
+        <v>-0.99</v>
       </c>
       <c r="D51" t="n">
-        <v>12.55</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="52">
@@ -1322,13 +1353,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>-12.21</v>
+        <v>-0.91</v>
       </c>
       <c r="C52" t="n">
-        <v>-5.51</v>
+        <v>-1.08</v>
       </c>
       <c r="D52" t="n">
-        <v>13.92</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="53">
@@ -1336,16 +1367,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>-12.5</v>
+        <v>-0.68</v>
       </c>
       <c r="C53" t="n">
-        <v>-6.55</v>
+        <v>-1.15</v>
       </c>
       <c r="D53" t="n">
-        <v>15.245</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0</v>
+        <v>1.84</v>
       </c>
     </row>
     <row r="54">
@@ -1353,16 +1381,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>-12.78</v>
+        <v>-0.5</v>
       </c>
       <c r="C54" t="n">
-        <v>-7.53</v>
+        <v>-1.19</v>
       </c>
       <c r="D54" t="n">
-        <v>16.51</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="55">
@@ -1370,16 +1395,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>-12.43</v>
+        <v>-0.5</v>
       </c>
       <c r="C55" t="n">
-        <v>-8.210000000000001</v>
+        <v>-1.16</v>
       </c>
       <c r="D55" t="n">
-        <v>16.835</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0.06666666666666667</v>
+        <v>1.66</v>
       </c>
     </row>
     <row r="56">
@@ -1387,16 +1409,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>-12.35</v>
+        <v>-0.57</v>
       </c>
       <c r="C56" t="n">
-        <v>-8.65</v>
+        <v>-1.12</v>
       </c>
       <c r="D56" t="n">
-        <v>17.18</v>
-      </c>
-      <c r="E56" t="n">
-        <v>0.5</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="57">
@@ -1404,16 +1423,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-12.31</v>
+        <v>-0.36</v>
       </c>
       <c r="C57" t="n">
-        <v>-9.220000000000001</v>
+        <v>-0.6899999999999999</v>
       </c>
       <c r="D57" t="n">
-        <v>17.525</v>
-      </c>
-      <c r="E57" t="n">
-        <v>-0.18</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="58">
@@ -1421,16 +1437,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>-12.31</v>
+        <v>0.02</v>
       </c>
       <c r="C58" t="n">
-        <v>-9.789999999999999</v>
+        <v>-0.25</v>
       </c>
       <c r="D58" t="n">
-        <v>18.39</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0.6333333333333334</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="59">
@@ -1438,16 +1451,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>-12.38</v>
+        <v>0.79</v>
       </c>
       <c r="C59" t="n">
-        <v>-10.2</v>
+        <v>-0.17</v>
       </c>
       <c r="D59" t="n">
-        <v>18.405</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0.9428571428571428</v>
+        <v>-0.77</v>
       </c>
     </row>
     <row r="60">
@@ -1455,16 +1465,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>-12.53</v>
+        <v>1.65</v>
       </c>
       <c r="C60" t="n">
-        <v>-10.6</v>
+        <v>-0.11</v>
       </c>
       <c r="D60" t="n">
-        <v>18.67</v>
-      </c>
-      <c r="E60" t="n">
-        <v>-0.4712499999999999</v>
+        <v>-1.69</v>
       </c>
     </row>
     <row r="61">
@@ -1472,16 +1479,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>-12.67</v>
+        <v>2.62</v>
       </c>
       <c r="C61" t="n">
-        <v>-8.859999999999999</v>
+        <v>-0.63</v>
       </c>
       <c r="D61" t="n">
-        <v>18.105</v>
-      </c>
-      <c r="E61" t="n">
-        <v>-1.482222222222222</v>
+        <v>-2.15</v>
       </c>
     </row>
     <row r="62">
@@ -1489,16 +1493,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>-12.88</v>
+        <v>3.6</v>
       </c>
       <c r="C62" t="n">
-        <v>-7.19</v>
+        <v>-0.99</v>
       </c>
       <c r="D62" t="n">
-        <v>17.6</v>
-      </c>
-      <c r="E62" t="n">
-        <v>-2.531</v>
+        <v>-2.77</v>
       </c>
     </row>
     <row r="63">
@@ -1506,16 +1507,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>-12.96</v>
+        <v>4.54</v>
       </c>
       <c r="C63" t="n">
-        <v>-5.52</v>
+        <v>-1.55</v>
       </c>
       <c r="D63" t="n">
-        <v>17.21</v>
-      </c>
-      <c r="E63" t="n">
-        <v>-2.531</v>
+        <v>-3.15</v>
       </c>
     </row>
     <row r="64">
@@ -1523,16 +1521,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>-13.12</v>
+        <v>5.41</v>
       </c>
       <c r="C64" t="n">
-        <v>-3.87</v>
+        <v>-2.09</v>
       </c>
       <c r="D64" t="n">
-        <v>16.94</v>
-      </c>
-      <c r="E64" t="n">
-        <v>-3.748</v>
+        <v>-3.47</v>
       </c>
     </row>
     <row r="65">
@@ -1540,16 +1535,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>-13.24</v>
+        <v>6.22</v>
       </c>
       <c r="C65" t="n">
-        <v>-2.52</v>
+        <v>-2.8</v>
       </c>
       <c r="D65" t="n">
-        <v>16.75</v>
-      </c>
-      <c r="E65" t="n">
-        <v>-4.784999999999999</v>
+        <v>-3.57</v>
       </c>
     </row>
     <row r="66">
@@ -1557,16 +1549,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>-13.42</v>
+        <v>7.06</v>
       </c>
       <c r="C66" t="n">
-        <v>-1.16</v>
+        <v>-3.4</v>
       </c>
       <c r="D66" t="n">
-        <v>16.62</v>
-      </c>
-      <c r="E66" t="n">
-        <v>-5.842</v>
+        <v>-3.66</v>
       </c>
     </row>
     <row r="67">
@@ -1574,16 +1563,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>-13.58</v>
+        <v>7.36</v>
       </c>
       <c r="C67" t="n">
-        <v>0.33</v>
+        <v>-4.13</v>
       </c>
       <c r="D67" t="n">
-        <v>16.58</v>
-      </c>
-      <c r="E67" t="n">
-        <v>-7.129</v>
+        <v>-3.23</v>
       </c>
     </row>
     <row r="68">
@@ -1591,16 +1577,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>-13.22</v>
+        <v>7.64</v>
       </c>
       <c r="C68" t="n">
-        <v>1.81</v>
+        <v>-4.91</v>
       </c>
       <c r="D68" t="n">
-        <v>16.01</v>
-      </c>
-      <c r="E68" t="n">
-        <v>-8.391</v>
+        <v>-2.73</v>
       </c>
     </row>
     <row r="69">
@@ -1608,16 +1591,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>-12.35</v>
+        <v>7.52</v>
       </c>
       <c r="C69" t="n">
-        <v>3.3</v>
+        <v>-5.3</v>
       </c>
       <c r="D69" t="n">
-        <v>16.11</v>
-      </c>
-      <c r="E69" t="n">
-        <v>-10.861</v>
+        <v>-2.22</v>
       </c>
     </row>
     <row r="70">
@@ -1625,16 +1605,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>-11.44</v>
+        <v>7.39</v>
       </c>
       <c r="C70" t="n">
-        <v>4.81</v>
+        <v>-5.76</v>
       </c>
       <c r="D70" t="n">
-        <v>15.97</v>
-      </c>
-      <c r="E70" t="n">
-        <v>-13.141</v>
+        <v>-1.63</v>
       </c>
     </row>
     <row r="71">
@@ -1642,16 +1619,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>-9.76</v>
+        <v>7.28</v>
       </c>
       <c r="C71" t="n">
-        <v>4.59</v>
+        <v>-6.14</v>
       </c>
       <c r="D71" t="n">
-        <v>16.09</v>
-      </c>
-      <c r="E71" t="n">
-        <v>-14.724</v>
+        <v>-1.14</v>
       </c>
     </row>
     <row r="72">
@@ -1659,16 +1633,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>-8.01</v>
+        <v>7.14</v>
       </c>
       <c r="C72" t="n">
-        <v>4.49</v>
+        <v>-6.5</v>
       </c>
       <c r="D72" t="n">
-        <v>16.13</v>
-      </c>
-      <c r="E72" t="n">
-        <v>-16.407</v>
+        <v>-0.64</v>
       </c>
     </row>
     <row r="73">
@@ -1676,16 +1647,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>-6.62</v>
+        <v>6.91</v>
       </c>
       <c r="C73" t="n">
-        <v>4.85</v>
+        <v>-6.67</v>
       </c>
       <c r="D73" t="n">
-        <v>16.18</v>
-      </c>
-      <c r="E73" t="n">
-        <v>-18.21</v>
+        <v>-0.24</v>
       </c>
     </row>
     <row r="74">
@@ -1693,16 +1661,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>-4.91</v>
+        <v>6.59</v>
       </c>
       <c r="C74" t="n">
-        <v>5.17</v>
+        <v>-6.83</v>
       </c>
       <c r="D74" t="n">
-        <v>15.93</v>
-      </c>
-      <c r="E74" t="n">
-        <v>-19.993</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="75">
@@ -1710,16 +1675,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>-3.17</v>
+        <v>6.33</v>
       </c>
       <c r="C75" t="n">
-        <v>5.33</v>
+        <v>-6.81</v>
       </c>
       <c r="D75" t="n">
-        <v>16</v>
-      </c>
-      <c r="E75" t="n">
-        <v>-21.956</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="76">
@@ -1727,16 +1689,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>-1.38</v>
+        <v>6.19</v>
       </c>
       <c r="C76" t="n">
-        <v>5.48</v>
+        <v>-6.84</v>
       </c>
       <c r="D76" t="n">
-        <v>16.354</v>
-      </c>
-      <c r="E76" t="n">
-        <v>-24.253</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="77">
@@ -1744,16 +1703,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.26</v>
+        <v>6.07</v>
       </c>
       <c r="C77" t="n">
-        <v>5.65</v>
+        <v>-6.89</v>
       </c>
       <c r="D77" t="n">
-        <v>16.618</v>
-      </c>
-      <c r="E77" t="n">
-        <v>-26.33</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="78">
@@ -1761,16 +1717,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>1.59</v>
+        <v>5.86</v>
       </c>
       <c r="C78" t="n">
-        <v>5.83</v>
+        <v>-6.87</v>
       </c>
       <c r="D78" t="n">
-        <v>16.812</v>
-      </c>
-      <c r="E78" t="n">
-        <v>-28.032</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="79">
@@ -1778,16 +1731,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>2.41</v>
+        <v>5.67</v>
       </c>
       <c r="C79" t="n">
-        <v>6.01</v>
+        <v>-6.87</v>
       </c>
       <c r="D79" t="n">
-        <v>17.626</v>
-      </c>
-      <c r="E79" t="n">
-        <v>-29.846</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="80">
@@ -1795,16 +1745,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>3.32</v>
+        <v>5.62</v>
       </c>
       <c r="C80" t="n">
-        <v>6.19</v>
+        <v>-6.79</v>
       </c>
       <c r="D80" t="n">
-        <v>18.43</v>
-      </c>
-      <c r="E80" t="n">
-        <v>-31.74</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="81">
@@ -1812,16 +1759,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>3.52</v>
+        <v>5.55</v>
       </c>
       <c r="C81" t="n">
-        <v>6.44</v>
+        <v>-6.81</v>
       </c>
       <c r="D81" t="n">
-        <v>18.819</v>
-      </c>
-      <c r="E81" t="n">
-        <v>-32.57899999999999</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="82">
@@ -1829,16 +1773,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>4.26</v>
+        <v>5.59</v>
       </c>
       <c r="C82" t="n">
-        <v>6.65</v>
+        <v>-6.86</v>
       </c>
       <c r="D82" t="n">
-        <v>18.948</v>
-      </c>
-      <c r="E82" t="n">
-        <v>-33.658</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="83">
@@ -1846,16 +1787,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>5.26</v>
+        <v>5.75</v>
       </c>
       <c r="C83" t="n">
-        <v>6.42</v>
+        <v>-6.87</v>
       </c>
       <c r="D83" t="n">
-        <v>19.077</v>
-      </c>
-      <c r="E83" t="n">
-        <v>-34.557</v>
+        <v>1.12</v>
       </c>
     </row>
     <row r="84">
@@ -1863,16 +1801,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>5.95</v>
+        <v>6.22</v>
       </c>
       <c r="C84" t="n">
-        <v>6.25</v>
+        <v>-6.9</v>
       </c>
       <c r="D84" t="n">
-        <v>19.261</v>
-      </c>
-      <c r="E84" t="n">
-        <v>-35.261</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="85">
@@ -1880,16 +1815,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>6.57</v>
+        <v>6.71</v>
       </c>
       <c r="C85" t="n">
-        <v>6.24</v>
+        <v>-6.95</v>
       </c>
       <c r="D85" t="n">
-        <v>19.275</v>
-      </c>
-      <c r="E85" t="n">
-        <v>-35.88500000000001</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="86">
@@ -1897,16 +1829,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>7.21</v>
+        <v>7.28</v>
       </c>
       <c r="C86" t="n">
-        <v>6.24</v>
+        <v>-7.06</v>
       </c>
       <c r="D86" t="n">
-        <v>18.945</v>
-      </c>
-      <c r="E86" t="n">
-        <v>-36.195</v>
+        <v>-0.21</v>
       </c>
     </row>
     <row r="87">
@@ -1914,16 +1843,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>8.18</v>
+        <v>7.92</v>
       </c>
       <c r="C87" t="n">
-        <v>6.24</v>
+        <v>-7.19</v>
       </c>
       <c r="D87" t="n">
-        <v>18.545</v>
-      </c>
-      <c r="E87" t="n">
-        <v>-36.765</v>
+        <v>-0.73</v>
       </c>
     </row>
     <row r="88">
@@ -1931,16 +1857,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>9.130000000000001</v>
+        <v>8.5</v>
       </c>
       <c r="C88" t="n">
-        <v>6.17</v>
+        <v>-7.34</v>
       </c>
       <c r="D88" t="n">
-        <v>18.195</v>
-      </c>
-      <c r="E88" t="n">
-        <v>-37.285</v>
+        <v>-1.17</v>
       </c>
     </row>
     <row r="89">
@@ -1948,16 +1871,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>10.11</v>
+        <v>9.27</v>
       </c>
       <c r="C89" t="n">
-        <v>6.01</v>
+        <v>-7.48</v>
       </c>
       <c r="D89" t="n">
-        <v>17.225</v>
-      </c>
-      <c r="E89" t="n">
-        <v>-37.145</v>
+        <v>-1.79</v>
       </c>
     </row>
     <row r="90">
@@ -1965,16 +1885,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>11</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="C90" t="n">
-        <v>5.9</v>
+        <v>-7.68</v>
       </c>
       <c r="D90" t="n">
-        <v>16.255</v>
-      </c>
-      <c r="E90" t="n">
-        <v>-36.94500000000001</v>
+        <v>-2.2</v>
       </c>
     </row>
     <row r="91">
@@ -1982,16 +1899,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>11.71</v>
+        <v>10.38</v>
       </c>
       <c r="C91" t="n">
-        <v>5.78</v>
+        <v>-7.84</v>
       </c>
       <c r="D91" t="n">
-        <v>14.97</v>
-      </c>
-      <c r="E91" t="n">
-        <v>-36.255</v>
+        <v>-2.54</v>
       </c>
     </row>
     <row r="92">
@@ -1999,16 +1913,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>11.83</v>
+        <v>10.88</v>
       </c>
       <c r="C92" t="n">
-        <v>5.65</v>
+        <v>-7.99</v>
       </c>
       <c r="D92" t="n">
-        <v>13.935</v>
-      </c>
-      <c r="E92" t="n">
-        <v>-35.205</v>
+        <v>-2.9</v>
       </c>
     </row>
     <row r="93">
@@ -2016,16 +1927,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>11.75</v>
+        <v>11.4</v>
       </c>
       <c r="C93" t="n">
-        <v>5.55</v>
+        <v>-8.16</v>
       </c>
       <c r="D93" t="n">
-        <v>12.9</v>
-      </c>
-      <c r="E93" t="n">
-        <v>-33.995</v>
+        <v>-3.24</v>
       </c>
     </row>
     <row r="94">
@@ -2033,16 +1941,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>11.66</v>
+        <v>11.82</v>
       </c>
       <c r="C94" t="n">
-        <v>5.92</v>
+        <v>-8.32</v>
       </c>
       <c r="D94" t="n">
-        <v>12.05</v>
-      </c>
-      <c r="E94" t="n">
-        <v>-33.42</v>
+        <v>-3.5</v>
       </c>
     </row>
     <row r="95">
@@ -2050,16 +1955,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>11.54</v>
+        <v>12.3</v>
       </c>
       <c r="C95" t="n">
-        <v>5.25</v>
+        <v>-8.470000000000001</v>
       </c>
       <c r="D95" t="n">
-        <v>11.12</v>
-      </c>
-      <c r="E95" t="n">
-        <v>-31.71</v>
+        <v>-3.83</v>
       </c>
     </row>
     <row r="96">
@@ -2067,16 +1969,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>11.25</v>
+        <v>12.76</v>
       </c>
       <c r="C96" t="n">
-        <v>2.31</v>
+        <v>-8.68</v>
       </c>
       <c r="D96" t="n">
-        <v>12.778</v>
-      </c>
-      <c r="E96" t="n">
-        <v>-30.14</v>
+        <v>-4.08</v>
       </c>
     </row>
     <row r="97">
@@ -2084,16 +1983,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>10.79</v>
+        <v>13.12</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.61</v>
+        <v>-8.720000000000001</v>
       </c>
       <c r="D97" t="n">
-        <v>14.506</v>
-      </c>
-      <c r="E97" t="n">
-        <v>-28.48</v>
+        <v>-4.4</v>
       </c>
     </row>
     <row r="98">
@@ -2101,16 +1997,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>10.2</v>
+        <v>13.55</v>
       </c>
       <c r="C98" t="n">
-        <v>-3.28</v>
+        <v>-8.75</v>
       </c>
       <c r="D98" t="n">
-        <v>16.168</v>
-      </c>
-      <c r="E98" t="n">
-        <v>-26.886</v>
+        <v>-4.8</v>
       </c>
     </row>
     <row r="99">
@@ -2118,16 +2011,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>9.630000000000001</v>
+        <v>13.78</v>
       </c>
       <c r="C99" t="n">
-        <v>-5.68</v>
+        <v>-8.76</v>
       </c>
       <c r="D99" t="n">
-        <v>17.83</v>
-      </c>
-      <c r="E99" t="n">
-        <v>-25.562</v>
+        <v>-5.02</v>
       </c>
     </row>
     <row r="100">
@@ -2135,16 +2025,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>9.140000000000001</v>
+        <v>14.05</v>
       </c>
       <c r="C100" t="n">
-        <v>-8.130000000000001</v>
+        <v>-8.720000000000001</v>
       </c>
       <c r="D100" t="n">
-        <v>19.492</v>
-      </c>
-      <c r="E100" t="n">
-        <v>-24.258</v>
+        <v>-5.33</v>
       </c>
     </row>
     <row r="101">
@@ -2152,16 +2039,13 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>8.81</v>
+        <v>14.33</v>
       </c>
       <c r="C101" t="n">
-        <v>-10.54</v>
+        <v>-8.619999999999999</v>
       </c>
       <c r="D101" t="n">
-        <v>21.894</v>
-      </c>
-      <c r="E101" t="n">
-        <v>-23.899</v>
+        <v>-5.71</v>
       </c>
     </row>
     <row r="102">
@@ -2169,16 +2053,13 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>8.380000000000001</v>
+        <v>14.47</v>
       </c>
       <c r="C102" t="n">
-        <v>-12.96</v>
+        <v>-8.460000000000001</v>
       </c>
       <c r="D102" t="n">
-        <v>24.306</v>
-      </c>
-      <c r="E102" t="n">
-        <v>-23.45</v>
+        <v>-6.01</v>
       </c>
     </row>
     <row r="103">
@@ -2186,16 +2067,13 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>7.97</v>
+        <v>14.65</v>
       </c>
       <c r="C103" t="n">
-        <v>-15.42</v>
+        <v>-8.32</v>
       </c>
       <c r="D103" t="n">
-        <v>26.718</v>
-      </c>
-      <c r="E103" t="n">
-        <v>-22.971</v>
+        <v>-6.33</v>
       </c>
     </row>
     <row r="104">
@@ -2203,16 +2081,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>7.68</v>
+        <v>14.68</v>
       </c>
       <c r="C104" t="n">
-        <v>-18.36</v>
+        <v>-8.17</v>
       </c>
       <c r="D104" t="n">
-        <v>29.13</v>
-      </c>
-      <c r="E104" t="n">
-        <v>-22.13200000000001</v>
+        <v>-6.51</v>
       </c>
     </row>
     <row r="105">
@@ -2220,16 +2095,13 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>7.05</v>
+        <v>15.29</v>
       </c>
       <c r="C105" t="n">
-        <v>-19.8</v>
+        <v>-8.66</v>
       </c>
       <c r="D105" t="n">
-        <v>31.63200000000001</v>
-      </c>
-      <c r="E105" t="n">
-        <v>-22.54800000000001</v>
+        <v>-6.63</v>
       </c>
     </row>
     <row r="106">
@@ -2237,16 +2109,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>6.58</v>
+        <v>15.84</v>
       </c>
       <c r="C106" t="n">
-        <v>-18.98</v>
+        <v>-9.07</v>
       </c>
       <c r="D106" t="n">
-        <v>31.546</v>
-      </c>
-      <c r="E106" t="n">
-        <v>-22.794</v>
+        <v>-6.77</v>
       </c>
     </row>
     <row r="107">
@@ -2254,16 +2123,13 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>6.1</v>
+        <v>16.31</v>
       </c>
       <c r="C107" t="n">
-        <v>-18.18</v>
+        <v>-9.630000000000001</v>
       </c>
       <c r="D107" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E107" t="n">
-        <v>-23</v>
+        <v>-6.68</v>
       </c>
     </row>
     <row r="108">
@@ -2271,16 +2137,13 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>6.02</v>
+        <v>17</v>
       </c>
       <c r="C108" t="n">
-        <v>-17.57</v>
+        <v>-10.21</v>
       </c>
       <c r="D108" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E108" t="n">
-        <v>-23.51</v>
+        <v>-6.79</v>
       </c>
     </row>
     <row r="109">
@@ -2288,16 +2151,13 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>5.92</v>
+        <v>17.63</v>
       </c>
       <c r="C109" t="n">
-        <v>-17.17</v>
+        <v>-10.71</v>
       </c>
       <c r="D109" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E109" t="n">
-        <v>-23.81</v>
+        <v>-6.92</v>
       </c>
     </row>
     <row r="110">
@@ -2305,16 +2165,13 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>5.57</v>
+        <v>17.99</v>
       </c>
       <c r="C110" t="n">
-        <v>-16.16</v>
+        <v>-11.2</v>
       </c>
       <c r="D110" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E110" t="n">
-        <v>-24.47</v>
+        <v>-6.79</v>
       </c>
     </row>
     <row r="111">
@@ -2322,16 +2179,13 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>5.57</v>
+        <v>18.33</v>
       </c>
       <c r="C111" t="n">
-        <v>-15.21</v>
+        <v>-11.52</v>
       </c>
       <c r="D111" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E111" t="n">
-        <v>-25.42</v>
+        <v>-6.81</v>
       </c>
     </row>
     <row r="112">
@@ -2339,16 +2193,13 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>5.6</v>
+        <v>19.19</v>
       </c>
       <c r="C112" t="n">
-        <v>-14.26</v>
+        <v>-12.35</v>
       </c>
       <c r="D112" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E112" t="n">
-        <v>-26.405</v>
+        <v>-6.84</v>
       </c>
     </row>
     <row r="113">
@@ -2356,16 +2207,13 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>5.55</v>
+        <v>20</v>
       </c>
       <c r="C113" t="n">
-        <v>-13.37</v>
+        <v>-13.13</v>
       </c>
       <c r="D113" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E113" t="n">
-        <v>-27.24</v>
+        <v>-6.87</v>
       </c>
     </row>
     <row r="114">
@@ -2373,16 +2221,13 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>6.21</v>
+        <v>20.95</v>
       </c>
       <c r="C114" t="n">
-        <v>-12.48</v>
+        <v>-13.97</v>
       </c>
       <c r="D114" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E114" t="n">
-        <v>-28.785</v>
+        <v>-6.98</v>
       </c>
     </row>
     <row r="115">
@@ -2390,16 +2235,13 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>7.21</v>
+        <v>21.26</v>
       </c>
       <c r="C115" t="n">
-        <v>-10.82</v>
+        <v>-14.19</v>
       </c>
       <c r="D115" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E115" t="n">
-        <v>-31.45499999999999</v>
+        <v>-7.06</v>
       </c>
     </row>
     <row r="116">
@@ -2407,16 +2249,13 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>8.390000000000001</v>
+        <v>21.75</v>
       </c>
       <c r="C116" t="n">
-        <v>-9.32</v>
+        <v>-14.44</v>
       </c>
       <c r="D116" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E116" t="n">
-        <v>-34.13499999999999</v>
+        <v>-7.31</v>
       </c>
     </row>
     <row r="117">
@@ -2424,16 +2263,13 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>9.539999999999999</v>
+        <v>22.02</v>
       </c>
       <c r="C117" t="n">
-        <v>-7.77</v>
+        <v>-14.38</v>
       </c>
       <c r="D117" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E117" t="n">
-        <v>-36.83499999999999</v>
+        <v>-7.64</v>
       </c>
     </row>
     <row r="118">
@@ -2441,16 +2277,13 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>10.21</v>
+        <v>22.07</v>
       </c>
       <c r="C118" t="n">
-        <v>-6.13</v>
+        <v>-14.31</v>
       </c>
       <c r="D118" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E118" t="n">
-        <v>-39.145</v>
+        <v>-7.76</v>
       </c>
     </row>
     <row r="119">
@@ -2458,16 +2291,13 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>10.93</v>
+        <v>22.13</v>
       </c>
       <c r="C119" t="n">
-        <v>-4.5</v>
+        <v>-14.27</v>
       </c>
       <c r="D119" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E119" t="n">
-        <v>-41.495</v>
+        <v>-7.86</v>
       </c>
     </row>
     <row r="120">
@@ -2475,16 +2305,13 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>11.48</v>
+        <v>22.42</v>
       </c>
       <c r="C120" t="n">
-        <v>-3.1</v>
+        <v>-14.21</v>
       </c>
       <c r="D120" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E120" t="n">
-        <v>-43.44500000000001</v>
+        <v>-8.210000000000001</v>
       </c>
     </row>
     <row r="121">
@@ -2492,16 +2319,13 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>11.61</v>
+        <v>22.7</v>
       </c>
       <c r="C121" t="n">
-        <v>-1.58</v>
+        <v>-14.57</v>
       </c>
       <c r="D121" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E121" t="n">
-        <v>-45.085</v>
+        <v>-8.130000000000001</v>
       </c>
     </row>
     <row r="122">
@@ -2509,16 +2333,13 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>11.89</v>
+        <v>22.59</v>
       </c>
       <c r="C122" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-14.55</v>
       </c>
       <c r="D122" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E122" t="n">
-        <v>-46.88</v>
+        <v>-8.039999999999999</v>
       </c>
     </row>
     <row r="123">
@@ -2526,16 +2347,13 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>12.13</v>
+        <v>22.49</v>
       </c>
       <c r="C123" t="n">
-        <v>1.65</v>
+        <v>-14.53</v>
       </c>
       <c r="D123" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E123" t="n">
-        <v>-48.835</v>
+        <v>-7.94</v>
       </c>
     </row>
     <row r="124">
@@ -2543,16 +2361,13 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>11.57</v>
+        <v>22.34</v>
       </c>
       <c r="C124" t="n">
-        <v>3.37</v>
+        <v>-14.47</v>
       </c>
       <c r="D124" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E124" t="n">
-        <v>-50</v>
+        <v>-7.83</v>
       </c>
     </row>
     <row r="125">
@@ -2560,16 +2375,13 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>11.39</v>
+        <v>22.17</v>
       </c>
       <c r="C125" t="n">
-        <v>3.55</v>
+        <v>-14.41</v>
       </c>
       <c r="D125" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E125" t="n">
-        <v>-50</v>
+        <v>-7.72</v>
       </c>
     </row>
     <row r="126">
@@ -2577,16 +2389,13 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>11.01</v>
+        <v>22.05</v>
       </c>
       <c r="C126" t="n">
-        <v>3.93</v>
+        <v>-14.57</v>
       </c>
       <c r="D126" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E126" t="n">
-        <v>-50</v>
+        <v>-7.44</v>
       </c>
     </row>
     <row r="127">
@@ -2594,16 +2403,13 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>10.68</v>
+        <v>22.71</v>
       </c>
       <c r="C127" t="n">
-        <v>4.26</v>
+        <v>-15.45</v>
       </c>
       <c r="D127" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E127" t="n">
-        <v>-50</v>
+        <v>-7.22</v>
       </c>
     </row>
     <row r="128">
@@ -2611,16 +2417,13 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>10.42</v>
+        <v>23.32</v>
       </c>
       <c r="C128" t="n">
-        <v>4.52</v>
+        <v>-16.34</v>
       </c>
       <c r="D128" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E128" t="n">
-        <v>-50</v>
+        <v>-6.94</v>
       </c>
     </row>
     <row r="129">
@@ -2628,16 +2431,13 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>10.23</v>
+        <v>24.01</v>
       </c>
       <c r="C129" t="n">
-        <v>4.71</v>
+        <v>-17.31</v>
       </c>
       <c r="D129" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E129" t="n">
-        <v>-50</v>
+        <v>-6.66</v>
       </c>
     </row>
     <row r="130">
@@ -2645,16 +2445,13 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>10.34</v>
+        <v>24.69</v>
       </c>
       <c r="C130" t="n">
-        <v>4.6</v>
+        <v>-18.3</v>
       </c>
       <c r="D130" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E130" t="n">
-        <v>-50</v>
+        <v>-6.35</v>
       </c>
     </row>
     <row r="131">
@@ -2662,16 +2459,13 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>10.54</v>
+        <v>25.2</v>
       </c>
       <c r="C131" t="n">
-        <v>4.4</v>
+        <v>-19.13</v>
       </c>
       <c r="D131" t="n">
-        <v>31.46</v>
-      </c>
-      <c r="E131" t="n">
-        <v>-50</v>
+        <v>-6.03</v>
       </c>
     </row>
     <row r="132">
@@ -2679,16 +2473,13 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>10.75</v>
+        <v>26.1</v>
       </c>
       <c r="C132" t="n">
-        <v>4.19</v>
+        <v>-19.9</v>
       </c>
       <c r="D132" t="n">
-        <v>31.44</v>
-      </c>
-      <c r="E132" t="n">
-        <v>-50</v>
+        <v>-6.16</v>
       </c>
     </row>
     <row r="133">
@@ -2696,16 +2487,13 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>10.55</v>
+        <v>26.8</v>
       </c>
       <c r="C133" t="n">
-        <v>4.42</v>
+        <v>-21.38</v>
       </c>
       <c r="D133" t="n">
-        <v>31.39</v>
-      </c>
-      <c r="E133" t="n">
-        <v>-50</v>
+        <v>-5.4</v>
       </c>
     </row>
     <row r="134">
@@ -2713,16 +2501,13 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>10.33</v>
+        <v>27.34</v>
       </c>
       <c r="C134" t="n">
-        <v>4.59</v>
+        <v>-22.67</v>
       </c>
       <c r="D134" t="n">
-        <v>31.42</v>
-      </c>
-      <c r="E134" t="n">
-        <v>-50</v>
+        <v>-4.67</v>
       </c>
     </row>
     <row r="135">
@@ -2730,16 +2515,13 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>9.74</v>
+        <v>27.84</v>
       </c>
       <c r="C135" t="n">
-        <v>5.07</v>
+        <v>-23.99</v>
       </c>
       <c r="D135" t="n">
-        <v>31.51</v>
-      </c>
-      <c r="E135" t="n">
-        <v>-50</v>
+        <v>-3.85</v>
       </c>
     </row>
     <row r="136">
@@ -2747,16 +2529,13 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>9.529999999999999</v>
+        <v>27.49</v>
       </c>
       <c r="C136" t="n">
-        <v>5.25</v>
+        <v>-25.11</v>
       </c>
       <c r="D136" t="n">
-        <v>31.52</v>
-      </c>
-      <c r="E136" t="n">
-        <v>-50</v>
+        <v>-2.37</v>
       </c>
     </row>
     <row r="137">
@@ -2764,16 +2543,13 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>9.33</v>
+        <v>26.56</v>
       </c>
       <c r="C137" t="n">
-        <v>5.4</v>
+        <v>-25.71</v>
       </c>
       <c r="D137" t="n">
-        <v>31.6</v>
-      </c>
-      <c r="E137" t="n">
-        <v>-50</v>
+        <v>-0.86</v>
       </c>
     </row>
     <row r="138">
@@ -2781,16 +2557,13 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>9.130000000000001</v>
+        <v>25.93</v>
       </c>
       <c r="C138" t="n">
-        <v>5.56</v>
+        <v>-26.51</v>
       </c>
       <c r="D138" t="n">
-        <v>31.69</v>
-      </c>
-      <c r="E138" t="n">
-        <v>-50</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="139">
@@ -2798,16 +2571,13 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>8.83</v>
+        <v>25.28</v>
       </c>
       <c r="C139" t="n">
-        <v>5.79</v>
+        <v>-27.37</v>
       </c>
       <c r="D139" t="n">
-        <v>31.8</v>
-      </c>
-      <c r="E139" t="n">
-        <v>-50</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="140">
@@ -2815,16 +2585,13 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>8.529999999999999</v>
+        <v>24.64</v>
       </c>
       <c r="C140" t="n">
-        <v>5.9</v>
+        <v>-28.22</v>
       </c>
       <c r="D140" t="n">
-        <v>31.96999999999999</v>
-      </c>
-      <c r="E140" t="n">
-        <v>-50</v>
+        <v>3.58</v>
       </c>
     </row>
     <row r="141">
@@ -2832,16 +2599,13 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>8.27</v>
+        <v>24.05</v>
       </c>
       <c r="C141" t="n">
-        <v>5.97</v>
+        <v>-28.99</v>
       </c>
       <c r="D141" t="n">
-        <v>32.14</v>
-      </c>
-      <c r="E141" t="n">
-        <v>-50</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="142">
@@ -2849,16 +2613,13 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>8.140000000000001</v>
+        <v>22.93</v>
       </c>
       <c r="C142" t="n">
-        <v>5.99</v>
+        <v>-29.71</v>
       </c>
       <c r="D142" t="n">
-        <v>32.25</v>
-      </c>
-      <c r="E142" t="n">
-        <v>-50</v>
+        <v>6.77</v>
       </c>
     </row>
     <row r="143">
@@ -2866,16 +2627,13 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>8.539999999999999</v>
+        <v>22.02</v>
       </c>
       <c r="C143" t="n">
-        <v>5.43</v>
+        <v>-29.66</v>
       </c>
       <c r="D143" t="n">
-        <v>32.41</v>
-      </c>
-      <c r="E143" t="n">
-        <v>-50</v>
+        <v>7.65</v>
       </c>
     </row>
     <row r="144">
@@ -2883,16 +2641,13 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>9.029999999999999</v>
+        <v>21.39</v>
       </c>
       <c r="C144" t="n">
-        <v>4.92</v>
+        <v>-29.81</v>
       </c>
       <c r="D144" t="n">
-        <v>32.43</v>
-      </c>
-      <c r="E144" t="n">
-        <v>-50</v>
+        <v>8.42</v>
       </c>
     </row>
     <row r="145">
@@ -2900,16 +2655,13 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>9.56</v>
+        <v>20.92</v>
       </c>
       <c r="C145" t="n">
-        <v>4.15</v>
+        <v>-29.92</v>
       </c>
       <c r="D145" t="n">
-        <v>32.67</v>
-      </c>
-      <c r="E145" t="n">
-        <v>-50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="146">
@@ -2917,16 +2669,13 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>9.710000000000001</v>
+        <v>21.07</v>
       </c>
       <c r="C146" t="n">
-        <v>3.64</v>
+        <v>-30.02</v>
       </c>
       <c r="D146" t="n">
-        <v>33.03</v>
-      </c>
-      <c r="E146" t="n">
-        <v>-50</v>
+        <v>8.949999999999999</v>
       </c>
     </row>
     <row r="147">
@@ -2934,16 +2683,13 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>9.9</v>
+        <v>21.49</v>
       </c>
       <c r="C147" t="n">
-        <v>3.1</v>
+        <v>-30.22</v>
       </c>
       <c r="D147" t="n">
-        <v>33.32</v>
-      </c>
-      <c r="E147" t="n">
-        <v>-50</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="148">
@@ -2951,16 +2697,13 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>10.07</v>
+        <v>21.62</v>
       </c>
       <c r="C148" t="n">
-        <v>2.49</v>
+        <v>-30.4</v>
       </c>
       <c r="D148" t="n">
-        <v>33.7</v>
-      </c>
-      <c r="E148" t="n">
-        <v>-50</v>
+        <v>8.779999999999999</v>
       </c>
     </row>
     <row r="149">
@@ -2968,16 +2711,13 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>9.82</v>
+        <v>21.76</v>
       </c>
       <c r="C149" t="n">
-        <v>1.88</v>
+        <v>-30.49</v>
       </c>
       <c r="D149" t="n">
-        <v>34.49499999999999</v>
-      </c>
-      <c r="E149" t="n">
-        <v>-50</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="150">
@@ -2985,16 +2725,13 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>9.58</v>
+        <v>21.88</v>
       </c>
       <c r="C150" t="n">
-        <v>1.45</v>
+        <v>-30.57</v>
       </c>
       <c r="D150" t="n">
-        <v>35.16999999999999</v>
-      </c>
-      <c r="E150" t="n">
-        <v>-50</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="151">
@@ -3002,16 +2739,13 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>9.43</v>
+        <v>22.17</v>
       </c>
       <c r="C151" t="n">
-        <v>0.95</v>
+        <v>-30.68</v>
       </c>
       <c r="D151" t="n">
-        <v>35.825</v>
-      </c>
-      <c r="E151" t="n">
-        <v>-50</v>
+        <v>8.51</v>
       </c>
     </row>
     <row r="152">
@@ -3019,16 +2753,13 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>9.050000000000001</v>
+        <v>22.75</v>
       </c>
       <c r="C152" t="n">
-        <v>0.65</v>
+        <v>-30.85</v>
       </c>
       <c r="D152" t="n">
-        <v>36.49999999999999</v>
-      </c>
-      <c r="E152" t="n">
-        <v>-50</v>
+        <v>8.109999999999999</v>
       </c>
     </row>
     <row r="153">
@@ -3036,16 +2767,13 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>8.68</v>
+        <v>23.21</v>
       </c>
       <c r="C153" t="n">
-        <v>0.36</v>
+        <v>-31.09</v>
       </c>
       <c r="D153" t="n">
-        <v>37.15499999999999</v>
-      </c>
-      <c r="E153" t="n">
-        <v>-50</v>
+        <v>7.88</v>
       </c>
     </row>
     <row r="154">
@@ -3053,16 +2781,13 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>8.27</v>
+        <v>23.49</v>
       </c>
       <c r="C154" t="n">
-        <v>0.08</v>
+        <v>-30.17</v>
       </c>
       <c r="D154" t="n">
-        <v>37.84999999999999</v>
-      </c>
-      <c r="E154" t="n">
-        <v>-50</v>
+        <v>6.68</v>
       </c>
     </row>
     <row r="155">
@@ -3070,16 +2795,13 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>7.88</v>
+        <v>23.6</v>
       </c>
       <c r="C155" t="n">
-        <v>0.16</v>
+        <v>-29.24</v>
       </c>
       <c r="D155" t="n">
-        <v>38.165</v>
-      </c>
-      <c r="E155" t="n">
-        <v>-50</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="156">
@@ -3087,16 +2809,13 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>7.52</v>
+        <v>23.65</v>
       </c>
       <c r="C156" t="n">
-        <v>0.24</v>
+        <v>-28.3</v>
       </c>
       <c r="D156" t="n">
-        <v>38.44</v>
-      </c>
-      <c r="E156" t="n">
-        <v>-50</v>
+        <v>4.65</v>
       </c>
     </row>
     <row r="157">
@@ -3104,16 +2823,13 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>6.96</v>
+        <v>23.53</v>
       </c>
       <c r="C157" t="n">
-        <v>0.36</v>
+        <v>-27.38</v>
       </c>
       <c r="D157" t="n">
-        <v>38.87499999999999</v>
-      </c>
-      <c r="E157" t="n">
-        <v>-50</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="158">
@@ -3121,16 +2837,13 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>6.41</v>
+        <v>24.38</v>
       </c>
       <c r="C158" t="n">
-        <v>0.54</v>
+        <v>-27.16</v>
       </c>
       <c r="D158" t="n">
-        <v>39.25</v>
-      </c>
-      <c r="E158" t="n">
-        <v>-50</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="159">
@@ -3138,16 +2851,13 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>6.28</v>
+        <v>25.25</v>
       </c>
       <c r="C159" t="n">
-        <v>0.73</v>
+        <v>-26.96</v>
       </c>
       <c r="D159" t="n">
-        <v>39.19</v>
-      </c>
-      <c r="E159" t="n">
-        <v>-50</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="160">
@@ -3155,16 +2865,13 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>6.17</v>
+        <v>26.01</v>
       </c>
       <c r="C160" t="n">
-        <v>-0.14</v>
+        <v>-26.58</v>
       </c>
       <c r="D160" t="n">
-        <v>40.17</v>
-      </c>
-      <c r="E160" t="n">
-        <v>-50</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="161">
@@ -3172,16 +2879,13 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>5.95</v>
+        <v>26.58</v>
       </c>
       <c r="C161" t="n">
-        <v>-0.47</v>
+        <v>-26</v>
       </c>
       <c r="D161" t="n">
-        <v>40.71999999999999</v>
-      </c>
-      <c r="E161" t="n">
-        <v>-50</v>
+        <v>-0.58</v>
       </c>
     </row>
     <row r="162">
@@ -3189,16 +2893,13 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>5.73</v>
+        <v>26.74</v>
       </c>
       <c r="C162" t="n">
-        <v>-0.33</v>
+        <v>-25.4</v>
       </c>
       <c r="D162" t="n">
-        <v>40.79799999999999</v>
-      </c>
-      <c r="E162" t="n">
-        <v>-50</v>
+        <v>-1.34</v>
       </c>
     </row>
     <row r="163">
@@ -3206,16 +2907,13 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>5.56</v>
+        <v>27.12</v>
       </c>
       <c r="C163" t="n">
-        <v>-0.18</v>
+        <v>-24.91</v>
       </c>
       <c r="D163" t="n">
-        <v>40.816</v>
-      </c>
-      <c r="E163" t="n">
-        <v>-50</v>
+        <v>-2.21</v>
       </c>
     </row>
     <row r="164">
@@ -3223,16 +2921,13 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>5.95</v>
+        <v>27.48</v>
       </c>
       <c r="C164" t="n">
-        <v>-0.04</v>
+        <v>-25.47</v>
       </c>
       <c r="D164" t="n">
-        <v>40.294</v>
-      </c>
-      <c r="E164" t="n">
-        <v>-50</v>
+        <v>-2.01</v>
       </c>
     </row>
     <row r="165">
@@ -3240,16 +2935,13 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>6.36</v>
+        <v>27.89</v>
       </c>
       <c r="C165" t="n">
-        <v>-0.03</v>
+        <v>-26.02</v>
       </c>
       <c r="D165" t="n">
-        <v>39.87199999999999</v>
-      </c>
-      <c r="E165" t="n">
-        <v>-50</v>
+        <v>-1.87</v>
       </c>
     </row>
     <row r="166">
@@ -3257,16 +2949,13 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>6.73</v>
+        <v>28.48</v>
       </c>
       <c r="C166" t="n">
-        <v>-0.14</v>
+        <v>-26.63</v>
       </c>
       <c r="D166" t="n">
-        <v>39.60999999999999</v>
-      </c>
-      <c r="E166" t="n">
-        <v>-50</v>
+        <v>-1.85</v>
       </c>
     </row>
     <row r="167">
@@ -3274,16 +2963,13 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>6.78</v>
+        <v>29.05</v>
       </c>
       <c r="C167" t="n">
-        <v>-0.33</v>
+        <v>-27.23</v>
       </c>
       <c r="D167" t="n">
-        <v>39.74799999999999</v>
-      </c>
-      <c r="E167" t="n">
-        <v>-50</v>
+        <v>-1.82</v>
       </c>
     </row>
     <row r="168">
@@ -3291,16 +2977,13 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>6.86</v>
+        <v>28.96</v>
       </c>
       <c r="C168" t="n">
-        <v>-0.51</v>
+        <v>-27.12</v>
       </c>
       <c r="D168" t="n">
-        <v>39.84599999999999</v>
-      </c>
-      <c r="E168" t="n">
-        <v>-50</v>
+        <v>-1.84</v>
       </c>
     </row>
     <row r="169">
@@ -3308,16 +2991,13 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>6.83</v>
+        <v>28.86</v>
       </c>
       <c r="C169" t="n">
-        <v>-0.67</v>
+        <v>-27.02</v>
       </c>
       <c r="D169" t="n">
-        <v>40.044</v>
-      </c>
-      <c r="E169" t="n">
-        <v>-50</v>
+        <v>-1.84</v>
       </c>
     </row>
     <row r="170">
@@ -3325,16 +3005,13 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>6.38</v>
+        <v>28.89</v>
       </c>
       <c r="C170" t="n">
-        <v>0.57</v>
+        <v>-27.11</v>
       </c>
       <c r="D170" t="n">
-        <v>39.242</v>
-      </c>
-      <c r="E170" t="n">
-        <v>-50</v>
+        <v>-1.79</v>
       </c>
     </row>
     <row r="171">
@@ -3342,16 +3019,13 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>5.75</v>
+        <v>29.34</v>
       </c>
       <c r="C171" t="n">
-        <v>1.36</v>
+        <v>-27.44</v>
       </c>
       <c r="D171" t="n">
-        <v>39.09</v>
-      </c>
-      <c r="E171" t="n">
-        <v>-50</v>
+        <v>-1.9</v>
       </c>
     </row>
     <row r="172">
@@ -3359,16 +3033,13 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>5.23</v>
+        <v>29.95</v>
       </c>
       <c r="C172" t="n">
-        <v>1.56</v>
+        <v>-27.79</v>
       </c>
       <c r="D172" t="n">
-        <v>39.41</v>
-      </c>
-      <c r="E172" t="n">
-        <v>-50</v>
+        <v>-2.16</v>
       </c>
     </row>
     <row r="173">
@@ -3376,16 +3047,13 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>4.63</v>
+        <v>30.46</v>
       </c>
       <c r="C173" t="n">
-        <v>1.86</v>
+        <v>-28.05</v>
       </c>
       <c r="D173" t="n">
-        <v>39.70999999999999</v>
-      </c>
-      <c r="E173" t="n">
-        <v>-50</v>
+        <v>-2.44</v>
       </c>
     </row>
     <row r="174">
@@ -3393,16 +3061,13 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>3.44</v>
+        <v>31.04</v>
       </c>
       <c r="C174" t="n">
-        <v>2.2</v>
+        <v>-28.39</v>
       </c>
       <c r="D174" t="n">
-        <v>40.57</v>
-      </c>
-      <c r="E174" t="n">
-        <v>-50</v>
+        <v>-2.71</v>
       </c>
     </row>
     <row r="175">
@@ -3410,16 +3075,13 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>2.28</v>
+        <v>31.65</v>
       </c>
       <c r="C175" t="n">
-        <v>2.55</v>
+        <v>-28.73</v>
       </c>
       <c r="D175" t="n">
-        <v>41.37</v>
-      </c>
-      <c r="E175" t="n">
-        <v>-50</v>
+        <v>-3.01</v>
       </c>
     </row>
     <row r="176">
@@ -3427,832 +3089,13 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>1.12</v>
+        <v>32.14</v>
       </c>
       <c r="C176" t="n">
-        <v>3.03</v>
+        <v>-28.7</v>
       </c>
       <c r="D176" t="n">
-        <v>42.05</v>
-      </c>
-      <c r="E176" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" s="1" t="n">
-        <v>175</v>
-      </c>
-      <c r="B177" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="C177" t="n">
-        <v>3.58</v>
-      </c>
-      <c r="D177" t="n">
-        <v>42.499</v>
-      </c>
-      <c r="E177" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" s="1" t="n">
-        <v>176</v>
-      </c>
-      <c r="B178" t="n">
-        <v>-0.89</v>
-      </c>
-      <c r="C178" t="n">
-        <v>4.13</v>
-      </c>
-      <c r="D178" t="n">
-        <v>42.95799999999999</v>
-      </c>
-      <c r="E178" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" s="1" t="n">
-        <v>177</v>
-      </c>
-      <c r="B179" t="n">
-        <v>-1.77</v>
-      </c>
-      <c r="C179" t="n">
-        <v>4.67</v>
-      </c>
-      <c r="D179" t="n">
-        <v>43.297</v>
-      </c>
-      <c r="E179" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" s="1" t="n">
-        <v>178</v>
-      </c>
-      <c r="B180" t="n">
-        <v>-2.17</v>
-      </c>
-      <c r="C180" t="n">
-        <v>4.71</v>
-      </c>
-      <c r="D180" t="n">
-        <v>43.656</v>
-      </c>
-      <c r="E180" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" s="1" t="n">
-        <v>179</v>
-      </c>
-      <c r="B181" t="n">
-        <v>-2.38</v>
-      </c>
-      <c r="C181" t="n">
-        <v>4.74</v>
-      </c>
-      <c r="D181" t="n">
-        <v>43.84500000000001</v>
-      </c>
-      <c r="E181" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="B182" t="n">
-        <v>-2.66</v>
-      </c>
-      <c r="C182" t="n">
-        <v>4.83</v>
-      </c>
-      <c r="D182" t="n">
-        <v>44.03400000000001</v>
-      </c>
-      <c r="E182" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="1" t="n">
-        <v>181</v>
-      </c>
-      <c r="B183" t="n">
-        <v>-2.94</v>
-      </c>
-      <c r="C183" t="n">
-        <v>4.84</v>
-      </c>
-      <c r="D183" t="n">
-        <v>44.303</v>
-      </c>
-      <c r="E183" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" s="1" t="n">
-        <v>182</v>
-      </c>
-      <c r="B184" t="n">
-        <v>-2.87</v>
-      </c>
-      <c r="C184" t="n">
-        <v>4.83</v>
-      </c>
-      <c r="D184" t="n">
-        <v>44.23800000000001</v>
-      </c>
-      <c r="E184" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" s="1" t="n">
-        <v>183</v>
-      </c>
-      <c r="B185" t="n">
-        <v>-2.87</v>
-      </c>
-      <c r="C185" t="n">
-        <v>4.86</v>
-      </c>
-      <c r="D185" t="n">
-        <v>44.213</v>
-      </c>
-      <c r="E185" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" s="1" t="n">
-        <v>184</v>
-      </c>
-      <c r="B186" t="n">
-        <v>-2.92</v>
-      </c>
-      <c r="C186" t="n">
-        <v>4.85</v>
-      </c>
-      <c r="D186" t="n">
-        <v>44.26799999999999</v>
-      </c>
-      <c r="E186" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" s="1" t="n">
-        <v>185</v>
-      </c>
-      <c r="B187" t="n">
-        <v>-3.18</v>
-      </c>
-      <c r="C187" t="n">
-        <v>4.85</v>
-      </c>
-      <c r="D187" t="n">
-        <v>44.53399999999999</v>
-      </c>
-      <c r="E187" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" s="1" t="n">
-        <v>186</v>
-      </c>
-      <c r="B188" t="n">
-        <v>-3.25</v>
-      </c>
-      <c r="C188" t="n">
-        <v>4.68</v>
-      </c>
-      <c r="D188" t="n">
-        <v>44.77</v>
-      </c>
-      <c r="E188" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" s="1" t="n">
-        <v>187</v>
-      </c>
-      <c r="B189" t="n">
-        <v>-3.38</v>
-      </c>
-      <c r="C189" t="n">
-        <v>4.47</v>
-      </c>
-      <c r="D189" t="n">
-        <v>45.10600000000001</v>
-      </c>
-      <c r="E189" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" s="1" t="n">
-        <v>188</v>
-      </c>
-      <c r="B190" t="n">
-        <v>-3.39</v>
-      </c>
-      <c r="C190" t="n">
-        <v>4.22</v>
-      </c>
-      <c r="D190" t="n">
-        <v>45.377</v>
-      </c>
-      <c r="E190" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" s="1" t="n">
-        <v>189</v>
-      </c>
-      <c r="B191" t="n">
-        <v>-3.11</v>
-      </c>
-      <c r="C191" t="n">
-        <v>3.71</v>
-      </c>
-      <c r="D191" t="n">
-        <v>45.598</v>
-      </c>
-      <c r="E191" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" s="1" t="n">
-        <v>190</v>
-      </c>
-      <c r="B192" t="n">
-        <v>-2.89</v>
-      </c>
-      <c r="C192" t="n">
-        <v>3.21</v>
-      </c>
-      <c r="D192" t="n">
-        <v>45.879</v>
-      </c>
-      <c r="E192" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" s="1" t="n">
-        <v>191</v>
-      </c>
-      <c r="B193" t="n">
-        <v>-2.74</v>
-      </c>
-      <c r="C193" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D193" t="n">
-        <v>46.44</v>
-      </c>
-      <c r="E193" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" s="1" t="n">
-        <v>192</v>
-      </c>
-      <c r="B194" t="n">
-        <v>-2.91</v>
-      </c>
-      <c r="C194" t="n">
-        <v>1.79</v>
-      </c>
-      <c r="D194" t="n">
-        <v>47.315</v>
-      </c>
-      <c r="E194" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" s="1" t="n">
-        <v>193</v>
-      </c>
-      <c r="B195" t="n">
-        <v>-2.52</v>
-      </c>
-      <c r="C195" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="D195" t="n">
-        <v>48.20999999999999</v>
-      </c>
-      <c r="E195" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" s="1" t="n">
-        <v>194</v>
-      </c>
-      <c r="B196" t="n">
-        <v>-2.1</v>
-      </c>
-      <c r="C196" t="n">
-        <v>-0.51</v>
-      </c>
-      <c r="D196" t="n">
-        <v>48.808</v>
-      </c>
-      <c r="E196" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" s="1" t="n">
-        <v>195</v>
-      </c>
-      <c r="B197" t="n">
-        <v>-1.13</v>
-      </c>
-      <c r="C197" t="n">
-        <v>-1.98</v>
-      </c>
-      <c r="D197" t="n">
-        <v>49.316</v>
-      </c>
-      <c r="E197" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" s="1" t="n">
-        <v>196</v>
-      </c>
-      <c r="B198" t="n">
-        <v>-0.22</v>
-      </c>
-      <c r="C198" t="n">
-        <v>-3.36</v>
-      </c>
-      <c r="D198" t="n">
-        <v>49.78400000000001</v>
-      </c>
-      <c r="E198" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" s="1" t="n">
-        <v>197</v>
-      </c>
-      <c r="B199" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="C199" t="n">
-        <v>-4.69</v>
-      </c>
-      <c r="D199" t="n">
-        <v>50.712</v>
-      </c>
-      <c r="E199" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" s="1" t="n">
-        <v>198</v>
-      </c>
-      <c r="B200" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="C200" t="n">
-        <v>-5.95</v>
-      </c>
-      <c r="D200" t="n">
-        <v>51.725</v>
-      </c>
-      <c r="E200" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" s="1" t="n">
-        <v>199</v>
-      </c>
-      <c r="B201" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="C201" t="n">
-        <v>-6.94</v>
-      </c>
-      <c r="D201" t="n">
-        <v>52.818</v>
-      </c>
-      <c r="E201" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="B202" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="C202" t="n">
-        <v>-7.99</v>
-      </c>
-      <c r="D202" t="n">
-        <v>53.461</v>
-      </c>
-      <c r="E202" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="B203" t="n">
-        <v>0.97</v>
-      </c>
-      <c r="C203" t="n">
-        <v>-8.869999999999999</v>
-      </c>
-      <c r="D203" t="n">
-        <v>54.104</v>
-      </c>
-      <c r="E203" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" s="1" t="n">
-        <v>202</v>
-      </c>
-      <c r="B204" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="C204" t="n">
-        <v>-9.619999999999999</v>
-      </c>
-      <c r="D204" t="n">
-        <v>54.617</v>
-      </c>
-      <c r="E204" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" s="1" t="n">
-        <v>203</v>
-      </c>
-      <c r="B205" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="C205" t="n">
-        <v>-9.84</v>
-      </c>
-      <c r="D205" t="n">
-        <v>55.11999999999999</v>
-      </c>
-      <c r="E205" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" s="1" t="n">
-        <v>204</v>
-      </c>
-      <c r="B206" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C206" t="n">
-        <v>-10.2</v>
-      </c>
-      <c r="D206" t="n">
-        <v>55.8</v>
-      </c>
-      <c r="E206" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" s="1" t="n">
-        <v>205</v>
-      </c>
-      <c r="B207" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="C207" t="n">
-        <v>-10.11</v>
-      </c>
-      <c r="D207" t="n">
-        <v>56.04000000000001</v>
-      </c>
-      <c r="E207" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" s="1" t="n">
-        <v>206</v>
-      </c>
-      <c r="B208" t="n">
-        <v>-0.61</v>
-      </c>
-      <c r="C208" t="n">
-        <v>-9.960000000000001</v>
-      </c>
-      <c r="D208" t="n">
-        <v>56.77</v>
-      </c>
-      <c r="E208" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" s="1" t="n">
-        <v>207</v>
-      </c>
-      <c r="B209" t="n">
-        <v>-0.65</v>
-      </c>
-      <c r="C209" t="n">
-        <v>-9.869999999999999</v>
-      </c>
-      <c r="D209" t="n">
-        <v>56.72000000000001</v>
-      </c>
-      <c r="E209" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" s="1" t="n">
-        <v>208</v>
-      </c>
-      <c r="B210" t="n">
-        <v>-0.68</v>
-      </c>
-      <c r="C210" t="n">
-        <v>-9.75</v>
-      </c>
-      <c r="D210" t="n">
-        <v>56.63000000000001</v>
-      </c>
-      <c r="E210" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" s="1" t="n">
-        <v>209</v>
-      </c>
-      <c r="B211" t="n">
-        <v>-0.65</v>
-      </c>
-      <c r="C211" t="n">
-        <v>-9.81</v>
-      </c>
-      <c r="D211" t="n">
-        <v>56.66</v>
-      </c>
-      <c r="E211" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" s="1" t="n">
-        <v>210</v>
-      </c>
-      <c r="B212" t="n">
-        <v>-1.09</v>
-      </c>
-      <c r="C212" t="n">
-        <v>-9.789999999999999</v>
-      </c>
-      <c r="D212" t="n">
-        <v>57.08</v>
-      </c>
-      <c r="E212" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" s="1" t="n">
-        <v>211</v>
-      </c>
-      <c r="B213" t="n">
-        <v>-1.36</v>
-      </c>
-      <c r="C213" t="n">
-        <v>-9.640000000000001</v>
-      </c>
-      <c r="D213" t="n">
-        <v>57.2</v>
-      </c>
-      <c r="E213" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" s="1" t="n">
-        <v>212</v>
-      </c>
-      <c r="B214" t="n">
-        <v>-0.85</v>
-      </c>
-      <c r="C214" t="n">
-        <v>-9.83</v>
-      </c>
-      <c r="D214" t="n">
-        <v>56.88499999999999</v>
-      </c>
-      <c r="E214" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" s="1" t="n">
-        <v>213</v>
-      </c>
-      <c r="B215" t="n">
-        <v>-0.4</v>
-      </c>
-      <c r="C215" t="n">
-        <v>-9.98</v>
-      </c>
-      <c r="D215" t="n">
-        <v>56.58</v>
-      </c>
-      <c r="E215" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" s="1" t="n">
-        <v>214</v>
-      </c>
-      <c r="B216" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C216" t="n">
-        <v>-10.27</v>
-      </c>
-      <c r="D216" t="n">
-        <v>56.255</v>
-      </c>
-      <c r="E216" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" s="1" t="n">
-        <v>215</v>
-      </c>
-      <c r="B217" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="C217" t="n">
-        <v>-10.62</v>
-      </c>
-      <c r="D217" t="n">
-        <v>55.98</v>
-      </c>
-      <c r="E217" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" s="1" t="n">
-        <v>216</v>
-      </c>
-      <c r="B218" t="n">
-        <v>2.02</v>
-      </c>
-      <c r="C218" t="n">
-        <v>-11.02</v>
-      </c>
-      <c r="D218" t="n">
-        <v>55.205</v>
-      </c>
-      <c r="E218" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" s="1" t="n">
-        <v>217</v>
-      </c>
-      <c r="B219" t="n">
-        <v>2.91</v>
-      </c>
-      <c r="C219" t="n">
-        <v>-11.36</v>
-      </c>
-      <c r="D219" t="n">
-        <v>54.65</v>
-      </c>
-      <c r="E219" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" s="1" t="n">
-        <v>218</v>
-      </c>
-      <c r="B220" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="C220" t="n">
-        <v>-11.64</v>
-      </c>
-      <c r="D220" t="n">
-        <v>54.09500000000001</v>
-      </c>
-      <c r="E220" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" s="1" t="n">
-        <v>219</v>
-      </c>
-      <c r="B221" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="C221" t="n">
-        <v>-11.76</v>
-      </c>
-      <c r="D221" t="n">
-        <v>53.56</v>
-      </c>
-      <c r="E221" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" s="1" t="n">
-        <v>220</v>
-      </c>
-      <c r="B222" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="C222" t="n">
-        <v>-12.21</v>
-      </c>
-      <c r="D222" t="n">
-        <v>53.425</v>
-      </c>
-      <c r="E222" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" s="1" t="n">
-        <v>221</v>
-      </c>
-      <c r="B223" t="n">
-        <v>5.6</v>
-      </c>
-      <c r="C223" t="n">
-        <v>-12.59</v>
-      </c>
-      <c r="D223" t="n">
-        <v>53.19</v>
-      </c>
-      <c r="E223" t="n">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" s="1" t="n">
-        <v>222</v>
-      </c>
-      <c r="B224" t="n">
-        <v>5.26</v>
-      </c>
-      <c r="C224" t="n">
-        <v>-12.61</v>
-      </c>
-      <c r="D224" t="n">
-        <v>53.54</v>
-      </c>
-      <c r="E224" t="n">
-        <v>-50</v>
+        <v>-3.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>